<commit_message>
Update automatico via Actualizar 06-07-2020 06-02-41
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1010" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7F343318-F019-E443-ABAE-1A7B7A63E314}"/>
+  <xr:revisionPtr revIDLastSave="1016" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F2759F86-4B9D-A245-BDE3-34E445021628}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
   <si>
     <t>Columna1</t>
   </si>
@@ -1006,7 +1006,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CJ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CL18" sqref="CL18"/>
+      <selection pane="topRight" activeCell="CL7" sqref="CL7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1708,7 +1708,9 @@
       <c r="CK2" s="8">
         <v>74231</v>
       </c>
-      <c r="CL2" s="8"/>
+      <c r="CL2" s="8">
+        <v>76003</v>
+      </c>
       <c r="CM2" s="8"/>
       <c r="CN2" s="8"/>
       <c r="CO2" s="8"/>
@@ -1981,7 +1983,9 @@
       <c r="CK3" s="8">
         <v>56277</v>
       </c>
-      <c r="CL3" s="8"/>
+      <c r="CL3" s="8">
+        <v>57480</v>
+      </c>
       <c r="CM3" s="8"/>
       <c r="CN3" s="8"/>
       <c r="CO3" s="8"/>
@@ -2236,7 +2240,9 @@
       <c r="CK4" s="8">
         <v>4357</v>
       </c>
-      <c r="CL4" s="8"/>
+      <c r="CL4" s="8">
+        <v>4472</v>
+      </c>
       <c r="CM4" s="8"/>
       <c r="CN4" s="8"/>
       <c r="CO4" s="8"/>
@@ -2418,7 +2424,9 @@
       <c r="CK5" s="8">
         <v>607</v>
       </c>
-      <c r="CL5" s="8"/>
+      <c r="CL5" s="8">
+        <v>623</v>
+      </c>
       <c r="CM5" s="8"/>
       <c r="CN5" s="8"/>
       <c r="CO5" s="8"/>
@@ -2683,7 +2691,9 @@
       <c r="CK6" s="8">
         <v>333</v>
       </c>
-      <c r="CL6" s="8"/>
+      <c r="CL6" s="8">
+        <v>323</v>
+      </c>
       <c r="CM6" s="8"/>
       <c r="CN6" s="8"/>
       <c r="CO6" s="8"/>
@@ -2950,7 +2960,9 @@
       <c r="CK7" s="8">
         <v>77</v>
       </c>
-      <c r="CL7" s="8"/>
+      <c r="CL7" s="8">
+        <v>82</v>
+      </c>
       <c r="CM7" s="8"/>
       <c r="CN7" s="8"/>
       <c r="CO7" s="8"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-08-2020 05-06-18
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1016" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F2759F86-4B9D-A245-BDE3-34E445021628}"/>
+  <xr:revisionPtr revIDLastSave="1022" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0796ED57-81B0-434C-ACF2-84C8322FEBA0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -1005,8 +1005,8 @@
   <dimension ref="A1:EK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CJ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CL7" sqref="CL7"/>
+      <pane xSplit="1" topLeftCell="CK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CN2" sqref="CN2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1711,7 +1711,9 @@
       <c r="CL2" s="8">
         <v>76003</v>
       </c>
-      <c r="CM2" s="8"/>
+      <c r="CM2" s="8">
+        <v>77592</v>
+      </c>
       <c r="CN2" s="8"/>
       <c r="CO2" s="8"/>
     </row>
@@ -1986,7 +1988,9 @@
       <c r="CL3" s="8">
         <v>57480</v>
       </c>
-      <c r="CM3" s="8"/>
+      <c r="CM3" s="8">
+        <v>58632</v>
+      </c>
       <c r="CN3" s="8"/>
       <c r="CO3" s="8"/>
     </row>
@@ -2243,7 +2247,9 @@
       <c r="CL4" s="8">
         <v>4472</v>
       </c>
-      <c r="CM4" s="8"/>
+      <c r="CM4" s="8">
+        <v>4726</v>
+      </c>
       <c r="CN4" s="8"/>
       <c r="CO4" s="8"/>
     </row>
@@ -2427,7 +2433,9 @@
       <c r="CL5" s="8">
         <v>623</v>
       </c>
-      <c r="CM5" s="8"/>
+      <c r="CM5" s="8">
+        <v>667</v>
+      </c>
       <c r="CN5" s="8"/>
       <c r="CO5" s="8"/>
     </row>
@@ -2694,7 +2702,9 @@
       <c r="CL6" s="8">
         <v>323</v>
       </c>
-      <c r="CM6" s="8"/>
+      <c r="CM6" s="8">
+        <v>337</v>
+      </c>
       <c r="CN6" s="8"/>
       <c r="CO6" s="8"/>
     </row>
@@ -2963,7 +2973,9 @@
       <c r="CL7" s="8">
         <v>82</v>
       </c>
-      <c r="CM7" s="8"/>
+      <c r="CM7" s="8">
+        <v>84</v>
+      </c>
       <c r="CN7" s="8"/>
       <c r="CO7" s="8"/>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-09-2020 01-17-53
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1022" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0796ED57-81B0-434C-ACF2-84C8322FEBA0}"/>
+  <xr:revisionPtr revIDLastSave="1028" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{987B14FC-0682-5543-BA80-D07E35CDA5D7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -1005,8 +1005,8 @@
   <dimension ref="A1:EK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CN2" sqref="CN2"/>
+      <pane xSplit="1" topLeftCell="CM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CN7" sqref="CN7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1714,7 +1714,9 @@
       <c r="CM2" s="8">
         <v>77592</v>
       </c>
-      <c r="CN2" s="8"/>
+      <c r="CN2" s="8">
+        <v>79268</v>
+      </c>
       <c r="CO2" s="8"/>
     </row>
     <row r="3" spans="1:141" x14ac:dyDescent="0.2">
@@ -1991,7 +1993,9 @@
       <c r="CM3" s="8">
         <v>58632</v>
       </c>
-      <c r="CN3" s="8"/>
+      <c r="CN3" s="8">
+        <v>59859</v>
+      </c>
       <c r="CO3" s="8"/>
     </row>
     <row r="4" spans="1:141" x14ac:dyDescent="0.2">
@@ -2250,7 +2254,9 @@
       <c r="CM4" s="8">
         <v>4726</v>
       </c>
-      <c r="CN4" s="8"/>
+      <c r="CN4" s="8">
+        <v>4942</v>
+      </c>
       <c r="CO4" s="8"/>
     </row>
     <row r="5" spans="1:141" x14ac:dyDescent="0.2">
@@ -2436,7 +2442,9 @@
       <c r="CM5" s="8">
         <v>667</v>
       </c>
-      <c r="CN5" s="8"/>
+      <c r="CN5" s="8">
+        <v>686</v>
+      </c>
       <c r="CO5" s="8"/>
     </row>
     <row r="6" spans="1:141" x14ac:dyDescent="0.2">
@@ -2705,7 +2713,9 @@
       <c r="CM6" s="8">
         <v>337</v>
       </c>
-      <c r="CN6" s="8"/>
+      <c r="CN6" s="8">
+        <v>340</v>
+      </c>
       <c r="CO6" s="8"/>
     </row>
     <row r="7" spans="1:141" x14ac:dyDescent="0.2">
@@ -2976,7 +2986,9 @@
       <c r="CM7" s="8">
         <v>84</v>
       </c>
-      <c r="CN7" s="8"/>
+      <c r="CN7" s="8">
+        <v>87</v>
+      </c>
       <c r="CO7" s="8"/>
     </row>
     <row r="8" spans="1:141" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-10-2020 20-47-39
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23007"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1051" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A7AFE3DE-BD4A-4B9B-9515-3E7215204ADE}"/>
+  <xr:revisionPtr revIDLastSave="1072" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9ED60AE3-547F-497E-BC1A-862D186498A5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -308,15 +308,12 @@
     <t>07-06-2020</t>
   </si>
   <si>
-    <t>08-06-20202</t>
-  </si>
-  <si>
-    <t>08-06-2020</t>
-  </si>
-  <si>
     <t>09-06-20203</t>
   </si>
   <si>
+    <t>10-06-202032</t>
+  </si>
+  <si>
     <t>10/6/2020</t>
   </si>
   <si>
@@ -396,6 +393,9 @@
   </si>
   <si>
     <t>Hospitalizados en UCI</t>
+  </si>
+  <si>
+    <t>8/6/2020</t>
   </si>
 </sst>
 </file>
@@ -403,9 +403,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,7 +459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,9 +572,9 @@
     <tableColumn id="2" xr3:uid="{31600888-D874-4B90-9270-CF9219D7F135}" name="05-06-20202"/>
     <tableColumn id="3" xr3:uid="{6415ECB6-E037-4BC3-9907-91C4C505CF37}" name="06-06-2020"/>
     <tableColumn id="4" xr3:uid="{2FE879E2-2128-42AE-A0E3-647EE2D0C94F}" name="07-06-2020"/>
-    <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="08-06-20202"/>
-    <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="08-06-2020"/>
-    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="09-06-20203"/>
+    <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="8/6/2020"/>
+    <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-20203"/>
+    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-202032"/>
     <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="10/6/2020"/>
     <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="11/6/2020"/>
     <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="12/6/2020"/>
@@ -602,7 +602,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -901,17 +901,17 @@
   <dimension ref="A1:DK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CL1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CP2" sqref="CP2"/>
+      <pane xSplit="1" topLeftCell="CD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CN2" sqref="CN2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="87" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
+    <col min="2" max="87" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:115">
+    <row r="1" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1186,81 +1186,81 @@
         <v>90</v>
       </c>
       <c r="CN1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="CO1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" s="1" t="s">
+      <c r="CP1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="CQ1" s="1" t="s">
+      <c r="CR1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" s="1" t="s">
+      <c r="CS1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" s="1" t="s">
+      <c r="CT1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="CT1" s="1" t="s">
+      <c r="CU1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" s="1" t="s">
+      <c r="CV1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="CW1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="CX1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="CY1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="DC1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="DC1" s="1" t="s">
+      <c r="DD1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="DE1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="DE1" s="1" t="s">
+      <c r="DF1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="DF1" s="1" t="s">
+      <c r="DG1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="DG1" s="1" t="s">
+      <c r="DH1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="DH1" s="1" t="s">
+      <c r="DI1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="DK1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:115" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:115">
-      <c r="A2" t="s">
-        <v>115</v>
       </c>
       <c r="B2" s="7">
         <v>146</v>
@@ -1539,9 +1539,9 @@
         <v>80720</v>
       </c>
     </row>
-    <row r="3" spans="1:115">
+    <row r="3" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="7">
         <v>138</v>
@@ -1820,16 +1820,22 @@
         <v>60899</v>
       </c>
     </row>
-    <row r="4" spans="1:115">
+    <row r="4" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+        <v>116</v>
+      </c>
+      <c r="B4" s="7">
+        <v>6</v>
+      </c>
+      <c r="C4" s="7">
+        <v>9</v>
+      </c>
       <c r="D4" s="7">
         <v>21</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="7">
+        <v>30</v>
+      </c>
       <c r="F4" s="7">
         <v>37</v>
       </c>
@@ -1854,7 +1860,9 @@
       <c r="M4" s="7">
         <v>209</v>
       </c>
-      <c r="N4" s="7"/>
+      <c r="N4" s="7">
+        <v>271</v>
+      </c>
       <c r="O4" s="7">
         <v>289</v>
       </c>
@@ -1870,7 +1878,9 @@
       <c r="S4" s="7">
         <v>662</v>
       </c>
-      <c r="T4" s="7"/>
+      <c r="T4" s="7">
+        <v>753</v>
+      </c>
       <c r="U4" s="7">
         <v>820</v>
       </c>
@@ -1904,7 +1914,9 @@
       <c r="AE4" s="7">
         <v>2154</v>
       </c>
-      <c r="AF4" s="7"/>
+      <c r="AF4" s="7">
+        <v>2367</v>
+      </c>
       <c r="AG4" s="7">
         <v>2579</v>
       </c>
@@ -1914,7 +1926,9 @@
       <c r="AI4" s="7">
         <v>2955</v>
       </c>
-      <c r="AJ4" s="7"/>
+      <c r="AJ4" s="7">
+        <v>2983</v>
+      </c>
       <c r="AK4" s="7">
         <v>3101</v>
       </c>
@@ -1930,8 +1944,12 @@
       <c r="AO4" s="7">
         <v>3664</v>
       </c>
-      <c r="AP4" s="7"/>
-      <c r="AQ4" s="7"/>
+      <c r="AP4" s="7">
+        <v>2010</v>
+      </c>
+      <c r="AQ4" s="7">
+        <v>2133</v>
+      </c>
       <c r="AR4" s="7">
         <v>4094</v>
       </c>
@@ -2083,9 +2101,9 @@
         <v>5122</v>
       </c>
     </row>
-    <row r="5" spans="1:115">
+    <row r="5" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2269,11 +2287,13 @@
       <c r="CN5" s="8">
         <v>686</v>
       </c>
-      <c r="CO5" s="8"/>
-    </row>
-    <row r="6" spans="1:115">
+      <c r="CO5" s="8">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="6" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -2325,7 +2345,9 @@
       <c r="S6" s="7">
         <v>108</v>
       </c>
-      <c r="T6" s="7"/>
+      <c r="T6" s="7">
+        <v>95</v>
+      </c>
       <c r="U6" s="7">
         <v>105</v>
       </c>
@@ -2347,7 +2369,9 @@
       <c r="AA6" s="7">
         <v>154</v>
       </c>
-      <c r="AB6" s="7"/>
+      <c r="AB6" s="7">
+        <v>163</v>
+      </c>
       <c r="AC6" s="7">
         <v>167</v>
       </c>
@@ -2540,13 +2564,17 @@
       <c r="CN6" s="8">
         <v>340</v>
       </c>
-      <c r="CO6" s="8"/>
-    </row>
-    <row r="7" spans="1:115">
+      <c r="CO6" s="8">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="7" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B7" s="7"/>
+        <v>119</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
       <c r="C7" s="7">
         <v>2</v>
       </c>
@@ -2596,7 +2624,9 @@
       <c r="S7" s="7">
         <v>28</v>
       </c>
-      <c r="T7" s="7"/>
+      <c r="T7" s="7">
+        <v>36</v>
+      </c>
       <c r="U7" s="7">
         <v>36</v>
       </c>
@@ -2813,9 +2843,11 @@
       <c r="CN7" s="8">
         <v>87</v>
       </c>
-      <c r="CO7" s="8"/>
-    </row>
-    <row r="8" spans="1:115">
+      <c r="CO7" s="8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2909,46 +2941,46 @@
       <c r="CN8" s="8"/>
       <c r="CO8" s="8"/>
     </row>
-    <row r="9" spans="1:115">
+    <row r="9" spans="1:115" x14ac:dyDescent="0.3">
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:115">
+    <row r="10" spans="1:115" x14ac:dyDescent="0.3">
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:115">
+    <row r="11" spans="1:115" x14ac:dyDescent="0.3">
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:115">
+    <row r="12" spans="1:115" x14ac:dyDescent="0.3">
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:115">
+    <row r="13" spans="1:115" x14ac:dyDescent="0.3">
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:115">
+    <row r="14" spans="1:115" x14ac:dyDescent="0.3">
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:115">
+    <row r="15" spans="1:115" x14ac:dyDescent="0.3">
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:115">
+    <row r="16" spans="1:115" x14ac:dyDescent="0.3">
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W17" s="3"/>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W18" s="3"/>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W19" s="3"/>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W20" s="3"/>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W21" s="3"/>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2971,52 +3003,52 @@
       <c r="T22" s="2"/>
       <c r="W22" s="3"/>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W23" s="3"/>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W24" s="3"/>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W25" s="4"/>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W26" s="4"/>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W27" s="4"/>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W28" s="4"/>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W29" s="4"/>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W30" s="4"/>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W31" s="4"/>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W32" s="4"/>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W33" s="4"/>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W34" s="4"/>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W35" s="1"/>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W36" s="1"/>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W37" s="1"/>
     </row>
-    <row r="38" spans="1:23">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -3039,7 +3071,7 @@
       <c r="T38" s="2"/>
       <c r="W38" s="1"/>
     </row>
-    <row r="39" spans="1:23">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -3062,7 +3094,7 @@
       <c r="T39" s="2"/>
       <c r="W39" s="1"/>
     </row>
-    <row r="40" spans="1:23">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -3085,7 +3117,7 @@
       <c r="T40" s="2"/>
       <c r="W40" s="1"/>
     </row>
-    <row r="41" spans="1:23">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -3108,7 +3140,7 @@
       <c r="T41" s="2"/>
       <c r="W41" s="1"/>
     </row>
-    <row r="42" spans="1:23">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -3131,7 +3163,7 @@
       <c r="T42" s="2"/>
       <c r="W42" s="1"/>
     </row>
-    <row r="43" spans="1:23">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -3154,7 +3186,7 @@
       <c r="T43" s="2"/>
       <c r="W43" s="1"/>
     </row>
-    <row r="44" spans="1:23">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -3177,7 +3209,7 @@
       <c r="T44" s="2"/>
       <c r="W44" s="1"/>
     </row>
-    <row r="45" spans="1:23">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -3200,7 +3232,7 @@
       <c r="T45" s="2"/>
       <c r="W45" s="1"/>
     </row>
-    <row r="46" spans="1:23">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -3223,7 +3255,7 @@
       <c r="T46" s="2"/>
       <c r="W46" s="1"/>
     </row>
-    <row r="47" spans="1:23">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -3246,7 +3278,7 @@
       <c r="T47" s="2"/>
       <c r="W47" s="3"/>
     </row>
-    <row r="48" spans="1:23">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -3269,7 +3301,7 @@
       <c r="T48" s="2"/>
       <c r="W48" s="3"/>
     </row>
-    <row r="49" spans="1:23">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -3292,7 +3324,7 @@
       <c r="T49" s="2"/>
       <c r="W49" s="3"/>
     </row>
-    <row r="50" spans="1:23">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -3315,7 +3347,7 @@
       <c r="T50" s="2"/>
       <c r="W50" s="3"/>
     </row>
-    <row r="51" spans="1:23">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -3338,7 +3370,7 @@
       <c r="T51" s="2"/>
       <c r="W51" s="3"/>
     </row>
-    <row r="52" spans="1:23">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="W52" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-11-2020 01-32-51
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1072" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9ED60AE3-547F-497E-BC1A-862D186498A5}"/>
+  <xr:revisionPtr revIDLastSave="1099" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B1EDAA3A-69C7-FC46-BCB1-85E30F2067CC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
+    <workbookView xWindow="2376" yWindow="0" windowWidth="14028" windowHeight="9216" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -296,31 +296,28 @@
     <t>03-06-2020</t>
   </si>
   <si>
-    <t>04-06-2020</t>
-  </si>
-  <si>
-    <t>05-06-20202</t>
-  </si>
-  <si>
     <t>06-06-2020</t>
   </si>
   <si>
     <t>07-06-2020</t>
   </si>
   <si>
-    <t>09-06-20203</t>
-  </si>
-  <si>
-    <t>10-06-202032</t>
-  </si>
-  <si>
-    <t>10/6/2020</t>
-  </si>
-  <si>
-    <t>11/6/2020</t>
-  </si>
-  <si>
-    <t>12/6/2020</t>
+    <t>Pruebas Realizadas</t>
+  </si>
+  <si>
+    <t>Pruebas Negativas</t>
+  </si>
+  <si>
+    <t>Aislamiento Domiciliario</t>
+  </si>
+  <si>
+    <t>Aislamiento en Hoteles</t>
+  </si>
+  <si>
+    <t>Hospitalizados en Sala</t>
+  </si>
+  <si>
+    <t>Hospitalizados en UCI</t>
   </si>
   <si>
     <t>13/6/2020</t>
@@ -377,25 +374,28 @@
     <t>30/6/2020</t>
   </si>
   <si>
-    <t>Pruebas Realizadas</t>
-  </si>
-  <si>
-    <t>Pruebas Negativas</t>
-  </si>
-  <si>
-    <t>Aislamiento Domiciliario</t>
-  </si>
-  <si>
-    <t>Aislamiento en Hoteles</t>
-  </si>
-  <si>
-    <t>Hospitalizados en Sala</t>
-  </si>
-  <si>
-    <t>Hospitalizados en UCI</t>
-  </si>
-  <si>
-    <t>8/6/2020</t>
+    <t>08-06-20</t>
+  </si>
+  <si>
+    <t>05-06-20</t>
+  </si>
+  <si>
+    <t>09-06-20</t>
+  </si>
+  <si>
+    <t>10-06-20</t>
+  </si>
+  <si>
+    <t>11-06-20</t>
+  </si>
+  <si>
+    <t>12-06-20</t>
+  </si>
+  <si>
+    <t>13-06-20</t>
+  </si>
+  <si>
+    <t>04-06-20</t>
   </si>
 </sst>
 </file>
@@ -568,16 +568,16 @@
     <tableColumn id="74" xr3:uid="{828D9632-D098-418C-8A67-CA98651BA254}" name="01-06-2020"/>
     <tableColumn id="75" xr3:uid="{2918382E-DC05-40AA-9D38-7D65EC299862}" name="02-06-2020"/>
     <tableColumn id="96" xr3:uid="{E4AB1F9C-8FD7-4413-867C-24D7D313240D}" name="03-06-2020"/>
-    <tableColumn id="1" xr3:uid="{0ED54AB8-E3B7-4C5E-A3D9-DC4FC5A90852}" name="04-06-2020"/>
-    <tableColumn id="2" xr3:uid="{31600888-D874-4B90-9270-CF9219D7F135}" name="05-06-20202"/>
+    <tableColumn id="1" xr3:uid="{0ED54AB8-E3B7-4C5E-A3D9-DC4FC5A90852}" name="04-06-20"/>
+    <tableColumn id="2" xr3:uid="{31600888-D874-4B90-9270-CF9219D7F135}" name="05-06-20"/>
     <tableColumn id="3" xr3:uid="{6415ECB6-E037-4BC3-9907-91C4C505CF37}" name="06-06-2020"/>
     <tableColumn id="4" xr3:uid="{2FE879E2-2128-42AE-A0E3-647EE2D0C94F}" name="07-06-2020"/>
-    <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="8/6/2020"/>
-    <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-20203"/>
-    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-202032"/>
-    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="10/6/2020"/>
-    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="11/6/2020"/>
-    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="12/6/2020"/>
+    <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="08-06-20"/>
+    <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-20"/>
+    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-20"/>
+    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-20"/>
+    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-20"/>
+    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20"/>
     <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="13/6/2020"/>
     <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="14/6/2020"/>
     <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="15/6/2020"/>
@@ -901,8 +901,8 @@
   <dimension ref="A1:DK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CN2" sqref="CN2"/>
+      <pane xSplit="1" topLeftCell="CN1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CN1" sqref="CN1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1174,93 +1174,93 @@
         <v>86</v>
       </c>
       <c r="CJ1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="CL1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CM1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="CM1" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="CN1" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="CO1" s="1" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="CP1" s="1" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="CQ1" s="1" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="CS1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="CT1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="CT1" s="1" t="s">
+      <c r="CU1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="CU1" s="1" t="s">
+      <c r="CV1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="CW1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="CX1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="CY1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="DC1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="DC1" s="1" t="s">
+      <c r="DD1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="DE1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="DE1" s="1" t="s">
+      <c r="DF1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="DF1" s="1" t="s">
+      <c r="DG1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="DG1" s="1" t="s">
+      <c r="DH1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="DH1" s="1" t="s">
+      <c r="DI1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="B2" s="7">
         <v>146</v>
@@ -1538,10 +1538,13 @@
       <c r="CO2" s="8">
         <v>80720</v>
       </c>
+      <c r="CP2">
+        <v>82774</v>
+      </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="B3" s="7">
         <v>138</v>
@@ -1819,10 +1822,13 @@
       <c r="CO3" s="8">
         <v>60899</v>
       </c>
+      <c r="CP3">
+        <v>62284</v>
+      </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="B4" s="7">
         <v>6</v>
@@ -2100,10 +2106,13 @@
       <c r="CO4" s="8">
         <v>5122</v>
       </c>
+      <c r="CP4">
+        <v>5315</v>
+      </c>
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2290,10 +2299,13 @@
       <c r="CO5" s="8">
         <v>692</v>
       </c>
+      <c r="CP5">
+        <v>712</v>
+      </c>
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -2567,10 +2579,13 @@
       <c r="CO6" s="8">
         <v>365</v>
       </c>
+      <c r="CP6">
+        <v>381</v>
+      </c>
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -2845,6 +2860,9 @@
       </c>
       <c r="CO7" s="8">
         <v>90</v>
+      </c>
+      <c r="CP7">
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:115" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-11-2020 01-53-17
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23007"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1099" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B1EDAA3A-69C7-FC46-BCB1-85E30F2067CC}"/>
+  <xr:revisionPtr revIDLastSave="1107" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{532FB329-B6BD-4820-BF6F-1982BB87A0E6}"/>
   <bookViews>
     <workbookView xWindow="2376" yWindow="0" windowWidth="14028" windowHeight="9216" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -296,12 +296,90 @@
     <t>03-06-2020</t>
   </si>
   <si>
+    <t>04-06-2020</t>
+  </si>
+  <si>
+    <t>05-06-2020</t>
+  </si>
+  <si>
     <t>06-06-2020</t>
   </si>
   <si>
     <t>07-06-2020</t>
   </si>
   <si>
+    <t>08-06-2020</t>
+  </si>
+  <si>
+    <t>09-06-2020</t>
+  </si>
+  <si>
+    <t>10-06-2020</t>
+  </si>
+  <si>
+    <t>11-06-2020</t>
+  </si>
+  <si>
+    <t>12-06-2020</t>
+  </si>
+  <si>
+    <t>13-06-2020</t>
+  </si>
+  <si>
+    <t>13/6/2020</t>
+  </si>
+  <si>
+    <t>14/6/2020</t>
+  </si>
+  <si>
+    <t>15/6/2020</t>
+  </si>
+  <si>
+    <t>16/6/2020</t>
+  </si>
+  <si>
+    <t>17/6/2020</t>
+  </si>
+  <si>
+    <t>18/6/2020</t>
+  </si>
+  <si>
+    <t>19/6/2020</t>
+  </si>
+  <si>
+    <t>20/6/2020</t>
+  </si>
+  <si>
+    <t>21/6/2020</t>
+  </si>
+  <si>
+    <t>22/6/2020</t>
+  </si>
+  <si>
+    <t>23/6/2020</t>
+  </si>
+  <si>
+    <t>24/6/2020</t>
+  </si>
+  <si>
+    <t>25/6/2020</t>
+  </si>
+  <si>
+    <t>26/6/2020</t>
+  </si>
+  <si>
+    <t>27/6/2020</t>
+  </si>
+  <si>
+    <t>28/6/2020</t>
+  </si>
+  <si>
+    <t>29/6/2020</t>
+  </si>
+  <si>
+    <t>30/6/2020</t>
+  </si>
+  <si>
     <t>Pruebas Realizadas</t>
   </si>
   <si>
@@ -318,84 +396,6 @@
   </si>
   <si>
     <t>Hospitalizados en UCI</t>
-  </si>
-  <si>
-    <t>13/6/2020</t>
-  </si>
-  <si>
-    <t>14/6/2020</t>
-  </si>
-  <si>
-    <t>15/6/2020</t>
-  </si>
-  <si>
-    <t>16/6/2020</t>
-  </si>
-  <si>
-    <t>17/6/2020</t>
-  </si>
-  <si>
-    <t>18/6/2020</t>
-  </si>
-  <si>
-    <t>19/6/2020</t>
-  </si>
-  <si>
-    <t>20/6/2020</t>
-  </si>
-  <si>
-    <t>21/6/2020</t>
-  </si>
-  <si>
-    <t>22/6/2020</t>
-  </si>
-  <si>
-    <t>23/6/2020</t>
-  </si>
-  <si>
-    <t>24/6/2020</t>
-  </si>
-  <si>
-    <t>25/6/2020</t>
-  </si>
-  <si>
-    <t>26/6/2020</t>
-  </si>
-  <si>
-    <t>27/6/2020</t>
-  </si>
-  <si>
-    <t>28/6/2020</t>
-  </si>
-  <si>
-    <t>29/6/2020</t>
-  </si>
-  <si>
-    <t>30/6/2020</t>
-  </si>
-  <si>
-    <t>08-06-20</t>
-  </si>
-  <si>
-    <t>05-06-20</t>
-  </si>
-  <si>
-    <t>09-06-20</t>
-  </si>
-  <si>
-    <t>10-06-20</t>
-  </si>
-  <si>
-    <t>11-06-20</t>
-  </si>
-  <si>
-    <t>12-06-20</t>
-  </si>
-  <si>
-    <t>13-06-20</t>
-  </si>
-  <si>
-    <t>04-06-20</t>
   </si>
 </sst>
 </file>
@@ -403,9 +403,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,7 +459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,16 +568,16 @@
     <tableColumn id="74" xr3:uid="{828D9632-D098-418C-8A67-CA98651BA254}" name="01-06-2020"/>
     <tableColumn id="75" xr3:uid="{2918382E-DC05-40AA-9D38-7D65EC299862}" name="02-06-2020"/>
     <tableColumn id="96" xr3:uid="{E4AB1F9C-8FD7-4413-867C-24D7D313240D}" name="03-06-2020"/>
-    <tableColumn id="1" xr3:uid="{0ED54AB8-E3B7-4C5E-A3D9-DC4FC5A90852}" name="04-06-20"/>
-    <tableColumn id="2" xr3:uid="{31600888-D874-4B90-9270-CF9219D7F135}" name="05-06-20"/>
+    <tableColumn id="1" xr3:uid="{0ED54AB8-E3B7-4C5E-A3D9-DC4FC5A90852}" name="04-06-2020"/>
+    <tableColumn id="2" xr3:uid="{31600888-D874-4B90-9270-CF9219D7F135}" name="05-06-2020"/>
     <tableColumn id="3" xr3:uid="{6415ECB6-E037-4BC3-9907-91C4C505CF37}" name="06-06-2020"/>
     <tableColumn id="4" xr3:uid="{2FE879E2-2128-42AE-A0E3-647EE2D0C94F}" name="07-06-2020"/>
-    <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="08-06-20"/>
-    <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-20"/>
-    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-20"/>
-    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-20"/>
-    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-20"/>
-    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20"/>
+    <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="08-06-2020"/>
+    <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-2020"/>
+    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020"/>
+    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020"/>
+    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020"/>
+    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-2020"/>
     <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="13/6/2020"/>
     <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="14/6/2020"/>
     <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="15/6/2020"/>
@@ -602,7 +602,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -902,16 +902,16 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CN1" sqref="CN1"/>
+      <selection pane="topRight" activeCell="CS2" sqref="CS2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="26.109375" customWidth="1"/>
-    <col min="2" max="87" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="87" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:115">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1174,93 +1174,93 @@
         <v>86</v>
       </c>
       <c r="CJ1" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="CK1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="CL1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CQ1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CR1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CS1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CT1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CU1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CV1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="CW1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CX1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CY1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="CZ1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="DA1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="DB1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="DC1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="DD1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="DE1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="DF1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="DG1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="DH1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="DI1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="DJ1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="DK1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="CL1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="CM1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="CN1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="CO1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:115">
+      <c r="A2" t="s">
         <v>115</v>
-      </c>
-      <c r="CP1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="CQ1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="CR1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="CS1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="CT1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="CU1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="CV1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="CW1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="CX1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="CY1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="CZ1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="DA1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="DB1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="DC1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="DD1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="DE1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="DF1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="DG1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="DH1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="DI1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="DJ1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:115" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>89</v>
       </c>
       <c r="B2" s="7">
         <v>146</v>
@@ -1542,9 +1542,9 @@
         <v>82774</v>
       </c>
     </row>
-    <row r="3" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:115">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="B3" s="7">
         <v>138</v>
@@ -1826,9 +1826,9 @@
         <v>62284</v>
       </c>
     </row>
-    <row r="4" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:115">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="B4" s="7">
         <v>6</v>
@@ -2110,9 +2110,9 @@
         <v>5315</v>
       </c>
     </row>
-    <row r="5" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:115">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2303,9 +2303,9 @@
         <v>712</v>
       </c>
     </row>
-    <row r="6" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:115">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -2583,9 +2583,9 @@
         <v>381</v>
       </c>
     </row>
-    <row r="7" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:115">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -2865,7 +2865,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:115">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2959,46 +2959,46 @@
       <c r="CN8" s="8"/>
       <c r="CO8" s="8"/>
     </row>
-    <row r="9" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:115">
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:115">
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:115">
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:115">
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:115">
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:115">
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:115">
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:115">
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23">
       <c r="W17" s="3"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23">
       <c r="W18" s="3"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23">
       <c r="W19" s="3"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23">
       <c r="W20" s="3"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23">
       <c r="W21" s="3"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3021,52 +3021,52 @@
       <c r="T22" s="2"/>
       <c r="W22" s="3"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23">
       <c r="W23" s="3"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23">
       <c r="W24" s="3"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23">
       <c r="W25" s="4"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23">
       <c r="W26" s="4"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23">
       <c r="W27" s="4"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23">
       <c r="W28" s="4"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23">
       <c r="W29" s="4"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23">
       <c r="W30" s="4"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23">
       <c r="W31" s="4"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23">
       <c r="W32" s="4"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23">
       <c r="W33" s="4"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23">
       <c r="W34" s="4"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23">
       <c r="W35" s="1"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23">
       <c r="W36" s="1"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23">
       <c r="W37" s="1"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -3089,7 +3089,7 @@
       <c r="T38" s="2"/>
       <c r="W38" s="1"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -3112,7 +3112,7 @@
       <c r="T39" s="2"/>
       <c r="W39" s="1"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -3135,7 +3135,7 @@
       <c r="T40" s="2"/>
       <c r="W40" s="1"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -3158,7 +3158,7 @@
       <c r="T41" s="2"/>
       <c r="W41" s="1"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -3181,7 +3181,7 @@
       <c r="T42" s="2"/>
       <c r="W42" s="1"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -3204,7 +3204,7 @@
       <c r="T43" s="2"/>
       <c r="W43" s="1"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -3227,7 +3227,7 @@
       <c r="T44" s="2"/>
       <c r="W44" s="1"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -3250,7 +3250,7 @@
       <c r="T45" s="2"/>
       <c r="W45" s="1"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -3273,7 +3273,7 @@
       <c r="T46" s="2"/>
       <c r="W46" s="1"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -3296,7 +3296,7 @@
       <c r="T47" s="2"/>
       <c r="W47" s="3"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -3319,7 +3319,7 @@
       <c r="T48" s="2"/>
       <c r="W48" s="3"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -3342,7 +3342,7 @@
       <c r="T49" s="2"/>
       <c r="W49" s="3"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -3365,7 +3365,7 @@
       <c r="T50" s="2"/>
       <c r="W50" s="3"/>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -3388,7 +3388,7 @@
       <c r="T51" s="2"/>
       <c r="W51" s="3"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23">
       <c r="W52" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-13-2020 13-12-30
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1113" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2C60A7A7-7962-164E-B101-842E2D728166}"/>
+  <xr:revisionPtr revIDLastSave="1119" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BDC794BD-FE29-5340-9E20-09614301EF72}"/>
   <bookViews>
     <workbookView xWindow="2376" yWindow="0" windowWidth="14028" windowHeight="9216" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -901,8 +901,8 @@
   <dimension ref="A1:DK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CQ7" sqref="CQ7"/>
+      <pane xSplit="1" topLeftCell="CP1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CS3" sqref="CS3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1544,6 +1544,9 @@
       <c r="CQ2">
         <v>85007</v>
       </c>
+      <c r="CR2">
+        <v>87041</v>
+      </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1831,6 +1834,9 @@
       <c r="CQ3">
         <v>63805</v>
       </c>
+      <c r="CR3">
+        <v>65209</v>
+      </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2117,6 +2123,9 @@
       </c>
       <c r="CQ4">
         <v>5910</v>
+      </c>
+      <c r="CR4">
+        <v>3798</v>
       </c>
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.2">
@@ -2314,6 +2323,9 @@
       <c r="CQ5">
         <v>695</v>
       </c>
+      <c r="CR5">
+        <v>739</v>
+      </c>
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -2597,6 +2609,9 @@
       <c r="CQ6">
         <v>390</v>
       </c>
+      <c r="CR6">
+        <v>398</v>
+      </c>
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -2880,6 +2895,9 @@
         <v>91</v>
       </c>
       <c r="CQ7">
+        <v>96</v>
+      </c>
+      <c r="CR7">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-13-2020 22-23-50
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1151" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AC714E4D-0ECA-48CA-9942-F225BA1F0C56}"/>
+  <xr:revisionPtr revIDLastSave="1164" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F64B851F-599D-4CAB-B7F9-CDDCB3A0C876}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -21672,14 +21672,6 @@
       <sheetData sheetId="10"/>
       <sheetData sheetId="11"/>
       <sheetData sheetId="12">
-        <row r="7">
-          <cell r="C7">
-            <v>4</v>
-          </cell>
-          <cell r="J7">
-            <v>1</v>
-          </cell>
-        </row>
         <row r="8">
           <cell r="C8">
             <v>5</v>
@@ -22127,7 +22119,7 @@
   <dimension ref="A1:DK52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="MF1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
@@ -24667,7 +24659,7 @@
   <dimension ref="A4:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24677,11 +24669,12 @@
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D4" s="9">
-        <f>+D7+COUNTA('[1]Casos Acum Corr'!$CP$3:$MO$3)</f>
+        <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
         <v>43994</v>
       </c>
       <c r="E4" s="10"/>
@@ -24750,25 +24743,25 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="str">
-        <f>+IF([1]!TODO_CORREGIMIENTO[[#This Row],[Fecha]]&gt;$D$1,"OUT TIME","ON")</f>
-        <v>OUT TIME</v>
+        <f>+IF(D7&gt;$D$4,"OUT TIME","ON")</f>
+        <v>ON</v>
       </c>
       <c r="B7" s="12" t="str">
-        <f>IF([1]!TODO_CORREGIMIENTO[[#This Row],[Fecha]]=$D$1,"ultima","no")</f>
+        <f>IF(D7=$D$4,"ultima","no")</f>
         <v>no</v>
       </c>
       <c r="C7" s="12">
         <v>1</v>
       </c>
       <c r="D7" s="1">
-        <v>43987</v>
+        <v>43900</v>
       </c>
       <c r="E7" s="11">
         <v>1</v>
       </c>
       <c r="F7" cm="1">
-        <f t="array" ref="F7">+INDEX('[1]Casos Acum Corr'!$CO$3:$MO$677,'[1]TODO CORREGIMIENTO'!C7+1,'[1]TODO CORREGIMIENTO'!J7)</f>
-        <v>574</v>
+        <f t="array" ref="F7">+INDEX(Hoja1!$B$2:$MO$7,C7+1,E7)</f>
+        <v>138</v>
       </c>
       <c r="L7" cm="1">
         <f t="array" ref="L7">+INDEX('[1]Muertes ACUM'!$H$3:$MO$677,$C7+1,$E7)</f>
@@ -24780,36 +24773,36 @@
       </c>
       <c r="P7">
         <f>+F7-L7-N7</f>
-        <v>22</v>
+        <v>-414</v>
       </c>
       <c r="R7" s="13">
         <f>+IFERROR(L7/F7,0)</f>
-        <v>2.7874564459930314E-2</v>
+        <v>0.11594202898550725</v>
       </c>
       <c r="S7" s="13">
         <f>+IFERROR(N7/F7,0)</f>
-        <v>0.93379790940766549</v>
+        <v>3.8840579710144927</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="str">
-        <f>+IF([1]!TODO_CORREGIMIENTO[[#This Row],[Fecha]]&gt;$D$1,"OUT TIME","ON")</f>
-        <v>OUT TIME</v>
+        <f t="shared" ref="A8:A9" si="0">+IF(D8&gt;$D$4,"OUT TIME","ON")</f>
+        <v>ON</v>
       </c>
       <c r="B8" s="12" t="str">
-        <f>IF([1]!TODO_CORREGIMIENTO[[#This Row],[Fecha]]=$D$1,"ultima","no")</f>
+        <f t="shared" ref="B8:B9" si="1">IF(D8=$D$4,"ultima","no")</f>
         <v>no</v>
       </c>
       <c r="C8" s="12">
         <v>2</v>
       </c>
       <c r="D8" s="1">
-        <f>+IF(C8=1,D7+1,D7)</f>
-        <v>43987</v>
+        <f>+D7+1</f>
+        <v>43901</v>
       </c>
       <c r="E8" s="11">
-        <f>+IF(C8=1,E7+1,E7)</f>
-        <v>1</v>
+        <f>+E7+1</f>
+        <v>2</v>
       </c>
       <c r="F8" cm="1">
         <f t="array" ref="F8">+INDEX('[1]Casos Acum Corr'!$CO$3:$MO$677,'[1]TODO CORREGIMIENTO'!C8+1,'[1]TODO CORREGIMIENTO'!J8)</f>
@@ -24824,37 +24817,37 @@
         <v>433</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8:P9" si="0">+F8-L8-N8</f>
+        <f t="shared" ref="P8:P9" si="2">+F8-L8-N8</f>
         <v>18</v>
       </c>
       <c r="R8" s="13">
-        <f t="shared" ref="R8:R9" si="1">+IFERROR(L8/F8,0)</f>
+        <f t="shared" ref="R8:R9" si="3">+IFERROR(L8/F8,0)</f>
         <v>0</v>
       </c>
       <c r="S8" s="13">
-        <f t="shared" ref="S8:S9" si="2">+IFERROR(N8/F8,0)</f>
+        <f t="shared" ref="S8:S9" si="4">+IFERROR(N8/F8,0)</f>
         <v>0.96008869179600886</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="str">
-        <f>+IF([1]!TODO_CORREGIMIENTO[[#This Row],[Fecha]]&gt;$D$1,"OUT TIME","ON")</f>
-        <v>OUT TIME</v>
+        <f t="shared" si="0"/>
+        <v>ON</v>
       </c>
       <c r="B9" s="12" t="str">
-        <f>IF([1]!TODO_CORREGIMIENTO[[#This Row],[Fecha]]=$D$1,"ultima","no")</f>
+        <f t="shared" si="1"/>
         <v>no</v>
       </c>
       <c r="C9" s="12">
         <v>3</v>
       </c>
       <c r="D9" s="1">
-        <f>+IF(C9=1,D8+1,D8)</f>
-        <v>43987</v>
+        <f>+D8+1</f>
+        <v>43902</v>
       </c>
       <c r="E9" s="11">
-        <f>+IF(C9=1,E8+1,E8)</f>
-        <v>1</v>
+        <f>+E8+1</f>
+        <v>3</v>
       </c>
       <c r="F9" cm="1">
         <f t="array" ref="F9">+INDEX('[1]Casos Acum Corr'!$CO$3:$MO$677,'[1]TODO CORREGIMIENTO'!C9+1,'[1]TODO CORREGIMIENTO'!J9)</f>
@@ -24866,19 +24859,19 @@
       </c>
       <c r="N9" cm="1">
         <f t="array" ref="N9">+INDEX('[1]Recuperados ACUM'!$H$3:$MO$677,$C9+1,$E9)</f>
-        <v>284</v>
+        <v>341</v>
       </c>
       <c r="P9">
-        <f t="shared" si="0"/>
-        <v>156</v>
+        <f t="shared" si="2"/>
+        <v>99</v>
       </c>
       <c r="R9" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S9" s="13">
-        <f t="shared" si="2"/>
-        <v>0.6454545454545455</v>
+        <f t="shared" si="4"/>
+        <v>0.77500000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-13-2020 22-56-39
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1271" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C96EFD8A-9683-4590-9175-871B6367AB1F}"/>
+  <xr:revisionPtr revIDLastSave="1277" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8A69EC1F-0BB4-40E1-A93D-9902A6017497}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -3566,8 +3566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8687142-640A-49EC-B5B6-1D4ED31D97B1}">
   <dimension ref="A4:AD304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K277" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8:AC303"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3822,8 +3822,8 @@
         <v>7.2164948453608241E-2</v>
       </c>
       <c r="R8">
-        <f>+I8-I7</f>
-        <v>42</v>
+        <f>+G8-G7</f>
+        <v>48</v>
       </c>
       <c r="S8">
         <f>+J8-J7</f>
@@ -3846,8 +3846,8 @@
         <v>2</v>
       </c>
       <c r="X8">
-        <f>+IFERROR(G8/G7,0)</f>
-        <v>0</v>
+        <f>+IFERROR(R8/F7,0)</f>
+        <v>0.32876712328767121</v>
       </c>
       <c r="Y8">
         <f>+IFERROR(K8/K7,0)</f>
@@ -3939,8 +3939,8 @@
         <v>6.7331670822942641E-2</v>
       </c>
       <c r="R9">
-        <f t="shared" ref="R9:R72" si="9">+I9-I8</f>
-        <v>152</v>
+        <f t="shared" ref="R9:R72" si="9">+G9-G8</f>
+        <v>159</v>
       </c>
       <c r="S9">
         <f t="shared" ref="S9:S72" si="10">+J9-J8</f>
@@ -3963,8 +3963,8 @@
         <v>0</v>
       </c>
       <c r="X9">
-        <f t="shared" ref="X9:X72" si="15">+IFERROR(G9/G8,0)</f>
-        <v>4.3125</v>
+        <f t="shared" ref="X9:X72" si="15">+IFERROR(R9/F8,0)</f>
+        <v>0.81958762886597936</v>
       </c>
       <c r="Y9">
         <f t="shared" ref="Y9:Y72" si="16">+IFERROR(K9/K8,0)</f>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="R10">
         <f t="shared" si="9"/>
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="S10">
         <f t="shared" si="10"/>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="X10">
         <f t="shared" si="15"/>
-        <v>1.1980676328502415</v>
+        <v>0.10224438902743142</v>
       </c>
       <c r="Y10">
         <f t="shared" si="16"/>
@@ -4174,7 +4174,7 @@
       </c>
       <c r="R11">
         <f t="shared" si="9"/>
-        <v>-38</v>
+        <v>-40</v>
       </c>
       <c r="S11">
         <f t="shared" si="10"/>
@@ -4198,7 +4198,7 @@
       </c>
       <c r="X11">
         <f t="shared" si="15"/>
-        <v>0.83870967741935487</v>
+        <v>-6.1633281972265024E-2</v>
       </c>
       <c r="Y11">
         <f t="shared" si="16"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="R12">
         <f t="shared" si="9"/>
-        <v>-94</v>
+        <v>-89</v>
       </c>
       <c r="S12">
         <f t="shared" si="10"/>
@@ -4315,7 +4315,7 @@
       </c>
       <c r="X12">
         <f t="shared" si="15"/>
-        <v>0.57211538461538458</v>
+        <v>-0.10385064177362893</v>
       </c>
       <c r="Y12">
         <f t="shared" si="16"/>
@@ -4408,7 +4408,7 @@
       </c>
       <c r="R13">
         <f t="shared" si="9"/>
-        <v>-24</v>
+        <v>-22</v>
       </c>
       <c r="S13">
         <f t="shared" si="10"/>
@@ -4432,7 +4432,7 @@
       </c>
       <c r="X13">
         <f t="shared" si="15"/>
-        <v>0.81512605042016806</v>
+        <v>-2.2540983606557378E-2</v>
       </c>
       <c r="Y13">
         <f t="shared" si="16"/>
@@ -4525,7 +4525,7 @@
       </c>
       <c r="R14">
         <f t="shared" si="9"/>
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="S14">
         <f t="shared" si="10"/>
@@ -4549,7 +4549,7 @@
       </c>
       <c r="X14">
         <f t="shared" si="15"/>
-        <v>1.6391752577319587</v>
+        <v>5.778191985088537E-2</v>
       </c>
       <c r="Y14">
         <f t="shared" si="16"/>
@@ -4642,7 +4642,7 @@
       </c>
       <c r="R15">
         <f t="shared" si="9"/>
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="S15">
         <f t="shared" si="10"/>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="X15">
         <f t="shared" si="15"/>
-        <v>1.4025157232704402</v>
+        <v>5.1948051948051951E-2</v>
       </c>
       <c r="Y15">
         <f t="shared" si="16"/>
@@ -4759,7 +4759,7 @@
       </c>
       <c r="R16">
         <f t="shared" si="9"/>
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="S16">
         <f t="shared" si="10"/>
@@ -4783,7 +4783,7 @@
       </c>
       <c r="X16">
         <f t="shared" si="15"/>
-        <v>1.4035874439461884</v>
+        <v>6.1855670103092786E-2</v>
       </c>
       <c r="Y16">
         <f t="shared" si="16"/>
@@ -4876,7 +4876,7 @@
       </c>
       <c r="R17">
         <f t="shared" si="9"/>
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="S17">
         <f t="shared" si="10"/>
@@ -4900,7 +4900,7 @@
       </c>
       <c r="X17">
         <f t="shared" si="15"/>
-        <v>1.281150159744409</v>
+        <v>4.9773755656108594E-2</v>
       </c>
       <c r="Y17">
         <f t="shared" si="16"/>
@@ -4993,7 +4993,7 @@
       </c>
       <c r="R18">
         <f t="shared" si="9"/>
-        <v>-81</v>
+        <v>-97</v>
       </c>
       <c r="S18">
         <f t="shared" si="10"/>
@@ -5017,7 +5017,7 @@
       </c>
       <c r="X18">
         <f t="shared" si="15"/>
-        <v>0.75810473815461343</v>
+        <v>-4.4721069617335178E-2</v>
       </c>
       <c r="Y18">
         <f t="shared" si="16"/>
@@ -5110,7 +5110,7 @@
       </c>
       <c r="R19">
         <f t="shared" si="9"/>
-        <v>300</v>
+        <v>322</v>
       </c>
       <c r="S19">
         <f t="shared" si="10"/>
@@ -5134,7 +5134,7 @@
       </c>
       <c r="X19">
         <f t="shared" si="15"/>
-        <v>2.0592105263157894</v>
+        <v>0.13020622725434694</v>
       </c>
       <c r="Y19">
         <f t="shared" si="16"/>
@@ -5227,7 +5227,7 @@
       </c>
       <c r="R20">
         <f t="shared" si="9"/>
-        <v>-450</v>
+        <v>-492</v>
       </c>
       <c r="S20">
         <f t="shared" si="10"/>
@@ -5251,7 +5251,7 @@
       </c>
       <c r="X20">
         <f t="shared" si="15"/>
-        <v>0.21405750798722045</v>
+        <v>-0.15876089060987417</v>
       </c>
       <c r="Y20">
         <f t="shared" si="16"/>
@@ -5344,7 +5344,7 @@
       </c>
       <c r="R21">
         <f t="shared" si="9"/>
-        <v>245</v>
+        <v>323</v>
       </c>
       <c r="S21">
         <f t="shared" si="10"/>
@@ -5368,7 +5368,7 @@
       </c>
       <c r="X21">
         <f t="shared" si="15"/>
-        <v>3.41044776119403</v>
+        <v>9.9907206928549333E-2</v>
       </c>
       <c r="Y21">
         <f t="shared" si="16"/>
@@ -5461,7 +5461,7 @@
       </c>
       <c r="R22">
         <f t="shared" si="9"/>
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="S22">
         <f t="shared" si="10"/>
@@ -5485,7 +5485,7 @@
       </c>
       <c r="X22">
         <f t="shared" si="15"/>
-        <v>1.2210065645514223</v>
+        <v>2.7371273712737128E-2</v>
       </c>
       <c r="Y22">
         <f t="shared" si="16"/>
@@ -5578,7 +5578,7 @@
       </c>
       <c r="R23">
         <f t="shared" si="9"/>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="S23">
         <f t="shared" si="10"/>
@@ -5602,7 +5602,7 @@
       </c>
       <c r="X23">
         <f t="shared" si="15"/>
-        <v>1.0896057347670252</v>
+        <v>1.1770244821092278E-2</v>
       </c>
       <c r="Y23">
         <f t="shared" si="16"/>
@@ -5695,7 +5695,7 @@
       </c>
       <c r="R24">
         <f t="shared" si="9"/>
-        <v>-235</v>
+        <v>-242</v>
       </c>
       <c r="S24">
         <f t="shared" si="10"/>
@@ -5719,7 +5719,7 @@
       </c>
       <c r="X24">
         <f t="shared" si="15"/>
-        <v>0.60197368421052633</v>
+        <v>-4.983525535420099E-2</v>
       </c>
       <c r="Y24">
         <f t="shared" si="16"/>
@@ -5812,7 +5812,7 @@
       </c>
       <c r="R25">
         <f t="shared" si="9"/>
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="S25">
         <f t="shared" si="10"/>
@@ -5836,7 +5836,7 @@
       </c>
       <c r="X25">
         <f t="shared" si="15"/>
-        <v>1.4754098360655739</v>
+        <v>3.3320566832631175E-2</v>
       </c>
       <c r="Y25">
         <f t="shared" si="16"/>
@@ -5929,7 +5929,7 @@
       </c>
       <c r="R26">
         <f t="shared" si="9"/>
-        <v>-47</v>
+        <v>-142</v>
       </c>
       <c r="S26">
         <f t="shared" si="10"/>
@@ -5953,7 +5953,7 @@
       </c>
       <c r="X26">
         <f t="shared" si="15"/>
-        <v>0.73703703703703705</v>
+        <v>-2.4644220756681708E-2</v>
       </c>
       <c r="Y26">
         <f t="shared" si="16"/>
@@ -6046,7 +6046,7 @@
       </c>
       <c r="R27">
         <f t="shared" si="9"/>
-        <v>-104</v>
+        <v>24</v>
       </c>
       <c r="S27">
         <f t="shared" si="10"/>
@@ -6070,7 +6070,7 @@
       </c>
       <c r="X27">
         <f t="shared" si="15"/>
-        <v>1.0603015075376885</v>
+        <v>3.8961038961038961E-3</v>
       </c>
       <c r="Y27">
         <f t="shared" si="16"/>
@@ -6163,7 +6163,7 @@
       </c>
       <c r="R28">
         <f t="shared" si="9"/>
-        <v>-15</v>
+        <v>-60</v>
       </c>
       <c r="S28">
         <f t="shared" si="10"/>
@@ -6187,7 +6187,7 @@
       </c>
       <c r="X28">
         <f t="shared" si="15"/>
-        <v>0.85781990521327012</v>
+        <v>-9.1157702825888781E-3</v>
       </c>
       <c r="Y28">
         <f t="shared" si="16"/>
@@ -6280,7 +6280,7 @@
       </c>
       <c r="R29">
         <f t="shared" si="9"/>
-        <v>-3</v>
+        <v>27</v>
       </c>
       <c r="S29">
         <f t="shared" si="10"/>
@@ -6304,7 +6304,7 @@
       </c>
       <c r="X29">
         <f t="shared" si="15"/>
-        <v>1.0745856353591161</v>
+        <v>3.8882488479262674E-3</v>
       </c>
       <c r="Y29">
         <f t="shared" si="16"/>
@@ -6397,7 +6397,7 @@
       </c>
       <c r="R30">
         <f t="shared" si="9"/>
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="S30">
         <f t="shared" si="10"/>
@@ -6421,7 +6421,7 @@
       </c>
       <c r="X30">
         <f t="shared" si="15"/>
-        <v>1.5629820051413881</v>
+        <v>2.9864993863357427E-2</v>
       </c>
       <c r="Y30">
         <f t="shared" si="16"/>
@@ -6514,7 +6514,7 @@
       </c>
       <c r="R31">
         <f t="shared" si="9"/>
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="S31">
         <f t="shared" si="10"/>
@@ -6538,7 +6538,7 @@
       </c>
       <c r="X31">
         <f t="shared" si="15"/>
-        <v>1.2384868421052631</v>
+        <v>1.8259665029593249E-2</v>
       </c>
       <c r="Y31">
         <f t="shared" si="16"/>
@@ -6631,7 +6631,7 @@
       </c>
       <c r="R32">
         <f t="shared" si="9"/>
-        <v>-123</v>
+        <v>-191</v>
       </c>
       <c r="S32">
         <f t="shared" si="10"/>
@@ -6655,7 +6655,7 @@
       </c>
       <c r="X32">
         <f t="shared" si="15"/>
-        <v>0.74634794156706508</v>
+        <v>-2.1969174143087185E-2</v>
       </c>
       <c r="Y32">
         <f t="shared" si="16"/>
@@ -6748,7 +6748,7 @@
       </c>
       <c r="R33">
         <f t="shared" si="9"/>
-        <v>-128</v>
+        <v>-69</v>
       </c>
       <c r="S33">
         <f t="shared" si="10"/>
@@ -6772,7 +6772,7 @@
       </c>
       <c r="X33">
         <f t="shared" si="15"/>
-        <v>0.87722419928825623</v>
+        <v>-7.4546240276577354E-3</v>
       </c>
       <c r="Y33">
         <f t="shared" si="16"/>
@@ -6865,7 +6865,7 @@
       </c>
       <c r="R34">
         <f t="shared" si="9"/>
-        <v>130</v>
+        <v>55</v>
       </c>
       <c r="S34">
         <f t="shared" si="10"/>
@@ -6889,7 +6889,7 @@
       </c>
       <c r="X34">
         <f t="shared" si="15"/>
-        <v>1.1115618661257607</v>
+        <v>5.6416042671043184E-3</v>
       </c>
       <c r="Y34">
         <f t="shared" si="16"/>
@@ -6982,7 +6982,7 @@
       </c>
       <c r="R35">
         <f t="shared" si="9"/>
-        <v>-201</v>
+        <v>-164</v>
       </c>
       <c r="S35">
         <f t="shared" si="10"/>
@@ -7006,7 +7006,7 @@
       </c>
       <c r="X35">
         <f t="shared" si="15"/>
-        <v>0.7007299270072993</v>
+        <v>-1.5926969020102943E-2</v>
       </c>
       <c r="Y35">
         <f t="shared" si="16"/>
@@ -7099,7 +7099,7 @@
       </c>
       <c r="R36">
         <f t="shared" si="9"/>
-        <v>581</v>
+        <v>711</v>
       </c>
       <c r="S36">
         <f t="shared" si="10"/>
@@ -7123,7 +7123,7 @@
       </c>
       <c r="X36">
         <f t="shared" si="15"/>
-        <v>2.8515625</v>
+        <v>6.6566800861342576E-2</v>
       </c>
       <c r="Y36">
         <f t="shared" si="16"/>
@@ -7216,7 +7216,7 @@
       </c>
       <c r="R37">
         <f t="shared" si="9"/>
-        <v>-364</v>
+        <v>-419</v>
       </c>
       <c r="S37">
         <f t="shared" si="10"/>
@@ -7240,7 +7240,7 @@
       </c>
       <c r="X37">
         <f t="shared" si="15"/>
-        <v>0.61735159817351604</v>
+        <v>-3.5580842391304345E-2</v>
       </c>
       <c r="Y37">
         <f t="shared" si="16"/>
@@ -7333,7 +7333,7 @@
       </c>
       <c r="R38">
         <f t="shared" si="9"/>
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="S38">
         <f t="shared" si="10"/>
@@ -7357,7 +7357,7 @@
       </c>
       <c r="X38">
         <f t="shared" si="15"/>
-        <v>1.5473372781065089</v>
+        <v>2.9714102152264697E-2</v>
       </c>
       <c r="Y38">
         <f t="shared" si="16"/>
@@ -7450,7 +7450,7 @@
       </c>
       <c r="R39">
         <f t="shared" si="9"/>
-        <v>-222</v>
+        <v>-184</v>
       </c>
       <c r="S39">
         <f t="shared" si="10"/>
@@ -7474,7 +7474,7 @@
       </c>
       <c r="X39">
         <f t="shared" si="15"/>
-        <v>0.82409177820267687</v>
+        <v>-1.3631649133204918E-2</v>
       </c>
       <c r="Y39">
         <f t="shared" si="16"/>
@@ -7567,7 +7567,7 @@
       </c>
       <c r="R40">
         <f t="shared" si="9"/>
-        <v>-143</v>
+        <v>-237</v>
       </c>
       <c r="S40">
         <f t="shared" si="10"/>
@@ -7591,7 +7591,7 @@
       </c>
       <c r="X40">
         <f t="shared" si="15"/>
-        <v>0.72505800464037118</v>
+        <v>-1.6504178272980501E-2</v>
       </c>
       <c r="Y40">
         <f t="shared" si="16"/>
@@ -7684,7 +7684,7 @@
       </c>
       <c r="R41">
         <f t="shared" si="9"/>
-        <v>-119</v>
+        <v>-43</v>
       </c>
       <c r="S41">
         <f t="shared" si="10"/>
@@ -7708,7 +7708,7 @@
       </c>
       <c r="X41">
         <f t="shared" si="15"/>
-        <v>0.93120000000000003</v>
+        <v>-2.8695362028695361E-3</v>
       </c>
       <c r="Y41">
         <f t="shared" si="16"/>
@@ -7801,7 +7801,7 @@
       </c>
       <c r="R42">
         <f t="shared" si="9"/>
-        <v>44</v>
+        <v>-96</v>
       </c>
       <c r="S42">
         <f t="shared" si="10"/>
@@ -7825,7 +7825,7 @@
       </c>
       <c r="X42">
         <f t="shared" si="15"/>
-        <v>0.83505154639175261</v>
+        <v>-6.1668915012526495E-3</v>
       </c>
       <c r="Y42">
         <f t="shared" si="16"/>
@@ -7918,7 +7918,7 @@
       </c>
       <c r="R43">
         <f t="shared" si="9"/>
-        <v>224</v>
+        <v>315</v>
       </c>
       <c r="S43">
         <f t="shared" si="10"/>
@@ -7942,7 +7942,7 @@
       </c>
       <c r="X43">
         <f t="shared" si="15"/>
-        <v>1.6481481481481481</v>
+        <v>1.9622500467202392E-2</v>
       </c>
       <c r="Y43">
         <f t="shared" si="16"/>
@@ -8035,7 +8035,7 @@
       </c>
       <c r="R44">
         <f t="shared" si="9"/>
-        <v>89</v>
+        <v>195</v>
       </c>
       <c r="S44">
         <f t="shared" si="10"/>
@@ -8059,7 +8059,7 @@
       </c>
       <c r="X44">
         <f t="shared" si="15"/>
-        <v>1.2434456928838951</v>
+        <v>1.1569953720185119E-2</v>
       </c>
       <c r="Y44">
         <f t="shared" si="16"/>
@@ -8152,7 +8152,7 @@
       </c>
       <c r="R45">
         <f t="shared" si="9"/>
-        <v>-180</v>
+        <v>-287</v>
       </c>
       <c r="S45">
         <f t="shared" si="10"/>
@@ -8176,7 +8176,7 @@
       </c>
       <c r="X45">
         <f t="shared" si="15"/>
-        <v>0.7118473895582329</v>
+        <v>-1.607843137254902E-2</v>
       </c>
       <c r="Y45">
         <f t="shared" si="16"/>
@@ -8269,7 +8269,7 @@
       </c>
       <c r="R46">
         <f t="shared" si="9"/>
-        <v>-83</v>
+        <v>-177</v>
       </c>
       <c r="S46">
         <f t="shared" si="10"/>
@@ -8293,7 +8293,7 @@
       </c>
       <c r="X46">
         <f t="shared" si="15"/>
-        <v>0.75035260930888581</v>
+        <v>-9.5371517861953768E-3</v>
       </c>
       <c r="Y46">
         <f t="shared" si="16"/>
@@ -8386,7 +8386,7 @@
       </c>
       <c r="R47">
         <f t="shared" si="9"/>
-        <v>385</v>
+        <v>514</v>
       </c>
       <c r="S47">
         <f t="shared" si="10"/>
@@ -8410,7 +8410,7 @@
       </c>
       <c r="X47">
         <f t="shared" si="15"/>
-        <v>1.9661654135338347</v>
+        <v>2.6923681315803256E-2</v>
       </c>
       <c r="Y47">
         <f t="shared" si="16"/>
@@ -8503,7 +8503,7 @@
       </c>
       <c r="R48">
         <f t="shared" si="9"/>
-        <v>-180</v>
+        <v>-187</v>
       </c>
       <c r="S48">
         <f t="shared" si="10"/>
@@ -8527,7 +8527,7 @@
       </c>
       <c r="X48">
         <f t="shared" si="15"/>
-        <v>0.82122370936902489</v>
+        <v>-9.2863882405522166E-3</v>
       </c>
       <c r="Y48">
         <f t="shared" si="16"/>
@@ -8620,7 +8620,7 @@
       </c>
       <c r="R49">
         <f t="shared" si="9"/>
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="S49">
         <f t="shared" si="10"/>
@@ -8644,7 +8644,7 @@
       </c>
       <c r="X49">
         <f t="shared" si="15"/>
-        <v>1.0547147846332945</v>
+        <v>2.2385216231663174E-3</v>
       </c>
       <c r="Y49">
         <f t="shared" si="16"/>
@@ -8737,7 +8737,7 @@
       </c>
       <c r="R50">
         <f t="shared" si="9"/>
-        <v>-97</v>
+        <v>-106</v>
       </c>
       <c r="S50">
         <f t="shared" si="10"/>
@@ -8761,7 +8761,7 @@
       </c>
       <c r="X50">
         <f t="shared" si="15"/>
-        <v>0.88300220750551872</v>
+        <v>-4.8397406629531545E-3</v>
       </c>
       <c r="Y50">
         <f t="shared" si="16"/>
@@ -8854,7 +8854,7 @@
       </c>
       <c r="R51">
         <f t="shared" si="9"/>
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="S51">
         <f t="shared" si="10"/>
@@ -8878,7 +8878,7 @@
       </c>
       <c r="X51">
         <f t="shared" si="15"/>
-        <v>1.04</v>
+        <v>1.4095674389921593E-3</v>
       </c>
       <c r="Y51">
         <f t="shared" si="16"/>
@@ -8971,7 +8971,7 @@
       </c>
       <c r="R52">
         <f t="shared" si="9"/>
-        <v>-49</v>
+        <v>-62</v>
       </c>
       <c r="S52">
         <f t="shared" si="10"/>
@@ -8995,7 +8995,7 @@
       </c>
       <c r="X52">
         <f t="shared" si="15"/>
-        <v>0.92548076923076927</v>
+        <v>-2.6344862751763406E-3</v>
       </c>
       <c r="Y52">
         <f t="shared" si="16"/>
@@ -9088,7 +9088,7 @@
       </c>
       <c r="R53">
         <f t="shared" si="9"/>
-        <v>248</v>
+        <v>326</v>
       </c>
       <c r="S53">
         <f t="shared" si="10"/>
@@ -9112,7 +9112,7 @@
       </c>
       <c r="X53">
         <f t="shared" si="15"/>
-        <v>1.4233766233766234</v>
+        <v>1.3413429888084265E-2</v>
       </c>
       <c r="Y53">
         <f t="shared" si="16"/>
@@ -9205,7 +9205,7 @@
       </c>
       <c r="R54">
         <f t="shared" si="9"/>
-        <v>109</v>
+        <v>146</v>
       </c>
       <c r="S54">
         <f t="shared" si="10"/>
@@ -9229,7 +9229,7 @@
       </c>
       <c r="X54">
         <f t="shared" si="15"/>
-        <v>1.1332116788321167</v>
+        <v>5.7480314960629917E-3</v>
       </c>
       <c r="Y54">
         <f t="shared" si="16"/>
@@ -9322,7 +9322,7 @@
       </c>
       <c r="R55">
         <f t="shared" si="9"/>
-        <v>-88</v>
+        <v>-50</v>
       </c>
       <c r="S55">
         <f t="shared" si="10"/>
@@ -9346,7 +9346,7 @@
       </c>
       <c r="X55">
         <f t="shared" si="15"/>
-        <v>0.95974235104669892</v>
+        <v>-1.8767359807822235E-3</v>
       </c>
       <c r="Y55">
         <f t="shared" si="16"/>
@@ -9439,7 +9439,7 @@
       </c>
       <c r="R56">
         <f t="shared" si="9"/>
-        <v>-122</v>
+        <v>-231</v>
       </c>
       <c r="S56">
         <f t="shared" si="10"/>
@@ -9463,7 +9463,7 @@
       </c>
       <c r="X56">
         <f t="shared" si="15"/>
-        <v>0.80620805369127513</v>
+        <v>-8.2992024143134294E-3</v>
       </c>
       <c r="Y56">
         <f t="shared" si="16"/>
@@ -9556,7 +9556,7 @@
       </c>
       <c r="R57">
         <f t="shared" si="9"/>
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="S57">
         <f t="shared" si="10"/>
@@ -9580,7 +9580,7 @@
       </c>
       <c r="X57">
         <f t="shared" si="15"/>
-        <v>1.0842872008324662</v>
+        <v>2.81298836603577E-3</v>
       </c>
       <c r="Y57">
         <f t="shared" si="16"/>
@@ -9673,7 +9673,7 @@
       </c>
       <c r="R58">
         <f t="shared" si="9"/>
-        <v>-103</v>
+        <v>-130</v>
       </c>
       <c r="S58">
         <f t="shared" si="10"/>
@@ -9697,7 +9697,7 @@
       </c>
       <c r="X58">
         <f t="shared" si="15"/>
-        <v>0.87523992322456812</v>
+        <v>-4.3570064014478663E-3</v>
       </c>
       <c r="Y58">
         <f t="shared" si="16"/>
@@ -9790,7 +9790,7 @@
       </c>
       <c r="R59">
         <f t="shared" si="9"/>
-        <v>130</v>
+        <v>234</v>
       </c>
       <c r="S59">
         <f t="shared" si="10"/>
@@ -9814,7 +9814,7 @@
       </c>
       <c r="X59">
         <f t="shared" si="15"/>
-        <v>1.256578947368421</v>
+        <v>7.6100035773521094E-3</v>
       </c>
       <c r="Y59">
         <f t="shared" si="16"/>
@@ -9907,7 +9907,7 @@
       </c>
       <c r="R60">
         <f t="shared" si="9"/>
-        <v>237</v>
+        <v>313</v>
       </c>
       <c r="S60">
         <f t="shared" si="10"/>
@@ -9931,7 +9931,7 @@
       </c>
       <c r="X60">
         <f t="shared" si="15"/>
-        <v>1.2731239092495636</v>
+        <v>9.8134503840727385E-3</v>
       </c>
       <c r="Y60">
         <f t="shared" si="16"/>
@@ -10024,7 +10024,7 @@
       </c>
       <c r="R61">
         <f t="shared" si="9"/>
-        <v>-207</v>
+        <v>-354</v>
       </c>
       <c r="S61">
         <f t="shared" si="10"/>
@@ -10048,7 +10048,7 @@
       </c>
       <c r="X61">
         <f t="shared" si="15"/>
-        <v>0.75736806031528447</v>
+        <v>-1.0613419679798525E-2</v>
       </c>
       <c r="Y61">
         <f t="shared" si="16"/>
@@ -10141,7 +10141,7 @@
       </c>
       <c r="R62">
         <f t="shared" si="9"/>
-        <v>-89</v>
+        <v>-8</v>
       </c>
       <c r="S62">
         <f t="shared" si="10"/>
@@ -10165,7 +10165,7 @@
       </c>
       <c r="X62">
         <f t="shared" si="15"/>
-        <v>0.99276018099547514</v>
+        <v>-2.3215995821120752E-4</v>
       </c>
       <c r="Y62">
         <f t="shared" si="16"/>
@@ -10258,7 +10258,7 @@
       </c>
       <c r="R63">
         <f t="shared" si="9"/>
-        <v>-22</v>
+        <v>-170</v>
       </c>
       <c r="S63">
         <f t="shared" si="10"/>
@@ -10282,7 +10282,7 @@
       </c>
       <c r="X63">
         <f t="shared" si="15"/>
-        <v>0.84503190519598903</v>
+        <v>-4.781190235122061E-3</v>
       </c>
       <c r="Y63">
         <f t="shared" si="16"/>
@@ -10375,7 +10375,7 @@
       </c>
       <c r="R64">
         <f t="shared" si="9"/>
-        <v>425</v>
+        <v>604</v>
       </c>
       <c r="S64">
         <f t="shared" si="10"/>
@@ -10399,7 +10399,7 @@
       </c>
       <c r="X64">
         <f t="shared" si="15"/>
-        <v>1.651564185544768</v>
+        <v>1.6555656058986377E-2</v>
       </c>
       <c r="Y64">
         <f t="shared" si="16"/>
@@ -10492,7 +10492,7 @@
       </c>
       <c r="R65">
         <f t="shared" si="9"/>
-        <v>-297</v>
+        <v>-452</v>
       </c>
       <c r="S65">
         <f t="shared" si="10"/>
@@ -10516,7 +10516,7 @@
       </c>
       <c r="X65">
         <f t="shared" si="15"/>
-        <v>0.70476812540822986</v>
+        <v>-1.1890356184563583E-2</v>
       </c>
       <c r="Y65">
         <f t="shared" si="16"/>
@@ -10609,7 +10609,7 @@
       </c>
       <c r="R66">
         <f t="shared" si="9"/>
-        <v>88</v>
+        <v>184</v>
       </c>
       <c r="S66">
         <f t="shared" si="10"/>
@@ -10633,7 +10633,7 @@
       </c>
       <c r="X66">
         <f t="shared" si="15"/>
-        <v>1.1705282669138091</v>
+        <v>4.7067249891284881E-3</v>
       </c>
       <c r="Y66">
         <f t="shared" si="16"/>
@@ -10726,7 +10726,7 @@
       </c>
       <c r="R67">
         <f t="shared" si="9"/>
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="S67">
         <f t="shared" si="10"/>
@@ -10750,7 +10750,7 @@
       </c>
       <c r="X67">
         <f t="shared" si="15"/>
-        <v>1.0237529691211402</v>
+        <v>7.4338388343740713E-4</v>
       </c>
       <c r="Y67">
         <f t="shared" si="16"/>
@@ -10843,7 +10843,7 @@
       </c>
       <c r="R68">
         <f t="shared" si="9"/>
-        <v>-392</v>
+        <v>-285</v>
       </c>
       <c r="S68">
         <f t="shared" si="10"/>
@@ -10867,7 +10867,7 @@
       </c>
       <c r="X68">
         <f t="shared" si="15"/>
-        <v>0.77958236658932711</v>
+        <v>-6.84290139018944E-3</v>
       </c>
       <c r="Y68">
         <f t="shared" si="16"/>
@@ -10960,7 +10960,7 @@
       </c>
       <c r="R69">
         <f t="shared" si="9"/>
-        <v>151</v>
+        <v>-2</v>
       </c>
       <c r="S69">
         <f t="shared" si="10"/>
@@ -10984,7 +10984,7 @@
       </c>
       <c r="X69">
         <f t="shared" si="15"/>
-        <v>0.99801587301587302</v>
+        <v>-4.688562252385306E-5</v>
       </c>
       <c r="Y69">
         <f t="shared" si="16"/>
@@ -11077,7 +11077,7 @@
       </c>
       <c r="R70">
         <f t="shared" si="9"/>
-        <v>-118</v>
+        <v>-108</v>
       </c>
       <c r="S70">
         <f t="shared" si="10"/>
@@ -11101,7 +11101,7 @@
       </c>
       <c r="X70">
         <f t="shared" si="15"/>
-        <v>0.89264413518886676</v>
+        <v>-2.4734901403934682E-3</v>
       </c>
       <c r="Y70">
         <f t="shared" si="16"/>
@@ -11218,7 +11218,7 @@
       </c>
       <c r="X71">
         <f t="shared" si="15"/>
-        <v>1.4610244988864143</v>
+        <v>9.2906353089024039E-3</v>
       </c>
       <c r="Y71">
         <f t="shared" si="16"/>
@@ -11311,7 +11311,7 @@
       </c>
       <c r="R72">
         <f t="shared" si="9"/>
-        <v>-363</v>
+        <v>-287</v>
       </c>
       <c r="S72">
         <f t="shared" si="10"/>
@@ -11335,7 +11335,7 @@
       </c>
       <c r="X72">
         <f t="shared" si="15"/>
-        <v>0.78125</v>
+        <v>-6.2564035489285639E-3</v>
       </c>
       <c r="Y72">
         <f t="shared" si="16"/>
@@ -11427,8 +11427,8 @@
         <v>0.22917015575280522</v>
       </c>
       <c r="R73">
-        <f t="shared" ref="R73:R136" si="31">+I73-I72</f>
-        <v>-27</v>
+        <f t="shared" ref="R73:R136" si="31">+G73-G72</f>
+        <v>-155</v>
       </c>
       <c r="S73">
         <f t="shared" ref="S73:S136" si="32">+J73-J72</f>
@@ -11451,8 +11451,8 @@
         <v>1</v>
       </c>
       <c r="X73">
-        <f t="shared" ref="X73:X136" si="37">+IFERROR(G73/G72,0)</f>
-        <v>0.84878048780487803</v>
+        <f t="shared" ref="X73:X136" si="37">+IFERROR(R73/F72,0)</f>
+        <v>-3.3050449912576229E-3</v>
       </c>
       <c r="Y73">
         <f t="shared" ref="Y73:Y136" si="38">+IFERROR(K73/K72,0)</f>
@@ -11545,7 +11545,7 @@
       </c>
       <c r="R74">
         <f t="shared" si="31"/>
-        <v>396</v>
+        <v>466</v>
       </c>
       <c r="S74">
         <f t="shared" si="32"/>
@@ -11569,7 +11569,7 @@
       </c>
       <c r="X74">
         <f t="shared" si="37"/>
-        <v>1.535632183908046</v>
+        <v>9.7554848434098142E-3</v>
       </c>
       <c r="Y74">
         <f t="shared" si="38"/>
@@ -11662,7 +11662,7 @@
       </c>
       <c r="R75">
         <f t="shared" si="31"/>
-        <v>-56</v>
+        <v>-92</v>
       </c>
       <c r="S75">
         <f t="shared" si="32"/>
@@ -11686,7 +11686,7 @@
       </c>
       <c r="X75">
         <f t="shared" si="37"/>
-        <v>0.93113772455089816</v>
+        <v>-1.8735744542196155E-3</v>
       </c>
       <c r="Y75">
         <f t="shared" si="38"/>
@@ -11779,7 +11779,7 @@
       </c>
       <c r="R76">
         <f t="shared" si="31"/>
-        <v>-462</v>
+        <v>-487</v>
       </c>
       <c r="S76">
         <f t="shared" si="32"/>
@@ -11803,7 +11803,7 @@
       </c>
       <c r="X76">
         <f t="shared" si="37"/>
-        <v>0.60852090032154338</v>
+        <v>-9.6726781600063559E-3</v>
       </c>
       <c r="Y76">
         <f t="shared" si="38"/>
@@ -11896,7 +11896,7 @@
       </c>
       <c r="R77">
         <f t="shared" si="31"/>
-        <v>-43</v>
+        <v>953</v>
       </c>
       <c r="S77">
         <f t="shared" si="32"/>
@@ -11920,7 +11920,7 @@
       </c>
       <c r="X77">
         <f t="shared" si="37"/>
-        <v>2.2589167767503304</v>
+        <v>1.8647881811955778E-2</v>
       </c>
       <c r="Y77">
         <f t="shared" si="38"/>
@@ -12013,7 +12013,7 @@
       </c>
       <c r="R78">
         <f t="shared" si="31"/>
-        <v>126</v>
+        <v>-1884</v>
       </c>
       <c r="S78">
         <f t="shared" si="32"/>
@@ -12037,7 +12037,7 @@
       </c>
       <c r="X78">
         <f t="shared" si="37"/>
-        <v>-0.10175438596491228</v>
+        <v>-3.5671684180630506E-2</v>
       </c>
       <c r="Y78">
         <f t="shared" si="38"/>
@@ -12130,7 +12130,7 @@
       </c>
       <c r="R79">
         <f t="shared" si="31"/>
-        <v>432</v>
+        <v>1461</v>
       </c>
       <c r="S79">
         <f t="shared" si="32"/>
@@ -12154,7 +12154,7 @@
       </c>
       <c r="X79">
         <f t="shared" si="37"/>
-        <v>-7.3965517241379306</v>
+        <v>2.7754032028266939E-2</v>
       </c>
       <c r="Y79">
         <f t="shared" si="38"/>
@@ -12247,7 +12247,7 @@
       </c>
       <c r="R80">
         <f t="shared" si="31"/>
-        <v>-237</v>
+        <v>-197</v>
       </c>
       <c r="S80">
         <f t="shared" si="32"/>
@@ -12271,7 +12271,7 @@
       </c>
       <c r="X80">
         <f t="shared" si="37"/>
-        <v>0.84693084693084697</v>
+        <v>-3.6530188399347277E-3</v>
       </c>
       <c r="Y80">
         <f t="shared" si="38"/>
@@ -12364,7 +12364,7 @@
       </c>
       <c r="R81">
         <f t="shared" si="31"/>
-        <v>485</v>
+        <v>647</v>
       </c>
       <c r="S81">
         <f t="shared" si="32"/>
@@ -12388,7 +12388,7 @@
       </c>
       <c r="X81">
         <f t="shared" si="37"/>
-        <v>1.5935779816513762</v>
+        <v>1.1759787705841724E-2</v>
       </c>
       <c r="Y81">
         <f t="shared" si="38"/>
@@ -12505,7 +12505,7 @@
       </c>
       <c r="X82">
         <f t="shared" si="37"/>
-        <v>0.85492227979274615</v>
+        <v>-4.4401374328253019E-3</v>
       </c>
       <c r="Y82">
         <f t="shared" si="38"/>
@@ -12598,7 +12598,7 @@
       </c>
       <c r="R83">
         <f t="shared" si="31"/>
-        <v>-308</v>
+        <v>-386</v>
       </c>
       <c r="S83">
         <f t="shared" si="32"/>
@@ -12622,7 +12622,7 @@
       </c>
       <c r="X83">
         <f t="shared" si="37"/>
-        <v>0.7400673400673401</v>
+        <v>-6.6277472527472526E-3</v>
       </c>
       <c r="Y83">
         <f t="shared" si="38"/>
@@ -12715,7 +12715,7 @@
       </c>
       <c r="R84">
         <f t="shared" si="31"/>
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="S84">
         <f t="shared" si="32"/>
@@ -12739,7 +12739,7 @@
       </c>
       <c r="X84">
         <f t="shared" si="37"/>
-        <v>1.1455868971792538</v>
+        <v>2.6963716948381336E-3</v>
       </c>
       <c r="Y84">
         <f t="shared" si="38"/>
@@ -12832,7 +12832,7 @@
       </c>
       <c r="R85">
         <f t="shared" si="31"/>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="S85">
         <f t="shared" si="32"/>
@@ -12856,7 +12856,7 @@
       </c>
       <c r="X85">
         <f t="shared" si="37"/>
-        <v>1.0301826846703732</v>
+        <v>6.270834020924783E-4</v>
       </c>
       <c r="Y85">
         <f t="shared" si="38"/>
@@ -12949,7 +12949,7 @@
       </c>
       <c r="R86">
         <f t="shared" si="31"/>
-        <v>-122</v>
+        <v>10</v>
       </c>
       <c r="S86">
         <f t="shared" si="32"/>
@@ -12973,7 +12973,7 @@
       </c>
       <c r="X86">
         <f t="shared" si="37"/>
-        <v>1.0077101002313029</v>
+        <v>1.6156393892883107E-4</v>
       </c>
       <c r="Y86">
         <f t="shared" si="38"/>
@@ -13066,7 +13066,7 @@
       </c>
       <c r="R87">
         <f t="shared" si="31"/>
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="S87">
         <f t="shared" si="32"/>
@@ -13090,7 +13090,7 @@
       </c>
       <c r="X87">
         <f t="shared" si="37"/>
-        <v>1.1009946442234124</v>
+        <v>2.088541501851207E-3</v>
       </c>
       <c r="Y87">
         <f t="shared" si="38"/>
@@ -13183,7 +13183,7 @@
       </c>
       <c r="R88">
         <f t="shared" si="31"/>
-        <v>-7</v>
+        <v>112</v>
       </c>
       <c r="S88">
         <f t="shared" si="32"/>
@@ -13207,7 +13207,7 @@
       </c>
       <c r="X88">
         <f t="shared" si="37"/>
-        <v>1.0778318276580958</v>
+        <v>1.7326464627713061E-3</v>
       </c>
       <c r="Y88">
         <f t="shared" si="38"/>
@@ -13300,7 +13300,7 @@
       </c>
       <c r="R89">
         <f t="shared" si="31"/>
-        <v>25</v>
+        <v>-13</v>
       </c>
       <c r="S89">
         <f t="shared" si="32"/>
@@ -13324,7 +13324,7 @@
       </c>
       <c r="X89">
         <f t="shared" si="37"/>
-        <v>0.99161831076724694</v>
+        <v>-1.9639835629683345E-4</v>
       </c>
       <c r="Y89">
         <f t="shared" si="38"/>
@@ -13417,7 +13417,7 @@
       </c>
       <c r="R90">
         <f t="shared" si="31"/>
-        <v>-471</v>
+        <v>-633</v>
       </c>
       <c r="S90">
         <f t="shared" si="32"/>
@@ -13441,7 +13441,7 @@
       </c>
       <c r="X90">
         <f t="shared" si="37"/>
-        <v>0.58842652795838757</v>
+        <v>-9.3459323785619365E-3</v>
       </c>
       <c r="Y90">
         <f t="shared" si="38"/>
@@ -13534,7 +13534,7 @@
       </c>
       <c r="R91">
         <f t="shared" si="31"/>
-        <v>18</v>
+        <v>-57</v>
       </c>
       <c r="S91">
         <f t="shared" si="32"/>
@@ -13558,7 +13558,7 @@
       </c>
       <c r="X91">
         <f t="shared" si="37"/>
-        <v>0.93701657458563536</v>
+        <v>-8.3048007576309467E-4</v>
       </c>
       <c r="Y91">
         <f t="shared" si="38"/>
@@ -13651,7 +13651,7 @@
       </c>
       <c r="R92">
         <f t="shared" si="31"/>
-        <v>533</v>
+        <v>808</v>
       </c>
       <c r="S92">
         <f t="shared" si="32"/>
@@ -13675,7 +13675,7 @@
       </c>
       <c r="X92">
         <f t="shared" si="37"/>
-        <v>1.9528301886792452</v>
+        <v>1.1628743721485832E-2</v>
       </c>
       <c r="Y92">
         <f t="shared" si="38"/>
@@ -13768,7 +13768,7 @@
       </c>
       <c r="R93">
         <f t="shared" si="31"/>
-        <v>-9</v>
+        <v>-98</v>
       </c>
       <c r="S93">
         <f t="shared" si="32"/>
@@ -13792,7 +13792,7 @@
       </c>
       <c r="X93">
         <f t="shared" si="37"/>
-        <v>0.9408212560386473</v>
+        <v>-1.3775847284892956E-3</v>
       </c>
       <c r="Y93">
         <f t="shared" si="38"/>
@@ -13885,7 +13885,7 @@
       </c>
       <c r="R94">
         <f t="shared" si="31"/>
-        <v>-20</v>
+        <v>-24</v>
       </c>
       <c r="S94">
         <f t="shared" si="32"/>
@@ -13909,7 +13909,7 @@
       </c>
       <c r="X94">
         <f t="shared" si="37"/>
-        <v>0.98459563543003847</v>
+        <v>-3.3013741970095052E-4</v>
       </c>
       <c r="Y94">
         <f t="shared" si="38"/>
@@ -14002,7 +14002,7 @@
       </c>
       <c r="R95">
         <f t="shared" si="31"/>
-        <v>127</v>
+        <v>238</v>
       </c>
       <c r="S95">
         <f t="shared" si="32"/>
@@ -14026,7 +14026,7 @@
       </c>
       <c r="X95">
         <f t="shared" si="37"/>
-        <v>1.1551499348109517</v>
+        <v>3.2062076490953916E-3</v>
       </c>
       <c r="Y95">
         <f t="shared" si="38"/>
@@ -14119,7 +14119,7 @@
       </c>
       <c r="R96">
         <f t="shared" si="31"/>
-        <v>-51</v>
+        <v>-183</v>
       </c>
       <c r="S96">
         <f t="shared" si="32"/>
@@ -14143,7 +14143,7 @@
       </c>
       <c r="X96">
         <f t="shared" si="37"/>
-        <v>0.89672686230248311</v>
+        <v>-2.4077996921174163E-3</v>
       </c>
       <c r="Y96">
         <f t="shared" si="38"/>
@@ -14236,7 +14236,7 @@
       </c>
       <c r="R97">
         <f t="shared" si="31"/>
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="S97">
         <f t="shared" si="32"/>
@@ -14260,7 +14260,7 @@
       </c>
       <c r="X97">
         <f t="shared" si="37"/>
-        <v>1.0547514159848961</v>
+        <v>1.1212496133622023E-3</v>
       </c>
       <c r="Y97">
         <f t="shared" si="38"/>
@@ -14353,7 +14353,7 @@
       </c>
       <c r="R98">
         <f t="shared" si="31"/>
-        <v>-187</v>
+        <v>-224</v>
       </c>
       <c r="S98">
         <f t="shared" si="32"/>
@@ -14377,7 +14377,7 @@
       </c>
       <c r="X98">
         <f t="shared" si="37"/>
-        <v>0.86634844868735084</v>
+        <v>-2.8258565877781702E-3</v>
       </c>
       <c r="Y98">
         <f t="shared" si="38"/>
@@ -14470,7 +14470,7 @@
       </c>
       <c r="R99">
         <f t="shared" si="31"/>
-        <v>345</v>
+        <v>602</v>
       </c>
       <c r="S99">
         <f t="shared" si="32"/>
@@ -14494,7 +14494,7 @@
       </c>
       <c r="X99">
         <f t="shared" si="37"/>
-        <v>1.4146005509641872</v>
+        <v>7.4578790882061444E-3</v>
       </c>
       <c r="Y99">
         <f t="shared" si="38"/>
@@ -14587,7 +14587,7 @@
       </c>
       <c r="R100">
         <f t="shared" si="31"/>
-        <v>136</v>
+        <v>179</v>
       </c>
       <c r="S100">
         <f t="shared" si="32"/>
@@ -14611,7 +14611,7 @@
       </c>
       <c r="X100">
         <f t="shared" si="37"/>
-        <v>1.0871470301850048</v>
+        <v>2.1625147993331239E-3</v>
       </c>
       <c r="Y100">
         <f t="shared" si="38"/>
@@ -14704,7 +14704,7 @@
       </c>
       <c r="R101">
         <f t="shared" si="31"/>
-        <v>-117</v>
+        <v>-199</v>
       </c>
       <c r="S101">
         <f t="shared" si="32"/>
@@ -14728,7 +14728,7 @@
       </c>
       <c r="X101">
         <f t="shared" si="37"/>
-        <v>0.91088222122704876</v>
+        <v>-2.3409836836966367E-3</v>
       </c>
       <c r="Y101">
         <f t="shared" si="38"/>
@@ -14821,7 +14821,7 @@
       </c>
       <c r="R102">
         <f t="shared" si="31"/>
-        <v>-66613</v>
+        <v>-89075</v>
       </c>
       <c r="S102">
         <f t="shared" si="32"/>
@@ -14845,7 +14845,7 @@
       </c>
       <c r="X102">
         <f t="shared" si="37"/>
-        <v>-42.793018682399214</v>
+        <v>-1.0233682976987857</v>
       </c>
       <c r="Y102">
         <f t="shared" si="38"/>
@@ -14938,7 +14938,7 @@
       </c>
       <c r="R103">
         <f t="shared" si="31"/>
-        <v>65209</v>
+        <v>87041</v>
       </c>
       <c r="S103">
         <f t="shared" si="32"/>
@@ -18915,7 +18915,7 @@
         <v>0</v>
       </c>
       <c r="R137">
-        <f t="shared" ref="R137:R200" si="53">+I137-I136</f>
+        <f t="shared" ref="R137:R200" si="53">+G137-G136</f>
         <v>0</v>
       </c>
       <c r="S137">
@@ -18939,7 +18939,7 @@
         <v>0</v>
       </c>
       <c r="X137">
-        <f t="shared" ref="X137:X200" si="59">+IFERROR(G137/G136,0)</f>
+        <f t="shared" ref="X137:X200" si="59">+IFERROR(R137/F136,0)</f>
         <v>0</v>
       </c>
       <c r="Y137">
@@ -26403,7 +26403,7 @@
         <v>0</v>
       </c>
       <c r="R201">
-        <f t="shared" ref="R201:R264" si="75">+I201-I200</f>
+        <f t="shared" ref="R201:R264" si="75">+G201-G200</f>
         <v>0</v>
       </c>
       <c r="S201">
@@ -26427,7 +26427,7 @@
         <v>0</v>
       </c>
       <c r="X201">
-        <f t="shared" ref="X201:X264" si="81">+IFERROR(G201/G200,0)</f>
+        <f t="shared" ref="X201:X264" si="81">+IFERROR(R201/F200,0)</f>
         <v>0</v>
       </c>
       <c r="Y201">
@@ -33891,7 +33891,7 @@
         <v>0</v>
       </c>
       <c r="R265">
-        <f t="shared" ref="R265:R303" si="97">+I265-I264</f>
+        <f t="shared" ref="R265:R303" si="97">+G265-G264</f>
         <v>0</v>
       </c>
       <c r="S265">
@@ -33915,7 +33915,7 @@
         <v>0</v>
       </c>
       <c r="X265">
-        <f t="shared" ref="X265:X303" si="103">+IFERROR(G265/G264,0)</f>
+        <f t="shared" ref="X265:X303" si="103">+IFERROR(R265/F264,0)</f>
         <v>0</v>
       </c>
       <c r="Y265">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-14-2020 16-09-15
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1375" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2EC650AA-1737-794F-AE7B-91D346562D06}"/>
+  <xr:revisionPtr revIDLastSave="1385" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3FB7A635-B02E-4E46-8923-4E5AA1EAC4D1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="161">
   <si>
     <t>Columna1</t>
   </si>
@@ -346,24 +346,6 @@
     <t>12-06-2020</t>
   </si>
   <si>
-    <t>13-06-2020</t>
-  </si>
-  <si>
-    <t>13/6/2020</t>
-  </si>
-  <si>
-    <t>14/6/2020</t>
-  </si>
-  <si>
-    <t>15/6/2020</t>
-  </si>
-  <si>
-    <t>16/6/2020</t>
-  </si>
-  <si>
-    <t>17/6/2020</t>
-  </si>
-  <si>
     <t>18/6/2020</t>
   </si>
   <si>
@@ -519,6 +501,24 @@
   <si>
     <t>%Variación Personas Medidas Sanitarias</t>
   </si>
+  <si>
+    <t>13-06-20</t>
+  </si>
+  <si>
+    <t>14-06-20</t>
+  </si>
+  <si>
+    <t>15-06-20</t>
+  </si>
+  <si>
+    <t>16-06-20</t>
+  </si>
+  <si>
+    <t>17-06-20</t>
+  </si>
+  <si>
+    <t>18-06-20</t>
+  </si>
 </sst>
 </file>
 
@@ -635,7 +635,31 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="16">
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -866,15 +890,15 @@
     <tableColumn id="4" xr3:uid="{2FE879E2-2128-42AE-A0E3-647EE2D0C94F}" name="07-06-2020"/>
     <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="08-06-2020"/>
     <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-2020"/>
-    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020"/>
-    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020"/>
-    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020"/>
-    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-2020"/>
-    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="13/6/2020"/>
-    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="14/6/2020"/>
-    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="15/6/2020"/>
-    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="16/6/2020"/>
-    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="17/6/2020"/>
+    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="5"/>
+    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="4"/>
+    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="3"/>
+    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="2"/>
+    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="1"/>
+    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="0"/>
+    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20"/>
     <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="18/6/2020"/>
     <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="19/6/2020"/>
     <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="20/6/2020"/>
@@ -894,20 +918,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="14">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="13">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="11">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="10">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -940,10 +964,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="1">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="9">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="8">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1313,14 +1337,15 @@
   <dimension ref="A1:DK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CR1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CS7" sqref="CS7"/>
+      <pane xSplit="1" topLeftCell="CW1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CX1" sqref="CX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.09765625" customWidth="1"/>
     <col min="2" max="87" width="11.296875" customWidth="1"/>
+    <col min="94" max="101" width="11.43359375" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:115" x14ac:dyDescent="0.2">
@@ -1603,76 +1628,76 @@
       <c r="CO1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="CP1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="CQ1" s="1" t="s">
+      <c r="CQ1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" s="1" t="s">
+      <c r="CR1" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" s="1" t="s">
+      <c r="CS1" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="CT1" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="CU1" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="CV1" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="CW1" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="CX1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="CY1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="CT1" s="1" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" s="1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="DC1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="DD1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="DE1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DF1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DG1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="DH1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="DC1" s="1" t="s">
+      <c r="DI1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="DE1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="DF1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="DG1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="DH1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="DI1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="DJ1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B2" s="7">
         <v>146</v>
@@ -1950,22 +1975,22 @@
       <c r="CO2" s="8">
         <v>80720</v>
       </c>
-      <c r="CP2">
+      <c r="CP2" s="8">
         <v>82774</v>
       </c>
-      <c r="CQ2">
+      <c r="CQ2" s="8">
         <v>85007</v>
       </c>
-      <c r="CR2">
+      <c r="CR2" s="8">
         <v>87041</v>
       </c>
-      <c r="CS2">
+      <c r="CS2" s="8">
         <v>89736</v>
       </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B3" s="7">
         <v>138</v>
@@ -2243,22 +2268,22 @@
       <c r="CO3" s="8">
         <v>60899</v>
       </c>
-      <c r="CP3">
+      <c r="CP3" s="8">
         <v>62284</v>
       </c>
-      <c r="CQ3">
+      <c r="CQ3" s="8">
         <v>63805</v>
       </c>
-      <c r="CR3">
+      <c r="CR3" s="8">
         <v>65209</v>
       </c>
-      <c r="CS3">
+      <c r="CS3" s="8">
         <v>67027</v>
       </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B4" s="7">
         <v>6</v>
@@ -2536,22 +2561,22 @@
       <c r="CO4" s="8">
         <v>5122</v>
       </c>
-      <c r="CP4">
+      <c r="CP4" s="8">
         <v>5315</v>
       </c>
-      <c r="CQ4">
+      <c r="CQ4" s="8">
         <v>5910</v>
       </c>
-      <c r="CR4">
+      <c r="CR4" s="8">
         <v>3798</v>
       </c>
-      <c r="CS4">
+      <c r="CS4" s="8">
         <v>4607</v>
       </c>
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2738,22 +2763,22 @@
       <c r="CO5" s="8">
         <v>692</v>
       </c>
-      <c r="CP5">
+      <c r="CP5" s="8">
         <v>712</v>
       </c>
-      <c r="CQ5">
+      <c r="CQ5" s="8">
         <v>695</v>
       </c>
-      <c r="CR5">
+      <c r="CR5" s="8">
         <v>739</v>
       </c>
-      <c r="CS5">
+      <c r="CS5" s="8">
         <v>755</v>
       </c>
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -3027,22 +3052,22 @@
       <c r="CO6" s="8">
         <v>365</v>
       </c>
-      <c r="CP6">
+      <c r="CP6" s="8">
         <v>381</v>
       </c>
-      <c r="CQ6">
+      <c r="CQ6" s="8">
         <v>390</v>
       </c>
-      <c r="CR6">
+      <c r="CR6" s="8">
         <v>398</v>
       </c>
-      <c r="CS6">
+      <c r="CS6" s="8">
         <v>412</v>
       </c>
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -3318,16 +3343,16 @@
       <c r="CO7" s="8">
         <v>90</v>
       </c>
-      <c r="CP7">
+      <c r="CP7" s="8">
         <v>91</v>
       </c>
-      <c r="CQ7">
+      <c r="CQ7" s="8">
         <v>96</v>
       </c>
-      <c r="CR7">
+      <c r="CR7" s="8">
         <v>96</v>
       </c>
-      <c r="CS7">
+      <c r="CS7" s="8">
         <v>97</v>
       </c>
     </row>
@@ -3922,121 +3947,121 @@
     </row>
     <row r="6" spans="1:39" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="I6" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="J6" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="K6" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="L6" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="P6" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="Q6" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="G6" s="14" t="s">
+      <c r="R6" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="S6" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="H6" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="J6" s="14" t="s">
+      <c r="T6" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="U6" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="L6" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="P6" s="14" t="s">
+      <c r="V6" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="W6" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="X6" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y6" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA6" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB6" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC6" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD6" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE6" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="S6" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="T6" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="U6" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="V6" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="W6" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="X6" s="14" t="s">
+      <c r="AF6" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="Y6" s="14" t="s">
+      <c r="AG6" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="Z6" s="14" t="s">
+      <c r="AH6" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="AA6" s="14" t="s">
+      <c r="AI6" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="AB6" s="14" t="s">
+      <c r="AJ6" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="AC6" s="14" t="s">
+      <c r="AK6" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="AL6" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="AD6" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="AE6" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="AF6" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="AG6" s="14" t="s">
+      <c r="AM6" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="AH6" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="AI6" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="AJ6" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="AK6" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="AL6" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="AM6" s="14" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-15-2020 01-36-40
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1385" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3FB7A635-B02E-4E46-8923-4E5AA1EAC4D1}"/>
+  <xr:revisionPtr revIDLastSave="1392" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FAED9310-4CAC-F543-B254-B94FDA5152AD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="154">
   <si>
     <t>Columna1</t>
   </si>
@@ -637,30 +637,6 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -780,6 +756,30 @@
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -890,14 +890,14 @@
     <tableColumn id="4" xr3:uid="{2FE879E2-2128-42AE-A0E3-647EE2D0C94F}" name="07-06-2020"/>
     <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="08-06-2020"/>
     <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-2020"/>
-    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="5"/>
-    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="4"/>
-    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="3"/>
-    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="2"/>
-    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="1"/>
-    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="13"/>
+    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="12"/>
+    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="11"/>
+    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="10"/>
+    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="9"/>
+    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="8"/>
     <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20"/>
     <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="18/6/2020"/>
     <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="19/6/2020"/>
@@ -918,20 +918,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="6">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="13">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="5">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="11">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="3">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="10">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="2">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -964,10 +964,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="9">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="1">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="8">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="0">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1337,8 +1337,8 @@
   <dimension ref="A1:DK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CW1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CX1" sqref="CX1"/>
+      <pane xSplit="1" topLeftCell="CS1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CT7" sqref="CT7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1987,6 +1987,9 @@
       <c r="CS2" s="8">
         <v>89736</v>
       </c>
+      <c r="CT2" s="8">
+        <v>91637</v>
+      </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2280,6 +2283,9 @@
       <c r="CS3" s="8">
         <v>67027</v>
       </c>
+      <c r="CT3" s="8">
+        <v>68280</v>
+      </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2572,6 +2578,9 @@
       </c>
       <c r="CS4" s="8">
         <v>4607</v>
+      </c>
+      <c r="CT4" s="8">
+        <v>5157</v>
       </c>
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.2">
@@ -2775,6 +2784,9 @@
       <c r="CS5" s="8">
         <v>755</v>
       </c>
+      <c r="CT5" s="8">
+        <v>804</v>
+      </c>
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3064,6 +3076,9 @@
       <c r="CS6" s="8">
         <v>412</v>
       </c>
+      <c r="CT6" s="8">
+        <v>420</v>
+      </c>
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -3354,6 +3369,9 @@
       </c>
       <c r="CS7" s="8">
         <v>97</v>
+      </c>
+      <c r="CT7" s="8">
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:115" x14ac:dyDescent="0.2">
@@ -3938,7 +3956,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>43995</v>
+        <v>43996</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -18917,7 +18935,7 @@
       </c>
       <c r="B102" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C102" s="12">
         <v>96</v>
@@ -19070,11 +19088,11 @@
     <row r="103" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A103" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B103" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C103" s="12">
         <v>97</v>
@@ -19089,139 +19107,139 @@
       </c>
       <c r="F103" cm="1">
         <f t="array" ref="F103">+INDEX(Hoja1!$B$2:$MO$7,1,E103)</f>
-        <v>0</v>
+        <v>91637</v>
       </c>
       <c r="G103">
         <f t="shared" si="41"/>
-        <v>-89736</v>
+        <v>1901</v>
       </c>
       <c r="H103" cm="1">
         <f t="array" ref="H103">+INDEX(Hoja1!$B$2:$MO$7,2,$E103)</f>
-        <v>0</v>
+        <v>68280</v>
       </c>
       <c r="I103">
         <f t="shared" si="42"/>
-        <v>-67027</v>
+        <v>1253</v>
       </c>
       <c r="J103">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>23357</v>
       </c>
       <c r="K103">
         <f t="shared" si="43"/>
-        <v>-22709</v>
+        <v>648</v>
       </c>
       <c r="L103" cm="1">
         <f t="array" ref="L103">+INDEX(Hoja1!$B$2:$MO$7,3,$E103)</f>
-        <v>0</v>
+        <v>5157</v>
       </c>
       <c r="M103" cm="1">
         <f t="array" ref="M103">+INDEX(Hoja1!$B$2:$MO$7,4,$E103)</f>
-        <v>0</v>
+        <v>804</v>
       </c>
       <c r="N103" cm="1">
         <f t="array" ref="N103">+INDEX(Hoja1!$B$2:$MO$7,5,$E103)</f>
-        <v>0</v>
+        <v>420</v>
       </c>
       <c r="O103" cm="1">
         <f t="array" ref="O103">+INDEX(Hoja1!$B$2:$MO$7,6,$E103)</f>
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="P103" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.74511387321715028</v>
       </c>
       <c r="Q103" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.25488612678284972</v>
       </c>
       <c r="R103">
         <f t="shared" si="44"/>
-        <v>-92431</v>
+        <v>-794</v>
       </c>
       <c r="S103">
         <f t="shared" si="45"/>
-        <v>-22709</v>
+        <v>648</v>
       </c>
       <c r="T103">
         <f t="shared" si="46"/>
-        <v>-4607</v>
+        <v>550</v>
       </c>
       <c r="U103">
         <f t="shared" si="47"/>
-        <v>-755</v>
+        <v>49</v>
       </c>
       <c r="V103">
         <f t="shared" si="48"/>
-        <v>-412</v>
+        <v>8</v>
       </c>
       <c r="W103">
         <f t="shared" si="49"/>
-        <v>-97</v>
+        <v>5</v>
       </c>
       <c r="X103">
         <f t="shared" si="50"/>
-        <v>-34.297217068645637</v>
+        <v>-0.29461966604823747</v>
       </c>
       <c r="Y103">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.8534942093443129E-2</v>
       </c>
       <c r="Z103">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.1193835467766442</v>
       </c>
       <c r="AA103">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1.0649006622516557</v>
       </c>
       <c r="AB103">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0194174757281553</v>
       </c>
       <c r="AC103">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.0515463917525774</v>
       </c>
       <c r="AD103">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>22033.421495551815</v>
       </c>
       <c r="AE103">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>5616.0134647751865</v>
       </c>
       <c r="AF103">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1239.9615292137535</v>
       </c>
       <c r="AG103">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>193.31570088963693</v>
       </c>
       <c r="AH103">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>100.98581389757153</v>
       </c>
       <c r="AI103">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>24.525126232267372</v>
       </c>
       <c r="AJ103">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>6483</v>
       </c>
       <c r="AK103">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>1558.7881702332293</v>
       </c>
       <c r="AL103">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ102</f>
-        <v>-5871</v>
+        <v>612</v>
       </c>
       <c r="AM103">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ102,0)</f>
-        <v>-1</v>
+        <v>0.10424118548799183</v>
       </c>
     </row>
     <row r="104" spans="1:39" x14ac:dyDescent="0.2">
@@ -19250,7 +19268,7 @@
       </c>
       <c r="G104">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-91637</v>
       </c>
       <c r="H104" cm="1">
         <f t="array" ref="H104">+INDEX(Hoja1!$B$2:$MO$7,2,$E104)</f>
@@ -19258,7 +19276,7 @@
       </c>
       <c r="I104">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-68280</v>
       </c>
       <c r="J104">
         <f t="shared" si="33"/>
@@ -19266,7 +19284,7 @@
       </c>
       <c r="K104">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-23357</v>
       </c>
       <c r="L104" cm="1">
         <f t="array" ref="L104">+INDEX(Hoja1!$B$2:$MO$7,3,$E104)</f>
@@ -19294,35 +19312,35 @@
       </c>
       <c r="R104">
         <f t="shared" si="44"/>
-        <v>89736</v>
+        <v>-93538</v>
       </c>
       <c r="S104">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-23357</v>
       </c>
       <c r="T104">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-5157</v>
       </c>
       <c r="U104">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-804</v>
       </c>
       <c r="V104">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-420</v>
       </c>
       <c r="W104">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-102</v>
       </c>
       <c r="X104">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-49.204629142556549</v>
       </c>
       <c r="Y104">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z104">
         <f t="shared" si="52"/>
@@ -19374,11 +19392,11 @@
       </c>
       <c r="AL104">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ103</f>
-        <v>0</v>
+        <v>-6483</v>
       </c>
       <c r="AM104">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ103,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="105" spans="1:39" x14ac:dyDescent="0.2">
@@ -19451,7 +19469,7 @@
       </c>
       <c r="R105">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>91637</v>
       </c>
       <c r="S105">
         <f t="shared" si="45"/>
@@ -19475,7 +19493,7 @@
       </c>
       <c r="X105">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y105">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-17-2020 16-31-55
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1398" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0A8BADC1-A59C-C941-9D59-723B5EEB81C0}"/>
+  <xr:revisionPtr revIDLastSave="1404" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{78DB8EBD-F3BC-084A-9CBA-DC3C37FE64F2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -1337,8 +1337,8 @@
   <dimension ref="A1:DK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CS1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CU8" sqref="CU8"/>
+      <pane xSplit="1" topLeftCell="CT1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CW6" sqref="CW6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1993,6 +1993,9 @@
       <c r="CU2" s="8">
         <v>93646</v>
       </c>
+      <c r="CV2" s="8">
+        <v>95299</v>
+      </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2292,6 +2295,9 @@
       <c r="CU3" s="8">
         <v>69528</v>
       </c>
+      <c r="CV3" s="8">
+        <v>70633</v>
+      </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2590,6 +2596,9 @@
       </c>
       <c r="CU4" s="8">
         <v>5824</v>
+      </c>
+      <c r="CV4" s="8">
+        <v>6325</v>
       </c>
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.2">
@@ -2799,6 +2808,9 @@
       <c r="CU5" s="8">
         <v>833</v>
       </c>
+      <c r="CV5" s="8">
+        <v>813</v>
+      </c>
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3094,6 +3106,9 @@
       <c r="CU6" s="8">
         <v>449</v>
       </c>
+      <c r="CV6" s="8">
+        <v>486</v>
+      </c>
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -3390,6 +3405,9 @@
       </c>
       <c r="CU7" s="8">
         <v>102</v>
+      </c>
+      <c r="CV7" s="8">
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:115" x14ac:dyDescent="0.2">
@@ -3974,7 +3992,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>43997</v>
+        <v>43998</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -19267,7 +19285,7 @@
       </c>
       <c r="B104" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C104" s="12">
         <v>98</v>
@@ -19420,11 +19438,11 @@
     <row r="105" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A105" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B105" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C105" s="12">
         <v>99</v>
@@ -19439,139 +19457,139 @@
       </c>
       <c r="F105" cm="1">
         <f t="array" ref="F105">+INDEX(Hoja1!$B$2:$MO$7,1,E105)</f>
-        <v>0</v>
+        <v>95299</v>
       </c>
       <c r="G105">
         <f t="shared" si="41"/>
-        <v>-93646</v>
+        <v>1653</v>
       </c>
       <c r="H105" cm="1">
         <f t="array" ref="H105">+INDEX(Hoja1!$B$2:$MO$7,2,$E105)</f>
-        <v>0</v>
+        <v>70633</v>
       </c>
       <c r="I105">
         <f t="shared" si="42"/>
-        <v>-69528</v>
+        <v>1105</v>
       </c>
       <c r="J105">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>24666</v>
       </c>
       <c r="K105">
         <f t="shared" si="43"/>
-        <v>-24118</v>
+        <v>548</v>
       </c>
       <c r="L105" cm="1">
         <f t="array" ref="L105">+INDEX(Hoja1!$B$2:$MO$7,3,$E105)</f>
-        <v>0</v>
+        <v>6325</v>
       </c>
       <c r="M105" cm="1">
         <f t="array" ref="M105">+INDEX(Hoja1!$B$2:$MO$7,4,$E105)</f>
-        <v>0</v>
+        <v>813</v>
       </c>
       <c r="N105" cm="1">
         <f t="array" ref="N105">+INDEX(Hoja1!$B$2:$MO$7,5,$E105)</f>
-        <v>0</v>
+        <v>486</v>
       </c>
       <c r="O105" cm="1">
         <f t="array" ref="O105">+INDEX(Hoja1!$B$2:$MO$7,6,$E105)</f>
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="P105" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.74117252017334911</v>
       </c>
       <c r="Q105" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.25882747982665083</v>
       </c>
       <c r="R105">
         <f t="shared" si="44"/>
-        <v>-95655</v>
+        <v>-356</v>
       </c>
       <c r="S105">
         <f t="shared" si="45"/>
-        <v>-24118</v>
+        <v>548</v>
       </c>
       <c r="T105">
         <f t="shared" si="46"/>
-        <v>-5824</v>
+        <v>501</v>
       </c>
       <c r="U105">
         <f t="shared" si="47"/>
-        <v>-833</v>
+        <v>-20</v>
       </c>
       <c r="V105">
         <f t="shared" si="48"/>
-        <v>-449</v>
+        <v>37</v>
       </c>
       <c r="W105">
         <f t="shared" si="49"/>
-        <v>-102</v>
+        <v>5</v>
       </c>
       <c r="X105">
         <f t="shared" si="50"/>
-        <v>-47.613240418118465</v>
+        <v>-0.17720258835241415</v>
       </c>
       <c r="Y105">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.2721618708018906E-2</v>
       </c>
       <c r="Z105">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0860233516483517</v>
       </c>
       <c r="AA105">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>0.97599039615846339</v>
       </c>
       <c r="AB105">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0824053452115814</v>
       </c>
       <c r="AC105">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.0490196078431373</v>
       </c>
       <c r="AD105">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>22913.921615773022</v>
       </c>
       <c r="AE105">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>5930.7525847559509</v>
       </c>
       <c r="AF105">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1520.798268814619</v>
       </c>
       <c r="AG105">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>195.47968261601346</v>
       </c>
       <c r="AH105">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>116.85501322433278</v>
       </c>
       <c r="AI105">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>25.727338302476557</v>
       </c>
       <c r="AJ105">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>7731</v>
       </c>
       <c r="AK105">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>1858.8603029574417</v>
       </c>
       <c r="AL105">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ104</f>
-        <v>-7208</v>
+        <v>523</v>
       </c>
       <c r="AM105">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ104,0)</f>
-        <v>-1</v>
+        <v>7.2558268590455055E-2</v>
       </c>
     </row>
     <row r="106" spans="1:39" x14ac:dyDescent="0.2">
@@ -19600,7 +19618,7 @@
       </c>
       <c r="G106">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-95299</v>
       </c>
       <c r="H106" cm="1">
         <f t="array" ref="H106">+INDEX(Hoja1!$B$2:$MO$7,2,$E106)</f>
@@ -19608,7 +19626,7 @@
       </c>
       <c r="I106">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-70633</v>
       </c>
       <c r="J106">
         <f t="shared" si="33"/>
@@ -19616,7 +19634,7 @@
       </c>
       <c r="K106">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-24666</v>
       </c>
       <c r="L106" cm="1">
         <f t="array" ref="L106">+INDEX(Hoja1!$B$2:$MO$7,3,$E106)</f>
@@ -19644,35 +19662,35 @@
       </c>
       <c r="R106">
         <f t="shared" si="44"/>
-        <v>93646</v>
+        <v>-96952</v>
       </c>
       <c r="S106">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-24666</v>
       </c>
       <c r="T106">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-6325</v>
       </c>
       <c r="U106">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-813</v>
       </c>
       <c r="V106">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-486</v>
       </c>
       <c r="W106">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-107</v>
       </c>
       <c r="X106">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-58.652147610405322</v>
       </c>
       <c r="Y106">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z106">
         <f t="shared" si="52"/>
@@ -19724,11 +19742,11 @@
       </c>
       <c r="AL106">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ105</f>
-        <v>0</v>
+        <v>-7731</v>
       </c>
       <c r="AM106">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ105,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="107" spans="1:39" x14ac:dyDescent="0.2">
@@ -19801,7 +19819,7 @@
       </c>
       <c r="R107">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>95299</v>
       </c>
       <c r="S107">
         <f t="shared" si="45"/>
@@ -19825,7 +19843,7 @@
       </c>
       <c r="X107">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y107">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-18-2020 20-36-28
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1404" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{78DB8EBD-F3BC-084A-9CBA-DC3C37FE64F2}"/>
+  <xr:revisionPtr revIDLastSave="1410" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DAFB6655-52E8-9B44-BA17-7E8E58245268}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -1338,7 +1338,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CT1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CW6" sqref="CW6"/>
+      <selection pane="topRight" activeCell="CW8" sqref="CW8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1996,6 +1996,9 @@
       <c r="CV2" s="8">
         <v>95299</v>
       </c>
+      <c r="CW2" s="8">
+        <v>97402</v>
+      </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2298,6 +2301,9 @@
       <c r="CV3" s="8">
         <v>70633</v>
       </c>
+      <c r="CW3" s="8">
+        <v>72084</v>
+      </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2599,6 +2605,9 @@
       </c>
       <c r="CV4" s="8">
         <v>6325</v>
+      </c>
+      <c r="CW4" s="8">
+        <v>6987</v>
       </c>
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.2">
@@ -2811,6 +2820,9 @@
       <c r="CV5" s="8">
         <v>813</v>
       </c>
+      <c r="CW5" s="8">
+        <v>773</v>
+      </c>
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3109,6 +3121,9 @@
       <c r="CV6" s="8">
         <v>486</v>
       </c>
+      <c r="CW6" s="8">
+        <v>484</v>
+      </c>
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -3408,6 +3423,9 @@
       </c>
       <c r="CV7" s="8">
         <v>107</v>
+      </c>
+      <c r="CW7" s="8">
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:115" x14ac:dyDescent="0.2">
@@ -3992,7 +4010,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>43998</v>
+        <v>43999</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -19442,7 +19460,7 @@
       </c>
       <c r="B105" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C105" s="12">
         <v>99</v>
@@ -19595,11 +19613,11 @@
     <row r="106" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A106" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B106" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C106" s="12">
         <v>100</v>
@@ -19614,139 +19632,139 @@
       </c>
       <c r="F106" cm="1">
         <f t="array" ref="F106">+INDEX(Hoja1!$B$2:$MO$7,1,E106)</f>
-        <v>0</v>
+        <v>97402</v>
       </c>
       <c r="G106">
         <f t="shared" si="41"/>
-        <v>-95299</v>
+        <v>2103</v>
       </c>
       <c r="H106" cm="1">
         <f t="array" ref="H106">+INDEX(Hoja1!$B$2:$MO$7,2,$E106)</f>
-        <v>0</v>
+        <v>72084</v>
       </c>
       <c r="I106">
         <f t="shared" si="42"/>
-        <v>-70633</v>
+        <v>1451</v>
       </c>
       <c r="J106">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>25318</v>
       </c>
       <c r="K106">
         <f t="shared" si="43"/>
-        <v>-24666</v>
+        <v>652</v>
       </c>
       <c r="L106" cm="1">
         <f t="array" ref="L106">+INDEX(Hoja1!$B$2:$MO$7,3,$E106)</f>
-        <v>0</v>
+        <v>6987</v>
       </c>
       <c r="M106" cm="1">
         <f t="array" ref="M106">+INDEX(Hoja1!$B$2:$MO$7,4,$E106)</f>
-        <v>0</v>
+        <v>773</v>
       </c>
       <c r="N106" cm="1">
         <f t="array" ref="N106">+INDEX(Hoja1!$B$2:$MO$7,5,$E106)</f>
-        <v>0</v>
+        <v>484</v>
       </c>
       <c r="O106" cm="1">
         <f t="array" ref="O106">+INDEX(Hoja1!$B$2:$MO$7,6,$E106)</f>
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="P106" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.74006693907722632</v>
       </c>
       <c r="Q106" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.25993306092277368</v>
       </c>
       <c r="R106">
         <f t="shared" si="44"/>
-        <v>-96952</v>
+        <v>450</v>
       </c>
       <c r="S106">
         <f t="shared" si="45"/>
-        <v>-24666</v>
+        <v>652</v>
       </c>
       <c r="T106">
         <f t="shared" si="46"/>
-        <v>-6325</v>
+        <v>662</v>
       </c>
       <c r="U106">
         <f t="shared" si="47"/>
-        <v>-813</v>
+        <v>-40</v>
       </c>
       <c r="V106">
         <f t="shared" si="48"/>
-        <v>-486</v>
+        <v>-2</v>
       </c>
       <c r="W106">
         <f t="shared" si="49"/>
-        <v>-107</v>
+        <v>2</v>
       </c>
       <c r="X106">
         <f t="shared" si="50"/>
-        <v>-58.652147610405322</v>
+        <v>0.27223230490018147</v>
       </c>
       <c r="Y106">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.6433146841806535E-2</v>
       </c>
       <c r="Z106">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.1046640316205534</v>
       </c>
       <c r="AA106">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>0.95079950799507995</v>
       </c>
       <c r="AB106">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>0.99588477366255146</v>
       </c>
       <c r="AC106">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.0186915887850467</v>
       </c>
       <c r="AD106">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>23419.572012503006</v>
       </c>
       <c r="AE106">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>6087.5210387112293</v>
       </c>
       <c r="AF106">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1679.9711469103152</v>
       </c>
       <c r="AG106">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>185.86198605434001</v>
       </c>
       <c r="AH106">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>116.37412839624911</v>
       </c>
       <c r="AI106">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>26.208223130560231</v>
       </c>
       <c r="AJ106">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>8353</v>
       </c>
       <c r="AK106">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>2008.4154844914644</v>
       </c>
       <c r="AL106">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ105</f>
-        <v>-7731</v>
+        <v>622</v>
       </c>
       <c r="AM106">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ105,0)</f>
-        <v>-1</v>
+        <v>8.0455309791747504E-2</v>
       </c>
     </row>
     <row r="107" spans="1:39" x14ac:dyDescent="0.2">
@@ -19775,7 +19793,7 @@
       </c>
       <c r="G107">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-97402</v>
       </c>
       <c r="H107" cm="1">
         <f t="array" ref="H107">+INDEX(Hoja1!$B$2:$MO$7,2,$E107)</f>
@@ -19783,7 +19801,7 @@
       </c>
       <c r="I107">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-72084</v>
       </c>
       <c r="J107">
         <f t="shared" si="33"/>
@@ -19791,7 +19809,7 @@
       </c>
       <c r="K107">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-25318</v>
       </c>
       <c r="L107" cm="1">
         <f t="array" ref="L107">+INDEX(Hoja1!$B$2:$MO$7,3,$E107)</f>
@@ -19819,35 +19837,35 @@
       </c>
       <c r="R107">
         <f t="shared" si="44"/>
-        <v>95299</v>
+        <v>-99505</v>
       </c>
       <c r="S107">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-25318</v>
       </c>
       <c r="T107">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-6987</v>
       </c>
       <c r="U107">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-773</v>
       </c>
       <c r="V107">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-484</v>
       </c>
       <c r="W107">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-109</v>
       </c>
       <c r="X107">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-47.315739419876365</v>
       </c>
       <c r="Y107">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z107">
         <f t="shared" si="52"/>
@@ -19899,11 +19917,11 @@
       </c>
       <c r="AL107">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ106</f>
-        <v>0</v>
+        <v>-8353</v>
       </c>
       <c r="AM107">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ106,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="108" spans="1:39" x14ac:dyDescent="0.2">
@@ -19976,7 +19994,7 @@
       </c>
       <c r="R108">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>97402</v>
       </c>
       <c r="S108">
         <f t="shared" si="45"/>
@@ -20000,7 +20018,7 @@
       </c>
       <c r="X108">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y108">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-19-2020 20-39-43
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1410" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DAFB6655-52E8-9B44-BA17-7E8E58245268}"/>
+  <xr:revisionPtr revIDLastSave="1418" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BB3A8740-856F-DA4A-A81F-D6A6CC03AFA3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -602,7 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -630,12 +630,59 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="27">
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -890,25 +937,25 @@
     <tableColumn id="4" xr3:uid="{2FE879E2-2128-42AE-A0E3-647EE2D0C94F}" name="07-06-2020"/>
     <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="08-06-2020"/>
     <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-2020"/>
-    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="13"/>
-    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="12"/>
-    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="11"/>
-    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="10"/>
-    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="9"/>
-    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="8"/>
-    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20"/>
-    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="18/6/2020"/>
-    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="19/6/2020"/>
-    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="20/6/2020"/>
-    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="21/6/2020"/>
-    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="22/6/2020"/>
-    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="23/6/2020"/>
-    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="24/6/2020"/>
-    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="25/6/2020"/>
-    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="26/6/2020"/>
-    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="27/6/2020"/>
+    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="24"/>
+    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="23"/>
+    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="22"/>
+    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="21"/>
+    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="20"/>
+    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="19"/>
+    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="10"/>
+    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="18/6/2020" dataDxfId="9"/>
+    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="19/6/2020" dataDxfId="8"/>
+    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="20/6/2020" dataDxfId="7"/>
+    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="21/6/2020" dataDxfId="6"/>
+    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="22/6/2020" dataDxfId="5"/>
+    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="23/6/2020" dataDxfId="4"/>
+    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="24/6/2020" dataDxfId="3"/>
+    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="25/6/2020" dataDxfId="2"/>
+    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="26/6/2020" dataDxfId="1"/>
+    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="27/6/2020" dataDxfId="0"/>
     <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="28/6/2020"/>
     <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="29/6/2020"/>
     <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="30/6/2020"/>
@@ -918,20 +965,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="17">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="16">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="14">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="13">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -964,10 +1011,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="1">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="12">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="11">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1337,8 +1384,8 @@
   <dimension ref="A1:DK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CT1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CW8" sqref="CW8"/>
+      <pane xSplit="1" topLeftCell="CX1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1346,6 +1393,7 @@
     <col min="1" max="1" width="26.09765625" customWidth="1"/>
     <col min="2" max="87" width="11.296875" customWidth="1"/>
     <col min="94" max="101" width="11.43359375" style="8"/>
+    <col min="102" max="112" width="11.43359375" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:115" x14ac:dyDescent="0.2">
@@ -1652,37 +1700,37 @@
       <c r="CW1" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="CX1" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="CY1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="CZ1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DA1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="DB1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="DC1" s="1" t="s">
+      <c r="DC1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="DD1" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="DE1" s="1" t="s">
+      <c r="DE1" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="DF1" s="1" t="s">
+      <c r="DF1" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="DG1" s="1" t="s">
+      <c r="DG1" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="DH1" s="1" t="s">
+      <c r="DH1" s="15" t="s">
         <v>105</v>
       </c>
       <c r="DI1" s="1" t="s">
@@ -1999,6 +2047,9 @@
       <c r="CW2" s="8">
         <v>97402</v>
       </c>
+      <c r="CX2" s="15">
+        <v>99870</v>
+      </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2304,6 +2355,9 @@
       <c r="CW3" s="8">
         <v>72084</v>
       </c>
+      <c r="CX3" s="15">
+        <v>73779</v>
+      </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2608,6 +2662,9 @@
       </c>
       <c r="CW4" s="8">
         <v>6987</v>
+      </c>
+      <c r="CX4" s="15">
+        <v>7717</v>
       </c>
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.2">
@@ -2823,6 +2880,9 @@
       <c r="CW5" s="8">
         <v>773</v>
       </c>
+      <c r="CX5" s="15">
+        <v>784</v>
+      </c>
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3124,6 +3184,9 @@
       <c r="CW6" s="8">
         <v>484</v>
       </c>
+      <c r="CX6" s="15">
+        <v>476</v>
+      </c>
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -3426,6 +3489,9 @@
       </c>
       <c r="CW7" s="8">
         <v>109</v>
+      </c>
+      <c r="CX7" s="15">
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:115" x14ac:dyDescent="0.2">
@@ -4010,7 +4076,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>43999</v>
+        <v>44000</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -19617,7 +19683,7 @@
       </c>
       <c r="B106" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C106" s="12">
         <v>100</v>
@@ -19770,11 +19836,11 @@
     <row r="107" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A107" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B107" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C107" s="12">
         <v>101</v>
@@ -19789,139 +19855,139 @@
       </c>
       <c r="F107" cm="1">
         <f t="array" ref="F107">+INDEX(Hoja1!$B$2:$MO$7,1,E107)</f>
-        <v>0</v>
+        <v>99870</v>
       </c>
       <c r="G107">
         <f t="shared" si="41"/>
-        <v>-97402</v>
+        <v>2468</v>
       </c>
       <c r="H107" cm="1">
         <f t="array" ref="H107">+INDEX(Hoja1!$B$2:$MO$7,2,$E107)</f>
-        <v>0</v>
+        <v>73779</v>
       </c>
       <c r="I107">
         <f t="shared" si="42"/>
-        <v>-72084</v>
+        <v>1695</v>
       </c>
       <c r="J107">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>26091</v>
       </c>
       <c r="K107">
         <f t="shared" si="43"/>
-        <v>-25318</v>
+        <v>773</v>
       </c>
       <c r="L107" cm="1">
         <f t="array" ref="L107">+INDEX(Hoja1!$B$2:$MO$7,3,$E107)</f>
-        <v>0</v>
+        <v>7717</v>
       </c>
       <c r="M107" cm="1">
         <f t="array" ref="M107">+INDEX(Hoja1!$B$2:$MO$7,4,$E107)</f>
-        <v>0</v>
+        <v>784</v>
       </c>
       <c r="N107" cm="1">
         <f t="array" ref="N107">+INDEX(Hoja1!$B$2:$MO$7,5,$E107)</f>
-        <v>0</v>
+        <v>476</v>
       </c>
       <c r="O107" cm="1">
         <f t="array" ref="O107">+INDEX(Hoja1!$B$2:$MO$7,6,$E107)</f>
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="P107" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.7387503754881346</v>
       </c>
       <c r="Q107" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.26124962451186545</v>
       </c>
       <c r="R107">
         <f t="shared" si="44"/>
-        <v>-99505</v>
+        <v>365</v>
       </c>
       <c r="S107">
         <f t="shared" si="45"/>
-        <v>-25318</v>
+        <v>773</v>
       </c>
       <c r="T107">
         <f t="shared" si="46"/>
-        <v>-6987</v>
+        <v>730</v>
       </c>
       <c r="U107">
         <f t="shared" si="47"/>
-        <v>-773</v>
+        <v>11</v>
       </c>
       <c r="V107">
         <f t="shared" si="48"/>
-        <v>-484</v>
+        <v>-8</v>
       </c>
       <c r="W107">
         <f t="shared" si="49"/>
-        <v>-109</v>
+        <v>8</v>
       </c>
       <c r="X107">
         <f t="shared" si="50"/>
-        <v>-47.315739419876365</v>
+        <v>0.17356157869709937</v>
       </c>
       <c r="Y107">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>3.0531637570108225E-2</v>
       </c>
       <c r="Z107">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.104479748103621</v>
       </c>
       <c r="AA107">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1.0142302716688227</v>
       </c>
       <c r="AB107">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>0.98347107438016534</v>
       </c>
       <c r="AC107">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.073394495412844</v>
       </c>
       <c r="AD107">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>24012.98389035826</v>
       </c>
       <c r="AE107">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>6273.3830247655687</v>
       </c>
       <c r="AF107">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1855.4941091608562</v>
       </c>
       <c r="AG107">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>188.50685260880019</v>
       </c>
       <c r="AH107">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>114.45058908391441</v>
       </c>
       <c r="AI107">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>28.131762442894928</v>
       </c>
       <c r="AJ107">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>9094</v>
       </c>
       <c r="AK107">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>2186.5833132964658</v>
       </c>
       <c r="AL107">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ106</f>
-        <v>-8353</v>
+        <v>741</v>
       </c>
       <c r="AM107">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ106,0)</f>
-        <v>-1</v>
+        <v>8.8710642882796606E-2</v>
       </c>
     </row>
     <row r="108" spans="1:39" x14ac:dyDescent="0.2">
@@ -19950,7 +20016,7 @@
       </c>
       <c r="G108">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-99870</v>
       </c>
       <c r="H108" cm="1">
         <f t="array" ref="H108">+INDEX(Hoja1!$B$2:$MO$7,2,$E108)</f>
@@ -19958,7 +20024,7 @@
       </c>
       <c r="I108">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-73779</v>
       </c>
       <c r="J108">
         <f t="shared" si="33"/>
@@ -19966,7 +20032,7 @@
       </c>
       <c r="K108">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-26091</v>
       </c>
       <c r="L108" cm="1">
         <f t="array" ref="L108">+INDEX(Hoja1!$B$2:$MO$7,3,$E108)</f>
@@ -19994,35 +20060,35 @@
       </c>
       <c r="R108">
         <f t="shared" si="44"/>
-        <v>97402</v>
+        <v>-102338</v>
       </c>
       <c r="S108">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-26091</v>
       </c>
       <c r="T108">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-7717</v>
       </c>
       <c r="U108">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-784</v>
       </c>
       <c r="V108">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-476</v>
       </c>
       <c r="W108">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-117</v>
       </c>
       <c r="X108">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-41.465964343598053</v>
       </c>
       <c r="Y108">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z108">
         <f t="shared" si="52"/>
@@ -20074,11 +20140,11 @@
       </c>
       <c r="AL108">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ107</f>
-        <v>0</v>
+        <v>-9094</v>
       </c>
       <c r="AM108">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ107,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="109" spans="1:39" x14ac:dyDescent="0.2">
@@ -20151,7 +20217,7 @@
       </c>
       <c r="R109">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>99870</v>
       </c>
       <c r="S109">
         <f t="shared" si="45"/>
@@ -20175,7 +20241,7 @@
       </c>
       <c r="X109">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y109">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-20-2020 06-06-55
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1418" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BB3A8740-856F-DA4A-A81F-D6A6CC03AFA3}"/>
+  <xr:revisionPtr revIDLastSave="1424" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2B5C9A70-230C-3F43-8885-A0D0AE508ABC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -640,50 +640,6 @@
   </cellStyles>
   <dxfs count="27">
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -802,6 +758,50 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment wrapText="1"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
@@ -945,17 +945,17 @@
     <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="21"/>
     <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="20"/>
     <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="19"/>
-    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="10"/>
-    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="18/6/2020" dataDxfId="9"/>
-    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="19/6/2020" dataDxfId="8"/>
-    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="20/6/2020" dataDxfId="7"/>
-    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="21/6/2020" dataDxfId="6"/>
-    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="22/6/2020" dataDxfId="5"/>
-    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="23/6/2020" dataDxfId="4"/>
-    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="24/6/2020" dataDxfId="3"/>
-    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="25/6/2020" dataDxfId="2"/>
-    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="26/6/2020" dataDxfId="1"/>
-    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="27/6/2020" dataDxfId="0"/>
+    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="18"/>
+    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="18/6/2020" dataDxfId="17"/>
+    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="19/6/2020" dataDxfId="16"/>
+    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="20/6/2020" dataDxfId="15"/>
+    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="21/6/2020" dataDxfId="14"/>
+    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="22/6/2020" dataDxfId="13"/>
+    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="23/6/2020" dataDxfId="12"/>
+    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="24/6/2020" dataDxfId="11"/>
+    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="25/6/2020" dataDxfId="10"/>
+    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="26/6/2020" dataDxfId="9"/>
+    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="27/6/2020" dataDxfId="8"/>
     <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="28/6/2020"/>
     <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="29/6/2020"/>
     <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="30/6/2020"/>
@@ -965,20 +965,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="6">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="16">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="5">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="3">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="13">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="2">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -1011,10 +1011,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="12">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="1">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="11">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="0">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1385,7 +1385,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CX1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A14" sqref="A14"/>
+      <selection pane="topRight" activeCell="CY8" sqref="CY8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2050,6 +2050,9 @@
       <c r="CX2" s="15">
         <v>99870</v>
       </c>
+      <c r="CY2" s="15">
+        <v>102703</v>
+      </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2358,6 +2361,9 @@
       <c r="CX3" s="15">
         <v>73779</v>
       </c>
+      <c r="CY3" s="15">
+        <v>75676</v>
+      </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2665,6 +2671,9 @@
       </c>
       <c r="CX4" s="15">
         <v>7717</v>
+      </c>
+      <c r="CY4" s="15">
+        <v>8056</v>
       </c>
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.2">
@@ -2883,6 +2892,9 @@
       <c r="CX5" s="15">
         <v>784</v>
       </c>
+      <c r="CY5" s="15">
+        <v>748</v>
+      </c>
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3187,6 +3199,9 @@
       <c r="CX6" s="15">
         <v>476</v>
       </c>
+      <c r="CY6" s="15">
+        <v>503</v>
+      </c>
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -3492,6 +3507,9 @@
       </c>
       <c r="CX7" s="15">
         <v>117</v>
+      </c>
+      <c r="CY7" s="15">
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:115" x14ac:dyDescent="0.2">
@@ -4076,7 +4094,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44000</v>
+        <v>44001</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -19840,7 +19858,7 @@
       </c>
       <c r="B107" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C107" s="12">
         <v>101</v>
@@ -19993,11 +20011,11 @@
     <row r="108" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A108" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B108" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C108" s="12">
         <v>102</v>
@@ -20012,139 +20030,139 @@
       </c>
       <c r="F108" cm="1">
         <f t="array" ref="F108">+INDEX(Hoja1!$B$2:$MO$7,1,E108)</f>
-        <v>0</v>
+        <v>102703</v>
       </c>
       <c r="G108">
         <f t="shared" si="41"/>
-        <v>-99870</v>
+        <v>2833</v>
       </c>
       <c r="H108" cm="1">
         <f t="array" ref="H108">+INDEX(Hoja1!$B$2:$MO$7,2,$E108)</f>
-        <v>0</v>
+        <v>75676</v>
       </c>
       <c r="I108">
         <f t="shared" si="42"/>
-        <v>-73779</v>
+        <v>1897</v>
       </c>
       <c r="J108">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>27027</v>
       </c>
       <c r="K108">
         <f t="shared" si="43"/>
-        <v>-26091</v>
+        <v>936</v>
       </c>
       <c r="L108" cm="1">
         <f t="array" ref="L108">+INDEX(Hoja1!$B$2:$MO$7,3,$E108)</f>
-        <v>0</v>
+        <v>8056</v>
       </c>
       <c r="M108" cm="1">
         <f t="array" ref="M108">+INDEX(Hoja1!$B$2:$MO$7,4,$E108)</f>
-        <v>0</v>
+        <v>748</v>
       </c>
       <c r="N108" cm="1">
         <f t="array" ref="N108">+INDEX(Hoja1!$B$2:$MO$7,5,$E108)</f>
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="O108" cm="1">
         <f t="array" ref="O108">+INDEX(Hoja1!$B$2:$MO$7,6,$E108)</f>
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="P108" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.73684313019093894</v>
       </c>
       <c r="Q108" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.26315686980906106</v>
       </c>
       <c r="R108">
         <f t="shared" si="44"/>
-        <v>-102338</v>
+        <v>365</v>
       </c>
       <c r="S108">
         <f t="shared" si="45"/>
-        <v>-26091</v>
+        <v>936</v>
       </c>
       <c r="T108">
         <f t="shared" si="46"/>
-        <v>-7717</v>
+        <v>339</v>
       </c>
       <c r="U108">
         <f t="shared" si="47"/>
-        <v>-784</v>
+        <v>-36</v>
       </c>
       <c r="V108">
         <f t="shared" si="48"/>
-        <v>-476</v>
+        <v>27</v>
       </c>
       <c r="W108">
         <f t="shared" si="49"/>
-        <v>-117</v>
+        <v>6</v>
       </c>
       <c r="X108">
         <f t="shared" si="50"/>
-        <v>-41.465964343598053</v>
+        <v>0.14789303079416533</v>
       </c>
       <c r="Y108">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>3.5874439461883408E-2</v>
       </c>
       <c r="Z108">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0439289879486848</v>
       </c>
       <c r="AA108">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>0.95408163265306123</v>
       </c>
       <c r="AB108">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0567226890756303</v>
       </c>
       <c r="AC108">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.0512820512820513</v>
       </c>
       <c r="AD108">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>24694.157249338783</v>
       </c>
       <c r="AE108">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>6498.437124308728</v>
       </c>
       <c r="AF108">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1937.0040875210389</v>
       </c>
       <c r="AG108">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>179.85092570329408</v>
       </c>
       <c r="AH108">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>120.94253426304401</v>
       </c>
       <c r="AI108">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>29.57441692714595</v>
       </c>
       <c r="AJ108">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>9430</v>
       </c>
       <c r="AK108">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>2267.3719644145226</v>
       </c>
       <c r="AL108">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ107</f>
-        <v>-9094</v>
+        <v>336</v>
       </c>
       <c r="AM108">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ107,0)</f>
-        <v>-1</v>
+        <v>3.6947437871123819E-2</v>
       </c>
     </row>
     <row r="109" spans="1:39" x14ac:dyDescent="0.2">
@@ -20173,7 +20191,7 @@
       </c>
       <c r="G109">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-102703</v>
       </c>
       <c r="H109" cm="1">
         <f t="array" ref="H109">+INDEX(Hoja1!$B$2:$MO$7,2,$E109)</f>
@@ -20181,7 +20199,7 @@
       </c>
       <c r="I109">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-75676</v>
       </c>
       <c r="J109">
         <f t="shared" si="33"/>
@@ -20189,7 +20207,7 @@
       </c>
       <c r="K109">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-27027</v>
       </c>
       <c r="L109" cm="1">
         <f t="array" ref="L109">+INDEX(Hoja1!$B$2:$MO$7,3,$E109)</f>
@@ -20217,35 +20235,35 @@
       </c>
       <c r="R109">
         <f t="shared" si="44"/>
-        <v>99870</v>
+        <v>-105536</v>
       </c>
       <c r="S109">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-27027</v>
       </c>
       <c r="T109">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-8056</v>
       </c>
       <c r="U109">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-748</v>
       </c>
       <c r="V109">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-503</v>
       </c>
       <c r="W109">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-123</v>
       </c>
       <c r="X109">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-37.252382633250974</v>
       </c>
       <c r="Y109">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z109">
         <f t="shared" si="52"/>
@@ -20297,11 +20315,11 @@
       </c>
       <c r="AL109">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ108</f>
-        <v>0</v>
+        <v>-9430</v>
       </c>
       <c r="AM109">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ108,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="110" spans="1:39" x14ac:dyDescent="0.2">
@@ -20374,7 +20392,7 @@
       </c>
       <c r="R110">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>102703</v>
       </c>
       <c r="S110">
         <f t="shared" si="45"/>
@@ -20398,7 +20416,7 @@
       </c>
       <c r="X110">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y110">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-21-2020 16-15-24
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1424" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2B5C9A70-230C-3F43-8885-A0D0AE508ABC}"/>
+  <xr:revisionPtr revIDLastSave="1433" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0A8E75AA-1D11-B04D-A46E-0CE22F3A5F60}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="156">
   <si>
     <t>Columna1</t>
   </si>
@@ -346,12 +346,6 @@
     <t>12-06-2020</t>
   </si>
   <si>
-    <t>18/6/2020</t>
-  </si>
-  <si>
-    <t>19/6/2020</t>
-  </si>
-  <si>
     <t>20/6/2020</t>
   </si>
   <si>
@@ -519,6 +513,12 @@
   <si>
     <t>18-06-20</t>
   </si>
+  <si>
+    <t>19-06-20</t>
+  </si>
+  <si>
+    <t>20-06-20</t>
+  </si>
 </sst>
 </file>
 
@@ -602,7 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -631,6 +631,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -946,8 +949,8 @@
     <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="20"/>
     <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="19"/>
     <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="18"/>
-    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="18/6/2020" dataDxfId="17"/>
-    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="19/6/2020" dataDxfId="16"/>
+    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="17"/>
+    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="16"/>
     <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="20/6/2020" dataDxfId="15"/>
     <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="21/6/2020" dataDxfId="14"/>
     <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="22/6/2020" dataDxfId="13"/>
@@ -1385,7 +1388,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CX1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CY8" sqref="CY8"/>
+      <selection pane="topRight" activeCell="CZ9" sqref="CZ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1393,7 +1396,9 @@
     <col min="1" max="1" width="26.09765625" customWidth="1"/>
     <col min="2" max="87" width="11.296875" customWidth="1"/>
     <col min="94" max="101" width="11.43359375" style="8"/>
-    <col min="102" max="112" width="11.43359375" style="15"/>
+    <col min="102" max="103" width="11.43359375" style="15"/>
+    <col min="104" max="104" width="12.9140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="105" max="112" width="11.43359375" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:115" x14ac:dyDescent="0.2">
@@ -1686,66 +1691,66 @@
         <v>95</v>
       </c>
       <c r="CS1" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="CT1" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="CU1" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="CT1" s="8" t="s">
+      <c r="CV1" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="CU1" s="8" t="s">
+      <c r="CW1" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="CV1" s="8" t="s">
+      <c r="CX1" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="CW1" s="8" t="s">
+      <c r="CY1" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="CX1" s="15" t="s">
+      <c r="CZ1" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="CY1" s="15" t="s">
+      <c r="DA1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="CZ1" s="15" t="s">
+      <c r="DB1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="DA1" s="15" t="s">
+      <c r="DC1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="DB1" s="15" t="s">
+      <c r="DD1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="DC1" s="15" t="s">
+      <c r="DE1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="DD1" s="15" t="s">
+      <c r="DF1" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="DE1" s="15" t="s">
+      <c r="DG1" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="DF1" s="15" t="s">
+      <c r="DH1" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="DG1" s="15" t="s">
+      <c r="DI1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="DH1" s="15" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="DJ1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B2" s="7">
         <v>146</v>
@@ -2052,11 +2057,14 @@
       </c>
       <c r="CY2" s="15">
         <v>102703</v>
+      </c>
+      <c r="CZ2" s="15">
+        <v>105470</v>
       </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3" s="7">
         <v>138</v>
@@ -2363,11 +2371,14 @@
       </c>
       <c r="CY3" s="15">
         <v>75676</v>
+      </c>
+      <c r="CZ3" s="15">
+        <v>77494</v>
       </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" s="7">
         <v>6</v>
@@ -2674,11 +2685,14 @@
       </c>
       <c r="CY4" s="15">
         <v>8056</v>
+      </c>
+      <c r="CZ4" s="15">
+        <v>9008</v>
       </c>
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2895,10 +2909,13 @@
       <c r="CY5" s="15">
         <v>748</v>
       </c>
+      <c r="CZ5" s="15">
+        <v>722</v>
+      </c>
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -3202,10 +3219,13 @@
       <c r="CY6" s="15">
         <v>503</v>
       </c>
+      <c r="CZ6" s="15">
+        <v>519</v>
+      </c>
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -3510,6 +3530,9 @@
       </c>
       <c r="CY7" s="15">
         <v>123</v>
+      </c>
+      <c r="CZ7" s="15">
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:115" x14ac:dyDescent="0.2">
@@ -4094,7 +4117,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44001</v>
+        <v>44002</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -4103,121 +4126,121 @@
     </row>
     <row r="6" spans="1:39" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="D6" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="F6" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="H6" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="J6" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="L6" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G6" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="H6" s="14" t="s">
+      <c r="M6" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="J6" s="14" t="s">
+      <c r="N6" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="P6" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="Q6" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="L6" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="P6" s="14" t="s">
+      <c r="R6" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="S6" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="Q6" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="R6" s="14" t="s">
+      <c r="T6" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="U6" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="S6" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="T6" s="14" t="s">
+      <c r="V6" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="W6" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="V6" s="14" t="s">
+      <c r="X6" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y6" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA6" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB6" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC6" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD6" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="W6" s="14" t="s">
+      <c r="AE6" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="X6" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y6" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="Z6" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="AA6" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB6" s="14" t="s">
+      <c r="AF6" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="AC6" s="14" t="s">
+      <c r="AG6" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="AD6" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="AE6" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="AF6" s="14" t="s">
+      <c r="AH6" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="AG6" s="14" t="s">
+      <c r="AI6" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="AH6" s="14" t="s">
+      <c r="AJ6" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="AI6" s="14" t="s">
+      <c r="AK6" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="AL6" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="AJ6" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="AK6" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="AL6" s="14" t="s">
+      <c r="AM6" s="14" t="s">
         <v>145</v>
-      </c>
-      <c r="AM6" s="14" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.2">
@@ -20015,7 +20038,7 @@
       </c>
       <c r="B108" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C108" s="12">
         <v>102</v>
@@ -20168,11 +20191,11 @@
     <row r="109" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A109" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B109" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C109" s="12">
         <v>103</v>
@@ -20187,139 +20210,139 @@
       </c>
       <c r="F109" cm="1">
         <f t="array" ref="F109">+INDEX(Hoja1!$B$2:$MO$7,1,E109)</f>
-        <v>0</v>
+        <v>105470</v>
       </c>
       <c r="G109">
         <f t="shared" si="41"/>
-        <v>-102703</v>
+        <v>2767</v>
       </c>
       <c r="H109" cm="1">
         <f t="array" ref="H109">+INDEX(Hoja1!$B$2:$MO$7,2,$E109)</f>
-        <v>0</v>
+        <v>77494</v>
       </c>
       <c r="I109">
         <f t="shared" si="42"/>
-        <v>-75676</v>
+        <v>1818</v>
       </c>
       <c r="J109">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>27976</v>
       </c>
       <c r="K109">
         <f t="shared" si="43"/>
-        <v>-27027</v>
+        <v>949</v>
       </c>
       <c r="L109" cm="1">
         <f t="array" ref="L109">+INDEX(Hoja1!$B$2:$MO$7,3,$E109)</f>
-        <v>0</v>
+        <v>9008</v>
       </c>
       <c r="M109" cm="1">
         <f t="array" ref="M109">+INDEX(Hoja1!$B$2:$MO$7,4,$E109)</f>
-        <v>0</v>
+        <v>722</v>
       </c>
       <c r="N109" cm="1">
         <f t="array" ref="N109">+INDEX(Hoja1!$B$2:$MO$7,5,$E109)</f>
-        <v>0</v>
+        <v>519</v>
       </c>
       <c r="O109" cm="1">
         <f t="array" ref="O109">+INDEX(Hoja1!$B$2:$MO$7,6,$E109)</f>
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="P109" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.73474921778704849</v>
       </c>
       <c r="Q109" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.26525078221295156</v>
       </c>
       <c r="R109">
         <f t="shared" si="44"/>
-        <v>-105536</v>
+        <v>-66</v>
       </c>
       <c r="S109">
         <f t="shared" si="45"/>
-        <v>-27027</v>
+        <v>949</v>
       </c>
       <c r="T109">
         <f t="shared" si="46"/>
-        <v>-8056</v>
+        <v>952</v>
       </c>
       <c r="U109">
         <f t="shared" si="47"/>
-        <v>-748</v>
+        <v>-26</v>
       </c>
       <c r="V109">
         <f t="shared" si="48"/>
-        <v>-503</v>
+        <v>16</v>
       </c>
       <c r="W109">
         <f t="shared" si="49"/>
-        <v>-123</v>
+        <v>-2</v>
       </c>
       <c r="X109">
         <f t="shared" si="50"/>
-        <v>-37.252382633250974</v>
+        <v>-2.3296858453935757E-2</v>
       </c>
       <c r="Y109">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>3.511303511303511E-2</v>
       </c>
       <c r="Z109">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.1181727904667329</v>
       </c>
       <c r="AA109">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>0.96524064171122992</v>
       </c>
       <c r="AB109">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0318091451292246</v>
       </c>
       <c r="AC109">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>0.98373983739837401</v>
       </c>
       <c r="AD109">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>25359.461408992549</v>
       </c>
       <c r="AE109">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>6726.6169752344313</v>
       </c>
       <c r="AF109">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>2165.9052656888675</v>
       </c>
       <c r="AG109">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>173.59942293820632</v>
       </c>
       <c r="AH109">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>124.7896128877134</v>
       </c>
       <c r="AI109">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>29.093532099062276</v>
       </c>
       <c r="AJ109">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>10370</v>
       </c>
       <c r="AK109">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>2493.3878336138496</v>
       </c>
       <c r="AL109">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ108</f>
-        <v>-9430</v>
+        <v>940</v>
       </c>
       <c r="AM109">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ108,0)</f>
-        <v>-1</v>
+        <v>9.9681866383881226E-2</v>
       </c>
     </row>
     <row r="110" spans="1:39" x14ac:dyDescent="0.2">
@@ -20348,7 +20371,7 @@
       </c>
       <c r="G110">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-105470</v>
       </c>
       <c r="H110" cm="1">
         <f t="array" ref="H110">+INDEX(Hoja1!$B$2:$MO$7,2,$E110)</f>
@@ -20356,7 +20379,7 @@
       </c>
       <c r="I110">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-77494</v>
       </c>
       <c r="J110">
         <f t="shared" si="33"/>
@@ -20364,7 +20387,7 @@
       </c>
       <c r="K110">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-27976</v>
       </c>
       <c r="L110" cm="1">
         <f t="array" ref="L110">+INDEX(Hoja1!$B$2:$MO$7,3,$E110)</f>
@@ -20392,35 +20415,35 @@
       </c>
       <c r="R110">
         <f t="shared" si="44"/>
-        <v>102703</v>
+        <v>-108237</v>
       </c>
       <c r="S110">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-27976</v>
       </c>
       <c r="T110">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-9008</v>
       </c>
       <c r="U110">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-722</v>
       </c>
       <c r="V110">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-519</v>
       </c>
       <c r="W110">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-121</v>
       </c>
       <c r="X110">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-39.117094325984823</v>
       </c>
       <c r="Y110">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z110">
         <f t="shared" si="52"/>
@@ -20472,11 +20495,11 @@
       </c>
       <c r="AL110">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ109</f>
-        <v>0</v>
+        <v>-10370</v>
       </c>
       <c r="AM110">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ109,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="111" spans="1:39" x14ac:dyDescent="0.2">
@@ -20549,7 +20572,7 @@
       </c>
       <c r="R111">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>105470</v>
       </c>
       <c r="S111">
         <f t="shared" si="45"/>
@@ -20573,7 +20596,7 @@
       </c>
       <c r="X111">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y111">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-22-2020 06-06-28
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1433" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0A8E75AA-1D11-B04D-A46E-0CE22F3A5F60}"/>
+  <xr:revisionPtr revIDLastSave="1444" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D41F1A85-9683-AC44-B343-2D2BF7C911F0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="157">
   <si>
     <t>Columna1</t>
   </si>
@@ -346,9 +346,6 @@
     <t>12-06-2020</t>
   </si>
   <si>
-    <t>20/6/2020</t>
-  </si>
-  <si>
     <t>21/6/2020</t>
   </si>
   <si>
@@ -518,6 +515,9 @@
   </si>
   <si>
     <t>20-06-20</t>
+  </si>
+  <si>
+    <t>21-06-20</t>
   </si>
 </sst>
 </file>
@@ -951,7 +951,7 @@
     <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="18"/>
     <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="17"/>
     <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="16"/>
-    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="20/6/2020" dataDxfId="15"/>
+    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="15"/>
     <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="21/6/2020" dataDxfId="14"/>
     <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="22/6/2020" dataDxfId="13"/>
     <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="23/6/2020" dataDxfId="12"/>
@@ -1387,8 +1387,8 @@
   <dimension ref="A1:DK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CX1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CZ9" sqref="CZ9"/>
+      <pane xSplit="1" topLeftCell="CY1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DA8" sqref="DA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1691,66 +1691,66 @@
         <v>95</v>
       </c>
       <c r="CS1" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="CT1" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="CT1" s="8" t="s">
+      <c r="CU1" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="CU1" s="8" t="s">
+      <c r="CV1" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="CV1" s="8" t="s">
+      <c r="CW1" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="CW1" s="8" t="s">
+      <c r="CX1" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="CX1" s="15" t="s">
+      <c r="CY1" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="CY1" s="16" t="s">
+      <c r="CZ1" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="CZ1" s="16" t="s">
+      <c r="DA1" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="DA1" s="15" t="s">
+      <c r="DB1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="DB1" s="15" t="s">
+      <c r="DC1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="DC1" s="15" t="s">
+      <c r="DD1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="DD1" s="15" t="s">
+      <c r="DE1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="DE1" s="15" t="s">
+      <c r="DF1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="DF1" s="15" t="s">
+      <c r="DG1" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="DG1" s="15" t="s">
+      <c r="DH1" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="DH1" s="15" t="s">
+      <c r="DI1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="7">
         <v>146</v>
@@ -2060,11 +2060,14 @@
       </c>
       <c r="CZ2" s="15">
         <v>105470</v>
+      </c>
+      <c r="DA2" s="15">
+        <v>107903</v>
       </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" s="7">
         <v>138</v>
@@ -2374,11 +2377,14 @@
       </c>
       <c r="CZ3" s="15">
         <v>77494</v>
+      </c>
+      <c r="DA3" s="15">
+        <v>79096</v>
       </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" s="7">
         <v>6</v>
@@ -2688,11 +2694,14 @@
       </c>
       <c r="CZ4" s="15">
         <v>9008</v>
+      </c>
+      <c r="DA4" s="15">
+        <v>9708</v>
       </c>
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2912,10 +2921,13 @@
       <c r="CZ5" s="15">
         <v>722</v>
       </c>
+      <c r="DA5" s="15">
+        <v>738</v>
+      </c>
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -3222,10 +3234,13 @@
       <c r="CZ6" s="15">
         <v>519</v>
       </c>
+      <c r="DA6" s="15">
+        <v>595</v>
+      </c>
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -3533,6 +3548,9 @@
       </c>
       <c r="CZ7" s="15">
         <v>121</v>
+      </c>
+      <c r="DA7" s="15">
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:115" x14ac:dyDescent="0.2">
@@ -4117,7 +4135,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44002</v>
+        <v>44003</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -4126,121 +4144,121 @@
     </row>
     <row r="6" spans="1:39" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="C6" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D6" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="F6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="J6" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="L6" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="K6" s="14" t="s">
+      <c r="M6" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="P6" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="L6" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="P6" s="14" t="s">
+      <c r="Q6" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="R6" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="S6" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="T6" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="S6" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="T6" s="14" t="s">
+      <c r="U6" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="V6" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="V6" s="14" t="s">
+      <c r="W6" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="W6" s="14" t="s">
+      <c r="X6" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y6" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA6" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB6" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC6" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD6" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="X6" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="Y6" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="Z6" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA6" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="AB6" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="AC6" s="14" t="s">
+      <c r="AE6" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF6" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="AD6" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="AE6" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="AF6" s="14" t="s">
+      <c r="AG6" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="AG6" s="14" t="s">
+      <c r="AH6" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="AH6" s="14" t="s">
+      <c r="AI6" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="AI6" s="14" t="s">
+      <c r="AJ6" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="AJ6" s="14" t="s">
+      <c r="AK6" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="AL6" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="AK6" s="14" t="s">
+      <c r="AM6" s="14" t="s">
         <v>144</v>
-      </c>
-      <c r="AL6" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="AM6" s="14" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.2">
@@ -20195,7 +20213,7 @@
       </c>
       <c r="B109" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C109" s="12">
         <v>103</v>
@@ -20348,11 +20366,11 @@
     <row r="110" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A110" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B110" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C110" s="12">
         <v>104</v>
@@ -20367,139 +20385,139 @@
       </c>
       <c r="F110" cm="1">
         <f t="array" ref="F110">+INDEX(Hoja1!$B$2:$MO$7,1,E110)</f>
-        <v>0</v>
+        <v>107903</v>
       </c>
       <c r="G110">
         <f t="shared" si="41"/>
-        <v>-105470</v>
+        <v>2433</v>
       </c>
       <c r="H110" cm="1">
         <f t="array" ref="H110">+INDEX(Hoja1!$B$2:$MO$7,2,$E110)</f>
-        <v>0</v>
+        <v>79096</v>
       </c>
       <c r="I110">
         <f t="shared" si="42"/>
-        <v>-77494</v>
+        <v>1602</v>
       </c>
       <c r="J110">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>28807</v>
       </c>
       <c r="K110">
         <f t="shared" si="43"/>
-        <v>-27976</v>
+        <v>831</v>
       </c>
       <c r="L110" cm="1">
         <f t="array" ref="L110">+INDEX(Hoja1!$B$2:$MO$7,3,$E110)</f>
-        <v>0</v>
+        <v>9708</v>
       </c>
       <c r="M110" cm="1">
         <f t="array" ref="M110">+INDEX(Hoja1!$B$2:$MO$7,4,$E110)</f>
-        <v>0</v>
+        <v>738</v>
       </c>
       <c r="N110" cm="1">
         <f t="array" ref="N110">+INDEX(Hoja1!$B$2:$MO$7,5,$E110)</f>
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="O110" cm="1">
         <f t="array" ref="O110">+INDEX(Hoja1!$B$2:$MO$7,6,$E110)</f>
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="P110" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.73302873877464014</v>
       </c>
       <c r="Q110" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.2669712612253598</v>
       </c>
       <c r="R110">
         <f t="shared" si="44"/>
-        <v>-108237</v>
+        <v>-334</v>
       </c>
       <c r="S110">
         <f t="shared" si="45"/>
-        <v>-27976</v>
+        <v>831</v>
       </c>
       <c r="T110">
         <f t="shared" si="46"/>
-        <v>-9008</v>
+        <v>700</v>
       </c>
       <c r="U110">
         <f t="shared" si="47"/>
-        <v>-722</v>
+        <v>16</v>
       </c>
       <c r="V110">
         <f t="shared" si="48"/>
-        <v>-519</v>
+        <v>76</v>
       </c>
       <c r="W110">
         <f t="shared" si="49"/>
-        <v>-121</v>
+        <v>8</v>
       </c>
       <c r="X110">
         <f t="shared" si="50"/>
-        <v>-39.117094325984823</v>
+        <v>-0.12070834839176003</v>
       </c>
       <c r="Y110">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.9704032027452101E-2</v>
       </c>
       <c r="Z110">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0777087033747779</v>
       </c>
       <c r="AA110">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1.0221606648199446</v>
       </c>
       <c r="AB110">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.1464354527938343</v>
       </c>
       <c r="AC110">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.0661157024793388</v>
       </c>
       <c r="AD110">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>25944.457802356337</v>
       </c>
       <c r="AE110">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>6926.4246213031984</v>
       </c>
       <c r="AF110">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>2334.2149555181536</v>
       </c>
       <c r="AG110">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>177.44650156287571</v>
       </c>
       <c r="AH110">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>143.06323635489301</v>
       </c>
       <c r="AI110">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>31.017071411396973</v>
       </c>
       <c r="AJ110">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>11170</v>
       </c>
       <c r="AK110">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>2685.7417648473192</v>
       </c>
       <c r="AL110">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ109</f>
-        <v>-10370</v>
+        <v>800</v>
       </c>
       <c r="AM110">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ109,0)</f>
-        <v>-1</v>
+        <v>7.7145612343297976E-2</v>
       </c>
     </row>
     <row r="111" spans="1:39" x14ac:dyDescent="0.2">
@@ -20528,7 +20546,7 @@
       </c>
       <c r="G111">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-107903</v>
       </c>
       <c r="H111" cm="1">
         <f t="array" ref="H111">+INDEX(Hoja1!$B$2:$MO$7,2,$E111)</f>
@@ -20536,7 +20554,7 @@
       </c>
       <c r="I111">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-79096</v>
       </c>
       <c r="J111">
         <f t="shared" si="33"/>
@@ -20544,7 +20562,7 @@
       </c>
       <c r="K111">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-28807</v>
       </c>
       <c r="L111" cm="1">
         <f t="array" ref="L111">+INDEX(Hoja1!$B$2:$MO$7,3,$E111)</f>
@@ -20572,35 +20590,35 @@
       </c>
       <c r="R111">
         <f t="shared" si="44"/>
-        <v>105470</v>
+        <v>-110336</v>
       </c>
       <c r="S111">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-28807</v>
       </c>
       <c r="T111">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-9708</v>
       </c>
       <c r="U111">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-738</v>
       </c>
       <c r="V111">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-595</v>
       </c>
       <c r="W111">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-129</v>
       </c>
       <c r="X111">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-45.349773941635839</v>
       </c>
       <c r="Y111">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z111">
         <f t="shared" si="52"/>
@@ -20652,11 +20670,11 @@
       </c>
       <c r="AL111">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ110</f>
-        <v>0</v>
+        <v>-11170</v>
       </c>
       <c r="AM111">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ110,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="112" spans="1:39" x14ac:dyDescent="0.2">
@@ -20729,7 +20747,7 @@
       </c>
       <c r="R112">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>107903</v>
       </c>
       <c r="S112">
         <f t="shared" si="45"/>
@@ -20753,7 +20771,7 @@
       </c>
       <c r="X112">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y112">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-23-2020 12-14-36
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1444" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D41F1A85-9683-AC44-B343-2D2BF7C911F0}"/>
+  <xr:revisionPtr revIDLastSave="1451" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1433EA04-84EF-964E-B450-3E72C0A32439}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="155">
   <si>
     <t>Columna1</t>
   </si>
@@ -346,9 +346,6 @@
     <t>12-06-2020</t>
   </si>
   <si>
-    <t>21/6/2020</t>
-  </si>
-  <si>
     <t>22/6/2020</t>
   </si>
   <si>
@@ -518,6 +515,9 @@
   </si>
   <si>
     <t>21-06-20</t>
+  </si>
+  <si>
+    <t>22-06-20</t>
   </si>
 </sst>
 </file>
@@ -952,7 +952,7 @@
     <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="17"/>
     <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="16"/>
     <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="15"/>
-    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="21/6/2020" dataDxfId="14"/>
+    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="14"/>
     <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="22/6/2020" dataDxfId="13"/>
     <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="23/6/2020" dataDxfId="12"/>
     <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="24/6/2020" dataDxfId="11"/>
@@ -1387,8 +1387,8 @@
   <dimension ref="A1:DK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CY1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DA8" sqref="DA8"/>
+      <pane xSplit="1" topLeftCell="CZ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DB9" sqref="DB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1691,66 +1691,66 @@
         <v>95</v>
       </c>
       <c r="CS1" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="CT1" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="CT1" s="8" t="s">
+      <c r="CU1" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="CU1" s="8" t="s">
+      <c r="CV1" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="CV1" s="8" t="s">
+      <c r="CW1" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="CW1" s="8" t="s">
+      <c r="CX1" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="CX1" s="15" t="s">
+      <c r="CY1" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="CY1" s="16" t="s">
+      <c r="CZ1" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="CZ1" s="16" t="s">
+      <c r="DA1" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="DA1" s="16" t="s">
+      <c r="DB1" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="DB1" s="15" t="s">
+      <c r="DC1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="DC1" s="15" t="s">
+      <c r="DD1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="DD1" s="15" t="s">
+      <c r="DE1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="DE1" s="15" t="s">
+      <c r="DF1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="DF1" s="15" t="s">
+      <c r="DG1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="DG1" s="15" t="s">
+      <c r="DH1" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="DH1" s="15" t="s">
+      <c r="DI1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="7">
         <v>146</v>
@@ -2063,11 +2063,14 @@
       </c>
       <c r="DA2" s="15">
         <v>107903</v>
+      </c>
+      <c r="DB2" s="15">
+        <v>109990</v>
       </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" s="7">
         <v>138</v>
@@ -2380,11 +2383,14 @@
       </c>
       <c r="DA3" s="15">
         <v>79096</v>
+      </c>
+      <c r="DB3" s="15">
+        <v>80449</v>
       </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" s="7">
         <v>6</v>
@@ -2697,11 +2703,14 @@
       </c>
       <c r="DA4" s="15">
         <v>9708</v>
+      </c>
+      <c r="DB4" s="15">
+        <v>10049</v>
       </c>
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2924,10 +2933,13 @@
       <c r="DA5" s="15">
         <v>738</v>
       </c>
+      <c r="DB5" s="15">
+        <v>771</v>
+      </c>
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -3237,10 +3249,13 @@
       <c r="DA6" s="15">
         <v>595</v>
       </c>
+      <c r="DB6" s="15">
+        <v>615</v>
+      </c>
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -3551,6 +3566,9 @@
       </c>
       <c r="DA7" s="15">
         <v>129</v>
+      </c>
+      <c r="DB7" s="15">
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:115" x14ac:dyDescent="0.2">
@@ -4135,7 +4153,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44003</v>
+        <v>44004</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -4144,121 +4162,121 @@
     </row>
     <row r="6" spans="1:39" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="C6" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D6" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="F6" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="J6" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="L6" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="K6" s="14" t="s">
+      <c r="M6" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="P6" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="L6" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="P6" s="14" t="s">
+      <c r="Q6" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="R6" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="S6" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="T6" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="S6" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="T6" s="14" t="s">
+      <c r="U6" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="V6" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="V6" s="14" t="s">
+      <c r="W6" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="W6" s="14" t="s">
+      <c r="X6" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y6" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA6" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB6" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="AC6" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD6" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="X6" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="Y6" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z6" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="AA6" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB6" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="AC6" s="14" t="s">
+      <c r="AE6" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF6" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="AD6" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="AE6" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="AF6" s="14" t="s">
+      <c r="AG6" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="AG6" s="14" t="s">
+      <c r="AH6" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="AH6" s="14" t="s">
+      <c r="AI6" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="AI6" s="14" t="s">
+      <c r="AJ6" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="AJ6" s="14" t="s">
+      <c r="AK6" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="AL6" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="AK6" s="14" t="s">
+      <c r="AM6" s="14" t="s">
         <v>143</v>
-      </c>
-      <c r="AL6" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="AM6" s="14" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.2">
@@ -20370,7 +20388,7 @@
       </c>
       <c r="B110" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C110" s="12">
         <v>104</v>
@@ -20523,11 +20541,11 @@
     <row r="111" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A111" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B111" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C111" s="12">
         <v>105</v>
@@ -20542,139 +20560,139 @@
       </c>
       <c r="F111" cm="1">
         <f t="array" ref="F111">+INDEX(Hoja1!$B$2:$MO$7,1,E111)</f>
-        <v>0</v>
+        <v>109990</v>
       </c>
       <c r="G111">
         <f t="shared" si="41"/>
-        <v>-107903</v>
+        <v>2087</v>
       </c>
       <c r="H111" cm="1">
         <f t="array" ref="H111">+INDEX(Hoja1!$B$2:$MO$7,2,$E111)</f>
-        <v>0</v>
+        <v>80449</v>
       </c>
       <c r="I111">
         <f t="shared" si="42"/>
-        <v>-79096</v>
+        <v>1353</v>
       </c>
       <c r="J111">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>29541</v>
       </c>
       <c r="K111">
         <f t="shared" si="43"/>
-        <v>-28807</v>
+        <v>734</v>
       </c>
       <c r="L111" cm="1">
         <f t="array" ref="L111">+INDEX(Hoja1!$B$2:$MO$7,3,$E111)</f>
-        <v>0</v>
+        <v>10049</v>
       </c>
       <c r="M111" cm="1">
         <f t="array" ref="M111">+INDEX(Hoja1!$B$2:$MO$7,4,$E111)</f>
-        <v>0</v>
+        <v>771</v>
       </c>
       <c r="N111" cm="1">
         <f t="array" ref="N111">+INDEX(Hoja1!$B$2:$MO$7,5,$E111)</f>
-        <v>0</v>
+        <v>615</v>
       </c>
       <c r="O111" cm="1">
         <f t="array" ref="O111">+INDEX(Hoja1!$B$2:$MO$7,6,$E111)</f>
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="P111" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.73142103827620697</v>
       </c>
       <c r="Q111" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.26857896172379309</v>
       </c>
       <c r="R111">
         <f t="shared" si="44"/>
-        <v>-110336</v>
+        <v>-346</v>
       </c>
       <c r="S111">
         <f t="shared" si="45"/>
-        <v>-28807</v>
+        <v>734</v>
       </c>
       <c r="T111">
         <f t="shared" si="46"/>
-        <v>-9708</v>
+        <v>341</v>
       </c>
       <c r="U111">
         <f t="shared" si="47"/>
-        <v>-738</v>
+        <v>33</v>
       </c>
       <c r="V111">
         <f t="shared" si="48"/>
-        <v>-595</v>
+        <v>20</v>
       </c>
       <c r="W111">
         <f t="shared" si="49"/>
-        <v>-129</v>
+        <v>3</v>
       </c>
       <c r="X111">
         <f t="shared" si="50"/>
-        <v>-45.349773941635839</v>
+        <v>-0.14221126181668722</v>
       </c>
       <c r="Y111">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.5479918075467768E-2</v>
       </c>
       <c r="Z111">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0351256695508859</v>
       </c>
       <c r="AA111">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1.0447154471544715</v>
       </c>
       <c r="AB111">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0336134453781514</v>
       </c>
       <c r="AC111">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.0232558139534884</v>
       </c>
       <c r="AD111">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>26446.261120461651</v>
       </c>
       <c r="AE111">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>7102.9093532099068</v>
       </c>
       <c r="AF111">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>2416.2058187064199</v>
       </c>
       <c r="AG111">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>185.38110122625633</v>
       </c>
       <c r="AH111">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>147.87208463572975</v>
       </c>
       <c r="AI111">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>31.738398653522484</v>
       </c>
       <c r="AJ111">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>11567</v>
       </c>
       <c r="AK111">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>2781.1974032219287</v>
       </c>
       <c r="AL111">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ110</f>
-        <v>-11170</v>
+        <v>397</v>
       </c>
       <c r="AM111">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ110,0)</f>
-        <v>-1</v>
+        <v>3.5541629364368846E-2</v>
       </c>
     </row>
     <row r="112" spans="1:39" x14ac:dyDescent="0.2">
@@ -20703,7 +20721,7 @@
       </c>
       <c r="G112">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-109990</v>
       </c>
       <c r="H112" cm="1">
         <f t="array" ref="H112">+INDEX(Hoja1!$B$2:$MO$7,2,$E112)</f>
@@ -20711,7 +20729,7 @@
       </c>
       <c r="I112">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-80449</v>
       </c>
       <c r="J112">
         <f t="shared" si="33"/>
@@ -20719,7 +20737,7 @@
       </c>
       <c r="K112">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-29541</v>
       </c>
       <c r="L112" cm="1">
         <f t="array" ref="L112">+INDEX(Hoja1!$B$2:$MO$7,3,$E112)</f>
@@ -20747,35 +20765,35 @@
       </c>
       <c r="R112">
         <f t="shared" si="44"/>
-        <v>107903</v>
+        <v>-112077</v>
       </c>
       <c r="S112">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-29541</v>
       </c>
       <c r="T112">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-10049</v>
       </c>
       <c r="U112">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-771</v>
       </c>
       <c r="V112">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-615</v>
       </c>
       <c r="W112">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-132</v>
       </c>
       <c r="X112">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-53.702443699089599</v>
       </c>
       <c r="Y112">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z112">
         <f t="shared" si="52"/>
@@ -20827,11 +20845,11 @@
       </c>
       <c r="AL112">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ111</f>
-        <v>0</v>
+        <v>-11567</v>
       </c>
       <c r="AM112">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ111,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="113" spans="1:39" x14ac:dyDescent="0.2">
@@ -20904,7 +20922,7 @@
       </c>
       <c r="R113">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>109990</v>
       </c>
       <c r="S113">
         <f t="shared" si="45"/>
@@ -20928,7 +20946,7 @@
       </c>
       <c r="X113">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y113">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-24-2020 03-03-40
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1451" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1433EA04-84EF-964E-B450-3E72C0A32439}"/>
+  <xr:revisionPtr revIDLastSave="1454" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2E6CC9C6-B33A-C94F-BE01-F7636144C11E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -346,9 +346,6 @@
     <t>12-06-2020</t>
   </si>
   <si>
-    <t>22/6/2020</t>
-  </si>
-  <si>
     <t>23/6/2020</t>
   </si>
   <si>
@@ -518,6 +515,9 @@
   </si>
   <si>
     <t>22-06-20</t>
+  </si>
+  <si>
+    <t>23-06-20</t>
   </si>
 </sst>
 </file>
@@ -953,7 +953,7 @@
     <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="16"/>
     <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="15"/>
     <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="14"/>
-    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="22/6/2020" dataDxfId="13"/>
+    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="13"/>
     <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="23/6/2020" dataDxfId="12"/>
     <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="24/6/2020" dataDxfId="11"/>
     <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="25/6/2020" dataDxfId="10"/>
@@ -1388,7 +1388,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CZ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DB9" sqref="DB9"/>
+      <selection pane="topRight" activeCell="DC4" sqref="DC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1691,66 +1691,66 @@
         <v>95</v>
       </c>
       <c r="CS1" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="CT1" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="CT1" s="8" t="s">
+      <c r="CU1" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="CU1" s="8" t="s">
+      <c r="CV1" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="CV1" s="8" t="s">
+      <c r="CW1" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="CW1" s="8" t="s">
+      <c r="CX1" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="CX1" s="15" t="s">
+      <c r="CY1" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="CY1" s="16" t="s">
+      <c r="CZ1" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="CZ1" s="16" t="s">
+      <c r="DA1" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="DA1" s="16" t="s">
+      <c r="DB1" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="DB1" s="16" t="s">
+      <c r="DC1" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="DC1" s="15" t="s">
+      <c r="DD1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="DD1" s="15" t="s">
+      <c r="DE1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="DE1" s="15" t="s">
+      <c r="DF1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="DF1" s="15" t="s">
+      <c r="DG1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="DG1" s="15" t="s">
+      <c r="DH1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="DH1" s="15" t="s">
+      <c r="DI1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="7">
         <v>146</v>
@@ -2066,11 +2066,14 @@
       </c>
       <c r="DB2" s="15">
         <v>109990</v>
+      </c>
+      <c r="DC2" s="15">
+        <v>111735</v>
       </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="7">
         <v>138</v>
@@ -2386,11 +2389,14 @@
       </c>
       <c r="DB3" s="15">
         <v>80449</v>
+      </c>
+      <c r="DC3" s="15">
+        <v>81588</v>
       </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="7">
         <v>6</v>
@@ -2710,7 +2716,7 @@
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2939,7 +2945,7 @@
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -3255,7 +3261,7 @@
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -4153,7 +4159,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -4162,121 +4168,121 @@
     </row>
     <row r="6" spans="1:39" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="C6" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D6" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="F6" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="J6" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="L6" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="K6" s="14" t="s">
+      <c r="M6" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="P6" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="L6" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="P6" s="14" t="s">
+      <c r="Q6" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="R6" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="S6" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="T6" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="S6" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="T6" s="14" t="s">
+      <c r="U6" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="V6" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="V6" s="14" t="s">
+      <c r="W6" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="W6" s="14" t="s">
+      <c r="X6" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y6" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA6" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB6" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC6" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD6" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="X6" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="Y6" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="Z6" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="AA6" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="AB6" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="AC6" s="14" t="s">
+      <c r="AE6" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="AF6" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="AD6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AE6" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="AF6" s="14" t="s">
+      <c r="AG6" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="AG6" s="14" t="s">
+      <c r="AH6" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="AH6" s="14" t="s">
+      <c r="AI6" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="AI6" s="14" t="s">
+      <c r="AJ6" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="AJ6" s="14" t="s">
+      <c r="AK6" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="AL6" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="AK6" s="14" t="s">
+      <c r="AM6" s="14" t="s">
         <v>142</v>
-      </c>
-      <c r="AL6" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="AM6" s="14" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.2">
@@ -20545,7 +20551,7 @@
       </c>
       <c r="B111" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C111" s="12">
         <v>105</v>
@@ -20698,11 +20704,11 @@
     <row r="112" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A112" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B112" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C112" s="12">
         <v>106</v>
@@ -20717,27 +20723,27 @@
       </c>
       <c r="F112" cm="1">
         <f t="array" ref="F112">+INDEX(Hoja1!$B$2:$MO$7,1,E112)</f>
-        <v>0</v>
+        <v>111735</v>
       </c>
       <c r="G112">
         <f t="shared" si="41"/>
-        <v>-109990</v>
+        <v>1745</v>
       </c>
       <c r="H112" cm="1">
         <f t="array" ref="H112">+INDEX(Hoja1!$B$2:$MO$7,2,$E112)</f>
-        <v>0</v>
+        <v>81588</v>
       </c>
       <c r="I112">
         <f t="shared" si="42"/>
-        <v>-80449</v>
+        <v>1139</v>
       </c>
       <c r="J112">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>30147</v>
       </c>
       <c r="K112">
         <f t="shared" si="43"/>
-        <v>-29541</v>
+        <v>606</v>
       </c>
       <c r="L112" cm="1">
         <f t="array" ref="L112">+INDEX(Hoja1!$B$2:$MO$7,3,$E112)</f>
@@ -20757,19 +20763,19 @@
       </c>
       <c r="P112" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.73019197207678888</v>
       </c>
       <c r="Q112" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.26980802792321118</v>
       </c>
       <c r="R112">
         <f t="shared" si="44"/>
-        <v>-112077</v>
+        <v>-342</v>
       </c>
       <c r="S112">
         <f t="shared" si="45"/>
-        <v>-29541</v>
+        <v>606</v>
       </c>
       <c r="T112">
         <f t="shared" si="46"/>
@@ -20789,11 +20795,11 @@
       </c>
       <c r="X112">
         <f t="shared" si="50"/>
-        <v>-53.702443699089599</v>
+        <v>-0.16387158600862481</v>
       </c>
       <c r="Y112">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.0513862089976641E-2</v>
       </c>
       <c r="Z112">
         <f t="shared" si="52"/>
@@ -20813,11 +20819,11 @@
       </c>
       <c r="AD112">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>26865.833132964657</v>
       </c>
       <c r="AE112">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>7248.6174561192602</v>
       </c>
       <c r="AF112">
         <f t="shared" si="36"/>
@@ -20878,7 +20884,7 @@
       </c>
       <c r="G113">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-111735</v>
       </c>
       <c r="H113" cm="1">
         <f t="array" ref="H113">+INDEX(Hoja1!$B$2:$MO$7,2,$E113)</f>
@@ -20886,7 +20892,7 @@
       </c>
       <c r="I113">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-81588</v>
       </c>
       <c r="J113">
         <f t="shared" si="33"/>
@@ -20894,7 +20900,7 @@
       </c>
       <c r="K113">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-30147</v>
       </c>
       <c r="L113" cm="1">
         <f t="array" ref="L113">+INDEX(Hoja1!$B$2:$MO$7,3,$E113)</f>
@@ -20922,11 +20928,11 @@
       </c>
       <c r="R113">
         <f t="shared" si="44"/>
-        <v>109990</v>
+        <v>-113480</v>
       </c>
       <c r="S113">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-30147</v>
       </c>
       <c r="T113">
         <f t="shared" si="46"/>
@@ -20946,11 +20952,11 @@
       </c>
       <c r="X113">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-65.031518624641834</v>
       </c>
       <c r="Y113">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z113">
         <f t="shared" si="52"/>
@@ -21079,7 +21085,7 @@
       </c>
       <c r="R114">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>111735</v>
       </c>
       <c r="S114">
         <f t="shared" si="45"/>
@@ -21103,7 +21109,7 @@
       </c>
       <c r="X114">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y114">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-26-2020 15-12-38
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1462" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C5399C8C-6A03-F54E-AC9C-956339A88FDB}"/>
+  <xr:revisionPtr revIDLastSave="1471" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A610E0E3-21AE-404D-91D4-EA1D2EA4D5BF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -346,9 +346,6 @@
     <t>12-06-2020</t>
   </si>
   <si>
-    <t>24/6/2020</t>
-  </si>
-  <si>
     <t>25/6/2020</t>
   </si>
   <si>
@@ -518,6 +515,9 @@
   </si>
   <si>
     <t>24-06-20</t>
+  </si>
+  <si>
+    <t>25-06-20</t>
   </si>
 </sst>
 </file>
@@ -955,7 +955,7 @@
     <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="14"/>
     <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="13"/>
     <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="12"/>
-    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="24/6/2020" dataDxfId="11"/>
+    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="11"/>
     <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="25/6/2020" dataDxfId="10"/>
     <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="26/6/2020" dataDxfId="9"/>
     <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="27/6/2020" dataDxfId="8"/>
@@ -1387,8 +1387,8 @@
   <dimension ref="A1:DK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DD4" sqref="DD4"/>
+      <pane xSplit="1" topLeftCell="DD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DE4" sqref="DE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1691,66 +1691,66 @@
         <v>95</v>
       </c>
       <c r="CS1" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="CT1" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="CT1" s="8" t="s">
+      <c r="CU1" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="CU1" s="8" t="s">
+      <c r="CV1" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="CV1" s="8" t="s">
+      <c r="CW1" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="CW1" s="8" t="s">
+      <c r="CX1" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="CX1" s="15" t="s">
+      <c r="CY1" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="CY1" s="16" t="s">
+      <c r="CZ1" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="CZ1" s="16" t="s">
+      <c r="DA1" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="DA1" s="16" t="s">
+      <c r="DB1" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="DB1" s="16" t="s">
+      <c r="DC1" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="DC1" s="16" t="s">
+      <c r="DD1" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="DD1" s="16" t="s">
+      <c r="DE1" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="DE1" s="15" t="s">
+      <c r="DF1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="DF1" s="15" t="s">
+      <c r="DG1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="DG1" s="15" t="s">
+      <c r="DH1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="DH1" s="15" t="s">
+      <c r="DI1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="7">
         <v>146</v>
@@ -2072,11 +2072,14 @@
       </c>
       <c r="DD2" s="15">
         <v>114042</v>
+      </c>
+      <c r="DE2" s="15">
+        <v>117266</v>
       </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="7">
         <v>138</v>
@@ -2398,11 +2401,14 @@
       </c>
       <c r="DD3" s="15">
         <v>83167</v>
+      </c>
+      <c r="DE3" s="15">
+        <v>85384</v>
       </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="7">
         <v>6</v>
@@ -2721,11 +2727,14 @@
       </c>
       <c r="DC4" s="15">
         <v>10548</v>
+      </c>
+      <c r="DD4" s="15">
+        <v>11135</v>
       </c>
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2954,10 +2963,13 @@
       <c r="DC5" s="15">
         <v>756</v>
       </c>
+      <c r="DD5" s="15">
+        <v>766</v>
+      </c>
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -3273,10 +3285,13 @@
       <c r="DC6" s="15">
         <v>649</v>
       </c>
+      <c r="DD6" s="15">
+        <v>649</v>
+      </c>
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -3593,6 +3608,9 @@
       </c>
       <c r="DC7" s="15">
         <v>131</v>
+      </c>
+      <c r="DD7" s="15">
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:115" x14ac:dyDescent="0.2">
@@ -4177,7 +4195,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -4186,121 +4204,121 @@
     </row>
     <row r="6" spans="1:39" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="C6" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D6" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="F6" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="J6" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="L6" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="K6" s="14" t="s">
+      <c r="M6" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="P6" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="L6" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="P6" s="14" t="s">
+      <c r="Q6" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="R6" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="S6" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="T6" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="S6" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="T6" s="14" t="s">
+      <c r="U6" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="V6" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="V6" s="14" t="s">
+      <c r="W6" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="W6" s="14" t="s">
+      <c r="X6" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y6" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA6" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB6" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC6" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD6" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="X6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y6" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z6" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="AA6" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="AB6" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="AC6" s="14" t="s">
+      <c r="AE6" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="AF6" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="AD6" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE6" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF6" s="14" t="s">
+      <c r="AG6" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="AG6" s="14" t="s">
+      <c r="AH6" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="AH6" s="14" t="s">
+      <c r="AI6" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="AI6" s="14" t="s">
+      <c r="AJ6" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="AJ6" s="14" t="s">
+      <c r="AK6" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="AL6" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="AK6" s="14" t="s">
+      <c r="AM6" s="14" t="s">
         <v>140</v>
-      </c>
-      <c r="AL6" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="AM6" s="14" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.2">
@@ -20883,7 +20901,7 @@
       </c>
       <c r="B113" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C113" s="12">
         <v>107</v>
@@ -20922,19 +20940,19 @@
       </c>
       <c r="L113" cm="1">
         <f t="array" ref="L113">+INDEX(Hoja1!$B$2:$MO$7,3,$E113)</f>
-        <v>0</v>
+        <v>11135</v>
       </c>
       <c r="M113" cm="1">
         <f t="array" ref="M113">+INDEX(Hoja1!$B$2:$MO$7,4,$E113)</f>
-        <v>0</v>
+        <v>766</v>
       </c>
       <c r="N113" cm="1">
         <f t="array" ref="N113">+INDEX(Hoja1!$B$2:$MO$7,5,$E113)</f>
-        <v>0</v>
+        <v>649</v>
       </c>
       <c r="O113" cm="1">
         <f t="array" ref="O113">+INDEX(Hoja1!$B$2:$MO$7,6,$E113)</f>
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="P113" s="13">
         <f t="shared" si="60"/>
@@ -20954,19 +20972,19 @@
       </c>
       <c r="T113">
         <f t="shared" si="46"/>
-        <v>-10548</v>
+        <v>587</v>
       </c>
       <c r="U113">
         <f t="shared" si="47"/>
-        <v>-756</v>
+        <v>10</v>
       </c>
       <c r="V113">
         <f t="shared" si="48"/>
-        <v>-649</v>
+        <v>0</v>
       </c>
       <c r="W113">
         <f t="shared" si="49"/>
-        <v>-131</v>
+        <v>-1</v>
       </c>
       <c r="X113">
         <f t="shared" si="50"/>
@@ -20978,19 +20996,19 @@
       </c>
       <c r="Z113">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0556503602578688</v>
       </c>
       <c r="AA113">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1.0132275132275133</v>
       </c>
       <c r="AB113">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC113">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>0.99236641221374045</v>
       </c>
       <c r="AD113">
         <f t="shared" si="34"/>
@@ -21002,45 +21020,45 @@
       </c>
       <c r="AF113">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>2677.326280355855</v>
       </c>
       <c r="AG113">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>184.17888915604715</v>
       </c>
       <c r="AH113">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>156.04712671315221</v>
       </c>
       <c r="AI113">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>31.25751382543881</v>
       </c>
       <c r="AJ113">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>12680</v>
       </c>
       <c r="AK113">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>3048.8098100504931</v>
       </c>
       <c r="AL113">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ112</f>
-        <v>-12084</v>
+        <v>596</v>
       </c>
       <c r="AM113">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ112,0)</f>
-        <v>-1</v>
+        <v>4.932141674942072E-2</v>
       </c>
     </row>
     <row r="114" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A114" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B114" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C114" s="12">
         <v>108</v>
@@ -21055,27 +21073,27 @@
       </c>
       <c r="F114" cm="1">
         <f t="array" ref="F114">+INDEX(Hoja1!$B$2:$MO$7,1,E114)</f>
-        <v>0</v>
+        <v>117266</v>
       </c>
       <c r="G114">
         <f t="shared" si="41"/>
-        <v>-114042</v>
+        <v>3224</v>
       </c>
       <c r="H114" cm="1">
         <f t="array" ref="H114">+INDEX(Hoja1!$B$2:$MO$7,2,$E114)</f>
-        <v>0</v>
+        <v>85384</v>
       </c>
       <c r="I114">
         <f t="shared" si="42"/>
-        <v>-83167</v>
+        <v>2217</v>
       </c>
       <c r="J114">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>31882</v>
       </c>
       <c r="K114">
         <f t="shared" si="43"/>
-        <v>-30875</v>
+        <v>1007</v>
       </c>
       <c r="L114" cm="1">
         <f t="array" ref="L114">+INDEX(Hoja1!$B$2:$MO$7,3,$E114)</f>
@@ -21095,43 +21113,43 @@
       </c>
       <c r="P114" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.72812238841607968</v>
       </c>
       <c r="Q114" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.27187761158392032</v>
       </c>
       <c r="R114">
         <f t="shared" si="44"/>
-        <v>-116349</v>
+        <v>917</v>
       </c>
       <c r="S114">
         <f t="shared" si="45"/>
-        <v>-30875</v>
+        <v>1007</v>
       </c>
       <c r="T114">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-11135</v>
       </c>
       <c r="U114">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-766</v>
       </c>
       <c r="V114">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-649</v>
       </c>
       <c r="W114">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-130</v>
       </c>
       <c r="X114">
         <f t="shared" si="50"/>
-        <v>-50.433029908972692</v>
+        <v>0.39748591244039877</v>
       </c>
       <c r="Y114">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>3.2615384615384616E-2</v>
       </c>
       <c r="Z114">
         <f t="shared" si="52"/>
@@ -21151,11 +21169,11 @@
       </c>
       <c r="AD114">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>28195.720125030057</v>
       </c>
       <c r="AE114">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>7665.7850444818469</v>
       </c>
       <c r="AF114">
         <f t="shared" si="36"/>
@@ -21183,11 +21201,11 @@
       </c>
       <c r="AL114">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ113</f>
-        <v>0</v>
+        <v>-12680</v>
       </c>
       <c r="AM114">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ113,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="115" spans="1:39" x14ac:dyDescent="0.2">
@@ -21216,7 +21234,7 @@
       </c>
       <c r="G115">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-117266</v>
       </c>
       <c r="H115" cm="1">
         <f t="array" ref="H115">+INDEX(Hoja1!$B$2:$MO$7,2,$E115)</f>
@@ -21224,7 +21242,7 @@
       </c>
       <c r="I115">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-85384</v>
       </c>
       <c r="J115">
         <f t="shared" si="33"/>
@@ -21232,7 +21250,7 @@
       </c>
       <c r="K115">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-31882</v>
       </c>
       <c r="L115" cm="1">
         <f t="array" ref="L115">+INDEX(Hoja1!$B$2:$MO$7,3,$E115)</f>
@@ -21260,11 +21278,11 @@
       </c>
       <c r="R115">
         <f t="shared" si="44"/>
-        <v>114042</v>
+        <v>-120490</v>
       </c>
       <c r="S115">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-31882</v>
       </c>
       <c r="T115">
         <f t="shared" si="46"/>
@@ -21284,11 +21302,11 @@
       </c>
       <c r="X115">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-37.372828784119108</v>
       </c>
       <c r="Y115">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z115">
         <f t="shared" si="52"/>
@@ -21417,7 +21435,7 @@
       </c>
       <c r="R116">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>117266</v>
       </c>
       <c r="S116">
         <f t="shared" si="45"/>
@@ -21441,7 +21459,7 @@
       </c>
       <c r="X116">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y116">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-27-2020 03-14-48
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1471" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A610E0E3-21AE-404D-91D4-EA1D2EA4D5BF}"/>
+  <xr:revisionPtr revIDLastSave="1478" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ACB448E2-C4EE-6B4C-B46F-60495156581E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -346,9 +346,6 @@
     <t>12-06-2020</t>
   </si>
   <si>
-    <t>25/6/2020</t>
-  </si>
-  <si>
     <t>26/6/2020</t>
   </si>
   <si>
@@ -518,6 +515,9 @@
   </si>
   <si>
     <t>25-06-20</t>
+  </si>
+  <si>
+    <t>26-06-20</t>
   </si>
 </sst>
 </file>
@@ -956,7 +956,7 @@
     <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="13"/>
     <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="12"/>
     <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="11"/>
-    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="25/6/2020" dataDxfId="10"/>
+    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="10"/>
     <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="26/6/2020" dataDxfId="9"/>
     <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="27/6/2020" dataDxfId="8"/>
     <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="28/6/2020"/>
@@ -1388,7 +1388,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="DD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DE4" sqref="DE4"/>
+      <selection pane="topRight" activeCell="DF4" sqref="DF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1691,66 +1691,66 @@
         <v>95</v>
       </c>
       <c r="CS1" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="CT1" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="CT1" s="8" t="s">
+      <c r="CU1" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="CU1" s="8" t="s">
+      <c r="CV1" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="CV1" s="8" t="s">
+      <c r="CW1" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="CW1" s="8" t="s">
+      <c r="CX1" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="CX1" s="15" t="s">
+      <c r="CY1" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="CY1" s="16" t="s">
+      <c r="CZ1" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="CZ1" s="16" t="s">
+      <c r="DA1" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="DA1" s="16" t="s">
+      <c r="DB1" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="DB1" s="16" t="s">
+      <c r="DC1" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="DC1" s="16" t="s">
+      <c r="DD1" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="DD1" s="16" t="s">
+      <c r="DE1" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="DE1" s="16" t="s">
+      <c r="DF1" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="DF1" s="15" t="s">
+      <c r="DG1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="DG1" s="15" t="s">
+      <c r="DH1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="DH1" s="15" t="s">
+      <c r="DI1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" s="7">
         <v>146</v>
@@ -2075,11 +2075,14 @@
       </c>
       <c r="DE2" s="15">
         <v>117266</v>
+      </c>
+      <c r="DF2" s="15">
+        <v>120303</v>
       </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="7">
         <v>138</v>
@@ -2404,11 +2407,14 @@
       </c>
       <c r="DE3" s="15">
         <v>85384</v>
+      </c>
+      <c r="DF3" s="15">
+        <v>87545</v>
       </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="7">
         <v>6</v>
@@ -2730,11 +2736,14 @@
       </c>
       <c r="DD4" s="15">
         <v>11135</v>
+      </c>
+      <c r="DE4" s="15">
+        <v>12111</v>
       </c>
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2966,10 +2975,13 @@
       <c r="DD5" s="15">
         <v>766</v>
       </c>
+      <c r="DE5" s="15">
+        <v>736</v>
+      </c>
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -3288,10 +3300,13 @@
       <c r="DD6" s="15">
         <v>649</v>
       </c>
+      <c r="DE6" s="15">
+        <v>686</v>
+      </c>
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -3611,6 +3626,9 @@
       </c>
       <c r="DD7" s="15">
         <v>130</v>
+      </c>
+      <c r="DE7" s="15">
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:115" x14ac:dyDescent="0.2">
@@ -4195,7 +4213,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -4204,121 +4222,121 @@
     </row>
     <row r="6" spans="1:39" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="C6" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D6" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="F6" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="J6" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="L6" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="K6" s="14" t="s">
+      <c r="M6" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="P6" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="L6" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="P6" s="14" t="s">
+      <c r="Q6" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="R6" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="S6" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="T6" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="S6" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="T6" s="14" t="s">
+      <c r="U6" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="V6" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="V6" s="14" t="s">
+      <c r="W6" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="W6" s="14" t="s">
+      <c r="X6" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y6" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA6" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB6" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC6" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="AD6" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="X6" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="Y6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z6" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="AA6" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="AB6" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="AC6" s="14" t="s">
+      <c r="AE6" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="AF6" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AD6" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="AE6" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF6" s="14" t="s">
+      <c r="AG6" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="AG6" s="14" t="s">
+      <c r="AH6" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="AH6" s="14" t="s">
+      <c r="AI6" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="AI6" s="14" t="s">
+      <c r="AJ6" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="AJ6" s="14" t="s">
+      <c r="AK6" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="AL6" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="AK6" s="14" t="s">
+      <c r="AM6" s="14" t="s">
         <v>139</v>
-      </c>
-      <c r="AL6" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="AM6" s="14" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.2">
@@ -21058,7 +21076,7 @@
       </c>
       <c r="B114" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C114" s="12">
         <v>108</v>
@@ -21097,19 +21115,19 @@
       </c>
       <c r="L114" cm="1">
         <f t="array" ref="L114">+INDEX(Hoja1!$B$2:$MO$7,3,$E114)</f>
-        <v>0</v>
+        <v>12111</v>
       </c>
       <c r="M114" cm="1">
         <f t="array" ref="M114">+INDEX(Hoja1!$B$2:$MO$7,4,$E114)</f>
-        <v>0</v>
+        <v>736</v>
       </c>
       <c r="N114" cm="1">
         <f t="array" ref="N114">+INDEX(Hoja1!$B$2:$MO$7,5,$E114)</f>
-        <v>0</v>
+        <v>686</v>
       </c>
       <c r="O114" cm="1">
         <f t="array" ref="O114">+INDEX(Hoja1!$B$2:$MO$7,6,$E114)</f>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="P114" s="13">
         <f t="shared" si="60"/>
@@ -21129,19 +21147,19 @@
       </c>
       <c r="T114">
         <f t="shared" si="46"/>
-        <v>-11135</v>
+        <v>976</v>
       </c>
       <c r="U114">
         <f t="shared" si="47"/>
-        <v>-766</v>
+        <v>-30</v>
       </c>
       <c r="V114">
         <f t="shared" si="48"/>
-        <v>-649</v>
+        <v>37</v>
       </c>
       <c r="W114">
         <f t="shared" si="49"/>
-        <v>-130</v>
+        <v>10</v>
       </c>
       <c r="X114">
         <f t="shared" si="50"/>
@@ -21153,19 +21171,19 @@
       </c>
       <c r="Z114">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.087651549169286</v>
       </c>
       <c r="AA114">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>0.96083550913838123</v>
       </c>
       <c r="AB114">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0570107858243452</v>
       </c>
       <c r="AC114">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.0769230769230769</v>
       </c>
       <c r="AD114">
         <f t="shared" si="34"/>
@@ -21177,45 +21195,45 @@
       </c>
       <c r="AF114">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>2911.998076460688</v>
       </c>
       <c r="AG114">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>176.96561673479204</v>
       </c>
       <c r="AH114">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>164.94349603270018</v>
       </c>
       <c r="AI114">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>33.661937965857177</v>
       </c>
       <c r="AJ114">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>13673</v>
       </c>
       <c r="AK114">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>3287.5691271940373</v>
       </c>
       <c r="AL114">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ113</f>
-        <v>-12680</v>
+        <v>993</v>
       </c>
       <c r="AM114">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ113,0)</f>
-        <v>-1</v>
+        <v>7.8312302839116721E-2</v>
       </c>
     </row>
     <row r="115" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A115" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B115" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C115" s="12">
         <v>109</v>
@@ -21230,27 +21248,27 @@
       </c>
       <c r="F115" cm="1">
         <f t="array" ref="F115">+INDEX(Hoja1!$B$2:$MO$7,1,E115)</f>
-        <v>0</v>
+        <v>120303</v>
       </c>
       <c r="G115">
         <f t="shared" si="41"/>
-        <v>-117266</v>
+        <v>3037</v>
       </c>
       <c r="H115" cm="1">
         <f t="array" ref="H115">+INDEX(Hoja1!$B$2:$MO$7,2,$E115)</f>
-        <v>0</v>
+        <v>87545</v>
       </c>
       <c r="I115">
         <f t="shared" si="42"/>
-        <v>-85384</v>
+        <v>2161</v>
       </c>
       <c r="J115">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>32758</v>
       </c>
       <c r="K115">
         <f t="shared" si="43"/>
-        <v>-31882</v>
+        <v>876</v>
       </c>
       <c r="L115" cm="1">
         <f t="array" ref="L115">+INDEX(Hoja1!$B$2:$MO$7,3,$E115)</f>
@@ -21270,43 +21288,43 @@
       </c>
       <c r="P115" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.72770421352750969</v>
       </c>
       <c r="Q115" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.27229578647249031</v>
       </c>
       <c r="R115">
         <f t="shared" si="44"/>
-        <v>-120490</v>
+        <v>-187</v>
       </c>
       <c r="S115">
         <f t="shared" si="45"/>
-        <v>-31882</v>
+        <v>876</v>
       </c>
       <c r="T115">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-12111</v>
       </c>
       <c r="U115">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-736</v>
       </c>
       <c r="V115">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-686</v>
       </c>
       <c r="W115">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-140</v>
       </c>
       <c r="X115">
         <f t="shared" si="50"/>
-        <v>-37.372828784119108</v>
+        <v>-5.8002481389578163E-2</v>
       </c>
       <c r="Y115">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.7476318926039772E-2</v>
       </c>
       <c r="Z115">
         <f t="shared" si="52"/>
@@ -21326,11 +21344,11 @@
       </c>
       <c r="AD115">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>28925.943736475114</v>
       </c>
       <c r="AE115">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>7876.4125991824958</v>
       </c>
       <c r="AF115">
         <f t="shared" si="36"/>
@@ -21358,11 +21376,11 @@
       </c>
       <c r="AL115">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ114</f>
-        <v>0</v>
+        <v>-13673</v>
       </c>
       <c r="AM115">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ114,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="116" spans="1:39" x14ac:dyDescent="0.2">
@@ -21391,7 +21409,7 @@
       </c>
       <c r="G116">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-120303</v>
       </c>
       <c r="H116" cm="1">
         <f t="array" ref="H116">+INDEX(Hoja1!$B$2:$MO$7,2,$E116)</f>
@@ -21399,7 +21417,7 @@
       </c>
       <c r="I116">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-87545</v>
       </c>
       <c r="J116">
         <f t="shared" si="33"/>
@@ -21407,7 +21425,7 @@
       </c>
       <c r="K116">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-32758</v>
       </c>
       <c r="L116" cm="1">
         <f t="array" ref="L116">+INDEX(Hoja1!$B$2:$MO$7,3,$E116)</f>
@@ -21435,11 +21453,11 @@
       </c>
       <c r="R116">
         <f t="shared" si="44"/>
-        <v>117266</v>
+        <v>-123340</v>
       </c>
       <c r="S116">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-32758</v>
       </c>
       <c r="T116">
         <f t="shared" si="46"/>
@@ -21459,11 +21477,11 @@
       </c>
       <c r="X116">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-40.612446493249919</v>
       </c>
       <c r="Y116">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z116">
         <f t="shared" si="52"/>
@@ -21592,7 +21610,7 @@
       </c>
       <c r="R117">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>120303</v>
       </c>
       <c r="S117">
         <f t="shared" si="45"/>
@@ -21616,7 +21634,7 @@
       </c>
       <c r="X117">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y117">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-28-2020 03-17-22
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1478" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ACB448E2-C4EE-6B4C-B46F-60495156581E}"/>
+  <xr:revisionPtr revIDLastSave="1489" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F1F4AEB3-BD32-4F41-B348-9E2204BB0D99}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -346,9 +346,6 @@
     <t>12-06-2020</t>
   </si>
   <si>
-    <t>26/6/2020</t>
-  </si>
-  <si>
     <t>27/6/2020</t>
   </si>
   <si>
@@ -518,6 +515,9 @@
   </si>
   <si>
     <t>26-06-20</t>
+  </si>
+  <si>
+    <t>27-06-20</t>
   </si>
 </sst>
 </file>
@@ -957,7 +957,7 @@
     <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="12"/>
     <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="11"/>
     <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="10"/>
-    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="26/6/2020" dataDxfId="9"/>
+    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="9"/>
     <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="27/6/2020" dataDxfId="8"/>
     <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="28/6/2020"/>
     <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="29/6/2020"/>
@@ -1388,7 +1388,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="DD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DF4" sqref="DF4"/>
+      <selection pane="topRight" activeCell="DG8" sqref="DG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1691,66 +1691,66 @@
         <v>95</v>
       </c>
       <c r="CS1" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="CT1" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="CT1" s="8" t="s">
+      <c r="CU1" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="CU1" s="8" t="s">
+      <c r="CV1" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="CV1" s="8" t="s">
+      <c r="CW1" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="CW1" s="8" t="s">
+      <c r="CX1" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="CX1" s="15" t="s">
+      <c r="CY1" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="CY1" s="16" t="s">
+      <c r="CZ1" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="CZ1" s="16" t="s">
+      <c r="DA1" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="DA1" s="16" t="s">
+      <c r="DB1" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="DB1" s="16" t="s">
+      <c r="DC1" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="DC1" s="16" t="s">
+      <c r="DD1" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="DD1" s="16" t="s">
+      <c r="DE1" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="DE1" s="16" t="s">
+      <c r="DF1" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="DF1" s="16" t="s">
+      <c r="DG1" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="DG1" s="15" t="s">
+      <c r="DH1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="DH1" s="15" t="s">
+      <c r="DI1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="7">
         <v>146</v>
@@ -2078,11 +2078,14 @@
       </c>
       <c r="DF2" s="15">
         <v>120303</v>
+      </c>
+      <c r="DG2" s="15">
+        <v>122668</v>
       </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="7">
         <v>138</v>
@@ -2410,11 +2413,14 @@
       </c>
       <c r="DF3" s="15">
         <v>87545</v>
+      </c>
+      <c r="DG3" s="15">
+        <v>89143</v>
       </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" s="7">
         <v>6</v>
@@ -2739,11 +2745,17 @@
       </c>
       <c r="DE4" s="15">
         <v>12111</v>
+      </c>
+      <c r="DF4" s="15">
+        <v>12457</v>
+      </c>
+      <c r="DG4" s="15">
+        <v>13116</v>
       </c>
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2978,10 +2990,16 @@
       <c r="DE5" s="15">
         <v>736</v>
       </c>
+      <c r="DF5" s="15">
+        <v>741</v>
+      </c>
+      <c r="DG5" s="15">
+        <v>712</v>
+      </c>
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -3303,10 +3321,16 @@
       <c r="DE6" s="15">
         <v>686</v>
       </c>
+      <c r="DF6" s="15">
+        <v>714</v>
+      </c>
+      <c r="DG6" s="15">
+        <v>727</v>
+      </c>
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -3629,6 +3653,12 @@
       </c>
       <c r="DE7" s="15">
         <v>140</v>
+      </c>
+      <c r="DF7" s="15">
+        <v>148</v>
+      </c>
+      <c r="DG7" s="15">
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:115" x14ac:dyDescent="0.2">
@@ -4213,7 +4243,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44008</v>
+        <v>44009</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -4222,121 +4252,121 @@
     </row>
     <row r="6" spans="1:39" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="C6" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D6" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="F6" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="J6" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="L6" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="K6" s="14" t="s">
+      <c r="M6" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="P6" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="L6" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="P6" s="14" t="s">
+      <c r="Q6" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="R6" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="S6" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="T6" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="S6" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="T6" s="14" t="s">
+      <c r="U6" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="V6" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="V6" s="14" t="s">
+      <c r="W6" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="W6" s="14" t="s">
+      <c r="X6" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y6" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA6" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB6" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC6" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD6" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="X6" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="Y6" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AA6" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="AB6" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="AC6" s="14" t="s">
+      <c r="AE6" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="AF6" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="AD6" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="AE6" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="AF6" s="14" t="s">
+      <c r="AG6" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AG6" s="14" t="s">
+      <c r="AH6" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="AH6" s="14" t="s">
+      <c r="AI6" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="AI6" s="14" t="s">
+      <c r="AJ6" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="AJ6" s="14" t="s">
+      <c r="AK6" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="AL6" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="AK6" s="14" t="s">
+      <c r="AM6" s="14" t="s">
         <v>138</v>
-      </c>
-      <c r="AL6" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="AM6" s="14" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.2">
@@ -21233,7 +21263,7 @@
       </c>
       <c r="B115" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C115" s="12">
         <v>109</v>
@@ -21272,19 +21302,19 @@
       </c>
       <c r="L115" cm="1">
         <f t="array" ref="L115">+INDEX(Hoja1!$B$2:$MO$7,3,$E115)</f>
-        <v>0</v>
+        <v>12457</v>
       </c>
       <c r="M115" cm="1">
         <f t="array" ref="M115">+INDEX(Hoja1!$B$2:$MO$7,4,$E115)</f>
-        <v>0</v>
+        <v>741</v>
       </c>
       <c r="N115" cm="1">
         <f t="array" ref="N115">+INDEX(Hoja1!$B$2:$MO$7,5,$E115)</f>
-        <v>0</v>
+        <v>714</v>
       </c>
       <c r="O115" cm="1">
         <f t="array" ref="O115">+INDEX(Hoja1!$B$2:$MO$7,6,$E115)</f>
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="P115" s="13">
         <f t="shared" si="60"/>
@@ -21304,19 +21334,19 @@
       </c>
       <c r="T115">
         <f t="shared" si="46"/>
-        <v>-12111</v>
+        <v>346</v>
       </c>
       <c r="U115">
         <f t="shared" si="47"/>
-        <v>-736</v>
+        <v>5</v>
       </c>
       <c r="V115">
         <f t="shared" si="48"/>
-        <v>-686</v>
+        <v>28</v>
       </c>
       <c r="W115">
         <f t="shared" si="49"/>
-        <v>-140</v>
+        <v>8</v>
       </c>
       <c r="X115">
         <f t="shared" si="50"/>
@@ -21328,19 +21358,19 @@
       </c>
       <c r="Z115">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0285690694410041</v>
       </c>
       <c r="AA115">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1.0067934782608696</v>
       </c>
       <c r="AB115">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0408163265306123</v>
       </c>
       <c r="AC115">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.0571428571428572</v>
       </c>
       <c r="AD115">
         <f t="shared" si="34"/>
@@ -21352,45 +21382,45 @@
       </c>
       <c r="AF115">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>2995.1911517191634</v>
       </c>
       <c r="AG115">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>178.16782880500122</v>
       </c>
       <c r="AH115">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>171.67588362587162</v>
       </c>
       <c r="AI115">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>35.585477278191874</v>
       </c>
       <c r="AJ115">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>14060</v>
       </c>
       <c r="AK115">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>3380.6203414282281</v>
       </c>
       <c r="AL115">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ114</f>
-        <v>-13673</v>
+        <v>387</v>
       </c>
       <c r="AM115">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ114,0)</f>
-        <v>-1</v>
+        <v>2.8303956702991295E-2</v>
       </c>
     </row>
     <row r="116" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A116" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B116" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C116" s="12">
         <v>110</v>
@@ -21405,139 +21435,139 @@
       </c>
       <c r="F116" cm="1">
         <f t="array" ref="F116">+INDEX(Hoja1!$B$2:$MO$7,1,E116)</f>
-        <v>0</v>
+        <v>122668</v>
       </c>
       <c r="G116">
         <f t="shared" si="41"/>
-        <v>-120303</v>
+        <v>2365</v>
       </c>
       <c r="H116" cm="1">
         <f t="array" ref="H116">+INDEX(Hoja1!$B$2:$MO$7,2,$E116)</f>
-        <v>0</v>
+        <v>89143</v>
       </c>
       <c r="I116">
         <f t="shared" si="42"/>
-        <v>-87545</v>
+        <v>1598</v>
       </c>
       <c r="J116">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>33525</v>
       </c>
       <c r="K116">
         <f t="shared" si="43"/>
-        <v>-32758</v>
+        <v>767</v>
       </c>
       <c r="L116" cm="1">
         <f t="array" ref="L116">+INDEX(Hoja1!$B$2:$MO$7,3,$E116)</f>
-        <v>0</v>
+        <v>13116</v>
       </c>
       <c r="M116" cm="1">
         <f t="array" ref="M116">+INDEX(Hoja1!$B$2:$MO$7,4,$E116)</f>
-        <v>0</v>
+        <v>712</v>
       </c>
       <c r="N116" cm="1">
         <f t="array" ref="N116">+INDEX(Hoja1!$B$2:$MO$7,5,$E116)</f>
-        <v>0</v>
+        <v>727</v>
       </c>
       <c r="O116" cm="1">
         <f t="array" ref="O116">+INDEX(Hoja1!$B$2:$MO$7,6,$E116)</f>
-        <v>0</v>
+        <v>141</v>
       </c>
       <c r="P116" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.72670134020282384</v>
       </c>
       <c r="Q116" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.2732986597971761</v>
       </c>
       <c r="R116">
         <f t="shared" si="44"/>
-        <v>-123340</v>
+        <v>-672</v>
       </c>
       <c r="S116">
         <f t="shared" si="45"/>
-        <v>-32758</v>
+        <v>767</v>
       </c>
       <c r="T116">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>659</v>
       </c>
       <c r="U116">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-29</v>
       </c>
       <c r="V116">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="W116">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-7</v>
       </c>
       <c r="X116">
         <f t="shared" si="50"/>
-        <v>-40.612446493249919</v>
+        <v>-0.22127099110964768</v>
       </c>
       <c r="Y116">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.3414127846632885E-2</v>
       </c>
       <c r="Z116">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0529019828209039</v>
       </c>
       <c r="AA116">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>0.96086369770580293</v>
       </c>
       <c r="AB116">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0182072829131652</v>
       </c>
       <c r="AC116">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>0.95270270270270274</v>
       </c>
       <c r="AD116">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>29494.590045684061</v>
       </c>
       <c r="AE116">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>8060.8319307525853</v>
       </c>
       <c r="AF116">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>3153.6427025727339</v>
       </c>
       <c r="AG116">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>171.19499879778795</v>
       </c>
       <c r="AH116">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>174.8016350084155</v>
       </c>
       <c r="AI116">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>33.902380379899014</v>
       </c>
       <c r="AJ116">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>14696</v>
       </c>
       <c r="AK116">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>3533.5417167588366</v>
       </c>
       <c r="AL116">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ115</f>
-        <v>0</v>
+        <v>636</v>
       </c>
       <c r="AM116">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ115,0)</f>
-        <v>0</v>
+        <v>4.5234708392603129E-2</v>
       </c>
     </row>
     <row r="117" spans="1:39" x14ac:dyDescent="0.2">
@@ -21566,7 +21596,7 @@
       </c>
       <c r="G117">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-122668</v>
       </c>
       <c r="H117" cm="1">
         <f t="array" ref="H117">+INDEX(Hoja1!$B$2:$MO$7,2,$E117)</f>
@@ -21574,7 +21604,7 @@
       </c>
       <c r="I117">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-89143</v>
       </c>
       <c r="J117">
         <f t="shared" si="33"/>
@@ -21582,7 +21612,7 @@
       </c>
       <c r="K117">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-33525</v>
       </c>
       <c r="L117" cm="1">
         <f t="array" ref="L117">+INDEX(Hoja1!$B$2:$MO$7,3,$E117)</f>
@@ -21610,35 +21640,35 @@
       </c>
       <c r="R117">
         <f t="shared" si="44"/>
-        <v>120303</v>
+        <v>-125033</v>
       </c>
       <c r="S117">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-33525</v>
       </c>
       <c r="T117">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-13116</v>
       </c>
       <c r="U117">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-712</v>
       </c>
       <c r="V117">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-727</v>
       </c>
       <c r="W117">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-141</v>
       </c>
       <c r="X117">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-52.868076109936574</v>
       </c>
       <c r="Y117">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z117">
         <f t="shared" si="52"/>
@@ -21690,11 +21720,11 @@
       </c>
       <c r="AL117">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ116</f>
-        <v>0</v>
+        <v>-14696</v>
       </c>
       <c r="AM117">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ116,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="118" spans="1:39" x14ac:dyDescent="0.2">
@@ -21767,7 +21797,7 @@
       </c>
       <c r="R118">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>122668</v>
       </c>
       <c r="S118">
         <f t="shared" si="45"/>
@@ -21791,7 +21821,7 @@
       </c>
       <c r="X118">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y118">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-29-2020 07-20-33
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1489" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F1F4AEB3-BD32-4F41-B348-9E2204BB0D99}"/>
+  <xr:revisionPtr revIDLastSave="1496" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5E0C1671-FC1C-A84E-A1F5-8CF6FFBCD339}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -346,9 +346,6 @@
     <t>12-06-2020</t>
   </si>
   <si>
-    <t>27/6/2020</t>
-  </si>
-  <si>
     <t>28/6/2020</t>
   </si>
   <si>
@@ -518,6 +515,9 @@
   </si>
   <si>
     <t>27-06-20</t>
+  </si>
+  <si>
+    <t>28-06-20</t>
   </si>
 </sst>
 </file>
@@ -958,7 +958,7 @@
     <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="11"/>
     <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="10"/>
     <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="9"/>
-    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="27/6/2020" dataDxfId="8"/>
+    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="8"/>
     <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="28/6/2020"/>
     <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="29/6/2020"/>
     <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="30/6/2020"/>
@@ -1387,8 +1387,8 @@
   <dimension ref="A1:DK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DG8" sqref="DG8"/>
+      <pane xSplit="1" topLeftCell="DF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DH17" sqref="DH17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1691,66 +1691,66 @@
         <v>95</v>
       </c>
       <c r="CS1" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="CT1" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="CT1" s="8" t="s">
+      <c r="CU1" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="CU1" s="8" t="s">
+      <c r="CV1" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="CV1" s="8" t="s">
+      <c r="CW1" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="CW1" s="8" t="s">
+      <c r="CX1" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="CX1" s="15" t="s">
+      <c r="CY1" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="CY1" s="16" t="s">
+      <c r="CZ1" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="CZ1" s="16" t="s">
+      <c r="DA1" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="DA1" s="16" t="s">
+      <c r="DB1" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="DB1" s="16" t="s">
+      <c r="DC1" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="DC1" s="16" t="s">
+      <c r="DD1" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="DD1" s="16" t="s">
+      <c r="DE1" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="DE1" s="16" t="s">
+      <c r="DF1" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="DF1" s="16" t="s">
+      <c r="DG1" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="DG1" s="16" t="s">
+      <c r="DH1" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="DH1" s="15" t="s">
+      <c r="DI1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="7">
         <v>146</v>
@@ -2081,11 +2081,14 @@
       </c>
       <c r="DG2" s="15">
         <v>122668</v>
+      </c>
+      <c r="DH2" s="15">
+        <v>125570</v>
       </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="7">
         <v>138</v>
@@ -2416,11 +2419,14 @@
       </c>
       <c r="DG3" s="15">
         <v>89143</v>
+      </c>
+      <c r="DH3" s="15">
+        <v>91023</v>
       </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="7">
         <v>6</v>
@@ -2751,11 +2757,14 @@
       </c>
       <c r="DG4" s="15">
         <v>13116</v>
+      </c>
+      <c r="DH4" s="15">
+        <v>13996</v>
       </c>
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2996,10 +3005,13 @@
       <c r="DG5" s="15">
         <v>712</v>
       </c>
+      <c r="DH5" s="15">
+        <v>764</v>
+      </c>
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -3327,10 +3339,13 @@
       <c r="DG6" s="15">
         <v>727</v>
       </c>
+      <c r="DH6" s="15">
+        <v>712</v>
+      </c>
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -3659,6 +3674,9 @@
       </c>
       <c r="DG7" s="15">
         <v>141</v>
+      </c>
+      <c r="DH7" s="15">
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:115" x14ac:dyDescent="0.2">
@@ -4243,7 +4261,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -4252,121 +4270,121 @@
     </row>
     <row r="6" spans="1:39" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="C6" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D6" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="F6" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="J6" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="L6" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="K6" s="14" t="s">
+      <c r="M6" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="P6" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="L6" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="P6" s="14" t="s">
+      <c r="Q6" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="R6" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="S6" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="T6" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="S6" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="T6" s="14" t="s">
+      <c r="U6" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="V6" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="V6" s="14" t="s">
+      <c r="W6" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="W6" s="14" t="s">
+      <c r="X6" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y6" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA6" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB6" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="AC6" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD6" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="X6" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="Y6" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z6" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="AA6" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB6" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="AC6" s="14" t="s">
+      <c r="AE6" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF6" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="AD6" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="AE6" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="AF6" s="14" t="s">
+      <c r="AG6" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="AG6" s="14" t="s">
+      <c r="AH6" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AH6" s="14" t="s">
+      <c r="AI6" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="AI6" s="14" t="s">
+      <c r="AJ6" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="AJ6" s="14" t="s">
+      <c r="AK6" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="AL6" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="AK6" s="14" t="s">
+      <c r="AM6" s="14" t="s">
         <v>137</v>
-      </c>
-      <c r="AL6" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="AM6" s="14" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.2">
@@ -21420,7 +21438,7 @@
       </c>
       <c r="B116" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C116" s="12">
         <v>110</v>
@@ -21573,11 +21591,11 @@
     <row r="117" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A117" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B117" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C117" s="12">
         <v>111</v>
@@ -21592,139 +21610,139 @@
       </c>
       <c r="F117" cm="1">
         <f t="array" ref="F117">+INDEX(Hoja1!$B$2:$MO$7,1,E117)</f>
-        <v>0</v>
+        <v>125570</v>
       </c>
       <c r="G117">
         <f t="shared" si="41"/>
-        <v>-122668</v>
+        <v>2902</v>
       </c>
       <c r="H117" cm="1">
         <f t="array" ref="H117">+INDEX(Hoja1!$B$2:$MO$7,2,$E117)</f>
-        <v>0</v>
+        <v>91023</v>
       </c>
       <c r="I117">
         <f t="shared" si="42"/>
-        <v>-89143</v>
+        <v>1880</v>
       </c>
       <c r="J117">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>34547</v>
       </c>
       <c r="K117">
         <f t="shared" si="43"/>
-        <v>-33525</v>
+        <v>1022</v>
       </c>
       <c r="L117" cm="1">
         <f t="array" ref="L117">+INDEX(Hoja1!$B$2:$MO$7,3,$E117)</f>
-        <v>0</v>
+        <v>13996</v>
       </c>
       <c r="M117" cm="1">
         <f t="array" ref="M117">+INDEX(Hoja1!$B$2:$MO$7,4,$E117)</f>
-        <v>0</v>
+        <v>764</v>
       </c>
       <c r="N117" cm="1">
         <f t="array" ref="N117">+INDEX(Hoja1!$B$2:$MO$7,5,$E117)</f>
-        <v>0</v>
+        <v>712</v>
       </c>
       <c r="O117" cm="1">
         <f t="array" ref="O117">+INDEX(Hoja1!$B$2:$MO$7,6,$E117)</f>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="P117" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.72487855379469623</v>
       </c>
       <c r="Q117" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.27512144620530382</v>
       </c>
       <c r="R117">
         <f t="shared" si="44"/>
-        <v>-125033</v>
+        <v>537</v>
       </c>
       <c r="S117">
         <f t="shared" si="45"/>
-        <v>-33525</v>
+        <v>1022</v>
       </c>
       <c r="T117">
         <f t="shared" si="46"/>
-        <v>-13116</v>
+        <v>880</v>
       </c>
       <c r="U117">
         <f t="shared" si="47"/>
-        <v>-712</v>
+        <v>52</v>
       </c>
       <c r="V117">
         <f t="shared" si="48"/>
-        <v>-727</v>
+        <v>-15</v>
       </c>
       <c r="W117">
         <f t="shared" si="49"/>
-        <v>-141</v>
+        <v>-1</v>
       </c>
       <c r="X117">
         <f t="shared" si="50"/>
-        <v>-52.868076109936574</v>
+        <v>0.22706131078224101</v>
       </c>
       <c r="Y117">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>3.0484712900820284E-2</v>
       </c>
       <c r="Z117">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0670936261055199</v>
       </c>
       <c r="AA117">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1.0730337078651686</v>
       </c>
       <c r="AB117">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>0.97936726272352137</v>
       </c>
       <c r="AC117">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>0.99290780141843971</v>
       </c>
       <c r="AD117">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>30192.353931233472</v>
       </c>
       <c r="AE117">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>8306.564077903342</v>
       </c>
       <c r="AF117">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>3365.2320269295506</v>
       </c>
       <c r="AG117">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>183.69800432796347</v>
       </c>
       <c r="AH117">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>171.19499879778795</v>
       </c>
       <c r="AI117">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>33.661937965857177</v>
       </c>
       <c r="AJ117">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>15612</v>
       </c>
       <c r="AK117">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>3753.7869680211593</v>
       </c>
       <c r="AL117">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ116</f>
-        <v>-14696</v>
+        <v>916</v>
       </c>
       <c r="AM117">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ116,0)</f>
-        <v>-1</v>
+        <v>6.2329885683179098E-2</v>
       </c>
     </row>
     <row r="118" spans="1:39" x14ac:dyDescent="0.2">
@@ -21753,7 +21771,7 @@
       </c>
       <c r="G118">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-125570</v>
       </c>
       <c r="H118" cm="1">
         <f t="array" ref="H118">+INDEX(Hoja1!$B$2:$MO$7,2,$E118)</f>
@@ -21761,7 +21779,7 @@
       </c>
       <c r="I118">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-91023</v>
       </c>
       <c r="J118">
         <f t="shared" si="33"/>
@@ -21769,7 +21787,7 @@
       </c>
       <c r="K118">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-34547</v>
       </c>
       <c r="L118" cm="1">
         <f t="array" ref="L118">+INDEX(Hoja1!$B$2:$MO$7,3,$E118)</f>
@@ -21797,35 +21815,35 @@
       </c>
       <c r="R118">
         <f t="shared" si="44"/>
-        <v>122668</v>
+        <v>-128472</v>
       </c>
       <c r="S118">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-34547</v>
       </c>
       <c r="T118">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-13996</v>
       </c>
       <c r="U118">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-764</v>
       </c>
       <c r="V118">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-712</v>
       </c>
       <c r="W118">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-140</v>
       </c>
       <c r="X118">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-44.27015851137147</v>
       </c>
       <c r="Y118">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z118">
         <f t="shared" si="52"/>
@@ -21877,11 +21895,11 @@
       </c>
       <c r="AL118">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ117</f>
-        <v>0</v>
+        <v>-15612</v>
       </c>
       <c r="AM118">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ117,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="119" spans="1:39" x14ac:dyDescent="0.2">
@@ -21954,7 +21972,7 @@
       </c>
       <c r="R119">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>125570</v>
       </c>
       <c r="S119">
         <f t="shared" si="45"/>
@@ -21978,7 +21996,7 @@
       </c>
       <c r="X119">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y119">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-30-2020 15-24-37
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1496" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5E0C1671-FC1C-A84E-A1F5-8CF6FFBCD339}"/>
+  <xr:revisionPtr revIDLastSave="1519" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8F9F04A8-AD55-694B-941C-1C245903ABE8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="165">
   <si>
     <t>Columna1</t>
   </si>
@@ -346,15 +346,6 @@
     <t>12-06-2020</t>
   </si>
   <si>
-    <t>28/6/2020</t>
-  </si>
-  <si>
-    <t>29/6/2020</t>
-  </si>
-  <si>
-    <t>30/6/2020</t>
-  </si>
-  <si>
     <t>Pruebas Realizadas</t>
   </si>
   <si>
@@ -519,6 +510,24 @@
   <si>
     <t>28-06-20</t>
   </si>
+  <si>
+    <t>29-06-20</t>
+  </si>
+  <si>
+    <t>30-06-20</t>
+  </si>
+  <si>
+    <t>01-07-20</t>
+  </si>
+  <si>
+    <t>02-07-20</t>
+  </si>
+  <si>
+    <t>03-07-20</t>
+  </si>
+  <si>
+    <t>04-07-20</t>
+  </si>
 </sst>
 </file>
 
@@ -641,7 +650,26 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="33">
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -844,9 +872,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:DK7" totalsRowShown="0">
-  <autoFilter ref="A1:DK7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
-  <tableColumns count="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:DN7" totalsRowShown="0">
+  <autoFilter ref="A1:DN7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
+  <tableColumns count="118">
     <tableColumn id="76" xr3:uid="{CA01250B-8685-4250-AAEF-D6E482663B6F}" name="Columna1"/>
     <tableColumn id="77" xr3:uid="{BC38B0B2-3229-42F8-9C9A-52EE74902839}" name="10-03-2020"/>
     <tableColumn id="78" xr3:uid="{4BB74E2E-62F3-4EED-8537-96C80CD1ED37}" name="11-03-2020"/>
@@ -940,48 +968,51 @@
     <tableColumn id="4" xr3:uid="{2FE879E2-2128-42AE-A0E3-647EE2D0C94F}" name="07-06-2020"/>
     <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="08-06-2020"/>
     <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-2020"/>
-    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="24"/>
-    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="23"/>
-    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="22"/>
-    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="21"/>
-    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="20"/>
-    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="19"/>
-    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="18"/>
-    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="17"/>
-    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="16"/>
-    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="15"/>
-    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="14"/>
-    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="13"/>
-    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="12"/>
-    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="11"/>
-    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="10"/>
-    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="9"/>
-    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="8"/>
-    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="28/6/2020"/>
-    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="29/6/2020"/>
-    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="30/6/2020"/>
+    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="30"/>
+    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="29"/>
+    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="28"/>
+    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="27"/>
+    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="26"/>
+    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="25"/>
+    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="24"/>
+    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="23"/>
+    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="22"/>
+    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="21"/>
+    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="20"/>
+    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="19"/>
+    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="18"/>
+    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="17"/>
+    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="16"/>
+    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="15"/>
+    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="14"/>
+    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="5"/>
+    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="4"/>
+    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="3"/>
+    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="2"/>
+    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="1"/>
+    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="12">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="11">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="9">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="8">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -1014,10 +1045,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="1">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="7">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="6">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1384,11 +1415,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B32E72-8F4B-408A-9B01-FAD2807C0C88}">
-  <dimension ref="A1:DK52"/>
+  <dimension ref="A1:DN52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DF1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DH17" sqref="DH17"/>
+      <pane xSplit="1" topLeftCell="DH1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1399,9 +1430,13 @@
     <col min="102" max="103" width="11.43359375" style="15"/>
     <col min="104" max="104" width="12.9140625" style="15" bestFit="1" customWidth="1"/>
     <col min="105" max="112" width="11.43359375" style="15"/>
+    <col min="113" max="113" width="11.43359375" style="8"/>
+    <col min="114" max="114" width="9.953125" style="8" customWidth="1"/>
+    <col min="115" max="115" width="10.89453125" style="8" customWidth="1"/>
+    <col min="116" max="118" width="11.43359375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1691,66 +1726,75 @@
         <v>95</v>
       </c>
       <c r="CS1" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="CT1" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="CU1" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="CV1" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="CT1" s="8" t="s">
+      <c r="CW1" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="CU1" s="8" t="s">
+      <c r="CX1" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="CV1" s="8" t="s">
+      <c r="CY1" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="CW1" s="8" t="s">
+      <c r="CZ1" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="CX1" s="15" t="s">
+      <c r="DA1" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="CY1" s="16" t="s">
+      <c r="DB1" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="CZ1" s="16" t="s">
+      <c r="DC1" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="DA1" s="16" t="s">
+      <c r="DD1" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="DB1" s="16" t="s">
+      <c r="DE1" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="DC1" s="16" t="s">
+      <c r="DF1" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="DD1" s="16" t="s">
+      <c r="DG1" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="DE1" s="16" t="s">
+      <c r="DH1" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="DF1" s="16" t="s">
+      <c r="DI1" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="DG1" s="16" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="DH1" s="16" t="s">
+      <c r="DK1" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DL1" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="DM1" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="DN1" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:118" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>96</v>
-      </c>
-      <c r="DJ1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:115" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>99</v>
       </c>
       <c r="B2" s="7">
         <v>146</v>
@@ -2085,10 +2129,13 @@
       <c r="DH2" s="15">
         <v>125570</v>
       </c>
+      <c r="DI2" s="8">
+        <v>128795</v>
+      </c>
     </row>
-    <row r="3" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B3" s="7">
         <v>138</v>
@@ -2423,10 +2470,13 @@
       <c r="DH3" s="15">
         <v>91023</v>
       </c>
+      <c r="DI3" s="8">
+        <v>93124</v>
+      </c>
     </row>
-    <row r="4" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B4" s="7">
         <v>6</v>
@@ -2761,10 +2811,13 @@
       <c r="DH4" s="15">
         <v>13996</v>
       </c>
+      <c r="DI4" s="8">
+        <v>14961</v>
+      </c>
     </row>
-    <row r="5" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -3008,10 +3061,13 @@
       <c r="DH5" s="15">
         <v>764</v>
       </c>
+      <c r="DI5" s="8">
+        <v>718</v>
+      </c>
     </row>
-    <row r="6" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -3342,10 +3398,13 @@
       <c r="DH6" s="15">
         <v>712</v>
       </c>
+      <c r="DI6" s="8">
+        <v>744</v>
+      </c>
     </row>
-    <row r="7" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -3678,8 +3737,11 @@
       <c r="DH7" s="15">
         <v>140</v>
       </c>
+      <c r="DI7" s="8">
+        <v>147</v>
+      </c>
     </row>
-    <row r="8" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -3773,28 +3835,28 @@
       <c r="CN8" s="8"/>
       <c r="CO8" s="8"/>
     </row>
-    <row r="9" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:118" x14ac:dyDescent="0.2">
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:118" x14ac:dyDescent="0.2">
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:118" x14ac:dyDescent="0.2">
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:118" x14ac:dyDescent="0.2">
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:118" x14ac:dyDescent="0.2">
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:118" x14ac:dyDescent="0.2">
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:118" x14ac:dyDescent="0.2">
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:118" x14ac:dyDescent="0.2">
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
@@ -4261,7 +4323,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -4270,121 +4332,121 @@
     </row>
     <row r="6" spans="1:39" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="F6" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="H6" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="J6" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="K6" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="M6" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="H6" s="14" t="s">
+      <c r="N6" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="O6" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="P6" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="Q6" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="R6" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="S6" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="L6" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="P6" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q6" s="14" t="s">
+      <c r="T6" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="U6" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="V6" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="S6" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="T6" s="14" t="s">
+      <c r="W6" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="X6" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y6" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA6" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB6" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC6" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD6" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="V6" s="14" t="s">
+      <c r="AE6" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="W6" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="X6" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="Y6" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z6" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA6" s="14" t="s">
+      <c r="AF6" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="AB6" s="14" t="s">
+      <c r="AG6" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="AC6" s="14" t="s">
+      <c r="AH6" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="AD6" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="AE6" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="AF6" s="14" t="s">
+      <c r="AI6" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="AG6" s="14" t="s">
+      <c r="AJ6" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="AH6" s="14" t="s">
+      <c r="AK6" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="AL6" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="AI6" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="AJ6" s="14" t="s">
+      <c r="AM6" s="14" t="s">
         <v>134</v>
-      </c>
-      <c r="AK6" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="AL6" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="AM6" s="14" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.2">
@@ -21595,7 +21657,7 @@
       </c>
       <c r="B117" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C117" s="12">
         <v>111</v>
@@ -21748,11 +21810,11 @@
     <row r="118" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A118" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B118" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C118" s="12">
         <v>112</v>
@@ -21767,139 +21829,139 @@
       </c>
       <c r="F118" cm="1">
         <f t="array" ref="F118">+INDEX(Hoja1!$B$2:$MO$7,1,E118)</f>
-        <v>0</v>
+        <v>128795</v>
       </c>
       <c r="G118">
         <f t="shared" si="41"/>
-        <v>-125570</v>
+        <v>3225</v>
       </c>
       <c r="H118" cm="1">
         <f t="array" ref="H118">+INDEX(Hoja1!$B$2:$MO$7,2,$E118)</f>
-        <v>0</v>
+        <v>93124</v>
       </c>
       <c r="I118">
         <f t="shared" si="42"/>
-        <v>-91023</v>
+        <v>2101</v>
       </c>
       <c r="J118">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>35671</v>
       </c>
       <c r="K118">
         <f t="shared" si="43"/>
-        <v>-34547</v>
+        <v>1124</v>
       </c>
       <c r="L118" cm="1">
         <f t="array" ref="L118">+INDEX(Hoja1!$B$2:$MO$7,3,$E118)</f>
-        <v>0</v>
+        <v>14961</v>
       </c>
       <c r="M118" cm="1">
         <f t="array" ref="M118">+INDEX(Hoja1!$B$2:$MO$7,4,$E118)</f>
-        <v>0</v>
+        <v>718</v>
       </c>
       <c r="N118" cm="1">
         <f t="array" ref="N118">+INDEX(Hoja1!$B$2:$MO$7,5,$E118)</f>
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="O118" cm="1">
         <f t="array" ref="O118">+INDEX(Hoja1!$B$2:$MO$7,6,$E118)</f>
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="P118" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.72304049070227883</v>
       </c>
       <c r="Q118" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.27695950929772117</v>
       </c>
       <c r="R118">
         <f t="shared" si="44"/>
-        <v>-128472</v>
+        <v>323</v>
       </c>
       <c r="S118">
         <f t="shared" si="45"/>
-        <v>-34547</v>
+        <v>1124</v>
       </c>
       <c r="T118">
         <f t="shared" si="46"/>
-        <v>-13996</v>
+        <v>965</v>
       </c>
       <c r="U118">
         <f t="shared" si="47"/>
-        <v>-764</v>
+        <v>-46</v>
       </c>
       <c r="V118">
         <f t="shared" si="48"/>
-        <v>-712</v>
+        <v>32</v>
       </c>
       <c r="W118">
         <f t="shared" si="49"/>
-        <v>-140</v>
+        <v>7</v>
       </c>
       <c r="X118">
         <f t="shared" si="50"/>
-        <v>-44.27015851137147</v>
+        <v>0.11130254996554101</v>
       </c>
       <c r="Y118">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>3.2535386574811129E-2</v>
       </c>
       <c r="Z118">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0689482709345528</v>
       </c>
       <c r="AA118">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>0.93979057591623039</v>
       </c>
       <c r="AB118">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0449438202247192</v>
       </c>
       <c r="AC118">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="AD118">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>30967.780716518395</v>
       </c>
       <c r="AE118">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>8576.8213512863676</v>
       </c>
       <c r="AF118">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>3597.2589564799232</v>
       </c>
       <c r="AG118">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>172.63765328203897</v>
       </c>
       <c r="AH118">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>178.88915604712673</v>
       </c>
       <c r="AI118">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>35.345034864150037</v>
       </c>
       <c r="AJ118">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>16570</v>
       </c>
       <c r="AK118">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>3984.1308006732388</v>
       </c>
       <c r="AL118">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ117</f>
-        <v>-15612</v>
+        <v>958</v>
       </c>
       <c r="AM118">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ117,0)</f>
-        <v>-1</v>
+        <v>6.1363054060978736E-2</v>
       </c>
     </row>
     <row r="119" spans="1:39" x14ac:dyDescent="0.2">
@@ -21928,7 +21990,7 @@
       </c>
       <c r="G119">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-128795</v>
       </c>
       <c r="H119" cm="1">
         <f t="array" ref="H119">+INDEX(Hoja1!$B$2:$MO$7,2,$E119)</f>
@@ -21936,7 +21998,7 @@
       </c>
       <c r="I119">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-93124</v>
       </c>
       <c r="J119">
         <f t="shared" si="33"/>
@@ -21944,7 +22006,7 @@
       </c>
       <c r="K119">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-35671</v>
       </c>
       <c r="L119" cm="1">
         <f t="array" ref="L119">+INDEX(Hoja1!$B$2:$MO$7,3,$E119)</f>
@@ -21972,35 +22034,35 @@
       </c>
       <c r="R119">
         <f t="shared" si="44"/>
-        <v>125570</v>
+        <v>-132020</v>
       </c>
       <c r="S119">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-35671</v>
       </c>
       <c r="T119">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-14961</v>
       </c>
       <c r="U119">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-718</v>
       </c>
       <c r="V119">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-744</v>
       </c>
       <c r="W119">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-147</v>
       </c>
       <c r="X119">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-40.936434108527131</v>
       </c>
       <c r="Y119">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z119">
         <f t="shared" si="52"/>
@@ -22052,11 +22114,11 @@
       </c>
       <c r="AL119">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ118</f>
-        <v>0</v>
+        <v>-16570</v>
       </c>
       <c r="AM119">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ118,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="120" spans="1:39" x14ac:dyDescent="0.2">
@@ -22129,7 +22191,7 @@
       </c>
       <c r="R120">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>128795</v>
       </c>
       <c r="S120">
         <f t="shared" si="45"/>
@@ -22153,7 +22215,7 @@
       </c>
       <c r="X120">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y120">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-01-2020 15-27-05
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1519" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8F9F04A8-AD55-694B-941C-1C245903ABE8}"/>
+  <xr:revisionPtr revIDLastSave="1527" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{481285EB-0637-1447-85E6-5001AAC49BD8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="157">
   <si>
     <t>Columna1</t>
   </si>
@@ -652,25 +652,6 @@
   </cellStyles>
   <dxfs count="33">
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -789,6 +770,25 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
@@ -987,32 +987,32 @@
     <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="16"/>
     <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="15"/>
     <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="14"/>
-    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="5"/>
-    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="4"/>
-    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="3"/>
-    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="2"/>
-    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="1"/>
-    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="0"/>
+    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="13"/>
+    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="12"/>
+    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="11"/>
+    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="10"/>
+    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="9"/>
+    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="6">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="11">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="5">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="9">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="3">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="8">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="2">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -1045,10 +1045,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="7">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="1">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="6">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="0">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1419,7 +1419,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="DH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A26" sqref="A26"/>
+      <selection pane="topRight" activeCell="DJ8" sqref="DJ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2132,6 +2132,9 @@
       <c r="DI2" s="8">
         <v>128795</v>
       </c>
+      <c r="DJ2" s="8">
+        <v>130776</v>
+      </c>
     </row>
     <row r="3" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2473,6 +2476,9 @@
       <c r="DI3" s="8">
         <v>93124</v>
       </c>
+      <c r="DJ3" s="8">
+        <v>94336</v>
+      </c>
     </row>
     <row r="4" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2813,6 +2819,9 @@
       </c>
       <c r="DI4" s="8">
         <v>14961</v>
+      </c>
+      <c r="DJ4" s="8">
+        <v>15590</v>
       </c>
     </row>
     <row r="5" spans="1:118" x14ac:dyDescent="0.2">
@@ -3064,6 +3073,9 @@
       <c r="DI5" s="8">
         <v>718</v>
       </c>
+      <c r="DJ5" s="8">
+        <v>664</v>
+      </c>
     </row>
     <row r="6" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3401,6 +3413,9 @@
       <c r="DI6" s="8">
         <v>744</v>
       </c>
+      <c r="DJ6" s="8">
+        <v>774</v>
+      </c>
     </row>
     <row r="7" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -3739,6 +3754,9 @@
       </c>
       <c r="DI7" s="8">
         <v>147</v>
+      </c>
+      <c r="DJ7" s="8">
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:118" x14ac:dyDescent="0.2">
@@ -4323,7 +4341,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44011</v>
+        <v>44012</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -21814,7 +21832,7 @@
       </c>
       <c r="B118" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C118" s="12">
         <v>112</v>
@@ -21967,11 +21985,11 @@
     <row r="119" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A119" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B119" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C119" s="12">
         <v>113</v>
@@ -21986,139 +22004,139 @@
       </c>
       <c r="F119" cm="1">
         <f t="array" ref="F119">+INDEX(Hoja1!$B$2:$MO$7,1,E119)</f>
-        <v>0</v>
+        <v>130776</v>
       </c>
       <c r="G119">
         <f t="shared" si="41"/>
-        <v>-128795</v>
+        <v>1981</v>
       </c>
       <c r="H119" cm="1">
         <f t="array" ref="H119">+INDEX(Hoja1!$B$2:$MO$7,2,$E119)</f>
-        <v>0</v>
+        <v>94336</v>
       </c>
       <c r="I119">
         <f t="shared" si="42"/>
-        <v>-93124</v>
+        <v>1212</v>
       </c>
       <c r="J119">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>36440</v>
       </c>
       <c r="K119">
         <f t="shared" si="43"/>
-        <v>-35671</v>
+        <v>769</v>
       </c>
       <c r="L119" cm="1">
         <f t="array" ref="L119">+INDEX(Hoja1!$B$2:$MO$7,3,$E119)</f>
-        <v>0</v>
+        <v>15590</v>
       </c>
       <c r="M119" cm="1">
         <f t="array" ref="M119">+INDEX(Hoja1!$B$2:$MO$7,4,$E119)</f>
-        <v>0</v>
+        <v>664</v>
       </c>
       <c r="N119" cm="1">
         <f t="array" ref="N119">+INDEX(Hoja1!$B$2:$MO$7,5,$E119)</f>
-        <v>0</v>
+        <v>774</v>
       </c>
       <c r="O119" cm="1">
         <f t="array" ref="O119">+INDEX(Hoja1!$B$2:$MO$7,6,$E119)</f>
-        <v>0</v>
+        <v>146</v>
       </c>
       <c r="P119" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.72135560041597846</v>
       </c>
       <c r="Q119" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.27864439958402154</v>
       </c>
       <c r="R119">
         <f t="shared" si="44"/>
-        <v>-132020</v>
+        <v>-1244</v>
       </c>
       <c r="S119">
         <f t="shared" si="45"/>
-        <v>-35671</v>
+        <v>769</v>
       </c>
       <c r="T119">
         <f t="shared" si="46"/>
-        <v>-14961</v>
+        <v>629</v>
       </c>
       <c r="U119">
         <f t="shared" si="47"/>
-        <v>-718</v>
+        <v>-54</v>
       </c>
       <c r="V119">
         <f t="shared" si="48"/>
-        <v>-744</v>
+        <v>30</v>
       </c>
       <c r="W119">
         <f t="shared" si="49"/>
-        <v>-147</v>
+        <v>-1</v>
       </c>
       <c r="X119">
         <f t="shared" si="50"/>
-        <v>-40.936434108527131</v>
+        <v>-0.38573643410852715</v>
       </c>
       <c r="Y119">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.155812845168344E-2</v>
       </c>
       <c r="Z119">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0420426442082749</v>
       </c>
       <c r="AA119">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>0.92479108635097496</v>
       </c>
       <c r="AB119">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0403225806451613</v>
       </c>
       <c r="AC119">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>0.99319727891156462</v>
       </c>
       <c r="AD119">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>31444.097138735273</v>
       </c>
       <c r="AE119">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>8761.7215676845408</v>
       </c>
       <c r="AF119">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>3748.4972349122386</v>
       </c>
       <c r="AG119">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>159.65376292377977</v>
       </c>
       <c r="AH119">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>186.10242846838185</v>
       </c>
       <c r="AI119">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>35.1045924501082</v>
       </c>
       <c r="AJ119">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>17174</v>
       </c>
       <c r="AK119">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>4129.3580187545085</v>
       </c>
       <c r="AL119">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ118</f>
-        <v>-16570</v>
+        <v>604</v>
       </c>
       <c r="AM119">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ118,0)</f>
-        <v>-1</v>
+        <v>3.645141822570911E-2</v>
       </c>
     </row>
     <row r="120" spans="1:39" x14ac:dyDescent="0.2">
@@ -22147,7 +22165,7 @@
       </c>
       <c r="G120">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-130776</v>
       </c>
       <c r="H120" cm="1">
         <f t="array" ref="H120">+INDEX(Hoja1!$B$2:$MO$7,2,$E120)</f>
@@ -22155,7 +22173,7 @@
       </c>
       <c r="I120">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-94336</v>
       </c>
       <c r="J120">
         <f t="shared" si="33"/>
@@ -22163,7 +22181,7 @@
       </c>
       <c r="K120">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-36440</v>
       </c>
       <c r="L120" cm="1">
         <f t="array" ref="L120">+INDEX(Hoja1!$B$2:$MO$7,3,$E120)</f>
@@ -22191,35 +22209,35 @@
       </c>
       <c r="R120">
         <f t="shared" si="44"/>
-        <v>128795</v>
+        <v>-132757</v>
       </c>
       <c r="S120">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-36440</v>
       </c>
       <c r="T120">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-15590</v>
       </c>
       <c r="U120">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-664</v>
       </c>
       <c r="V120">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-774</v>
       </c>
       <c r="W120">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-146</v>
       </c>
       <c r="X120">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-67.015143866733979</v>
       </c>
       <c r="Y120">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z120">
         <f t="shared" si="52"/>
@@ -22271,11 +22289,11 @@
       </c>
       <c r="AL120">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ119</f>
-        <v>0</v>
+        <v>-17174</v>
       </c>
       <c r="AM120">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ119,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="121" spans="1:39" x14ac:dyDescent="0.2">
@@ -22348,7 +22366,7 @@
       </c>
       <c r="R121">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>130776</v>
       </c>
       <c r="S121">
         <f t="shared" si="45"/>
@@ -22372,7 +22390,7 @@
       </c>
       <c r="X121">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y121">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-02-2020 03-28-24
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1527" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{481285EB-0637-1447-85E6-5001AAC49BD8}"/>
+  <xr:revisionPtr revIDLastSave="1528" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{091CD34D-DA7C-2845-A854-4CA57BEE7C91}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -1418,8 +1418,8 @@
   <dimension ref="A1:DN52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DJ8" sqref="DJ8"/>
+      <pane xSplit="1" topLeftCell="DI1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DK3" sqref="DK3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2134,6 +2134,9 @@
       </c>
       <c r="DJ2" s="8">
         <v>130776</v>
+      </c>
+      <c r="DK2" s="8">
+        <v>133449</v>
       </c>
     </row>
     <row r="3" spans="1:118" x14ac:dyDescent="0.2">
@@ -4341,7 +4344,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44012</v>
+        <v>44013</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -21989,7 +21992,7 @@
       </c>
       <c r="B119" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C119" s="12">
         <v>113</v>
@@ -22142,11 +22145,11 @@
     <row r="120" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A120" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B120" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C120" s="12">
         <v>114</v>
@@ -22161,11 +22164,11 @@
       </c>
       <c r="F120" cm="1">
         <f t="array" ref="F120">+INDEX(Hoja1!$B$2:$MO$7,1,E120)</f>
-        <v>0</v>
+        <v>133449</v>
       </c>
       <c r="G120">
         <f t="shared" si="41"/>
-        <v>-130776</v>
+        <v>2673</v>
       </c>
       <c r="H120" cm="1">
         <f t="array" ref="H120">+INDEX(Hoja1!$B$2:$MO$7,2,$E120)</f>
@@ -22177,11 +22180,11 @@
       </c>
       <c r="J120">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>133449</v>
       </c>
       <c r="K120">
         <f t="shared" si="43"/>
-        <v>-36440</v>
+        <v>97009</v>
       </c>
       <c r="L120" cm="1">
         <f t="array" ref="L120">+INDEX(Hoja1!$B$2:$MO$7,3,$E120)</f>
@@ -22205,15 +22208,15 @@
       </c>
       <c r="Q120" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R120">
         <f t="shared" si="44"/>
-        <v>-132757</v>
+        <v>692</v>
       </c>
       <c r="S120">
         <f t="shared" si="45"/>
-        <v>-36440</v>
+        <v>97009</v>
       </c>
       <c r="T120">
         <f t="shared" si="46"/>
@@ -22233,11 +22236,11 @@
       </c>
       <c r="X120">
         <f t="shared" si="50"/>
-        <v>-67.015143866733979</v>
+        <v>0.34931852599697122</v>
       </c>
       <c r="Y120">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.6621569703622394</v>
       </c>
       <c r="Z120">
         <f t="shared" si="52"/>
@@ -22257,11 +22260,11 @@
       </c>
       <c r="AD120">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>32086.799711469106</v>
       </c>
       <c r="AE120">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>32086.799711469106</v>
       </c>
       <c r="AF120">
         <f t="shared" si="36"/>
@@ -22322,7 +22325,7 @@
       </c>
       <c r="G121">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-133449</v>
       </c>
       <c r="H121" cm="1">
         <f t="array" ref="H121">+INDEX(Hoja1!$B$2:$MO$7,2,$E121)</f>
@@ -22338,7 +22341,7 @@
       </c>
       <c r="K121">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-133449</v>
       </c>
       <c r="L121" cm="1">
         <f t="array" ref="L121">+INDEX(Hoja1!$B$2:$MO$7,3,$E121)</f>
@@ -22366,11 +22369,11 @@
       </c>
       <c r="R121">
         <f t="shared" si="44"/>
-        <v>130776</v>
+        <v>-136122</v>
       </c>
       <c r="S121">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-133449</v>
       </c>
       <c r="T121">
         <f t="shared" si="46"/>
@@ -22390,11 +22393,11 @@
       </c>
       <c r="X121">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-50.924803591470258</v>
       </c>
       <c r="Y121">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z121">
         <f t="shared" si="52"/>
@@ -22523,7 +22526,7 @@
       </c>
       <c r="R122">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>133449</v>
       </c>
       <c r="S122">
         <f t="shared" si="45"/>
@@ -22547,7 +22550,7 @@
       </c>
       <c r="X122">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y122">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-04-2020 05-38-40
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1540" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C1CBDD8A-1817-1549-A9D3-2ABF290FFB1A}"/>
+  <xr:revisionPtr revIDLastSave="1546" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{49705E11-8439-204A-A769-058CDEA82278}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -1418,8 +1418,8 @@
   <dimension ref="A1:DN52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DL8" sqref="DL8"/>
+      <pane xSplit="1" topLeftCell="DJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DM8" sqref="DM8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2141,6 +2141,9 @@
       <c r="DL2" s="8">
         <v>135801</v>
       </c>
+      <c r="DM2" s="8">
+        <v>138081</v>
+      </c>
     </row>
     <row r="3" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2491,6 +2494,9 @@
       <c r="DL3" s="8">
         <v>97666</v>
       </c>
+      <c r="DM3" s="8">
+        <v>99169</v>
+      </c>
     </row>
     <row r="4" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2840,6 +2846,9 @@
       </c>
       <c r="DL4" s="8">
         <v>16508</v>
+      </c>
+      <c r="DM4" s="8">
+        <v>16678</v>
       </c>
     </row>
     <row r="5" spans="1:118" x14ac:dyDescent="0.2">
@@ -3100,6 +3109,9 @@
       <c r="DL5" s="8">
         <v>673</v>
       </c>
+      <c r="DM5" s="8">
+        <v>705</v>
+      </c>
     </row>
     <row r="6" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3446,6 +3458,9 @@
       <c r="DL6" s="8">
         <v>795</v>
       </c>
+      <c r="DM6" s="8">
+        <v>823</v>
+      </c>
     </row>
     <row r="7" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -3793,6 +3808,9 @@
       </c>
       <c r="DL7" s="8">
         <v>149</v>
+      </c>
+      <c r="DM7" s="8">
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:118" x14ac:dyDescent="0.2">
@@ -4377,7 +4395,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -22339,7 +22357,7 @@
       </c>
       <c r="B121" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C121" s="12">
         <v>115</v>
@@ -22492,11 +22510,11 @@
     <row r="122" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A122" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B122" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C122" s="12">
         <v>116</v>
@@ -22511,139 +22529,139 @@
       </c>
       <c r="F122" cm="1">
         <f t="array" ref="F122">+INDEX(Hoja1!$B$2:$MO$7,1,E122)</f>
-        <v>0</v>
+        <v>138081</v>
       </c>
       <c r="G122">
         <f t="shared" si="41"/>
-        <v>-135801</v>
+        <v>2280</v>
       </c>
       <c r="H122" cm="1">
         <f t="array" ref="H122">+INDEX(Hoja1!$B$2:$MO$7,2,$E122)</f>
-        <v>0</v>
+        <v>99169</v>
       </c>
       <c r="I122">
         <f t="shared" si="42"/>
-        <v>-97666</v>
+        <v>1503</v>
       </c>
       <c r="J122">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>38912</v>
       </c>
       <c r="K122">
         <f t="shared" si="43"/>
-        <v>-38135</v>
+        <v>777</v>
       </c>
       <c r="L122" cm="1">
         <f t="array" ref="L122">+INDEX(Hoja1!$B$2:$MO$7,3,$E122)</f>
-        <v>0</v>
+        <v>16678</v>
       </c>
       <c r="M122" cm="1">
         <f t="array" ref="M122">+INDEX(Hoja1!$B$2:$MO$7,4,$E122)</f>
-        <v>0</v>
+        <v>705</v>
       </c>
       <c r="N122" cm="1">
         <f t="array" ref="N122">+INDEX(Hoja1!$B$2:$MO$7,5,$E122)</f>
-        <v>0</v>
+        <v>823</v>
       </c>
       <c r="O122" cm="1">
         <f t="array" ref="O122">+INDEX(Hoja1!$B$2:$MO$7,6,$E122)</f>
-        <v>0</v>
+        <v>146</v>
       </c>
       <c r="P122" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.71819439314605193</v>
       </c>
       <c r="Q122" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.28180560685394807</v>
       </c>
       <c r="R122">
         <f t="shared" si="44"/>
-        <v>-138153</v>
+        <v>-72</v>
       </c>
       <c r="S122">
         <f t="shared" si="45"/>
-        <v>-38135</v>
+        <v>777</v>
       </c>
       <c r="T122">
         <f t="shared" si="46"/>
-        <v>-16508</v>
+        <v>170</v>
       </c>
       <c r="U122">
         <f t="shared" si="47"/>
-        <v>-673</v>
+        <v>32</v>
       </c>
       <c r="V122">
         <f t="shared" si="48"/>
-        <v>-795</v>
+        <v>28</v>
       </c>
       <c r="W122">
         <f t="shared" si="49"/>
-        <v>-149</v>
+        <v>-3</v>
       </c>
       <c r="X122">
         <f t="shared" si="50"/>
-        <v>-58.738520408163268</v>
+        <v>-3.0612244897959183E-2</v>
       </c>
       <c r="Y122">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.037498361085617E-2</v>
       </c>
       <c r="Z122">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.010298037315241</v>
       </c>
       <c r="AA122">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1.0475482912332839</v>
       </c>
       <c r="AB122">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0352201257861635</v>
       </c>
       <c r="AC122">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>0.97986577181208057</v>
       </c>
       <c r="AD122">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>33200.528973310895</v>
       </c>
       <c r="AE122">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>9356.0952151959609</v>
       </c>
       <c r="AF122">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>4010.0985813897573</v>
       </c>
       <c r="AG122">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>169.51190189949509</v>
       </c>
       <c r="AH122">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>197.88410675643183</v>
       </c>
       <c r="AI122">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>35.1045924501082</v>
       </c>
       <c r="AJ122">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>18352</v>
       </c>
       <c r="AK122">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>4412.5991824957928</v>
       </c>
       <c r="AL122">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ121</f>
-        <v>-18125</v>
+        <v>227</v>
       </c>
       <c r="AM122">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ121,0)</f>
-        <v>-1</v>
+        <v>1.2524137931034483E-2</v>
       </c>
     </row>
     <row r="123" spans="1:39" x14ac:dyDescent="0.2">
@@ -22672,7 +22690,7 @@
       </c>
       <c r="G123">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-138081</v>
       </c>
       <c r="H123" cm="1">
         <f t="array" ref="H123">+INDEX(Hoja1!$B$2:$MO$7,2,$E123)</f>
@@ -22680,7 +22698,7 @@
       </c>
       <c r="I123">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-99169</v>
       </c>
       <c r="J123">
         <f t="shared" si="33"/>
@@ -22688,7 +22706,7 @@
       </c>
       <c r="K123">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-38912</v>
       </c>
       <c r="L123" cm="1">
         <f t="array" ref="L123">+INDEX(Hoja1!$B$2:$MO$7,3,$E123)</f>
@@ -22716,35 +22734,35 @@
       </c>
       <c r="R123">
         <f t="shared" si="44"/>
-        <v>135801</v>
+        <v>-140361</v>
       </c>
       <c r="S123">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-38912</v>
       </c>
       <c r="T123">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-16678</v>
       </c>
       <c r="U123">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-705</v>
       </c>
       <c r="V123">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-823</v>
       </c>
       <c r="W123">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-146</v>
       </c>
       <c r="X123">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-61.56184210526316</v>
       </c>
       <c r="Y123">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z123">
         <f t="shared" si="52"/>
@@ -22796,11 +22814,11 @@
       </c>
       <c r="AL123">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ122</f>
-        <v>0</v>
+        <v>-18352</v>
       </c>
       <c r="AM123">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ122,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="124" spans="1:39" x14ac:dyDescent="0.2">
@@ -22873,7 +22891,7 @@
       </c>
       <c r="R124">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>138081</v>
       </c>
       <c r="S124">
         <f t="shared" si="45"/>
@@ -22897,7 +22915,7 @@
       </c>
       <c r="X124">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y124">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-06-2020 13-46-37
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1546" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{49705E11-8439-204A-A769-058CDEA82278}"/>
+  <xr:revisionPtr revIDLastSave="1553" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C7408779-0627-1F44-8E36-DAFDB5114E74}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -1418,8 +1418,8 @@
   <dimension ref="A1:DN52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DJ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DM8" sqref="DM8"/>
+      <pane xSplit="1" topLeftCell="DL1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DN8" sqref="DN8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2144,6 +2144,9 @@
       <c r="DM2" s="8">
         <v>138081</v>
       </c>
+      <c r="DN2" s="8">
+        <v>144918</v>
+      </c>
     </row>
     <row r="3" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2497,6 +2500,9 @@
       <c r="DM3" s="8">
         <v>99169</v>
       </c>
+      <c r="DN3" s="8">
+        <v>103818</v>
+      </c>
     </row>
     <row r="4" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2849,6 +2855,9 @@
       </c>
       <c r="DM4" s="8">
         <v>16678</v>
+      </c>
+      <c r="DN4" s="8">
+        <v>17759</v>
       </c>
     </row>
     <row r="5" spans="1:118" x14ac:dyDescent="0.2">
@@ -3112,6 +3121,9 @@
       <c r="DM5" s="8">
         <v>705</v>
       </c>
+      <c r="DN5" s="8">
+        <v>661</v>
+      </c>
     </row>
     <row r="6" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3461,6 +3473,9 @@
       <c r="DM6" s="8">
         <v>823</v>
       </c>
+      <c r="DN6" s="8">
+        <v>843</v>
+      </c>
     </row>
     <row r="7" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -3811,6 +3826,9 @@
       </c>
       <c r="DM7" s="8">
         <v>146</v>
+      </c>
+      <c r="DN7" s="8">
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:118" x14ac:dyDescent="0.2">
@@ -4395,7 +4413,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -22514,7 +22532,7 @@
       </c>
       <c r="B122" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C122" s="12">
         <v>116</v>
@@ -22667,11 +22685,11 @@
     <row r="123" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A123" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B123" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C123" s="12">
         <v>117</v>
@@ -22686,139 +22704,139 @@
       </c>
       <c r="F123" cm="1">
         <f t="array" ref="F123">+INDEX(Hoja1!$B$2:$MO$7,1,E123)</f>
-        <v>0</v>
+        <v>144918</v>
       </c>
       <c r="G123">
         <f t="shared" si="41"/>
-        <v>-138081</v>
+        <v>6837</v>
       </c>
       <c r="H123" cm="1">
         <f t="array" ref="H123">+INDEX(Hoja1!$B$2:$MO$7,2,$E123)</f>
-        <v>0</v>
+        <v>103818</v>
       </c>
       <c r="I123">
         <f t="shared" si="42"/>
-        <v>-99169</v>
+        <v>4649</v>
       </c>
       <c r="J123">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>41100</v>
       </c>
       <c r="K123">
         <f t="shared" si="43"/>
-        <v>-38912</v>
+        <v>2188</v>
       </c>
       <c r="L123" cm="1">
         <f t="array" ref="L123">+INDEX(Hoja1!$B$2:$MO$7,3,$E123)</f>
-        <v>0</v>
+        <v>17759</v>
       </c>
       <c r="M123" cm="1">
         <f t="array" ref="M123">+INDEX(Hoja1!$B$2:$MO$7,4,$E123)</f>
-        <v>0</v>
+        <v>661</v>
       </c>
       <c r="N123" cm="1">
         <f t="array" ref="N123">+INDEX(Hoja1!$B$2:$MO$7,5,$E123)</f>
-        <v>0</v>
+        <v>843</v>
       </c>
       <c r="O123" cm="1">
         <f t="array" ref="O123">+INDEX(Hoja1!$B$2:$MO$7,6,$E123)</f>
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="P123" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.71639133855007664</v>
       </c>
       <c r="Q123" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.28360866144992342</v>
       </c>
       <c r="R123">
         <f t="shared" si="44"/>
-        <v>-140361</v>
+        <v>4557</v>
       </c>
       <c r="S123">
         <f t="shared" si="45"/>
-        <v>-38912</v>
+        <v>2188</v>
       </c>
       <c r="T123">
         <f t="shared" si="46"/>
-        <v>-16678</v>
+        <v>1081</v>
       </c>
       <c r="U123">
         <f t="shared" si="47"/>
-        <v>-705</v>
+        <v>-44</v>
       </c>
       <c r="V123">
         <f t="shared" si="48"/>
-        <v>-823</v>
+        <v>20</v>
       </c>
       <c r="W123">
         <f t="shared" si="49"/>
-        <v>-146</v>
+        <v>7</v>
       </c>
       <c r="X123">
         <f t="shared" si="50"/>
-        <v>-61.56184210526316</v>
+        <v>1.9986842105263158</v>
       </c>
       <c r="Y123">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>5.6229440789473686E-2</v>
       </c>
       <c r="Z123">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0648159251708837</v>
       </c>
       <c r="AA123">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>0.93758865248226952</v>
       </c>
       <c r="AB123">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0243013365735116</v>
       </c>
       <c r="AC123">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.047945205479452</v>
       </c>
       <c r="AD123">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>34844.43375811493</v>
       </c>
       <c r="AE123">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>9882.1832171195001</v>
       </c>
       <c r="AF123">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>4270.0168309689834</v>
       </c>
       <c r="AG123">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>158.93243568165425</v>
       </c>
       <c r="AH123">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>202.69295503726858</v>
       </c>
       <c r="AI123">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>36.787689348401059</v>
       </c>
       <c r="AJ123">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>19416</v>
       </c>
       <c r="AK123">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>4668.4299110363072</v>
       </c>
       <c r="AL123">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ122</f>
-        <v>-18352</v>
+        <v>1064</v>
       </c>
       <c r="AM123">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ122,0)</f>
-        <v>-1</v>
+        <v>5.7977332170880559E-2</v>
       </c>
     </row>
     <row r="124" spans="1:39" x14ac:dyDescent="0.2">
@@ -22847,7 +22865,7 @@
       </c>
       <c r="G124">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-144918</v>
       </c>
       <c r="H124" cm="1">
         <f t="array" ref="H124">+INDEX(Hoja1!$B$2:$MO$7,2,$E124)</f>
@@ -22855,7 +22873,7 @@
       </c>
       <c r="I124">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-103818</v>
       </c>
       <c r="J124">
         <f t="shared" si="33"/>
@@ -22863,7 +22881,7 @@
       </c>
       <c r="K124">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-41100</v>
       </c>
       <c r="L124" cm="1">
         <f t="array" ref="L124">+INDEX(Hoja1!$B$2:$MO$7,3,$E124)</f>
@@ -22891,35 +22909,35 @@
       </c>
       <c r="R124">
         <f t="shared" si="44"/>
-        <v>138081</v>
+        <v>-151755</v>
       </c>
       <c r="S124">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-41100</v>
       </c>
       <c r="T124">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-17759</v>
       </c>
       <c r="U124">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-661</v>
       </c>
       <c r="V124">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-843</v>
       </c>
       <c r="W124">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-153</v>
       </c>
       <c r="X124">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-22.196138657305834</v>
       </c>
       <c r="Y124">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z124">
         <f t="shared" si="52"/>
@@ -22971,11 +22989,11 @@
       </c>
       <c r="AL124">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ123</f>
-        <v>0</v>
+        <v>-19416</v>
       </c>
       <c r="AM124">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ123,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="125" spans="1:39" x14ac:dyDescent="0.2">
@@ -23048,7 +23066,7 @@
       </c>
       <c r="R125">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>144918</v>
       </c>
       <c r="S125">
         <f t="shared" si="45"/>
@@ -23072,7 +23090,7 @@
       </c>
       <c r="X125">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y125">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-07-2020 17-50-37
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1553" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C7408779-0627-1F44-8E36-DAFDB5114E74}"/>
+  <xr:revisionPtr revIDLastSave="1575" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C3FED109-B87C-6047-A1B4-C87D4EA0F878}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="164">
   <si>
     <t>Columna1</t>
   </si>
@@ -528,6 +528,18 @@
   <si>
     <t>04-07-20</t>
   </si>
+  <si>
+    <t>04-07-24</t>
+  </si>
+  <si>
+    <t>05-07-20</t>
+  </si>
+  <si>
+    <t>06-07-20</t>
+  </si>
+  <si>
+    <t>07-06-20</t>
+  </si>
 </sst>
 </file>
 
@@ -650,7 +662,19 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="37">
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -872,9 +896,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:DN7" totalsRowShown="0">
-  <autoFilter ref="A1:DN7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
-  <tableColumns count="118">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:DR7" totalsRowShown="0">
+  <autoFilter ref="A1:DR7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
+  <tableColumns count="122">
     <tableColumn id="76" xr3:uid="{CA01250B-8685-4250-AAEF-D6E482663B6F}" name="Columna1"/>
     <tableColumn id="77" xr3:uid="{BC38B0B2-3229-42F8-9C9A-52EE74902839}" name="10-03-2020"/>
     <tableColumn id="78" xr3:uid="{4BB74E2E-62F3-4EED-8537-96C80CD1ED37}" name="11-03-2020"/>
@@ -968,51 +992,55 @@
     <tableColumn id="4" xr3:uid="{2FE879E2-2128-42AE-A0E3-647EE2D0C94F}" name="07-06-2020"/>
     <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="08-06-2020"/>
     <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-2020"/>
-    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="30"/>
-    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="29"/>
-    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="28"/>
-    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="27"/>
-    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="26"/>
-    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="25"/>
-    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="24"/>
-    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="23"/>
-    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="22"/>
-    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="21"/>
-    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="20"/>
-    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="19"/>
-    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="18"/>
-    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="17"/>
-    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="16"/>
-    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="15"/>
-    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="14"/>
-    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="13"/>
-    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="12"/>
-    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="11"/>
-    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="10"/>
-    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="9"/>
-    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="34"/>
+    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="33"/>
+    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="32"/>
+    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="31"/>
+    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="30"/>
+    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="29"/>
+    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="28"/>
+    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="27"/>
+    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="26"/>
+    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="25"/>
+    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="24"/>
+    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="23"/>
+    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="22"/>
+    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="21"/>
+    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="20"/>
+    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="19"/>
+    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="18"/>
+    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="17"/>
+    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="16"/>
+    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="15"/>
+    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="14"/>
+    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="13"/>
+    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="12"/>
+    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="0"/>
+    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="3"/>
+    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="2"/>
+    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="04-07-24" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="10">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="9">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="7">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="6">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -1045,10 +1073,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="1">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="5">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="4">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1415,11 +1443,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B32E72-8F4B-408A-9B01-FAD2807C0C88}">
-  <dimension ref="A1:DN52"/>
+  <dimension ref="A1:DR52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DL1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DN8" sqref="DN8"/>
+      <pane xSplit="1" topLeftCell="DN1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DP8" sqref="DP8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1436,7 +1464,7 @@
     <col min="116" max="118" width="11.43359375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1791,8 +1819,20 @@
       <c r="DN1" s="8" t="s">
         <v>156</v>
       </c>
+      <c r="DO1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="DP1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="DR1" t="s">
+        <v>157</v>
+      </c>
     </row>
-    <row r="2" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2145,10 +2185,18 @@
         <v>138081</v>
       </c>
       <c r="DN2" s="8">
+        <v>141283</v>
+      </c>
+      <c r="DO2" s="8">
         <v>144918</v>
       </c>
+      <c r="DP2" s="8">
+        <v>148115</v>
+      </c>
+      <c r="DQ2" s="8"/>
+      <c r="DR2" s="8"/>
     </row>
-    <row r="3" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -2501,10 +2549,18 @@
         <v>99169</v>
       </c>
       <c r="DN3" s="8">
+        <v>101362</v>
+      </c>
+      <c r="DO3" s="8">
         <v>103818</v>
       </c>
+      <c r="DP3" s="8">
+        <v>105805</v>
+      </c>
+      <c r="DQ3" s="8"/>
+      <c r="DR3" s="8"/>
     </row>
-    <row r="4" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -2857,10 +2913,18 @@
         <v>16678</v>
       </c>
       <c r="DN4" s="8">
+        <v>16878</v>
+      </c>
+      <c r="DO4" s="8">
         <v>17759</v>
       </c>
+      <c r="DP4" s="8">
+        <v>18844</v>
+      </c>
+      <c r="DQ4" s="8"/>
+      <c r="DR4" s="8"/>
     </row>
-    <row r="5" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -3122,10 +3186,18 @@
         <v>705</v>
       </c>
       <c r="DN5" s="8">
+        <v>645</v>
+      </c>
+      <c r="DO5" s="8">
         <v>661</v>
       </c>
+      <c r="DP5" s="8">
+        <v>676</v>
+      </c>
+      <c r="DQ5" s="8"/>
+      <c r="DR5" s="8"/>
     </row>
-    <row r="6" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -3474,10 +3546,18 @@
         <v>823</v>
       </c>
       <c r="DN6" s="8">
+        <v>825</v>
+      </c>
+      <c r="DO6" s="8">
         <v>843</v>
       </c>
+      <c r="DP6" s="8">
+        <v>846</v>
+      </c>
+      <c r="DQ6" s="8"/>
+      <c r="DR6" s="8"/>
     </row>
-    <row r="7" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -3828,10 +3908,18 @@
         <v>146</v>
       </c>
       <c r="DN7" s="8">
+        <v>154</v>
+      </c>
+      <c r="DO7" s="8">
         <v>153</v>
       </c>
+      <c r="DP7" s="8">
+        <v>162</v>
+      </c>
+      <c r="DQ7" s="8"/>
+      <c r="DR7" s="8"/>
     </row>
-    <row r="8" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -3924,29 +4012,31 @@
       <c r="CM8" s="8"/>
       <c r="CN8" s="8"/>
       <c r="CO8" s="8"/>
+      <c r="DI8" s="15"/>
+      <c r="DO8" s="8"/>
     </row>
-    <row r="9" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:122" x14ac:dyDescent="0.2">
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:122" x14ac:dyDescent="0.2">
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:122" x14ac:dyDescent="0.2">
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:122" x14ac:dyDescent="0.2">
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:122" x14ac:dyDescent="0.2">
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:122" x14ac:dyDescent="0.2">
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:122" x14ac:dyDescent="0.2">
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:122" x14ac:dyDescent="0.2">
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
@@ -4413,7 +4503,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44016</v>
+        <v>44018</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -22689,7 +22779,7 @@
       </c>
       <c r="B123" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C123" s="12">
         <v>117</v>
@@ -22704,145 +22794,145 @@
       </c>
       <c r="F123" cm="1">
         <f t="array" ref="F123">+INDEX(Hoja1!$B$2:$MO$7,1,E123)</f>
-        <v>144918</v>
+        <v>141283</v>
       </c>
       <c r="G123">
         <f t="shared" si="41"/>
-        <v>6837</v>
+        <v>3202</v>
       </c>
       <c r="H123" cm="1">
         <f t="array" ref="H123">+INDEX(Hoja1!$B$2:$MO$7,2,$E123)</f>
-        <v>103818</v>
+        <v>101362</v>
       </c>
       <c r="I123">
         <f t="shared" si="42"/>
-        <v>4649</v>
+        <v>2193</v>
       </c>
       <c r="J123">
         <f t="shared" si="33"/>
-        <v>41100</v>
+        <v>39921</v>
       </c>
       <c r="K123">
         <f t="shared" si="43"/>
-        <v>2188</v>
+        <v>1009</v>
       </c>
       <c r="L123" cm="1">
         <f t="array" ref="L123">+INDEX(Hoja1!$B$2:$MO$7,3,$E123)</f>
-        <v>17759</v>
+        <v>16878</v>
       </c>
       <c r="M123" cm="1">
         <f t="array" ref="M123">+INDEX(Hoja1!$B$2:$MO$7,4,$E123)</f>
-        <v>661</v>
+        <v>645</v>
       </c>
       <c r="N123" cm="1">
         <f t="array" ref="N123">+INDEX(Hoja1!$B$2:$MO$7,5,$E123)</f>
-        <v>843</v>
+        <v>825</v>
       </c>
       <c r="O123" cm="1">
         <f t="array" ref="O123">+INDEX(Hoja1!$B$2:$MO$7,6,$E123)</f>
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="P123" s="13">
         <f t="shared" si="60"/>
-        <v>0.71639133855007664</v>
+        <v>0.71743946547001414</v>
       </c>
       <c r="Q123" s="13">
         <f t="shared" si="61"/>
-        <v>0.28360866144992342</v>
+        <v>0.28256053452998592</v>
       </c>
       <c r="R123">
         <f t="shared" si="44"/>
-        <v>4557</v>
+        <v>922</v>
       </c>
       <c r="S123">
         <f t="shared" si="45"/>
-        <v>2188</v>
+        <v>1009</v>
       </c>
       <c r="T123">
         <f t="shared" si="46"/>
-        <v>1081</v>
+        <v>200</v>
       </c>
       <c r="U123">
         <f t="shared" si="47"/>
-        <v>-44</v>
+        <v>-60</v>
       </c>
       <c r="V123">
         <f t="shared" si="48"/>
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="W123">
         <f t="shared" si="49"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="X123">
         <f t="shared" si="50"/>
-        <v>1.9986842105263158</v>
+        <v>0.40438596491228068</v>
       </c>
       <c r="Y123">
         <f t="shared" si="51"/>
-        <v>5.6229440789473686E-2</v>
+        <v>2.5930304276315791E-2</v>
       </c>
       <c r="Z123">
         <f t="shared" si="52"/>
-        <v>1.0648159251708837</v>
+        <v>1.0119918455450294</v>
       </c>
       <c r="AA123">
         <f t="shared" si="53"/>
-        <v>0.93758865248226952</v>
+        <v>0.91489361702127658</v>
       </c>
       <c r="AB123">
         <f t="shared" si="54"/>
-        <v>1.0243013365735116</v>
+        <v>1.0024301336573511</v>
       </c>
       <c r="AC123">
         <f t="shared" si="55"/>
-        <v>1.047945205479452</v>
+        <v>1.0547945205479452</v>
       </c>
       <c r="AD123">
         <f t="shared" si="34"/>
-        <v>34844.43375811493</v>
+        <v>33970.425583072858</v>
       </c>
       <c r="AE123">
         <f t="shared" si="35"/>
-        <v>9882.1832171195001</v>
+        <v>9598.7016109641754</v>
       </c>
       <c r="AF123">
         <f t="shared" si="36"/>
-        <v>4270.0168309689834</v>
+        <v>4058.1870641981245</v>
       </c>
       <c r="AG123">
         <f t="shared" si="37"/>
-        <v>158.93243568165425</v>
+        <v>155.08535705698486</v>
       </c>
       <c r="AH123">
         <f t="shared" si="38"/>
-        <v>202.69295503726858</v>
+        <v>198.36499158451551</v>
       </c>
       <c r="AI123">
         <f t="shared" si="39"/>
-        <v>36.787689348401059</v>
+        <v>37.028131762442897</v>
       </c>
       <c r="AJ123">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>19416</v>
+        <v>18502</v>
       </c>
       <c r="AK123">
         <f t="shared" si="40"/>
-        <v>4668.4299110363072</v>
+        <v>4448.6655446020677</v>
       </c>
       <c r="AL123">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ122</f>
-        <v>1064</v>
+        <v>150</v>
       </c>
       <c r="AM123">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ122,0)</f>
-        <v>5.7977332170880559E-2</v>
+        <v>8.1734960767218829E-3</v>
       </c>
     </row>
     <row r="124" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A124" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B124" s="12" t="str">
         <f t="shared" si="57"/>
@@ -22861,149 +22951,149 @@
       </c>
       <c r="F124" cm="1">
         <f t="array" ref="F124">+INDEX(Hoja1!$B$2:$MO$7,1,E124)</f>
-        <v>0</v>
+        <v>144918</v>
       </c>
       <c r="G124">
         <f t="shared" si="41"/>
-        <v>-144918</v>
+        <v>3635</v>
       </c>
       <c r="H124" cm="1">
         <f t="array" ref="H124">+INDEX(Hoja1!$B$2:$MO$7,2,$E124)</f>
-        <v>0</v>
+        <v>103818</v>
       </c>
       <c r="I124">
         <f t="shared" si="42"/>
-        <v>-103818</v>
+        <v>2456</v>
       </c>
       <c r="J124">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>41100</v>
       </c>
       <c r="K124">
         <f t="shared" si="43"/>
-        <v>-41100</v>
+        <v>1179</v>
       </c>
       <c r="L124" cm="1">
         <f t="array" ref="L124">+INDEX(Hoja1!$B$2:$MO$7,3,$E124)</f>
-        <v>0</v>
+        <v>17759</v>
       </c>
       <c r="M124" cm="1">
         <f t="array" ref="M124">+INDEX(Hoja1!$B$2:$MO$7,4,$E124)</f>
-        <v>0</v>
+        <v>661</v>
       </c>
       <c r="N124" cm="1">
         <f t="array" ref="N124">+INDEX(Hoja1!$B$2:$MO$7,5,$E124)</f>
-        <v>0</v>
+        <v>843</v>
       </c>
       <c r="O124" cm="1">
         <f t="array" ref="O124">+INDEX(Hoja1!$B$2:$MO$7,6,$E124)</f>
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="P124" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.71639133855007664</v>
       </c>
       <c r="Q124" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.28360866144992342</v>
       </c>
       <c r="R124">
         <f t="shared" si="44"/>
-        <v>-151755</v>
+        <v>433</v>
       </c>
       <c r="S124">
         <f t="shared" si="45"/>
-        <v>-41100</v>
+        <v>1179</v>
       </c>
       <c r="T124">
         <f t="shared" si="46"/>
-        <v>-17759</v>
+        <v>881</v>
       </c>
       <c r="U124">
         <f t="shared" si="47"/>
-        <v>-661</v>
+        <v>16</v>
       </c>
       <c r="V124">
         <f t="shared" si="48"/>
-        <v>-843</v>
+        <v>18</v>
       </c>
       <c r="W124">
         <f t="shared" si="49"/>
-        <v>-153</v>
+        <v>-1</v>
       </c>
       <c r="X124">
         <f t="shared" si="50"/>
-        <v>-22.196138657305834</v>
+        <v>0.13522798251093066</v>
       </c>
       <c r="Y124">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.9533328323438791E-2</v>
       </c>
       <c r="Z124">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0521981277402537</v>
       </c>
       <c r="AA124">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1.0248062015503876</v>
       </c>
       <c r="AB124">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0218181818181817</v>
       </c>
       <c r="AC124">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>0.99350649350649356</v>
       </c>
       <c r="AD124">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>34844.43375811493</v>
       </c>
       <c r="AE124">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>9882.1832171195001</v>
       </c>
       <c r="AF124">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>4270.0168309689834</v>
       </c>
       <c r="AG124">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>158.93243568165425</v>
       </c>
       <c r="AH124">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>202.69295503726858</v>
       </c>
       <c r="AI124">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>36.787689348401059</v>
       </c>
       <c r="AJ124">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>19416</v>
       </c>
       <c r="AK124">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>4668.4299110363072</v>
       </c>
       <c r="AL124">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ123</f>
-        <v>-19416</v>
+        <v>914</v>
       </c>
       <c r="AM124">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ123,0)</f>
-        <v>-1</v>
+        <v>4.9400064857853206E-2</v>
       </c>
     </row>
     <row r="125" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A125" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B125" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C125" s="12">
         <v>119</v>
@@ -23018,139 +23108,139 @@
       </c>
       <c r="F125" cm="1">
         <f t="array" ref="F125">+INDEX(Hoja1!$B$2:$MO$7,1,E125)</f>
-        <v>0</v>
+        <v>148115</v>
       </c>
       <c r="G125">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>3197</v>
       </c>
       <c r="H125" cm="1">
         <f t="array" ref="H125">+INDEX(Hoja1!$B$2:$MO$7,2,$E125)</f>
-        <v>0</v>
+        <v>105805</v>
       </c>
       <c r="I125">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>1987</v>
       </c>
       <c r="J125">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>42310</v>
       </c>
       <c r="K125">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1210</v>
       </c>
       <c r="L125" cm="1">
         <f t="array" ref="L125">+INDEX(Hoja1!$B$2:$MO$7,3,$E125)</f>
-        <v>0</v>
+        <v>18844</v>
       </c>
       <c r="M125" cm="1">
         <f t="array" ref="M125">+INDEX(Hoja1!$B$2:$MO$7,4,$E125)</f>
-        <v>0</v>
+        <v>676</v>
       </c>
       <c r="N125" cm="1">
         <f t="array" ref="N125">+INDEX(Hoja1!$B$2:$MO$7,5,$E125)</f>
-        <v>0</v>
+        <v>846</v>
       </c>
       <c r="O125" cm="1">
         <f t="array" ref="O125">+INDEX(Hoja1!$B$2:$MO$7,6,$E125)</f>
-        <v>0</v>
+        <v>162</v>
       </c>
       <c r="P125" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.7143435843770044</v>
       </c>
       <c r="Q125" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.28565641562299565</v>
       </c>
       <c r="R125">
         <f t="shared" si="44"/>
-        <v>144918</v>
+        <v>-438</v>
       </c>
       <c r="S125">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>1210</v>
       </c>
       <c r="T125">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>1085</v>
       </c>
       <c r="U125">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="V125">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W125">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="X125">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-0.12049518569463549</v>
       </c>
       <c r="Y125">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>2.9440389294403894E-2</v>
       </c>
       <c r="Z125">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0610957824201812</v>
       </c>
       <c r="AA125">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1.0226928895612708</v>
       </c>
       <c r="AB125">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0035587188612101</v>
       </c>
       <c r="AC125">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.0588235294117647</v>
       </c>
       <c r="AD125">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>35613.128155806684</v>
       </c>
       <c r="AE125">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>10173.118538110122</v>
       </c>
       <c r="AF125">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>4530.8968502043763</v>
       </c>
       <c r="AG125">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>162.53907189228181</v>
       </c>
       <c r="AH125">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>203.41428227939409</v>
       </c>
       <c r="AI125">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>38.951671074777593</v>
       </c>
       <c r="AJ125">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>20528</v>
       </c>
       <c r="AK125">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>4935.8018754508294</v>
       </c>
       <c r="AL125">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ124</f>
-        <v>0</v>
+        <v>1112</v>
       </c>
       <c r="AM125">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ124,0)</f>
-        <v>0</v>
+        <v>5.727235269880511E-2</v>
       </c>
     </row>
     <row r="126" spans="1:39" x14ac:dyDescent="0.2">
@@ -23179,7 +23269,7 @@
       </c>
       <c r="G126">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-148115</v>
       </c>
       <c r="H126" cm="1">
         <f t="array" ref="H126">+INDEX(Hoja1!$B$2:$MO$7,2,$E126)</f>
@@ -23187,7 +23277,7 @@
       </c>
       <c r="I126">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-105805</v>
       </c>
       <c r="J126">
         <f t="shared" si="33"/>
@@ -23195,7 +23285,7 @@
       </c>
       <c r="K126">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-42310</v>
       </c>
       <c r="L126" cm="1">
         <f t="array" ref="L126">+INDEX(Hoja1!$B$2:$MO$7,3,$E126)</f>
@@ -23223,35 +23313,35 @@
       </c>
       <c r="R126">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>-151312</v>
       </c>
       <c r="S126">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-42310</v>
       </c>
       <c r="T126">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-18844</v>
       </c>
       <c r="U126">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-676</v>
       </c>
       <c r="V126">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-846</v>
       </c>
       <c r="W126">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-162</v>
       </c>
       <c r="X126">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-47.32937128558023</v>
       </c>
       <c r="Y126">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z126">
         <f t="shared" si="52"/>
@@ -23303,11 +23393,11 @@
       </c>
       <c r="AL126">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ125</f>
-        <v>0</v>
+        <v>-20528</v>
       </c>
       <c r="AM126">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ125,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="127" spans="1:39" x14ac:dyDescent="0.2">
@@ -23380,7 +23470,7 @@
       </c>
       <c r="R127">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>148115</v>
       </c>
       <c r="S127">
         <f t="shared" si="45"/>
@@ -23404,7 +23494,7 @@
       </c>
       <c r="X127">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y127">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-08-2020 17-54-29
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1575" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C3FED109-B87C-6047-A1B4-C87D4EA0F878}"/>
+  <xr:revisionPtr revIDLastSave="1581" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{024451AB-6F72-2046-B65E-2C93A596AEB5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="161">
   <si>
     <t>Columna1</t>
   </si>
@@ -664,18 +664,6 @@
   </cellStyles>
   <dxfs count="37">
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -794,6 +782,18 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
@@ -1017,30 +1017,30 @@
     <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="14"/>
     <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="13"/>
     <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="12"/>
-    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="0"/>
-    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="3"/>
-    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="2"/>
-    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="04-07-24" dataDxfId="1"/>
+    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="11"/>
+    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="10"/>
+    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="9"/>
+    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="04-07-24" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="6">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="9">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="5">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="3">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="6">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="2">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -1073,10 +1073,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="5">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="1">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="4">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="0">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1446,8 +1446,8 @@
   <dimension ref="A1:DR52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DP8" sqref="DP8"/>
+      <pane xSplit="1" topLeftCell="DO1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DQ8" sqref="DQ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2193,7 +2193,9 @@
       <c r="DP2" s="8">
         <v>148115</v>
       </c>
-      <c r="DQ2" s="8"/>
+      <c r="DQ2" s="8">
+        <v>150542</v>
+      </c>
       <c r="DR2" s="8"/>
     </row>
     <row r="3" spans="1:122" x14ac:dyDescent="0.2">
@@ -2557,7 +2559,9 @@
       <c r="DP3" s="8">
         <v>105805</v>
       </c>
-      <c r="DQ3" s="8"/>
+      <c r="DQ3" s="8">
+        <v>107269</v>
+      </c>
       <c r="DR3" s="8"/>
     </row>
     <row r="4" spans="1:122" x14ac:dyDescent="0.2">
@@ -2921,7 +2925,9 @@
       <c r="DP4" s="8">
         <v>18844</v>
       </c>
-      <c r="DQ4" s="8"/>
+      <c r="DQ4" s="8">
+        <v>19012</v>
+      </c>
       <c r="DR4" s="8"/>
     </row>
     <row r="5" spans="1:122" x14ac:dyDescent="0.2">
@@ -3194,7 +3200,9 @@
       <c r="DP5" s="8">
         <v>676</v>
       </c>
-      <c r="DQ5" s="8"/>
+      <c r="DQ5" s="8">
+        <v>732</v>
+      </c>
       <c r="DR5" s="8"/>
     </row>
     <row r="6" spans="1:122" x14ac:dyDescent="0.2">
@@ -3554,7 +3562,9 @@
       <c r="DP6" s="8">
         <v>846</v>
       </c>
-      <c r="DQ6" s="8"/>
+      <c r="DQ6" s="8">
+        <v>862</v>
+      </c>
       <c r="DR6" s="8"/>
     </row>
     <row r="7" spans="1:122" x14ac:dyDescent="0.2">
@@ -3916,7 +3926,9 @@
       <c r="DP7" s="8">
         <v>162</v>
       </c>
-      <c r="DQ7" s="8"/>
+      <c r="DQ7" s="8">
+        <v>160</v>
+      </c>
       <c r="DR7" s="8"/>
     </row>
     <row r="8" spans="1:122" x14ac:dyDescent="0.2">
@@ -4503,7 +4515,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -23093,7 +23105,7 @@
       </c>
       <c r="B125" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C125" s="12">
         <v>119</v>
@@ -23246,11 +23258,11 @@
     <row r="126" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A126" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B126" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C126" s="12">
         <v>120</v>
@@ -23265,139 +23277,139 @@
       </c>
       <c r="F126" cm="1">
         <f t="array" ref="F126">+INDEX(Hoja1!$B$2:$MO$7,1,E126)</f>
-        <v>0</v>
+        <v>150542</v>
       </c>
       <c r="G126">
         <f t="shared" si="41"/>
-        <v>-148115</v>
+        <v>2427</v>
       </c>
       <c r="H126" cm="1">
         <f t="array" ref="H126">+INDEX(Hoja1!$B$2:$MO$7,2,$E126)</f>
-        <v>0</v>
+        <v>107269</v>
       </c>
       <c r="I126">
         <f t="shared" si="42"/>
-        <v>-105805</v>
+        <v>1464</v>
       </c>
       <c r="J126">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>43273</v>
       </c>
       <c r="K126">
         <f t="shared" si="43"/>
-        <v>-42310</v>
+        <v>963</v>
       </c>
       <c r="L126" cm="1">
         <f t="array" ref="L126">+INDEX(Hoja1!$B$2:$MO$7,3,$E126)</f>
-        <v>0</v>
+        <v>19012</v>
       </c>
       <c r="M126" cm="1">
         <f t="array" ref="M126">+INDEX(Hoja1!$B$2:$MO$7,4,$E126)</f>
-        <v>0</v>
+        <v>732</v>
       </c>
       <c r="N126" cm="1">
         <f t="array" ref="N126">+INDEX(Hoja1!$B$2:$MO$7,5,$E126)</f>
-        <v>0</v>
+        <v>862</v>
       </c>
       <c r="O126" cm="1">
         <f t="array" ref="O126">+INDEX(Hoja1!$B$2:$MO$7,6,$E126)</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="P126" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.71255197884975618</v>
       </c>
       <c r="Q126" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.28744802115024376</v>
       </c>
       <c r="R126">
         <f t="shared" si="44"/>
-        <v>-151312</v>
+        <v>-770</v>
       </c>
       <c r="S126">
         <f t="shared" si="45"/>
-        <v>-42310</v>
+        <v>963</v>
       </c>
       <c r="T126">
         <f t="shared" si="46"/>
-        <v>-18844</v>
+        <v>168</v>
       </c>
       <c r="U126">
         <f t="shared" si="47"/>
-        <v>-676</v>
+        <v>56</v>
       </c>
       <c r="V126">
         <f t="shared" si="48"/>
-        <v>-846</v>
+        <v>16</v>
       </c>
       <c r="W126">
         <f t="shared" si="49"/>
-        <v>-162</v>
+        <v>-2</v>
       </c>
       <c r="X126">
         <f t="shared" si="50"/>
-        <v>-47.32937128558023</v>
+        <v>-0.24085079762277134</v>
       </c>
       <c r="Y126">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.2760576695816593E-2</v>
       </c>
       <c r="Z126">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0089153046062407</v>
       </c>
       <c r="AA126">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1.0828402366863905</v>
       </c>
       <c r="AB126">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0189125295508275</v>
       </c>
       <c r="AC126">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>0.98765432098765427</v>
       </c>
       <c r="AD126">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>36196.681894686226</v>
       </c>
       <c r="AE126">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>10404.664582832413</v>
       </c>
       <c r="AF126">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>4571.2911757634047</v>
       </c>
       <c r="AG126">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>176.00384707862469</v>
       </c>
       <c r="AH126">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>207.26136090406348</v>
       </c>
       <c r="AI126">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>38.470786246693919</v>
       </c>
       <c r="AJ126">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>20766</v>
       </c>
       <c r="AK126">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>4993.0271699927871</v>
       </c>
       <c r="AL126">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ125</f>
-        <v>-20528</v>
+        <v>238</v>
       </c>
       <c r="AM126">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ125,0)</f>
-        <v>-1</v>
+        <v>1.1593920498830864E-2</v>
       </c>
     </row>
     <row r="127" spans="1:39" x14ac:dyDescent="0.2">
@@ -23426,7 +23438,7 @@
       </c>
       <c r="G127">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-150542</v>
       </c>
       <c r="H127" cm="1">
         <f t="array" ref="H127">+INDEX(Hoja1!$B$2:$MO$7,2,$E127)</f>
@@ -23434,7 +23446,7 @@
       </c>
       <c r="I127">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-107269</v>
       </c>
       <c r="J127">
         <f t="shared" si="33"/>
@@ -23442,7 +23454,7 @@
       </c>
       <c r="K127">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-43273</v>
       </c>
       <c r="L127" cm="1">
         <f t="array" ref="L127">+INDEX(Hoja1!$B$2:$MO$7,3,$E127)</f>
@@ -23470,35 +23482,35 @@
       </c>
       <c r="R127">
         <f t="shared" si="44"/>
-        <v>148115</v>
+        <v>-152969</v>
       </c>
       <c r="S127">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-43273</v>
       </c>
       <c r="T127">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-19012</v>
       </c>
       <c r="U127">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-732</v>
       </c>
       <c r="V127">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-862</v>
       </c>
       <c r="W127">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-160</v>
       </c>
       <c r="X127">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-63.028018129377834</v>
       </c>
       <c r="Y127">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z127">
         <f t="shared" si="52"/>
@@ -23550,11 +23562,11 @@
       </c>
       <c r="AL127">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ126</f>
-        <v>0</v>
+        <v>-20766</v>
       </c>
       <c r="AM127">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ126,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="128" spans="1:39" x14ac:dyDescent="0.2">
@@ -23627,7 +23639,7 @@
       </c>
       <c r="R128">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>150542</v>
       </c>
       <c r="S128">
         <f t="shared" si="45"/>
@@ -23651,7 +23663,7 @@
       </c>
       <c r="X128">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y128">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-09-2020 05-56-34
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1581" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{024451AB-6F72-2046-B65E-2C93A596AEB5}"/>
+  <xr:revisionPtr revIDLastSave="1588" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B2B0BEFB-6F63-3248-985C-8C84315D8480}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="162">
   <si>
     <t>Columna1</t>
   </si>
@@ -529,9 +529,6 @@
     <t>04-07-20</t>
   </si>
   <si>
-    <t>04-07-24</t>
-  </si>
-  <si>
     <t>05-07-20</t>
   </si>
   <si>
@@ -539,6 +536,9 @@
   </si>
   <si>
     <t>07-06-20</t>
+  </si>
+  <si>
+    <t>08-07-20</t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1020,7 @@
     <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="11"/>
     <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="10"/>
     <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="9"/>
-    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="04-07-24" dataDxfId="8"/>
+    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1446,8 +1446,8 @@
   <dimension ref="A1:DR52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DQ8" sqref="DQ8"/>
+      <pane xSplit="1" topLeftCell="DP1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DS1" sqref="DS1:DS1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1820,16 +1820,16 @@
         <v>156</v>
       </c>
       <c r="DO1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="DP1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="DP1" s="1" t="s">
+      <c r="DQ1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="DQ1" s="1" t="s">
+      <c r="DR1" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="DR1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:122" x14ac:dyDescent="0.2">
@@ -2196,7 +2196,9 @@
       <c r="DQ2" s="8">
         <v>150542</v>
       </c>
-      <c r="DR2" s="8"/>
+      <c r="DR2" s="8">
+        <v>153148</v>
+      </c>
     </row>
     <row r="3" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2562,7 +2564,9 @@
       <c r="DQ3" s="8">
         <v>107269</v>
       </c>
-      <c r="DR3" s="8"/>
+      <c r="DR3" s="8">
+        <v>108893</v>
+      </c>
     </row>
     <row r="4" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2928,7 +2932,9 @@
       <c r="DQ4" s="8">
         <v>19012</v>
       </c>
-      <c r="DR4" s="8"/>
+      <c r="DR4" s="8">
+        <v>19211</v>
+      </c>
     </row>
     <row r="5" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -3203,7 +3209,9 @@
       <c r="DQ5" s="8">
         <v>732</v>
       </c>
-      <c r="DR5" s="8"/>
+      <c r="DR5" s="8">
+        <v>734</v>
+      </c>
     </row>
     <row r="6" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3565,7 +3573,9 @@
       <c r="DQ6" s="8">
         <v>862</v>
       </c>
-      <c r="DR6" s="8"/>
+      <c r="DR6" s="8">
+        <v>860</v>
+      </c>
     </row>
     <row r="7" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -3929,7 +3939,9 @@
       <c r="DQ7" s="8">
         <v>160</v>
       </c>
-      <c r="DR7" s="8"/>
+      <c r="DR7" s="8">
+        <v>158</v>
+      </c>
     </row>
     <row r="8" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
@@ -4515,7 +4527,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -23262,7 +23274,7 @@
       </c>
       <c r="B126" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C126" s="12">
         <v>120</v>
@@ -23415,11 +23427,11 @@
     <row r="127" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A127" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B127" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C127" s="12">
         <v>121</v>
@@ -23434,139 +23446,139 @@
       </c>
       <c r="F127" cm="1">
         <f t="array" ref="F127">+INDEX(Hoja1!$B$2:$MO$7,1,E127)</f>
-        <v>0</v>
+        <v>153148</v>
       </c>
       <c r="G127">
         <f t="shared" si="41"/>
-        <v>-150542</v>
+        <v>2606</v>
       </c>
       <c r="H127" cm="1">
         <f t="array" ref="H127">+INDEX(Hoja1!$B$2:$MO$7,2,$E127)</f>
-        <v>0</v>
+        <v>108893</v>
       </c>
       <c r="I127">
         <f t="shared" si="42"/>
-        <v>-107269</v>
+        <v>1624</v>
       </c>
       <c r="J127">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>44255</v>
       </c>
       <c r="K127">
         <f t="shared" si="43"/>
-        <v>-43273</v>
+        <v>982</v>
       </c>
       <c r="L127" cm="1">
         <f t="array" ref="L127">+INDEX(Hoja1!$B$2:$MO$7,3,$E127)</f>
-        <v>0</v>
+        <v>19211</v>
       </c>
       <c r="M127" cm="1">
         <f t="array" ref="M127">+INDEX(Hoja1!$B$2:$MO$7,4,$E127)</f>
-        <v>0</v>
+        <v>734</v>
       </c>
       <c r="N127" cm="1">
         <f t="array" ref="N127">+INDEX(Hoja1!$B$2:$MO$7,5,$E127)</f>
-        <v>0</v>
+        <v>860</v>
       </c>
       <c r="O127" cm="1">
         <f t="array" ref="O127">+INDEX(Hoja1!$B$2:$MO$7,6,$E127)</f>
-        <v>0</v>
+        <v>158</v>
       </c>
       <c r="P127" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.71103115940136341</v>
       </c>
       <c r="Q127" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.28896884059863659</v>
       </c>
       <c r="R127">
         <f t="shared" si="44"/>
-        <v>-152969</v>
+        <v>179</v>
       </c>
       <c r="S127">
         <f t="shared" si="45"/>
-        <v>-43273</v>
+        <v>982</v>
       </c>
       <c r="T127">
         <f t="shared" si="46"/>
-        <v>-19012</v>
+        <v>199</v>
       </c>
       <c r="U127">
         <f t="shared" si="47"/>
-        <v>-732</v>
+        <v>2</v>
       </c>
       <c r="V127">
         <f t="shared" si="48"/>
-        <v>-862</v>
+        <v>-2</v>
       </c>
       <c r="W127">
         <f t="shared" si="49"/>
-        <v>-160</v>
+        <v>-2</v>
       </c>
       <c r="X127">
         <f t="shared" si="50"/>
-        <v>-63.028018129377834</v>
+        <v>7.3753605274000822E-2</v>
       </c>
       <c r="Y127">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.2693134286968779E-2</v>
       </c>
       <c r="Z127">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0104670734273091</v>
       </c>
       <c r="AA127">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1.0027322404371584</v>
       </c>
       <c r="AB127">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>0.99767981438515085</v>
       </c>
       <c r="AC127">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="AD127">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>36823.274825679255</v>
       </c>
       <c r="AE127">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>10640.779033421497</v>
       </c>
       <c r="AF127">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>4619.1392161577305</v>
       </c>
       <c r="AG127">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>176.48473190670836</v>
       </c>
       <c r="AH127">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>206.78047607597981</v>
       </c>
       <c r="AI127">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>37.989901418610245</v>
       </c>
       <c r="AJ127">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>20963</v>
       </c>
       <c r="AK127">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>5040.3943255590284</v>
       </c>
       <c r="AL127">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ126</f>
-        <v>-20766</v>
+        <v>197</v>
       </c>
       <c r="AM127">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ126,0)</f>
-        <v>-1</v>
+        <v>9.4866608879899828E-3</v>
       </c>
     </row>
     <row r="128" spans="1:39" x14ac:dyDescent="0.2">
@@ -23595,7 +23607,7 @@
       </c>
       <c r="G128">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-153148</v>
       </c>
       <c r="H128" cm="1">
         <f t="array" ref="H128">+INDEX(Hoja1!$B$2:$MO$7,2,$E128)</f>
@@ -23603,7 +23615,7 @@
       </c>
       <c r="I128">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-108893</v>
       </c>
       <c r="J128">
         <f t="shared" si="33"/>
@@ -23611,7 +23623,7 @@
       </c>
       <c r="K128">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-44255</v>
       </c>
       <c r="L128" cm="1">
         <f t="array" ref="L128">+INDEX(Hoja1!$B$2:$MO$7,3,$E128)</f>
@@ -23639,35 +23651,35 @@
       </c>
       <c r="R128">
         <f t="shared" si="44"/>
-        <v>150542</v>
+        <v>-155754</v>
       </c>
       <c r="S128">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-44255</v>
       </c>
       <c r="T128">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-19211</v>
       </c>
       <c r="U128">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-734</v>
       </c>
       <c r="V128">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-860</v>
       </c>
       <c r="W128">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-158</v>
       </c>
       <c r="X128">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-59.767459708365308</v>
       </c>
       <c r="Y128">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z128">
         <f t="shared" si="52"/>
@@ -23719,11 +23731,11 @@
       </c>
       <c r="AL128">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ127</f>
-        <v>0</v>
+        <v>-20963</v>
       </c>
       <c r="AM128">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ127,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="129" spans="1:39" x14ac:dyDescent="0.2">
@@ -23796,7 +23808,7 @@
       </c>
       <c r="R129">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>153148</v>
       </c>
       <c r="S129">
         <f t="shared" si="45"/>
@@ -23820,7 +23832,7 @@
       </c>
       <c r="X129">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y129">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-10-2020 01-59-02
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1588" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B2B0BEFB-6F63-3248-985C-8C84315D8480}"/>
+  <xr:revisionPtr revIDLastSave="1597" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{83B1D84E-1B23-0942-905D-5407A6369D0B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="167">
   <si>
     <t>Columna1</t>
   </si>
@@ -540,6 +540,18 @@
   <si>
     <t>08-07-20</t>
   </si>
+  <si>
+    <t>08-07-22</t>
+  </si>
+  <si>
+    <t>08-07-23</t>
+  </si>
+  <si>
+    <t>08-07-24</t>
+  </si>
+  <si>
+    <t>09-07-20</t>
+  </si>
 </sst>
 </file>
 
@@ -662,7 +674,19 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="41">
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -896,9 +920,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:DR7" totalsRowShown="0">
-  <autoFilter ref="A1:DR7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
-  <tableColumns count="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:DV7" totalsRowShown="0">
+  <autoFilter ref="A1:DV7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
+  <tableColumns count="126">
     <tableColumn id="76" xr3:uid="{CA01250B-8685-4250-AAEF-D6E482663B6F}" name="Columna1"/>
     <tableColumn id="77" xr3:uid="{BC38B0B2-3229-42F8-9C9A-52EE74902839}" name="10-03-2020"/>
     <tableColumn id="78" xr3:uid="{4BB74E2E-62F3-4EED-8537-96C80CD1ED37}" name="11-03-2020"/>
@@ -992,55 +1016,59 @@
     <tableColumn id="4" xr3:uid="{2FE879E2-2128-42AE-A0E3-647EE2D0C94F}" name="07-06-2020"/>
     <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="08-06-2020"/>
     <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-2020"/>
-    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="34"/>
-    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="33"/>
-    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="32"/>
-    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="31"/>
-    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="30"/>
-    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="29"/>
-    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="28"/>
-    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="27"/>
-    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="26"/>
-    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="25"/>
-    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="24"/>
-    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="23"/>
-    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="22"/>
-    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="21"/>
-    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="20"/>
-    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="19"/>
-    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="18"/>
-    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="17"/>
-    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="16"/>
-    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="15"/>
-    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="14"/>
-    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="13"/>
-    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="12"/>
-    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="11"/>
-    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="10"/>
-    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="9"/>
-    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="39"/>
+    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="38"/>
+    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="37"/>
+    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="36"/>
+    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="35"/>
+    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="34"/>
+    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="33"/>
+    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="32"/>
+    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="31"/>
+    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="30"/>
+    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="29"/>
+    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="28"/>
+    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="27"/>
+    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="26"/>
+    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="25"/>
+    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="24"/>
+    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="23"/>
+    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="22"/>
+    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="21"/>
+    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="20"/>
+    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="19"/>
+    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="18"/>
+    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="17"/>
+    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="16"/>
+    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="15"/>
+    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="14"/>
+    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="13"/>
+    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="12"/>
+    <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="3"/>
+    <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="08-07-22" dataDxfId="2"/>
+    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="08-07-23" dataDxfId="1"/>
+    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="08-07-24" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="10">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="9">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="7">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="6">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -1073,10 +1101,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="1">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="5">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="4">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1443,11 +1471,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B32E72-8F4B-408A-9B01-FAD2807C0C88}">
-  <dimension ref="A1:DR52"/>
+  <dimension ref="A1:DV52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DS1" sqref="DS1:DS1048576"/>
+      <pane xSplit="1" topLeftCell="DQ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DS8" sqref="DS8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1464,7 +1492,7 @@
     <col min="116" max="118" width="11.43359375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:122" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1831,8 +1859,20 @@
       <c r="DR1" s="1" t="s">
         <v>160</v>
       </c>
+      <c r="DS1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="DT1" t="s">
+        <v>161</v>
+      </c>
+      <c r="DU1" t="s">
+        <v>162</v>
+      </c>
+      <c r="DV1" t="s">
+        <v>163</v>
+      </c>
     </row>
-    <row r="2" spans="1:122" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2199,8 +2239,14 @@
       <c r="DR2" s="8">
         <v>153148</v>
       </c>
+      <c r="DS2" s="8">
+        <v>155605</v>
+      </c>
+      <c r="DT2" s="8"/>
+      <c r="DU2" s="8"/>
+      <c r="DV2" s="8"/>
     </row>
-    <row r="3" spans="1:122" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -2567,8 +2613,14 @@
       <c r="DR3" s="8">
         <v>108893</v>
       </c>
+      <c r="DS3" s="8">
+        <v>110426</v>
+      </c>
+      <c r="DT3" s="8"/>
+      <c r="DU3" s="8"/>
+      <c r="DV3" s="8"/>
     </row>
-    <row r="4" spans="1:122" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -2935,8 +2987,14 @@
       <c r="DR4" s="8">
         <v>19211</v>
       </c>
+      <c r="DS4" s="8">
+        <v>19182</v>
+      </c>
+      <c r="DT4" s="8"/>
+      <c r="DU4" s="8"/>
+      <c r="DV4" s="8"/>
     </row>
-    <row r="5" spans="1:122" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -3212,8 +3270,14 @@
       <c r="DR5" s="8">
         <v>734</v>
       </c>
+      <c r="DS5" s="8">
+        <v>709</v>
+      </c>
+      <c r="DT5" s="8"/>
+      <c r="DU5" s="8"/>
+      <c r="DV5" s="8"/>
     </row>
-    <row r="6" spans="1:122" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -3576,8 +3640,14 @@
       <c r="DR6" s="8">
         <v>860</v>
       </c>
+      <c r="DS6" s="8">
+        <v>890</v>
+      </c>
+      <c r="DT6" s="8"/>
+      <c r="DU6" s="8"/>
+      <c r="DV6" s="8"/>
     </row>
-    <row r="7" spans="1:122" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -3942,8 +4012,14 @@
       <c r="DR7" s="8">
         <v>158</v>
       </c>
+      <c r="DS7" s="8">
+        <v>159</v>
+      </c>
+      <c r="DT7" s="8"/>
+      <c r="DU7" s="8"/>
+      <c r="DV7" s="8"/>
     </row>
-    <row r="8" spans="1:122" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4039,28 +4115,28 @@
       <c r="DI8" s="15"/>
       <c r="DO8" s="8"/>
     </row>
-    <row r="9" spans="1:122" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:126" x14ac:dyDescent="0.2">
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:122" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:126" x14ac:dyDescent="0.2">
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:122" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:126" x14ac:dyDescent="0.2">
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:122" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:126" x14ac:dyDescent="0.2">
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:122" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:126" x14ac:dyDescent="0.2">
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:122" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:126" x14ac:dyDescent="0.2">
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:122" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:126" x14ac:dyDescent="0.2">
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:122" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:126" x14ac:dyDescent="0.2">
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
@@ -4527,7 +4603,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -23431,7 +23507,7 @@
       </c>
       <c r="B127" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C127" s="12">
         <v>121</v>
@@ -23584,11 +23660,11 @@
     <row r="128" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A128" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B128" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C128" s="12">
         <v>122</v>
@@ -23603,139 +23679,139 @@
       </c>
       <c r="F128" cm="1">
         <f t="array" ref="F128">+INDEX(Hoja1!$B$2:$MO$7,1,E128)</f>
-        <v>0</v>
+        <v>155605</v>
       </c>
       <c r="G128">
         <f t="shared" si="41"/>
-        <v>-153148</v>
+        <v>2457</v>
       </c>
       <c r="H128" cm="1">
         <f t="array" ref="H128">+INDEX(Hoja1!$B$2:$MO$7,2,$E128)</f>
-        <v>0</v>
+        <v>110426</v>
       </c>
       <c r="I128">
         <f t="shared" si="42"/>
-        <v>-108893</v>
+        <v>1533</v>
       </c>
       <c r="J128">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>45179</v>
       </c>
       <c r="K128">
         <f t="shared" si="43"/>
-        <v>-44255</v>
+        <v>924</v>
       </c>
       <c r="L128" cm="1">
         <f t="array" ref="L128">+INDEX(Hoja1!$B$2:$MO$7,3,$E128)</f>
-        <v>0</v>
+        <v>19182</v>
       </c>
       <c r="M128" cm="1">
         <f t="array" ref="M128">+INDEX(Hoja1!$B$2:$MO$7,4,$E128)</f>
-        <v>0</v>
+        <v>709</v>
       </c>
       <c r="N128" cm="1">
         <f t="array" ref="N128">+INDEX(Hoja1!$B$2:$MO$7,5,$E128)</f>
-        <v>0</v>
+        <v>890</v>
       </c>
       <c r="O128" cm="1">
         <f t="array" ref="O128">+INDEX(Hoja1!$B$2:$MO$7,6,$E128)</f>
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="P128" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.70965585938755182</v>
       </c>
       <c r="Q128" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.29034414061244818</v>
       </c>
       <c r="R128">
         <f t="shared" si="44"/>
-        <v>-155754</v>
+        <v>-149</v>
       </c>
       <c r="S128">
         <f t="shared" si="45"/>
-        <v>-44255</v>
+        <v>924</v>
       </c>
       <c r="T128">
         <f t="shared" si="46"/>
-        <v>-19211</v>
+        <v>-29</v>
       </c>
       <c r="U128">
         <f t="shared" si="47"/>
-        <v>-734</v>
+        <v>-25</v>
       </c>
       <c r="V128">
         <f t="shared" si="48"/>
-        <v>-860</v>
+        <v>30</v>
       </c>
       <c r="W128">
         <f t="shared" si="49"/>
-        <v>-158</v>
+        <v>1</v>
       </c>
       <c r="X128">
         <f t="shared" si="50"/>
-        <v>-59.767459708365308</v>
+        <v>-5.7175748273215657E-2</v>
       </c>
       <c r="Y128">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.0878996723534063E-2</v>
       </c>
       <c r="Z128">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>0.99849044818072974</v>
       </c>
       <c r="AA128">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>0.9659400544959128</v>
       </c>
       <c r="AB128">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0348837209302326</v>
       </c>
       <c r="AC128">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.0063291139240507</v>
       </c>
       <c r="AD128">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>37414.041836980046</v>
       </c>
       <c r="AE128">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>10862.947823996154</v>
       </c>
       <c r="AF128">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>4612.1663861505176</v>
       </c>
       <c r="AG128">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>170.47367155566243</v>
       </c>
       <c r="AH128">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>213.99374849723492</v>
       </c>
       <c r="AI128">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>38.230343832652082</v>
       </c>
       <c r="AJ128">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>20940</v>
       </c>
       <c r="AK128">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>5034.8641500360663</v>
       </c>
       <c r="AL128">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ127</f>
-        <v>-20963</v>
+        <v>-23</v>
       </c>
       <c r="AM128">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ127,0)</f>
-        <v>-1</v>
+        <v>-1.0971712064112961E-3</v>
       </c>
     </row>
     <row r="129" spans="1:39" x14ac:dyDescent="0.2">
@@ -23764,7 +23840,7 @@
       </c>
       <c r="G129">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-155605</v>
       </c>
       <c r="H129" cm="1">
         <f t="array" ref="H129">+INDEX(Hoja1!$B$2:$MO$7,2,$E129)</f>
@@ -23772,7 +23848,7 @@
       </c>
       <c r="I129">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-110426</v>
       </c>
       <c r="J129">
         <f t="shared" si="33"/>
@@ -23780,7 +23856,7 @@
       </c>
       <c r="K129">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-45179</v>
       </c>
       <c r="L129" cm="1">
         <f t="array" ref="L129">+INDEX(Hoja1!$B$2:$MO$7,3,$E129)</f>
@@ -23808,35 +23884,35 @@
       </c>
       <c r="R129">
         <f t="shared" si="44"/>
-        <v>153148</v>
+        <v>-158062</v>
       </c>
       <c r="S129">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-45179</v>
       </c>
       <c r="T129">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-19182</v>
       </c>
       <c r="U129">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-709</v>
       </c>
       <c r="V129">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-890</v>
       </c>
       <c r="W129">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-159</v>
       </c>
       <c r="X129">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-64.331298331298328</v>
       </c>
       <c r="Y129">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z129">
         <f t="shared" si="52"/>
@@ -23888,11 +23964,11 @@
       </c>
       <c r="AL129">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ128</f>
-        <v>0</v>
+        <v>-20940</v>
       </c>
       <c r="AM129">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ128,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="130" spans="1:39" x14ac:dyDescent="0.2">
@@ -23965,7 +24041,7 @@
       </c>
       <c r="R130">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>155605</v>
       </c>
       <c r="S130">
         <f t="shared" si="45"/>
@@ -23989,7 +24065,7 @@
       </c>
       <c r="X130">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y130">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-11-2020 22-04-57
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1597" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{83B1D84E-1B23-0942-905D-5407A6369D0B}"/>
+  <xr:revisionPtr revIDLastSave="1599" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D01EFF1F-10AD-BB47-8F3C-753FFD765E92}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="166">
   <si>
     <t>Columna1</t>
   </si>
@@ -541,9 +541,6 @@
     <t>08-07-20</t>
   </si>
   <si>
-    <t>08-07-22</t>
-  </si>
-  <si>
     <t>08-07-23</t>
   </si>
   <si>
@@ -551,6 +548,9 @@
   </si>
   <si>
     <t>09-07-20</t>
+  </si>
+  <si>
+    <t>10-07-20</t>
   </si>
 </sst>
 </file>
@@ -676,18 +676,6 @@
   </cellStyles>
   <dxfs count="41">
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -806,6 +794,18 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
@@ -1045,30 +1045,30 @@
     <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="14"/>
     <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="13"/>
     <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="12"/>
-    <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="3"/>
-    <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="08-07-22" dataDxfId="2"/>
-    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="08-07-23" dataDxfId="1"/>
-    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="08-07-24" dataDxfId="0"/>
+    <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="11"/>
+    <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="10-07-20" dataDxfId="10"/>
+    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="08-07-23" dataDxfId="9"/>
+    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="08-07-24" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="6">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="9">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="5">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="3">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="6">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="2">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -1101,10 +1101,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="5">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="1">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="4">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="0">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1475,7 +1475,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="DQ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DS8" sqref="DS8"/>
+      <selection pane="topRight" activeCell="DT3" sqref="DT3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1860,16 +1860,16 @@
         <v>160</v>
       </c>
       <c r="DS1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="DT1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="DT1" t="s">
+      <c r="DU1" t="s">
         <v>161</v>
       </c>
-      <c r="DU1" t="s">
+      <c r="DV1" t="s">
         <v>162</v>
-      </c>
-      <c r="DV1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:126" x14ac:dyDescent="0.2">
@@ -2242,7 +2242,9 @@
       <c r="DS2" s="8">
         <v>155605</v>
       </c>
-      <c r="DT2" s="8"/>
+      <c r="DT2" s="8">
+        <v>158669</v>
+      </c>
       <c r="DU2" s="8"/>
       <c r="DV2" s="8"/>
     </row>
@@ -4603,7 +4605,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44021</v>
+        <v>44022</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -23664,7 +23666,7 @@
       </c>
       <c r="B128" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C128" s="12">
         <v>122</v>
@@ -23817,11 +23819,11 @@
     <row r="129" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A129" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B129" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C129" s="12">
         <v>123</v>
@@ -23836,11 +23838,11 @@
       </c>
       <c r="F129" cm="1">
         <f t="array" ref="F129">+INDEX(Hoja1!$B$2:$MO$7,1,E129)</f>
-        <v>0</v>
+        <v>158669</v>
       </c>
       <c r="G129">
         <f t="shared" si="41"/>
-        <v>-155605</v>
+        <v>3064</v>
       </c>
       <c r="H129" cm="1">
         <f t="array" ref="H129">+INDEX(Hoja1!$B$2:$MO$7,2,$E129)</f>
@@ -23852,11 +23854,11 @@
       </c>
       <c r="J129">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>158669</v>
       </c>
       <c r="K129">
         <f t="shared" si="43"/>
-        <v>-45179</v>
+        <v>113490</v>
       </c>
       <c r="L129" cm="1">
         <f t="array" ref="L129">+INDEX(Hoja1!$B$2:$MO$7,3,$E129)</f>
@@ -23880,15 +23882,15 @@
       </c>
       <c r="Q129" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R129">
         <f t="shared" si="44"/>
-        <v>-158062</v>
+        <v>607</v>
       </c>
       <c r="S129">
         <f t="shared" si="45"/>
-        <v>-45179</v>
+        <v>113490</v>
       </c>
       <c r="T129">
         <f t="shared" si="46"/>
@@ -23908,11 +23910,11 @@
       </c>
       <c r="X129">
         <f t="shared" si="50"/>
-        <v>-64.331298331298328</v>
+        <v>0.24704924704924705</v>
       </c>
       <c r="Y129">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.512007791230439</v>
       </c>
       <c r="Z129">
         <f t="shared" si="52"/>
@@ -23932,11 +23934,11 @@
       </c>
       <c r="AD129">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>38150.757393604232</v>
       </c>
       <c r="AE129">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>38150.757393604232</v>
       </c>
       <c r="AF129">
         <f t="shared" si="36"/>
@@ -23997,7 +23999,7 @@
       </c>
       <c r="G130">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-158669</v>
       </c>
       <c r="H130" cm="1">
         <f t="array" ref="H130">+INDEX(Hoja1!$B$2:$MO$7,2,$E130)</f>
@@ -24013,7 +24015,7 @@
       </c>
       <c r="K130">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-158669</v>
       </c>
       <c r="L130" cm="1">
         <f t="array" ref="L130">+INDEX(Hoja1!$B$2:$MO$7,3,$E130)</f>
@@ -24041,11 +24043,11 @@
       </c>
       <c r="R130">
         <f t="shared" si="44"/>
-        <v>155605</v>
+        <v>-161733</v>
       </c>
       <c r="S130">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-158669</v>
       </c>
       <c r="T130">
         <f t="shared" si="46"/>
@@ -24065,11 +24067,11 @@
       </c>
       <c r="X130">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-52.784921671018274</v>
       </c>
       <c r="Y130">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z130">
         <f t="shared" si="52"/>
@@ -24198,7 +24200,7 @@
       </c>
       <c r="R131">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>158669</v>
       </c>
       <c r="S131">
         <f t="shared" si="45"/>
@@ -24222,7 +24224,7 @@
       </c>
       <c r="X131">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y131">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-12-2020 06-05-52
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1599" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D01EFF1F-10AD-BB47-8F3C-753FFD765E92}"/>
+  <xr:revisionPtr revIDLastSave="1608" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FA356C5C-82C1-AF4D-B3F7-FC2493C4C3F4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -541,9 +541,6 @@
     <t>08-07-20</t>
   </si>
   <si>
-    <t>08-07-23</t>
-  </si>
-  <si>
     <t>08-07-24</t>
   </si>
   <si>
@@ -551,6 +548,9 @@
   </si>
   <si>
     <t>10-07-20</t>
+  </si>
+  <si>
+    <t>11-07-20</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1047,7 @@
     <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="12"/>
     <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="11"/>
     <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="10-07-20" dataDxfId="10"/>
-    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="08-07-23" dataDxfId="9"/>
+    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="11-07-20" dataDxfId="9"/>
     <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="08-07-24" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1474,8 +1474,8 @@
   <dimension ref="A1:DV52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DQ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DT3" sqref="DT3"/>
+      <pane xSplit="1" topLeftCell="DR1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DU4" sqref="DU4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1860,16 +1860,16 @@
         <v>160</v>
       </c>
       <c r="DS1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="DT1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="DT1" s="1" t="s">
+      <c r="DU1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="DU1" t="s">
+      <c r="DV1" t="s">
         <v>161</v>
-      </c>
-      <c r="DV1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:126" x14ac:dyDescent="0.2">
@@ -2245,7 +2245,9 @@
       <c r="DT2" s="8">
         <v>158669</v>
       </c>
-      <c r="DU2" s="8"/>
+      <c r="DU2" s="8">
+        <v>161466</v>
+      </c>
       <c r="DV2" s="8"/>
     </row>
     <row r="3" spans="1:126" x14ac:dyDescent="0.2">
@@ -2618,8 +2620,12 @@
       <c r="DS3" s="8">
         <v>110426</v>
       </c>
-      <c r="DT3" s="8"/>
-      <c r="DU3" s="8"/>
+      <c r="DT3" s="8">
+        <v>112407</v>
+      </c>
+      <c r="DU3" s="8">
+        <v>114238</v>
+      </c>
       <c r="DV3" s="8"/>
     </row>
     <row r="4" spans="1:126" x14ac:dyDescent="0.2">
@@ -2992,7 +2998,9 @@
       <c r="DS4" s="8">
         <v>19182</v>
       </c>
-      <c r="DT4" s="8"/>
+      <c r="DT4" s="8">
+        <v>19193</v>
+      </c>
       <c r="DU4" s="8"/>
       <c r="DV4" s="8"/>
     </row>
@@ -3275,7 +3283,9 @@
       <c r="DS5" s="8">
         <v>709</v>
       </c>
-      <c r="DT5" s="8"/>
+      <c r="DT5" s="8">
+        <v>656</v>
+      </c>
       <c r="DU5" s="8"/>
       <c r="DV5" s="8"/>
     </row>
@@ -3645,7 +3655,9 @@
       <c r="DS6" s="8">
         <v>890</v>
       </c>
-      <c r="DT6" s="8"/>
+      <c r="DT6" s="8">
+        <v>959</v>
+      </c>
       <c r="DU6" s="8"/>
       <c r="DV6" s="8"/>
     </row>
@@ -4017,7 +4029,9 @@
       <c r="DS7" s="8">
         <v>159</v>
       </c>
-      <c r="DT7" s="8"/>
+      <c r="DT7" s="8">
+        <v>160</v>
+      </c>
       <c r="DU7" s="8"/>
       <c r="DV7" s="8"/>
     </row>
@@ -4605,7 +4619,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -23823,7 +23837,7 @@
       </c>
       <c r="B129" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C129" s="12">
         <v>123</v>
@@ -23846,43 +23860,43 @@
       </c>
       <c r="H129" cm="1">
         <f t="array" ref="H129">+INDEX(Hoja1!$B$2:$MO$7,2,$E129)</f>
-        <v>0</v>
+        <v>112407</v>
       </c>
       <c r="I129">
         <f t="shared" si="42"/>
-        <v>-110426</v>
+        <v>1981</v>
       </c>
       <c r="J129">
         <f t="shared" si="33"/>
-        <v>158669</v>
+        <v>46262</v>
       </c>
       <c r="K129">
         <f t="shared" si="43"/>
-        <v>113490</v>
+        <v>1083</v>
       </c>
       <c r="L129" cm="1">
         <f t="array" ref="L129">+INDEX(Hoja1!$B$2:$MO$7,3,$E129)</f>
-        <v>0</v>
+        <v>19193</v>
       </c>
       <c r="M129" cm="1">
         <f t="array" ref="M129">+INDEX(Hoja1!$B$2:$MO$7,4,$E129)</f>
-        <v>0</v>
+        <v>656</v>
       </c>
       <c r="N129" cm="1">
         <f t="array" ref="N129">+INDEX(Hoja1!$B$2:$MO$7,5,$E129)</f>
-        <v>0</v>
+        <v>959</v>
       </c>
       <c r="O129" cm="1">
         <f t="array" ref="O129">+INDEX(Hoja1!$B$2:$MO$7,6,$E129)</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="P129" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.70843706079952606</v>
       </c>
       <c r="Q129" s="13">
         <f t="shared" si="61"/>
-        <v>1</v>
+        <v>0.29156293920047394</v>
       </c>
       <c r="R129">
         <f t="shared" si="44"/>
@@ -23890,23 +23904,23 @@
       </c>
       <c r="S129">
         <f t="shared" si="45"/>
-        <v>113490</v>
+        <v>1083</v>
       </c>
       <c r="T129">
         <f t="shared" si="46"/>
-        <v>-19182</v>
+        <v>11</v>
       </c>
       <c r="U129">
         <f t="shared" si="47"/>
-        <v>-709</v>
+        <v>-53</v>
       </c>
       <c r="V129">
         <f t="shared" si="48"/>
-        <v>-890</v>
+        <v>69</v>
       </c>
       <c r="W129">
         <f t="shared" si="49"/>
-        <v>-159</v>
+        <v>1</v>
       </c>
       <c r="X129">
         <f t="shared" si="50"/>
@@ -23914,23 +23928,23 @@
       </c>
       <c r="Y129">
         <f t="shared" si="51"/>
-        <v>2.512007791230439</v>
+        <v>2.3971314106111245E-2</v>
       </c>
       <c r="Z129">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0005734542800542</v>
       </c>
       <c r="AA129">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>0.92524682651622003</v>
       </c>
       <c r="AB129">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0775280898876405</v>
       </c>
       <c r="AC129">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.0062893081761006</v>
       </c>
       <c r="AD129">
         <f t="shared" si="34"/>
@@ -23938,49 +23952,49 @@
       </c>
       <c r="AE129">
         <f t="shared" si="35"/>
-        <v>38150.757393604232</v>
+        <v>11123.346958403463</v>
       </c>
       <c r="AF129">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>4614.8112527049771</v>
       </c>
       <c r="AG129">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>157.73022361144507</v>
       </c>
       <c r="AH129">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>230.58427506612168</v>
       </c>
       <c r="AI129">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>38.470786246693919</v>
       </c>
       <c r="AJ129">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>20968</v>
       </c>
       <c r="AK129">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>5041.5965376292379</v>
       </c>
       <c r="AL129">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ128</f>
-        <v>-20940</v>
+        <v>28</v>
       </c>
       <c r="AM129">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ128,0)</f>
-        <v>-1</v>
+        <v>1.3371537726838587E-3</v>
       </c>
     </row>
     <row r="130" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A130" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B130" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C130" s="12">
         <v>124</v>
@@ -23995,27 +24009,27 @@
       </c>
       <c r="F130" cm="1">
         <f t="array" ref="F130">+INDEX(Hoja1!$B$2:$MO$7,1,E130)</f>
-        <v>0</v>
+        <v>161466</v>
       </c>
       <c r="G130">
         <f t="shared" si="41"/>
-        <v>-158669</v>
+        <v>2797</v>
       </c>
       <c r="H130" cm="1">
         <f t="array" ref="H130">+INDEX(Hoja1!$B$2:$MO$7,2,$E130)</f>
-        <v>0</v>
+        <v>114238</v>
       </c>
       <c r="I130">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>1831</v>
       </c>
       <c r="J130">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>47228</v>
       </c>
       <c r="K130">
         <f t="shared" si="43"/>
-        <v>-158669</v>
+        <v>966</v>
       </c>
       <c r="L130" cm="1">
         <f t="array" ref="L130">+INDEX(Hoja1!$B$2:$MO$7,3,$E130)</f>
@@ -24035,43 +24049,43 @@
       </c>
       <c r="P130" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.70750498556971742</v>
       </c>
       <c r="Q130" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.29249501443028253</v>
       </c>
       <c r="R130">
         <f t="shared" si="44"/>
-        <v>-161733</v>
+        <v>-267</v>
       </c>
       <c r="S130">
         <f t="shared" si="45"/>
-        <v>-158669</v>
+        <v>966</v>
       </c>
       <c r="T130">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-19193</v>
       </c>
       <c r="U130">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-656</v>
       </c>
       <c r="V130">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-959</v>
       </c>
       <c r="W130">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-160</v>
       </c>
       <c r="X130">
         <f t="shared" si="50"/>
-        <v>-52.784921671018274</v>
+        <v>-8.7140992167101833E-2</v>
       </c>
       <c r="Y130">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.0881068695689765E-2</v>
       </c>
       <c r="Z130">
         <f t="shared" si="52"/>
@@ -24091,11 +24105,11 @@
       </c>
       <c r="AD130">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>38823.274825679255</v>
       </c>
       <c r="AE130">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>11355.614330367878</v>
       </c>
       <c r="AF130">
         <f t="shared" si="36"/>
@@ -24123,11 +24137,11 @@
       </c>
       <c r="AL130">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ129</f>
-        <v>0</v>
+        <v>-20968</v>
       </c>
       <c r="AM130">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ129,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="131" spans="1:39" x14ac:dyDescent="0.2">
@@ -24156,7 +24170,7 @@
       </c>
       <c r="G131">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-161466</v>
       </c>
       <c r="H131" cm="1">
         <f t="array" ref="H131">+INDEX(Hoja1!$B$2:$MO$7,2,$E131)</f>
@@ -24164,7 +24178,7 @@
       </c>
       <c r="I131">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-114238</v>
       </c>
       <c r="J131">
         <f t="shared" si="33"/>
@@ -24172,7 +24186,7 @@
       </c>
       <c r="K131">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-47228</v>
       </c>
       <c r="L131" cm="1">
         <f t="array" ref="L131">+INDEX(Hoja1!$B$2:$MO$7,3,$E131)</f>
@@ -24200,11 +24214,11 @@
       </c>
       <c r="R131">
         <f t="shared" si="44"/>
-        <v>158669</v>
+        <v>-164263</v>
       </c>
       <c r="S131">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-47228</v>
       </c>
       <c r="T131">
         <f t="shared" si="46"/>
@@ -24224,11 +24238,11 @@
       </c>
       <c r="X131">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-58.728280300321771</v>
       </c>
       <c r="Y131">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z131">
         <f t="shared" si="52"/>
@@ -24357,7 +24371,7 @@
       </c>
       <c r="R132">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>161466</v>
       </c>
       <c r="S132">
         <f t="shared" si="45"/>
@@ -24381,7 +24395,7 @@
       </c>
       <c r="X132">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y132">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-13-2020 06-09-15
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1608" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FA356C5C-82C1-AF4D-B3F7-FC2493C4C3F4}"/>
+  <xr:revisionPtr revIDLastSave="1619" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0032DF64-1B51-0644-B935-833635DFB017}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -541,9 +541,6 @@
     <t>08-07-20</t>
   </si>
   <si>
-    <t>08-07-24</t>
-  </si>
-  <si>
     <t>09-07-20</t>
   </si>
   <si>
@@ -551,6 +548,9 @@
   </si>
   <si>
     <t>11-07-20</t>
+  </si>
+  <si>
+    <t>12-07-20</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1048,7 @@
     <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="11"/>
     <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="10-07-20" dataDxfId="10"/>
     <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="11-07-20" dataDxfId="9"/>
-    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="08-07-24" dataDxfId="8"/>
+    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="12-07-20" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1474,8 +1474,8 @@
   <dimension ref="A1:DV52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DR1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DU4" sqref="DU4"/>
+      <pane xSplit="1" topLeftCell="DT1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DV1" sqref="DV1:DV7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1860,16 +1860,16 @@
         <v>160</v>
       </c>
       <c r="DS1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="DT1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="DT1" s="1" t="s">
+      <c r="DU1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="DU1" s="1" t="s">
+      <c r="DV1" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="DV1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:126" x14ac:dyDescent="0.2">
@@ -2248,7 +2248,9 @@
       <c r="DU2" s="8">
         <v>161466</v>
       </c>
-      <c r="DV2" s="8"/>
+      <c r="DV2" s="8">
+        <v>164927</v>
+      </c>
     </row>
     <row r="3" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2626,7 +2628,9 @@
       <c r="DU3" s="8">
         <v>114238</v>
       </c>
-      <c r="DV3" s="8"/>
+      <c r="DV3" s="8">
+        <v>116372</v>
+      </c>
     </row>
     <row r="4" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -3001,8 +3005,12 @@
       <c r="DT4" s="8">
         <v>19193</v>
       </c>
-      <c r="DU4" s="8"/>
-      <c r="DV4" s="8"/>
+      <c r="DU4" s="8">
+        <v>19497</v>
+      </c>
+      <c r="DV4" s="8">
+        <v>19867</v>
+      </c>
     </row>
     <row r="5" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -3286,8 +3294,12 @@
       <c r="DT5" s="8">
         <v>656</v>
       </c>
-      <c r="DU5" s="8"/>
-      <c r="DV5" s="8"/>
+      <c r="DU5" s="8">
+        <v>678</v>
+      </c>
+      <c r="DV5" s="8">
+        <v>672</v>
+      </c>
     </row>
     <row r="6" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3658,8 +3670,12 @@
       <c r="DT6" s="8">
         <v>959</v>
       </c>
-      <c r="DU6" s="8"/>
-      <c r="DV6" s="8"/>
+      <c r="DU6" s="8">
+        <v>936</v>
+      </c>
+      <c r="DV6" s="8">
+        <v>987</v>
+      </c>
     </row>
     <row r="7" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -4032,8 +4048,12 @@
       <c r="DT7" s="8">
         <v>160</v>
       </c>
-      <c r="DU7" s="8"/>
-      <c r="DV7" s="8"/>
+      <c r="DU7" s="8">
+        <v>158</v>
+      </c>
+      <c r="DV7" s="8">
+        <v>159</v>
+      </c>
     </row>
     <row r="8" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
@@ -4619,7 +4639,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44023</v>
+        <v>44024</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -23994,7 +24014,7 @@
       </c>
       <c r="B130" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C130" s="12">
         <v>124</v>
@@ -24033,19 +24053,19 @@
       </c>
       <c r="L130" cm="1">
         <f t="array" ref="L130">+INDEX(Hoja1!$B$2:$MO$7,3,$E130)</f>
-        <v>0</v>
+        <v>19497</v>
       </c>
       <c r="M130" cm="1">
         <f t="array" ref="M130">+INDEX(Hoja1!$B$2:$MO$7,4,$E130)</f>
-        <v>0</v>
+        <v>678</v>
       </c>
       <c r="N130" cm="1">
         <f t="array" ref="N130">+INDEX(Hoja1!$B$2:$MO$7,5,$E130)</f>
-        <v>0</v>
+        <v>936</v>
       </c>
       <c r="O130" cm="1">
         <f t="array" ref="O130">+INDEX(Hoja1!$B$2:$MO$7,6,$E130)</f>
-        <v>0</v>
+        <v>158</v>
       </c>
       <c r="P130" s="13">
         <f t="shared" si="60"/>
@@ -24065,19 +24085,19 @@
       </c>
       <c r="T130">
         <f t="shared" si="46"/>
-        <v>-19193</v>
+        <v>304</v>
       </c>
       <c r="U130">
         <f t="shared" si="47"/>
-        <v>-656</v>
+        <v>22</v>
       </c>
       <c r="V130">
         <f t="shared" si="48"/>
-        <v>-959</v>
+        <v>-23</v>
       </c>
       <c r="W130">
         <f t="shared" si="49"/>
-        <v>-160</v>
+        <v>-2</v>
       </c>
       <c r="X130">
         <f t="shared" si="50"/>
@@ -24089,19 +24109,19 @@
       </c>
       <c r="Z130">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0158391080081279</v>
       </c>
       <c r="AA130">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1.0335365853658536</v>
       </c>
       <c r="AB130">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>0.97601668404588116</v>
       </c>
       <c r="AC130">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="AD130">
         <f t="shared" si="34"/>
@@ -24113,45 +24133,45 @@
       </c>
       <c r="AF130">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>4687.905746573696</v>
       </c>
       <c r="AG130">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>163.01995672036549</v>
       </c>
       <c r="AH130">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>225.05409954315942</v>
       </c>
       <c r="AI130">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>37.989901418610245</v>
       </c>
       <c r="AJ130">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>21269</v>
       </c>
       <c r="AK130">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>5113.9697042558309</v>
       </c>
       <c r="AL130">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ129</f>
-        <v>-20968</v>
+        <v>301</v>
       </c>
       <c r="AM130">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ129,0)</f>
-        <v>-1</v>
+        <v>1.4355207935902328E-2</v>
       </c>
     </row>
     <row r="131" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A131" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B131" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C131" s="12">
         <v>125</v>
@@ -24166,139 +24186,139 @@
       </c>
       <c r="F131" cm="1">
         <f t="array" ref="F131">+INDEX(Hoja1!$B$2:$MO$7,1,E131)</f>
-        <v>0</v>
+        <v>164927</v>
       </c>
       <c r="G131">
         <f t="shared" si="41"/>
-        <v>-161466</v>
+        <v>3461</v>
       </c>
       <c r="H131" cm="1">
         <f t="array" ref="H131">+INDEX(Hoja1!$B$2:$MO$7,2,$E131)</f>
-        <v>0</v>
+        <v>116372</v>
       </c>
       <c r="I131">
         <f t="shared" si="42"/>
-        <v>-114238</v>
+        <v>2134</v>
       </c>
       <c r="J131">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>48555</v>
       </c>
       <c r="K131">
         <f t="shared" si="43"/>
-        <v>-47228</v>
+        <v>1327</v>
       </c>
       <c r="L131" cm="1">
         <f t="array" ref="L131">+INDEX(Hoja1!$B$2:$MO$7,3,$E131)</f>
-        <v>0</v>
+        <v>19867</v>
       </c>
       <c r="M131" cm="1">
         <f t="array" ref="M131">+INDEX(Hoja1!$B$2:$MO$7,4,$E131)</f>
-        <v>0</v>
+        <v>672</v>
       </c>
       <c r="N131" cm="1">
         <f t="array" ref="N131">+INDEX(Hoja1!$B$2:$MO$7,5,$E131)</f>
-        <v>0</v>
+        <v>987</v>
       </c>
       <c r="O131" cm="1">
         <f t="array" ref="O131">+INDEX(Hoja1!$B$2:$MO$7,6,$E131)</f>
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="P131" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.7055970217126365</v>
       </c>
       <c r="Q131" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.2944029782873635</v>
       </c>
       <c r="R131">
         <f t="shared" si="44"/>
-        <v>-164263</v>
+        <v>664</v>
       </c>
       <c r="S131">
         <f t="shared" si="45"/>
-        <v>-47228</v>
+        <v>1327</v>
       </c>
       <c r="T131">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>370</v>
       </c>
       <c r="U131">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="V131">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="W131">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X131">
         <f t="shared" si="50"/>
-        <v>-58.728280300321771</v>
+        <v>0.2373972112978191</v>
       </c>
       <c r="Y131">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.8097738629626494E-2</v>
       </c>
       <c r="Z131">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0189772785556752</v>
       </c>
       <c r="AA131">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>0.99115044247787609</v>
       </c>
       <c r="AB131">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0544871794871795</v>
       </c>
       <c r="AC131">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.0063291139240507</v>
       </c>
       <c r="AD131">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>39655.44602067805</v>
       </c>
       <c r="AE131">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>11674.681413801394</v>
       </c>
       <c r="AF131">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>4776.8694397691752</v>
       </c>
       <c r="AG131">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>161.57730223611446</v>
       </c>
       <c r="AH131">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>237.31666265929312</v>
       </c>
       <c r="AI131">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>38.230343832652082</v>
       </c>
       <c r="AJ131">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>21685</v>
       </c>
       <c r="AK131">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>5213.9937484972352</v>
       </c>
       <c r="AL131">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ130</f>
-        <v>0</v>
+        <v>416</v>
       </c>
       <c r="AM131">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ130,0)</f>
-        <v>0</v>
+        <v>1.9558982556772769E-2</v>
       </c>
     </row>
     <row r="132" spans="1:39" x14ac:dyDescent="0.2">
@@ -24327,7 +24347,7 @@
       </c>
       <c r="G132">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-164927</v>
       </c>
       <c r="H132" cm="1">
         <f t="array" ref="H132">+INDEX(Hoja1!$B$2:$MO$7,2,$E132)</f>
@@ -24335,7 +24355,7 @@
       </c>
       <c r="I132">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-116372</v>
       </c>
       <c r="J132">
         <f t="shared" si="33"/>
@@ -24343,7 +24363,7 @@
       </c>
       <c r="K132">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-48555</v>
       </c>
       <c r="L132" cm="1">
         <f t="array" ref="L132">+INDEX(Hoja1!$B$2:$MO$7,3,$E132)</f>
@@ -24371,35 +24391,35 @@
       </c>
       <c r="R132">
         <f t="shared" si="44"/>
-        <v>161466</v>
+        <v>-168388</v>
       </c>
       <c r="S132">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-48555</v>
       </c>
       <c r="T132">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-19867</v>
       </c>
       <c r="U132">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-672</v>
       </c>
       <c r="V132">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-987</v>
       </c>
       <c r="W132">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-159</v>
       </c>
       <c r="X132">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-48.652990465183471</v>
       </c>
       <c r="Y132">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z132">
         <f t="shared" si="52"/>
@@ -24451,11 +24471,11 @@
       </c>
       <c r="AL132">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ131</f>
-        <v>0</v>
+        <v>-21685</v>
       </c>
       <c r="AM132">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ131,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="133" spans="1:39" x14ac:dyDescent="0.2">
@@ -24528,7 +24548,7 @@
       </c>
       <c r="R133">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>164927</v>
       </c>
       <c r="S133">
         <f t="shared" si="45"/>
@@ -24552,7 +24572,7 @@
       </c>
       <c r="X133">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y133">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-15-2020 14-17-02
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1619" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0032DF64-1B51-0644-B935-833635DFB017}"/>
+  <xr:revisionPtr revIDLastSave="1635" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F5604B6A-D351-0B43-B1B6-82D5833A9F6F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="174">
   <si>
     <t>Columna1</t>
   </si>
@@ -552,6 +552,27 @@
   <si>
     <t>12-07-20</t>
   </si>
+  <si>
+    <t>12-07-23</t>
+  </si>
+  <si>
+    <t>12-07-24</t>
+  </si>
+  <si>
+    <t>12-07-25</t>
+  </si>
+  <si>
+    <t>12-07-26</t>
+  </si>
+  <si>
+    <t>12-07-27</t>
+  </si>
+  <si>
+    <t>13-07-20</t>
+  </si>
+  <si>
+    <t>14-07-20</t>
+  </si>
 </sst>
 </file>
 
@@ -674,7 +695,28 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="48">
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -920,9 +962,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:DV7" totalsRowShown="0">
-  <autoFilter ref="A1:DV7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
-  <tableColumns count="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:EC7" totalsRowShown="0">
+  <autoFilter ref="A1:EC7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
+  <tableColumns count="133">
     <tableColumn id="76" xr3:uid="{CA01250B-8685-4250-AAEF-D6E482663B6F}" name="Columna1"/>
     <tableColumn id="77" xr3:uid="{BC38B0B2-3229-42F8-9C9A-52EE74902839}" name="10-03-2020"/>
     <tableColumn id="78" xr3:uid="{4BB74E2E-62F3-4EED-8537-96C80CD1ED37}" name="11-03-2020"/>
@@ -1016,59 +1058,66 @@
     <tableColumn id="4" xr3:uid="{2FE879E2-2128-42AE-A0E3-647EE2D0C94F}" name="07-06-2020"/>
     <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="08-06-2020"/>
     <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-2020"/>
-    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="40"/>
-    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="39"/>
-    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="38"/>
-    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="37"/>
-    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="36"/>
-    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="35"/>
-    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="34"/>
-    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="33"/>
-    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="32"/>
-    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="31"/>
-    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="30"/>
-    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="29"/>
-    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="28"/>
-    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="27"/>
-    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="26"/>
-    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="25"/>
-    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="24"/>
-    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="23"/>
-    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="22"/>
-    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="21"/>
-    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="20"/>
-    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="19"/>
-    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="18"/>
-    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="17"/>
-    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="16"/>
-    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="15"/>
-    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="14"/>
-    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="13"/>
-    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="12"/>
-    <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="11"/>
-    <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="10-07-20" dataDxfId="10"/>
-    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="11-07-20" dataDxfId="9"/>
-    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="12-07-20" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="47"/>
+    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="46"/>
+    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="45"/>
+    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="44"/>
+    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="43"/>
+    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="42"/>
+    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="41"/>
+    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="40"/>
+    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="39"/>
+    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="38"/>
+    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="37"/>
+    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="36"/>
+    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="35"/>
+    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="34"/>
+    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="33"/>
+    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="32"/>
+    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="31"/>
+    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="30"/>
+    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="29"/>
+    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="28"/>
+    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="27"/>
+    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="26"/>
+    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="25"/>
+    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="24"/>
+    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="23"/>
+    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="22"/>
+    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="21"/>
+    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="20"/>
+    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="19"/>
+    <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="18"/>
+    <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="10-07-20" dataDxfId="17"/>
+    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="11-07-20" dataDxfId="16"/>
+    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="12-07-20" dataDxfId="15"/>
+    <tableColumn id="127" xr3:uid="{2B284A50-3213-EF46-904E-73679622D22C}" name="13-07-20" dataDxfId="6"/>
+    <tableColumn id="128" xr3:uid="{30C66AA6-47A6-FB40-A335-1BA9A696E85B}" name="14-07-20" dataDxfId="5"/>
+    <tableColumn id="129" xr3:uid="{041D18C8-807A-0949-898D-C4880EDA94DD}" name="12-07-23" dataDxfId="4"/>
+    <tableColumn id="130" xr3:uid="{61B56DA5-913C-EF4F-B703-9A52B436E7DD}" name="12-07-24" dataDxfId="3"/>
+    <tableColumn id="131" xr3:uid="{877B5AA5-D97A-8D40-B352-6FFA59645351}" name="12-07-25" dataDxfId="2"/>
+    <tableColumn id="132" xr3:uid="{3FADF8C3-57FC-5D47-913A-C0C36C8E59FE}" name="12-07-26" dataDxfId="1"/>
+    <tableColumn id="133" xr3:uid="{1226D8E9-4582-2342-A7CC-4D09D093B768}" name="12-07-27" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="13">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="12">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="10">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="9">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -1101,10 +1150,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="1">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="8">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="7">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1471,11 +1520,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B32E72-8F4B-408A-9B01-FAD2807C0C88}">
-  <dimension ref="A1:DV52"/>
+  <dimension ref="A1:EC52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DT1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DV1" sqref="DV1:DV7"/>
+      <pane xSplit="1" topLeftCell="DU1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DX6" sqref="DX6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1492,7 +1541,7 @@
     <col min="116" max="118" width="11.43359375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:126" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:133" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1871,8 +1920,29 @@
       <c r="DV1" s="1" t="s">
         <v>164</v>
       </c>
+      <c r="DW1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="DX1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="DY1" t="s">
+        <v>165</v>
+      </c>
+      <c r="DZ1" t="s">
+        <v>166</v>
+      </c>
+      <c r="EA1" t="s">
+        <v>167</v>
+      </c>
+      <c r="EB1" t="s">
+        <v>168</v>
+      </c>
+      <c r="EC1" t="s">
+        <v>169</v>
+      </c>
     </row>
-    <row r="2" spans="1:126" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:133" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2251,8 +2321,19 @@
       <c r="DV2" s="8">
         <v>164927</v>
       </c>
+      <c r="DW2" s="8">
+        <v>168517</v>
+      </c>
+      <c r="DX2" s="8">
+        <v>171116</v>
+      </c>
+      <c r="DY2" s="8"/>
+      <c r="DZ2" s="8"/>
+      <c r="EA2" s="8"/>
+      <c r="EB2" s="8"/>
+      <c r="EC2" s="8"/>
     </row>
-    <row r="3" spans="1:126" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:133" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -2631,8 +2712,19 @@
       <c r="DV3" s="8">
         <v>116372</v>
       </c>
+      <c r="DW3" s="8">
+        <v>118412</v>
+      </c>
+      <c r="DX3" s="8">
+        <v>120068</v>
+      </c>
+      <c r="DY3" s="8"/>
+      <c r="DZ3" s="8"/>
+      <c r="EA3" s="8"/>
+      <c r="EB3" s="8"/>
+      <c r="EC3" s="8"/>
     </row>
-    <row r="4" spans="1:126" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:133" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -3011,8 +3103,19 @@
       <c r="DV4" s="8">
         <v>19867</v>
       </c>
+      <c r="DW4" s="8">
+        <v>20500</v>
+      </c>
+      <c r="DX4" s="8">
+        <v>20639</v>
+      </c>
+      <c r="DY4" s="8"/>
+      <c r="DZ4" s="8"/>
+      <c r="EA4" s="8"/>
+      <c r="EB4" s="8"/>
+      <c r="EC4" s="8"/>
     </row>
-    <row r="5" spans="1:126" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:133" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -3300,8 +3403,19 @@
       <c r="DV5" s="8">
         <v>672</v>
       </c>
+      <c r="DW5" s="8">
+        <v>658</v>
+      </c>
+      <c r="DX5" s="8">
+        <v>658</v>
+      </c>
+      <c r="DY5" s="8"/>
+      <c r="DZ5" s="8"/>
+      <c r="EA5" s="8"/>
+      <c r="EB5" s="8"/>
+      <c r="EC5" s="8"/>
     </row>
-    <row r="6" spans="1:126" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:133" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -3676,8 +3790,17 @@
       <c r="DV6" s="8">
         <v>987</v>
       </c>
+      <c r="DW6" s="8">
+        <v>1005</v>
+      </c>
+      <c r="DX6" s="8"/>
+      <c r="DY6" s="8"/>
+      <c r="DZ6" s="8"/>
+      <c r="EA6" s="8"/>
+      <c r="EB6" s="8"/>
+      <c r="EC6" s="8"/>
     </row>
-    <row r="7" spans="1:126" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:133" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -4012,7 +4135,7 @@
       <c r="DH7" s="15">
         <v>140</v>
       </c>
-      <c r="DI7" s="8">
+      <c r="DI7" s="15">
         <v>147</v>
       </c>
       <c r="DJ7" s="8">
@@ -4054,8 +4177,17 @@
       <c r="DV7" s="8">
         <v>159</v>
       </c>
+      <c r="DW7" s="8">
+        <v>159</v>
+      </c>
+      <c r="DX7" s="8"/>
+      <c r="DY7" s="8"/>
+      <c r="DZ7" s="8"/>
+      <c r="EA7" s="8"/>
+      <c r="EB7" s="8"/>
+      <c r="EC7" s="8"/>
     </row>
-    <row r="8" spans="1:126" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:133" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4151,28 +4283,28 @@
       <c r="DI8" s="15"/>
       <c r="DO8" s="8"/>
     </row>
-    <row r="9" spans="1:126" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:133" x14ac:dyDescent="0.2">
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:126" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:133" x14ac:dyDescent="0.2">
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:126" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:133" x14ac:dyDescent="0.2">
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:126" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:133" x14ac:dyDescent="0.2">
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:126" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:133" x14ac:dyDescent="0.2">
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:126" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:133" x14ac:dyDescent="0.2">
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:126" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:133" x14ac:dyDescent="0.2">
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:126" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:133" x14ac:dyDescent="0.2">
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
@@ -4639,7 +4771,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44024</v>
+        <v>44026</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -24171,7 +24303,7 @@
       </c>
       <c r="B131" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C131" s="12">
         <v>125</v>
@@ -24324,7 +24456,7 @@
     <row r="132" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A132" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B132" s="12" t="str">
         <f t="shared" si="57"/>
@@ -24343,149 +24475,149 @@
       </c>
       <c r="F132" cm="1">
         <f t="array" ref="F132">+INDEX(Hoja1!$B$2:$MO$7,1,E132)</f>
-        <v>0</v>
+        <v>168517</v>
       </c>
       <c r="G132">
         <f t="shared" si="41"/>
-        <v>-164927</v>
+        <v>3590</v>
       </c>
       <c r="H132" cm="1">
         <f t="array" ref="H132">+INDEX(Hoja1!$B$2:$MO$7,2,$E132)</f>
-        <v>0</v>
+        <v>118412</v>
       </c>
       <c r="I132">
         <f t="shared" si="42"/>
-        <v>-116372</v>
+        <v>2040</v>
       </c>
       <c r="J132">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>50105</v>
       </c>
       <c r="K132">
         <f t="shared" si="43"/>
-        <v>-48555</v>
+        <v>1550</v>
       </c>
       <c r="L132" cm="1">
         <f t="array" ref="L132">+INDEX(Hoja1!$B$2:$MO$7,3,$E132)</f>
-        <v>0</v>
+        <v>20500</v>
       </c>
       <c r="M132" cm="1">
         <f t="array" ref="M132">+INDEX(Hoja1!$B$2:$MO$7,4,$E132)</f>
-        <v>0</v>
+        <v>658</v>
       </c>
       <c r="N132" cm="1">
         <f t="array" ref="N132">+INDEX(Hoja1!$B$2:$MO$7,5,$E132)</f>
-        <v>0</v>
+        <v>1005</v>
       </c>
       <c r="O132" cm="1">
         <f t="array" ref="O132">+INDEX(Hoja1!$B$2:$MO$7,6,$E132)</f>
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="P132" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.7026709471447985</v>
       </c>
       <c r="Q132" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.29732905285520156</v>
       </c>
       <c r="R132">
         <f t="shared" si="44"/>
-        <v>-168388</v>
+        <v>129</v>
       </c>
       <c r="S132">
         <f t="shared" si="45"/>
-        <v>-48555</v>
+        <v>1550</v>
       </c>
       <c r="T132">
         <f t="shared" si="46"/>
-        <v>-19867</v>
+        <v>633</v>
       </c>
       <c r="U132">
         <f t="shared" si="47"/>
-        <v>-672</v>
+        <v>-14</v>
       </c>
       <c r="V132">
         <f t="shared" si="48"/>
-        <v>-987</v>
+        <v>18</v>
       </c>
       <c r="W132">
         <f t="shared" si="49"/>
-        <v>-159</v>
+        <v>0</v>
       </c>
       <c r="X132">
         <f t="shared" si="50"/>
-        <v>-48.652990465183471</v>
+        <v>3.7272464605605314E-2</v>
       </c>
       <c r="Y132">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>3.1922562043043973E-2</v>
       </c>
       <c r="Z132">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0318618815120553</v>
       </c>
       <c r="AA132">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>0.97916666666666663</v>
       </c>
       <c r="AB132">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0182370820668694</v>
       </c>
       <c r="AC132">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD132">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>40518.634287088244</v>
       </c>
       <c r="AE132">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>12047.367155566242</v>
       </c>
       <c r="AF132">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>4929.0694878576587</v>
       </c>
       <c r="AG132">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>158.21110843952874</v>
       </c>
       <c r="AH132">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>241.64462611204618</v>
       </c>
       <c r="AI132">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>38.230343832652082</v>
       </c>
       <c r="AJ132">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>22322</v>
       </c>
       <c r="AK132">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>5367.155566241885</v>
       </c>
       <c r="AL132">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ131</f>
-        <v>-21685</v>
+        <v>637</v>
       </c>
       <c r="AM132">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ131,0)</f>
-        <v>-1</v>
+        <v>2.9375144108830988E-2</v>
       </c>
     </row>
     <row r="133" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A133" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B133" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C133" s="12">
         <v>127</v>
@@ -24500,35 +24632,35 @@
       </c>
       <c r="F133" cm="1">
         <f t="array" ref="F133">+INDEX(Hoja1!$B$2:$MO$7,1,E133)</f>
-        <v>0</v>
+        <v>171116</v>
       </c>
       <c r="G133">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>2599</v>
       </c>
       <c r="H133" cm="1">
         <f t="array" ref="H133">+INDEX(Hoja1!$B$2:$MO$7,2,$E133)</f>
-        <v>0</v>
+        <v>120068</v>
       </c>
       <c r="I133">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>1656</v>
       </c>
       <c r="J133">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>51048</v>
       </c>
       <c r="K133">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>943</v>
       </c>
       <c r="L133" cm="1">
         <f t="array" ref="L133">+INDEX(Hoja1!$B$2:$MO$7,3,$E133)</f>
-        <v>0</v>
+        <v>20639</v>
       </c>
       <c r="M133" cm="1">
         <f t="array" ref="M133">+INDEX(Hoja1!$B$2:$MO$7,4,$E133)</f>
-        <v>0</v>
+        <v>658</v>
       </c>
       <c r="N133" cm="1">
         <f t="array" ref="N133">+INDEX(Hoja1!$B$2:$MO$7,5,$E133)</f>
@@ -24540,23 +24672,23 @@
       </c>
       <c r="P133" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.70167605600878935</v>
       </c>
       <c r="Q133" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.29832394399121065</v>
       </c>
       <c r="R133">
         <f t="shared" si="44"/>
-        <v>164927</v>
+        <v>-991</v>
       </c>
       <c r="S133">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>943</v>
       </c>
       <c r="T133">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="U133">
         <f t="shared" si="47"/>
@@ -24564,27 +24696,27 @@
       </c>
       <c r="V133">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-1005</v>
       </c>
       <c r="W133">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-159</v>
       </c>
       <c r="X133">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-0.27604456824512535</v>
       </c>
       <c r="Y133">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1.8820476998303564E-2</v>
       </c>
       <c r="Z133">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0067804878048781</v>
       </c>
       <c r="AA133">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB133">
         <f t="shared" si="54"/>
@@ -24596,19 +24728,19 @@
       </c>
       <c r="AD133">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>41143.544121182982</v>
       </c>
       <c r="AE133">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>12274.104352007695</v>
       </c>
       <c r="AF133">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>4962.4909834094733</v>
       </c>
       <c r="AG133">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>158.21110843952874</v>
       </c>
       <c r="AH133">
         <f t="shared" si="38"/>
@@ -24620,19 +24752,19 @@
       </c>
       <c r="AJ133">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>21297</v>
       </c>
       <c r="AK133">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>5120.7020918490025</v>
       </c>
       <c r="AL133">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ132</f>
-        <v>0</v>
+        <v>-1025</v>
       </c>
       <c r="AM133">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ132,0)</f>
-        <v>0</v>
+        <v>-4.591882447809336E-2</v>
       </c>
     </row>
     <row r="134" spans="1:39" x14ac:dyDescent="0.2">
@@ -24661,7 +24793,7 @@
       </c>
       <c r="G134">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-171116</v>
       </c>
       <c r="H134" cm="1">
         <f t="array" ref="H134">+INDEX(Hoja1!$B$2:$MO$7,2,$E134)</f>
@@ -24669,7 +24801,7 @@
       </c>
       <c r="I134">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-120068</v>
       </c>
       <c r="J134">
         <f t="shared" si="33"/>
@@ -24677,7 +24809,7 @@
       </c>
       <c r="K134">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-51048</v>
       </c>
       <c r="L134" cm="1">
         <f t="array" ref="L134">+INDEX(Hoja1!$B$2:$MO$7,3,$E134)</f>
@@ -24705,19 +24837,19 @@
       </c>
       <c r="R134">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>-173715</v>
       </c>
       <c r="S134">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-51048</v>
       </c>
       <c r="T134">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-20639</v>
       </c>
       <c r="U134">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-658</v>
       </c>
       <c r="V134">
         <f t="shared" si="48"/>
@@ -24729,11 +24861,11 @@
       </c>
       <c r="X134">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-66.839168911119657</v>
       </c>
       <c r="Y134">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z134">
         <f t="shared" si="52"/>
@@ -24785,11 +24917,11 @@
       </c>
       <c r="AL134">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ133</f>
-        <v>0</v>
+        <v>-21297</v>
       </c>
       <c r="AM134">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ133,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="135" spans="1:39" x14ac:dyDescent="0.2">
@@ -24862,7 +24994,7 @@
       </c>
       <c r="R135">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>171116</v>
       </c>
       <c r="S135">
         <f t="shared" si="45"/>
@@ -24886,7 +25018,7 @@
       </c>
       <c r="X135">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y135">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-17-2020 02-24-43
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1635" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F5604B6A-D351-0B43-B1B6-82D5833A9F6F}"/>
+  <xr:revisionPtr revIDLastSave="1644" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3F538821-4AC4-4345-AF4F-285E15368F9D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="173">
   <si>
     <t>Columna1</t>
   </si>
@@ -553,9 +553,6 @@
     <t>12-07-20</t>
   </si>
   <si>
-    <t>12-07-23</t>
-  </si>
-  <si>
     <t>12-07-24</t>
   </si>
   <si>
@@ -572,6 +569,9 @@
   </si>
   <si>
     <t>14-07-20</t>
+  </si>
+  <si>
+    <t>15-07-20</t>
   </si>
 </sst>
 </file>
@@ -697,27 +697,6 @@
   </cellStyles>
   <dxfs count="48">
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -836,6 +815,27 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
@@ -1091,33 +1091,33 @@
     <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="10-07-20" dataDxfId="17"/>
     <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="11-07-20" dataDxfId="16"/>
     <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="12-07-20" dataDxfId="15"/>
-    <tableColumn id="127" xr3:uid="{2B284A50-3213-EF46-904E-73679622D22C}" name="13-07-20" dataDxfId="6"/>
-    <tableColumn id="128" xr3:uid="{30C66AA6-47A6-FB40-A335-1BA9A696E85B}" name="14-07-20" dataDxfId="5"/>
-    <tableColumn id="129" xr3:uid="{041D18C8-807A-0949-898D-C4880EDA94DD}" name="12-07-23" dataDxfId="4"/>
-    <tableColumn id="130" xr3:uid="{61B56DA5-913C-EF4F-B703-9A52B436E7DD}" name="12-07-24" dataDxfId="3"/>
-    <tableColumn id="131" xr3:uid="{877B5AA5-D97A-8D40-B352-6FFA59645351}" name="12-07-25" dataDxfId="2"/>
-    <tableColumn id="132" xr3:uid="{3FADF8C3-57FC-5D47-913A-C0C36C8E59FE}" name="12-07-26" dataDxfId="1"/>
-    <tableColumn id="133" xr3:uid="{1226D8E9-4582-2342-A7CC-4D09D093B768}" name="12-07-27" dataDxfId="0"/>
+    <tableColumn id="127" xr3:uid="{2B284A50-3213-EF46-904E-73679622D22C}" name="13-07-20" dataDxfId="14"/>
+    <tableColumn id="128" xr3:uid="{30C66AA6-47A6-FB40-A335-1BA9A696E85B}" name="14-07-20" dataDxfId="13"/>
+    <tableColumn id="129" xr3:uid="{041D18C8-807A-0949-898D-C4880EDA94DD}" name="15-07-20" dataDxfId="12"/>
+    <tableColumn id="130" xr3:uid="{61B56DA5-913C-EF4F-B703-9A52B436E7DD}" name="12-07-24" dataDxfId="11"/>
+    <tableColumn id="131" xr3:uid="{877B5AA5-D97A-8D40-B352-6FFA59645351}" name="12-07-25" dataDxfId="10"/>
+    <tableColumn id="132" xr3:uid="{3FADF8C3-57FC-5D47-913A-C0C36C8E59FE}" name="12-07-26" dataDxfId="9"/>
+    <tableColumn id="133" xr3:uid="{1226D8E9-4582-2342-A7CC-4D09D093B768}" name="12-07-27" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="6">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="12">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="5">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="10">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="3">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="9">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="2">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -1150,10 +1150,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="8">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="1">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="7">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="0">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1523,8 +1523,9 @@
   <dimension ref="A1:EC52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DU1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DX6" sqref="DX6"/>
+      <pane xSplit="1" topLeftCell="DW1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="DY1" sqref="DY1:DY7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1921,25 +1922,25 @@
         <v>164</v>
       </c>
       <c r="DW1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="DX1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="DX1" s="1" t="s">
+      <c r="DY1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="DY1" t="s">
+      <c r="DZ1" t="s">
         <v>165</v>
       </c>
-      <c r="DZ1" t="s">
+      <c r="EA1" t="s">
         <v>166</v>
       </c>
-      <c r="EA1" t="s">
+      <c r="EB1" t="s">
         <v>167</v>
       </c>
-      <c r="EB1" t="s">
+      <c r="EC1" t="s">
         <v>168</v>
-      </c>
-      <c r="EC1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:133" x14ac:dyDescent="0.2">
@@ -2327,7 +2328,9 @@
       <c r="DX2" s="8">
         <v>171116</v>
       </c>
-      <c r="DY2" s="8"/>
+      <c r="DY2" s="8">
+        <v>174345</v>
+      </c>
       <c r="DZ2" s="8"/>
       <c r="EA2" s="8"/>
       <c r="EB2" s="8"/>
@@ -2718,7 +2721,9 @@
       <c r="DX3" s="8">
         <v>120068</v>
       </c>
-      <c r="DY3" s="8"/>
+      <c r="DY3" s="8">
+        <v>122190</v>
+      </c>
       <c r="DZ3" s="8"/>
       <c r="EA3" s="8"/>
       <c r="EB3" s="8"/>
@@ -3109,7 +3114,9 @@
       <c r="DX4" s="8">
         <v>20639</v>
       </c>
-      <c r="DY4" s="8"/>
+      <c r="DY4" s="8">
+        <v>21009</v>
+      </c>
       <c r="DZ4" s="8"/>
       <c r="EA4" s="8"/>
       <c r="EB4" s="8"/>
@@ -3409,7 +3416,9 @@
       <c r="DX5" s="8">
         <v>658</v>
       </c>
-      <c r="DY5" s="8"/>
+      <c r="DY5" s="8">
+        <v>616</v>
+      </c>
       <c r="DZ5" s="8"/>
       <c r="EA5" s="8"/>
       <c r="EB5" s="8"/>
@@ -3793,8 +3802,12 @@
       <c r="DW6" s="8">
         <v>1005</v>
       </c>
-      <c r="DX6" s="8"/>
-      <c r="DY6" s="8"/>
+      <c r="DX6" s="8">
+        <v>1015</v>
+      </c>
+      <c r="DY6" s="8">
+        <v>1056</v>
+      </c>
       <c r="DZ6" s="8"/>
       <c r="EA6" s="8"/>
       <c r="EB6" s="8"/>
@@ -4180,8 +4193,12 @@
       <c r="DW7" s="8">
         <v>159</v>
       </c>
-      <c r="DX7" s="8"/>
-      <c r="DY7" s="8"/>
+      <c r="DX7" s="8">
+        <v>157</v>
+      </c>
+      <c r="DY7" s="8">
+        <v>163</v>
+      </c>
       <c r="DZ7" s="8"/>
       <c r="EA7" s="8"/>
       <c r="EB7" s="8"/>
@@ -4771,7 +4788,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -24617,7 +24634,7 @@
       </c>
       <c r="B133" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C133" s="12">
         <v>127</v>
@@ -24664,11 +24681,11 @@
       </c>
       <c r="N133" cm="1">
         <f t="array" ref="N133">+INDEX(Hoja1!$B$2:$MO$7,5,$E133)</f>
-        <v>0</v>
+        <v>1015</v>
       </c>
       <c r="O133" cm="1">
         <f t="array" ref="O133">+INDEX(Hoja1!$B$2:$MO$7,6,$E133)</f>
-        <v>0</v>
+        <v>157</v>
       </c>
       <c r="P133" s="13">
         <f t="shared" si="60"/>
@@ -24696,11 +24713,11 @@
       </c>
       <c r="V133">
         <f t="shared" si="48"/>
-        <v>-1005</v>
+        <v>10</v>
       </c>
       <c r="W133">
         <f t="shared" si="49"/>
-        <v>-159</v>
+        <v>-2</v>
       </c>
       <c r="X133">
         <f t="shared" si="50"/>
@@ -24720,11 +24737,11 @@
       </c>
       <c r="AB133">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0099502487562189</v>
       </c>
       <c r="AC133">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>0.98742138364779874</v>
       </c>
       <c r="AD133">
         <f t="shared" si="34"/>
@@ -24744,37 +24761,37 @@
       </c>
       <c r="AH133">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>244.04905025246455</v>
       </c>
       <c r="AI133">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>37.749459004568408</v>
       </c>
       <c r="AJ133">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>21297</v>
+        <v>22469</v>
       </c>
       <c r="AK133">
         <f t="shared" si="40"/>
-        <v>5120.7020918490025</v>
+        <v>5402.500601106035</v>
       </c>
       <c r="AL133">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ132</f>
-        <v>-1025</v>
+        <v>147</v>
       </c>
       <c r="AM133">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ132,0)</f>
-        <v>-4.591882447809336E-2</v>
+        <v>6.5854314129558285E-3</v>
       </c>
     </row>
     <row r="134" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A134" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B134" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C134" s="12">
         <v>128</v>
@@ -24789,139 +24806,139 @@
       </c>
       <c r="F134" cm="1">
         <f t="array" ref="F134">+INDEX(Hoja1!$B$2:$MO$7,1,E134)</f>
-        <v>0</v>
+        <v>174345</v>
       </c>
       <c r="G134">
         <f t="shared" si="41"/>
-        <v>-171116</v>
+        <v>3229</v>
       </c>
       <c r="H134" cm="1">
         <f t="array" ref="H134">+INDEX(Hoja1!$B$2:$MO$7,2,$E134)</f>
-        <v>0</v>
+        <v>122190</v>
       </c>
       <c r="I134">
         <f t="shared" si="42"/>
-        <v>-120068</v>
+        <v>2122</v>
       </c>
       <c r="J134">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>52155</v>
       </c>
       <c r="K134">
         <f t="shared" si="43"/>
-        <v>-51048</v>
+        <v>1107</v>
       </c>
       <c r="L134" cm="1">
         <f t="array" ref="L134">+INDEX(Hoja1!$B$2:$MO$7,3,$E134)</f>
-        <v>0</v>
+        <v>21009</v>
       </c>
       <c r="M134" cm="1">
         <f t="array" ref="M134">+INDEX(Hoja1!$B$2:$MO$7,4,$E134)</f>
-        <v>0</v>
+        <v>616</v>
       </c>
       <c r="N134" cm="1">
         <f t="array" ref="N134">+INDEX(Hoja1!$B$2:$MO$7,5,$E134)</f>
-        <v>0</v>
+        <v>1056</v>
       </c>
       <c r="O134" cm="1">
         <f t="array" ref="O134">+INDEX(Hoja1!$B$2:$MO$7,6,$E134)</f>
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="P134" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.70085175944248468</v>
       </c>
       <c r="Q134" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.29914824055751527</v>
       </c>
       <c r="R134">
         <f t="shared" si="44"/>
-        <v>-173715</v>
+        <v>630</v>
       </c>
       <c r="S134">
         <f t="shared" si="45"/>
-        <v>-51048</v>
+        <v>1107</v>
       </c>
       <c r="T134">
         <f t="shared" si="46"/>
-        <v>-20639</v>
+        <v>370</v>
       </c>
       <c r="U134">
         <f t="shared" si="47"/>
-        <v>-658</v>
+        <v>-42</v>
       </c>
       <c r="V134">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="W134">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="X134">
         <f t="shared" si="50"/>
-        <v>-66.839168911119657</v>
+        <v>0.24240092343208927</v>
       </c>
       <c r="Y134">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.1685472496473908E-2</v>
       </c>
       <c r="Z134">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0179272251562577</v>
       </c>
       <c r="AA134">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>0.93617021276595747</v>
       </c>
       <c r="AB134">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0403940886699508</v>
       </c>
       <c r="AC134">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.0382165605095541</v>
       </c>
       <c r="AD134">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>41919.932676124074</v>
       </c>
       <c r="AE134">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>12540.274104352009</v>
       </c>
       <c r="AF134">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>5051.4546766049534</v>
       </c>
       <c r="AG134">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>148.11252704977159</v>
       </c>
       <c r="AH134">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>253.90718922817987</v>
       </c>
       <c r="AI134">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>39.19211348881943</v>
       </c>
       <c r="AJ134">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>22844</v>
       </c>
       <c r="AK134">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>5492.6665063717246</v>
       </c>
       <c r="AL134">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ133</f>
-        <v>-21297</v>
+        <v>375</v>
       </c>
       <c r="AM134">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ133,0)</f>
-        <v>-1</v>
+        <v>1.6689661311139792E-2</v>
       </c>
     </row>
     <row r="135" spans="1:39" x14ac:dyDescent="0.2">
@@ -24950,7 +24967,7 @@
       </c>
       <c r="G135">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-174345</v>
       </c>
       <c r="H135" cm="1">
         <f t="array" ref="H135">+INDEX(Hoja1!$B$2:$MO$7,2,$E135)</f>
@@ -24958,7 +24975,7 @@
       </c>
       <c r="I135">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>-122190</v>
       </c>
       <c r="J135">
         <f t="shared" si="33"/>
@@ -24966,7 +24983,7 @@
       </c>
       <c r="K135">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>-52155</v>
       </c>
       <c r="L135" cm="1">
         <f t="array" ref="L135">+INDEX(Hoja1!$B$2:$MO$7,3,$E135)</f>
@@ -24994,35 +25011,35 @@
       </c>
       <c r="R135">
         <f t="shared" si="44"/>
-        <v>171116</v>
+        <v>-177574</v>
       </c>
       <c r="S135">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>-52155</v>
       </c>
       <c r="T135">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-21009</v>
       </c>
       <c r="U135">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-616</v>
       </c>
       <c r="V135">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>-1056</v>
       </c>
       <c r="W135">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>-163</v>
       </c>
       <c r="X135">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-54.99349643852586</v>
       </c>
       <c r="Y135">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z135">
         <f t="shared" si="52"/>
@@ -25074,11 +25091,11 @@
       </c>
       <c r="AL135">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ134</f>
-        <v>0</v>
+        <v>-22844</v>
       </c>
       <c r="AM135">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ134,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="136" spans="1:39" x14ac:dyDescent="0.2">
@@ -25151,7 +25168,7 @@
       </c>
       <c r="R136">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>174345</v>
       </c>
       <c r="S136">
         <f t="shared" si="45"/>
@@ -25175,7 +25192,7 @@
       </c>
       <c r="X136">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y136">
         <f t="shared" si="51"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-18-2020 22-31-22
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1644" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3F538821-4AC4-4345-AF4F-285E15368F9D}"/>
+  <xr:revisionPtr revIDLastSave="1658" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6F61A3E2-0346-9148-93F6-8C4433DC0593}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="174">
   <si>
     <t>Columna1</t>
   </si>
@@ -553,12 +553,6 @@
     <t>12-07-20</t>
   </si>
   <si>
-    <t>12-07-24</t>
-  </si>
-  <si>
-    <t>12-07-25</t>
-  </si>
-  <si>
     <t>12-07-26</t>
   </si>
   <si>
@@ -572,6 +566,12 @@
   </si>
   <si>
     <t>15-07-20</t>
+  </si>
+  <si>
+    <t>16-07-20</t>
+  </si>
+  <si>
+    <t>17-07-20</t>
   </si>
 </sst>
 </file>
@@ -1094,8 +1094,8 @@
     <tableColumn id="127" xr3:uid="{2B284A50-3213-EF46-904E-73679622D22C}" name="13-07-20" dataDxfId="14"/>
     <tableColumn id="128" xr3:uid="{30C66AA6-47A6-FB40-A335-1BA9A696E85B}" name="14-07-20" dataDxfId="13"/>
     <tableColumn id="129" xr3:uid="{041D18C8-807A-0949-898D-C4880EDA94DD}" name="15-07-20" dataDxfId="12"/>
-    <tableColumn id="130" xr3:uid="{61B56DA5-913C-EF4F-B703-9A52B436E7DD}" name="12-07-24" dataDxfId="11"/>
-    <tableColumn id="131" xr3:uid="{877B5AA5-D97A-8D40-B352-6FFA59645351}" name="12-07-25" dataDxfId="10"/>
+    <tableColumn id="130" xr3:uid="{61B56DA5-913C-EF4F-B703-9A52B436E7DD}" name="16-07-20" dataDxfId="11"/>
+    <tableColumn id="131" xr3:uid="{877B5AA5-D97A-8D40-B352-6FFA59645351}" name="17-07-20" dataDxfId="10"/>
     <tableColumn id="132" xr3:uid="{3FADF8C3-57FC-5D47-913A-C0C36C8E59FE}" name="12-07-26" dataDxfId="9"/>
     <tableColumn id="133" xr3:uid="{1226D8E9-4582-2342-A7CC-4D09D093B768}" name="12-07-27" dataDxfId="8"/>
   </tableColumns>
@@ -1523,9 +1523,9 @@
   <dimension ref="A1:EC52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DW1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="DY1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="DY1" sqref="DY1:DY7"/>
+      <selection pane="topRight" activeCell="EA7" sqref="EA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1922,25 +1922,25 @@
         <v>164</v>
       </c>
       <c r="DW1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="DX1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="DY1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="DX1" s="1" t="s">
+      <c r="DZ1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="DY1" s="1" t="s">
+      <c r="EA1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="DZ1" t="s">
+      <c r="EB1" t="s">
         <v>165</v>
       </c>
-      <c r="EA1" t="s">
+      <c r="EC1" t="s">
         <v>166</v>
-      </c>
-      <c r="EB1" t="s">
-        <v>167</v>
-      </c>
-      <c r="EC1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:133" x14ac:dyDescent="0.2">
@@ -2331,8 +2331,12 @@
       <c r="DY2" s="8">
         <v>174345</v>
       </c>
-      <c r="DZ2" s="8"/>
-      <c r="EA2" s="8"/>
+      <c r="DZ2" s="8">
+        <v>177843</v>
+      </c>
+      <c r="EA2" s="8">
+        <v>180814</v>
+      </c>
       <c r="EB2" s="8"/>
       <c r="EC2" s="8"/>
     </row>
@@ -2724,8 +2728,12 @@
       <c r="DY3" s="8">
         <v>122190</v>
       </c>
-      <c r="DZ3" s="8"/>
-      <c r="EA3" s="8"/>
+      <c r="DZ3" s="8">
+        <v>124504</v>
+      </c>
+      <c r="EA3" s="8">
+        <v>126411</v>
+      </c>
       <c r="EB3" s="8"/>
       <c r="EC3" s="8"/>
     </row>
@@ -3117,8 +3125,12 @@
       <c r="DY4" s="8">
         <v>21009</v>
       </c>
-      <c r="DZ4" s="8"/>
-      <c r="EA4" s="8"/>
+      <c r="DZ4" s="8">
+        <v>21665</v>
+      </c>
+      <c r="EA4" s="8">
+        <v>21946</v>
+      </c>
       <c r="EB4" s="8"/>
       <c r="EC4" s="8"/>
     </row>
@@ -3419,8 +3431,12 @@
       <c r="DY5" s="8">
         <v>616</v>
       </c>
-      <c r="DZ5" s="8"/>
-      <c r="EA5" s="8"/>
+      <c r="DZ5" s="8">
+        <v>622</v>
+      </c>
+      <c r="EA5" s="8">
+        <v>620</v>
+      </c>
       <c r="EB5" s="8"/>
       <c r="EC5" s="8"/>
     </row>
@@ -3808,8 +3824,12 @@
       <c r="DY6" s="8">
         <v>1056</v>
       </c>
-      <c r="DZ6" s="8"/>
-      <c r="EA6" s="8"/>
+      <c r="DZ6" s="8">
+        <v>1078</v>
+      </c>
+      <c r="EA6" s="8">
+        <v>1117</v>
+      </c>
       <c r="EB6" s="8"/>
       <c r="EC6" s="8"/>
     </row>
@@ -4199,8 +4219,12 @@
       <c r="DY7" s="8">
         <v>163</v>
       </c>
-      <c r="DZ7" s="8"/>
-      <c r="EA7" s="8"/>
+      <c r="DZ7" s="8">
+        <v>166</v>
+      </c>
+      <c r="EA7" s="8">
+        <v>167</v>
+      </c>
       <c r="EB7" s="8"/>
       <c r="EC7" s="8"/>
     </row>
@@ -4788,7 +4812,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44027</v>
+        <v>44029</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -24791,7 +24815,7 @@
       </c>
       <c r="B134" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C134" s="12">
         <v>128</v>
@@ -24944,7 +24968,7 @@
     <row r="135" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A135" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B135" s="12" t="str">
         <f t="shared" si="57"/>
@@ -24963,149 +24987,149 @@
       </c>
       <c r="F135" cm="1">
         <f t="array" ref="F135">+INDEX(Hoja1!$B$2:$MO$7,1,E135)</f>
-        <v>0</v>
+        <v>177843</v>
       </c>
       <c r="G135">
         <f t="shared" si="41"/>
-        <v>-174345</v>
+        <v>3498</v>
       </c>
       <c r="H135" cm="1">
         <f t="array" ref="H135">+INDEX(Hoja1!$B$2:$MO$7,2,$E135)</f>
-        <v>0</v>
+        <v>124504</v>
       </c>
       <c r="I135">
         <f t="shared" si="42"/>
-        <v>-122190</v>
+        <v>2314</v>
       </c>
       <c r="J135">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>53339</v>
       </c>
       <c r="K135">
         <f t="shared" si="43"/>
-        <v>-52155</v>
+        <v>1184</v>
       </c>
       <c r="L135" cm="1">
         <f t="array" ref="L135">+INDEX(Hoja1!$B$2:$MO$7,3,$E135)</f>
-        <v>0</v>
+        <v>21665</v>
       </c>
       <c r="M135" cm="1">
         <f t="array" ref="M135">+INDEX(Hoja1!$B$2:$MO$7,4,$E135)</f>
-        <v>0</v>
+        <v>622</v>
       </c>
       <c r="N135" cm="1">
         <f t="array" ref="N135">+INDEX(Hoja1!$B$2:$MO$7,5,$E135)</f>
-        <v>0</v>
+        <v>1078</v>
       </c>
       <c r="O135" cm="1">
         <f t="array" ref="O135">+INDEX(Hoja1!$B$2:$MO$7,6,$E135)</f>
-        <v>0</v>
+        <v>166</v>
       </c>
       <c r="P135" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.70007815882548086</v>
       </c>
       <c r="Q135" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.29992184117451909</v>
       </c>
       <c r="R135">
         <f t="shared" si="44"/>
-        <v>-177574</v>
+        <v>269</v>
       </c>
       <c r="S135">
         <f t="shared" si="45"/>
-        <v>-52155</v>
+        <v>1184</v>
       </c>
       <c r="T135">
         <f t="shared" si="46"/>
-        <v>-21009</v>
+        <v>656</v>
       </c>
       <c r="U135">
         <f t="shared" si="47"/>
-        <v>-616</v>
+        <v>6</v>
       </c>
       <c r="V135">
         <f t="shared" si="48"/>
-        <v>-1056</v>
+        <v>22</v>
       </c>
       <c r="W135">
         <f t="shared" si="49"/>
-        <v>-163</v>
+        <v>3</v>
       </c>
       <c r="X135">
         <f t="shared" si="50"/>
-        <v>-54.99349643852586</v>
+        <v>8.3307525549705788E-2</v>
       </c>
       <c r="Y135">
         <f t="shared" si="51"/>
-        <v>-1</v>
+        <v>2.2701562649793883E-2</v>
       </c>
       <c r="Z135">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0312247132181447</v>
       </c>
       <c r="AA135">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1.0097402597402598</v>
       </c>
       <c r="AB135">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0208333333333333</v>
       </c>
       <c r="AC135">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.01840490797546</v>
       </c>
       <c r="AD135">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>42761.000240442416</v>
       </c>
       <c r="AE135">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>12824.957922577543</v>
       </c>
       <c r="AF135">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>5209.1849002163981</v>
       </c>
       <c r="AG135">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>149.55518153402261</v>
       </c>
       <c r="AH135">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>259.19692233710026</v>
       </c>
       <c r="AI135">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>39.913440730944941</v>
       </c>
       <c r="AJ135">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>23531</v>
       </c>
       <c r="AK135">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>5657.8504448184658</v>
       </c>
       <c r="AL135">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ134</f>
-        <v>-22844</v>
+        <v>687</v>
       </c>
       <c r="AM135">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ134,0)</f>
-        <v>-1</v>
+        <v>3.0073542286814917E-2</v>
       </c>
     </row>
     <row r="136" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A136" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B136" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C136" s="12">
         <v>130</v>
@@ -25120,139 +25144,139 @@
       </c>
       <c r="F136" cm="1">
         <f t="array" ref="F136">+INDEX(Hoja1!$B$2:$MO$7,1,E136)</f>
-        <v>0</v>
+        <v>180814</v>
       </c>
       <c r="G136">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>2971</v>
       </c>
       <c r="H136" cm="1">
         <f t="array" ref="H136">+INDEX(Hoja1!$B$2:$MO$7,2,$E136)</f>
-        <v>0</v>
+        <v>126411</v>
       </c>
       <c r="I136">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>1907</v>
       </c>
       <c r="J136">
         <f t="shared" ref="J136:J199" si="62">+F136-H136</f>
-        <v>0</v>
+        <v>54403</v>
       </c>
       <c r="K136">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1064</v>
       </c>
       <c r="L136" cm="1">
         <f t="array" ref="L136">+INDEX(Hoja1!$B$2:$MO$7,3,$E136)</f>
-        <v>0</v>
+        <v>21946</v>
       </c>
       <c r="M136" cm="1">
         <f t="array" ref="M136">+INDEX(Hoja1!$B$2:$MO$7,4,$E136)</f>
-        <v>0</v>
+        <v>620</v>
       </c>
       <c r="N136" cm="1">
         <f t="array" ref="N136">+INDEX(Hoja1!$B$2:$MO$7,5,$E136)</f>
-        <v>0</v>
+        <v>1117</v>
       </c>
       <c r="O136" cm="1">
         <f t="array" ref="O136">+INDEX(Hoja1!$B$2:$MO$7,6,$E136)</f>
-        <v>0</v>
+        <v>167</v>
       </c>
       <c r="P136" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.69912174942205807</v>
       </c>
       <c r="Q136" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.30087825057794199</v>
       </c>
       <c r="R136">
         <f t="shared" si="44"/>
-        <v>174345</v>
+        <v>-527</v>
       </c>
       <c r="S136">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>1064</v>
       </c>
       <c r="T136">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>281</v>
       </c>
       <c r="U136">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="V136">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="W136">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X136">
         <f t="shared" si="50"/>
-        <v>-1</v>
+        <v>-0.15065751858204687</v>
       </c>
       <c r="Y136">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1.9947880537692871E-2</v>
       </c>
       <c r="Z136">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1.0129702284791138</v>
       </c>
       <c r="AA136">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>0.99678456591639875</v>
       </c>
       <c r="AB136">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1.0361781076066789</v>
       </c>
       <c r="AC136">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1.0060240963855422</v>
       </c>
       <c r="AD136">
         <f t="shared" ref="AD136:AD199" si="63">+IFERROR(F136/4.159,0)</f>
-        <v>0</v>
+        <v>43475.354652560716</v>
       </c>
       <c r="AE136">
         <f t="shared" ref="AE136:AE199" si="64">+IFERROR(J136/4.159,0)</f>
-        <v>0</v>
+        <v>13080.788651118059</v>
       </c>
       <c r="AF136">
         <f t="shared" ref="AF136:AF199" si="65">+IFERROR(L136/4.159,0)</f>
-        <v>0</v>
+        <v>5276.749218562155</v>
       </c>
       <c r="AG136">
         <f t="shared" ref="AG136:AG199" si="66">+IFERROR(M136/4.159,0)</f>
-        <v>0</v>
+        <v>149.07429670593893</v>
       </c>
       <c r="AH136">
         <f t="shared" ref="AH136:AH199" si="67">+IFERROR(N136/4.159,0)</f>
-        <v>0</v>
+        <v>268.57417648473194</v>
       </c>
       <c r="AI136">
         <f t="shared" ref="AI136:AI199" si="68">+IFERROR(O136/4.159,0)</f>
-        <v>0</v>
+        <v>40.153883144986779</v>
       </c>
       <c r="AJ136">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>23850</v>
       </c>
       <c r="AK136">
         <f t="shared" ref="AK136:AK199" si="69">+IFERROR(AJ136/4.159,0)</f>
-        <v>0</v>
+        <v>5734.5515748978123</v>
       </c>
       <c r="AL136">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ135</f>
-        <v>0</v>
+        <v>319</v>
       </c>
       <c r="AM136">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ135,0)</f>
-        <v>0</v>
+        <v>1.3556584930517189E-2</v>
       </c>
     </row>
     <row r="137" spans="1:39" x14ac:dyDescent="0.2">
@@ -25281,7 +25305,7 @@
       </c>
       <c r="G137">
         <f t="shared" ref="G137:G200" si="70">+F137-F136</f>
-        <v>0</v>
+        <v>-180814</v>
       </c>
       <c r="H137" cm="1">
         <f t="array" ref="H137">+INDEX(Hoja1!$B$2:$MO$7,2,$E137)</f>
@@ -25289,7 +25313,7 @@
       </c>
       <c r="I137">
         <f t="shared" ref="I137:I200" si="71">+H137-H136</f>
-        <v>0</v>
+        <v>-126411</v>
       </c>
       <c r="J137">
         <f t="shared" si="62"/>
@@ -25297,7 +25321,7 @@
       </c>
       <c r="K137">
         <f t="shared" ref="K137:K200" si="72">+J137-J136</f>
-        <v>0</v>
+        <v>-54403</v>
       </c>
       <c r="L137" cm="1">
         <f t="array" ref="L137">+INDEX(Hoja1!$B$2:$MO$7,3,$E137)</f>
@@ -25325,35 +25349,35 @@
       </c>
       <c r="R137">
         <f t="shared" ref="R137:R200" si="73">+G137-G136</f>
-        <v>0</v>
+        <v>-183785</v>
       </c>
       <c r="S137">
         <f t="shared" ref="S137:S200" si="74">+J137-J136</f>
-        <v>0</v>
+        <v>-54403</v>
       </c>
       <c r="T137">
         <f t="shared" ref="T137:T200" si="75">+L137-L136</f>
-        <v>0</v>
+        <v>-21946</v>
       </c>
       <c r="U137">
         <f t="shared" ref="U137:U200" si="76">+M137-M136</f>
-        <v>0</v>
+        <v>-620</v>
       </c>
       <c r="V137">
         <f t="shared" ref="V137:V200" si="77">+N137-N136</f>
-        <v>0</v>
+        <v>-1117</v>
       </c>
       <c r="W137">
         <f t="shared" ref="W137:W200" si="78">+O137-O136</f>
-        <v>0</v>
+        <v>-167</v>
       </c>
       <c r="X137">
         <f t="shared" ref="X137:X200" si="79">+IFERROR(R137/G136,0)</f>
-        <v>0</v>
+        <v>-61.859643217771797</v>
       </c>
       <c r="Y137">
         <f t="shared" ref="Y137:Y200" si="80">+IFERROR(S137/J136,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z137">
         <f t="shared" ref="Z137:Z200" si="81">+IFERROR(L137/L136,0)</f>
@@ -25405,11 +25429,11 @@
       </c>
       <c r="AL137">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ136</f>
-        <v>0</v>
+        <v>-23850</v>
       </c>
       <c r="AM137">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ136,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="138" spans="1:39" x14ac:dyDescent="0.2">
@@ -25482,7 +25506,7 @@
       </c>
       <c r="R138">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>180814</v>
       </c>
       <c r="S138">
         <f t="shared" si="74"/>
@@ -25506,7 +25530,7 @@
       </c>
       <c r="X138">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y138">
         <f t="shared" si="80"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-20-2020 06-35-47
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1658" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6F61A3E2-0346-9148-93F6-8C4433DC0593}"/>
+  <xr:revisionPtr revIDLastSave="1659" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ED2B7776-95E3-184F-AC1B-3790B91D2A5D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="173">
   <si>
     <t>Columna1</t>
   </si>
@@ -553,9 +553,6 @@
     <t>12-07-20</t>
   </si>
   <si>
-    <t>12-07-26</t>
-  </si>
-  <si>
     <t>12-07-27</t>
   </si>
   <si>
@@ -572,6 +569,9 @@
   </si>
   <si>
     <t>17-07-20</t>
+  </si>
+  <si>
+    <t>18-07-20</t>
   </si>
 </sst>
 </file>
@@ -1096,7 +1096,7 @@
     <tableColumn id="129" xr3:uid="{041D18C8-807A-0949-898D-C4880EDA94DD}" name="15-07-20" dataDxfId="12"/>
     <tableColumn id="130" xr3:uid="{61B56DA5-913C-EF4F-B703-9A52B436E7DD}" name="16-07-20" dataDxfId="11"/>
     <tableColumn id="131" xr3:uid="{877B5AA5-D97A-8D40-B352-6FFA59645351}" name="17-07-20" dataDxfId="10"/>
-    <tableColumn id="132" xr3:uid="{3FADF8C3-57FC-5D47-913A-C0C36C8E59FE}" name="12-07-26" dataDxfId="9"/>
+    <tableColumn id="132" xr3:uid="{3FADF8C3-57FC-5D47-913A-C0C36C8E59FE}" name="18-07-20" dataDxfId="9"/>
     <tableColumn id="133" xr3:uid="{1226D8E9-4582-2342-A7CC-4D09D093B768}" name="12-07-27" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1525,7 +1525,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="DY1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="EA7" sqref="EA7"/>
+      <selection pane="topRight" activeCell="EB2" sqref="EB1:EB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1922,25 +1922,25 @@
         <v>164</v>
       </c>
       <c r="DW1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="DX1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="DX1" s="1" t="s">
+      <c r="DY1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="DY1" s="1" t="s">
+      <c r="DZ1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="DZ1" s="1" t="s">
+      <c r="EA1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="EA1" s="1" t="s">
+      <c r="EB1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="EB1" t="s">
+      <c r="EC1" t="s">
         <v>165</v>
-      </c>
-      <c r="EC1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:133" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-24-2020 02-47-02
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1659" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ED2B7776-95E3-184F-AC1B-3790B91D2A5D}"/>
+  <xr:revisionPtr revIDLastSave="1698" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0E71B09F-D36B-D04F-AF93-2195303FF2ED}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="177">
   <si>
     <t>Columna1</t>
   </si>
@@ -553,9 +553,6 @@
     <t>12-07-20</t>
   </si>
   <si>
-    <t>12-07-27</t>
-  </si>
-  <si>
     <t>13-07-20</t>
   </si>
   <si>
@@ -572,6 +569,24 @@
   </si>
   <si>
     <t>18-07-20</t>
+  </si>
+  <si>
+    <t>19-07-20</t>
+  </si>
+  <si>
+    <t>19-07-24</t>
+  </si>
+  <si>
+    <t>19-07-25</t>
+  </si>
+  <si>
+    <t>20-07-20</t>
+  </si>
+  <si>
+    <t>21-07-20</t>
+  </si>
+  <si>
+    <t>22-07-20</t>
   </si>
 </sst>
 </file>
@@ -695,7 +710,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="53">
     <dxf>
       <font>
         <b val="0"/>
@@ -878,6 +893,21 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -962,9 +992,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:EC7" totalsRowShown="0">
-  <autoFilter ref="A1:EC7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
-  <tableColumns count="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:EH7" totalsRowShown="0">
+  <autoFilter ref="A1:EH7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
+  <tableColumns count="138">
     <tableColumn id="76" xr3:uid="{CA01250B-8685-4250-AAEF-D6E482663B6F}" name="Columna1"/>
     <tableColumn id="77" xr3:uid="{BC38B0B2-3229-42F8-9C9A-52EE74902839}" name="10-03-2020"/>
     <tableColumn id="78" xr3:uid="{4BB74E2E-62F3-4EED-8537-96C80CD1ED37}" name="11-03-2020"/>
@@ -1058,46 +1088,51 @@
     <tableColumn id="4" xr3:uid="{2FE879E2-2128-42AE-A0E3-647EE2D0C94F}" name="07-06-2020"/>
     <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="08-06-2020"/>
     <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-2020"/>
-    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="47"/>
-    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="46"/>
-    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="45"/>
-    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="44"/>
-    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="43"/>
-    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="42"/>
-    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="41"/>
-    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="40"/>
-    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="39"/>
-    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="38"/>
-    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="37"/>
-    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="36"/>
-    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="35"/>
-    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="34"/>
-    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="33"/>
-    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="32"/>
-    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="31"/>
-    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="30"/>
-    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="29"/>
-    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="28"/>
-    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="27"/>
-    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="26"/>
-    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="25"/>
-    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="24"/>
-    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="23"/>
-    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="22"/>
-    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="21"/>
-    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="20"/>
-    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="19"/>
-    <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="18"/>
-    <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="10-07-20" dataDxfId="17"/>
-    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="11-07-20" dataDxfId="16"/>
-    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="12-07-20" dataDxfId="15"/>
-    <tableColumn id="127" xr3:uid="{2B284A50-3213-EF46-904E-73679622D22C}" name="13-07-20" dataDxfId="14"/>
-    <tableColumn id="128" xr3:uid="{30C66AA6-47A6-FB40-A335-1BA9A696E85B}" name="14-07-20" dataDxfId="13"/>
-    <tableColumn id="129" xr3:uid="{041D18C8-807A-0949-898D-C4880EDA94DD}" name="15-07-20" dataDxfId="12"/>
-    <tableColumn id="130" xr3:uid="{61B56DA5-913C-EF4F-B703-9A52B436E7DD}" name="16-07-20" dataDxfId="11"/>
-    <tableColumn id="131" xr3:uid="{877B5AA5-D97A-8D40-B352-6FFA59645351}" name="17-07-20" dataDxfId="10"/>
-    <tableColumn id="132" xr3:uid="{3FADF8C3-57FC-5D47-913A-C0C36C8E59FE}" name="18-07-20" dataDxfId="9"/>
-    <tableColumn id="133" xr3:uid="{1226D8E9-4582-2342-A7CC-4D09D093B768}" name="12-07-27" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="52"/>
+    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="50"/>
+    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="49"/>
+    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="48"/>
+    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="47"/>
+    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="46"/>
+    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="45"/>
+    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="44"/>
+    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="43"/>
+    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="42"/>
+    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="41"/>
+    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="40"/>
+    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="39"/>
+    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="38"/>
+    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="37"/>
+    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="36"/>
+    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="35"/>
+    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="34"/>
+    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="33"/>
+    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="32"/>
+    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="31"/>
+    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="30"/>
+    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="29"/>
+    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="28"/>
+    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="27"/>
+    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="26"/>
+    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="25"/>
+    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="24"/>
+    <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="23"/>
+    <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="10-07-20" dataDxfId="22"/>
+    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="11-07-20" dataDxfId="21"/>
+    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="12-07-20" dataDxfId="20"/>
+    <tableColumn id="127" xr3:uid="{2B284A50-3213-EF46-904E-73679622D22C}" name="13-07-20" dataDxfId="19"/>
+    <tableColumn id="128" xr3:uid="{30C66AA6-47A6-FB40-A335-1BA9A696E85B}" name="14-07-20" dataDxfId="18"/>
+    <tableColumn id="129" xr3:uid="{041D18C8-807A-0949-898D-C4880EDA94DD}" name="15-07-20" dataDxfId="17"/>
+    <tableColumn id="130" xr3:uid="{61B56DA5-913C-EF4F-B703-9A52B436E7DD}" name="16-07-20" dataDxfId="16"/>
+    <tableColumn id="131" xr3:uid="{877B5AA5-D97A-8D40-B352-6FFA59645351}" name="17-07-20" dataDxfId="15"/>
+    <tableColumn id="132" xr3:uid="{3FADF8C3-57FC-5D47-913A-C0C36C8E59FE}" name="18-07-20" dataDxfId="14"/>
+    <tableColumn id="133" xr3:uid="{1226D8E9-4582-2342-A7CC-4D09D093B768}" name="19-07-20" dataDxfId="13"/>
+    <tableColumn id="134" xr3:uid="{7101E8B8-49A5-1A49-8532-994B0A3FB01B}" name="20-07-20" dataDxfId="12"/>
+    <tableColumn id="135" xr3:uid="{94611A1B-D923-9546-A8DC-9CCC7B65A729}" name="21-07-20" dataDxfId="11"/>
+    <tableColumn id="136" xr3:uid="{58AE38DE-BFD7-4249-AB7A-15BF37E8B591}" name="22-07-20" dataDxfId="10"/>
+    <tableColumn id="137" xr3:uid="{55C5FB87-1CA4-3F45-887B-DBB3DAAA5369}" name="19-07-24" dataDxfId="9"/>
+    <tableColumn id="138" xr3:uid="{437CA53C-B11E-BF47-AF09-040913B3FCD0}" name="19-07-25" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1520,12 +1555,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B32E72-8F4B-408A-9B01-FAD2807C0C88}">
-  <dimension ref="A1:EC52"/>
+  <dimension ref="A1:EH52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DY1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="ED1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="EB2" sqref="EB1:EB7"/>
+      <selection pane="topRight" activeCell="EF8" sqref="EF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1542,7 +1577,7 @@
     <col min="116" max="118" width="11.43359375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:133" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:138" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1922,28 +1957,43 @@
         <v>164</v>
       </c>
       <c r="DW1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="DX1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="DX1" s="1" t="s">
+      <c r="DY1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="DY1" s="1" t="s">
+      <c r="DZ1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="DZ1" s="1" t="s">
+      <c r="EA1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="EA1" s="1" t="s">
+      <c r="EB1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="EB1" s="1" t="s">
+      <c r="EC1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="EC1" t="s">
-        <v>165</v>
+      <c r="ED1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="EE1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="EF1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="EG1" t="s">
+        <v>172</v>
+      </c>
+      <c r="EH1" t="s">
+        <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:133" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:138" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2337,10 +2387,25 @@
       <c r="EA2" s="8">
         <v>180814</v>
       </c>
-      <c r="EB2" s="8"/>
-      <c r="EC2" s="8"/>
+      <c r="EB2" s="8">
+        <v>183261</v>
+      </c>
+      <c r="EC2" s="8">
+        <v>187041</v>
+      </c>
+      <c r="ED2" s="8">
+        <v>189941</v>
+      </c>
+      <c r="EE2" s="8">
+        <v>192085</v>
+      </c>
+      <c r="EF2" s="8">
+        <v>194599</v>
+      </c>
+      <c r="EG2" s="8"/>
+      <c r="EH2" s="8"/>
     </row>
-    <row r="3" spans="1:133" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:138" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -2734,10 +2799,25 @@
       <c r="EA3" s="8">
         <v>126411</v>
       </c>
-      <c r="EB3" s="8"/>
-      <c r="EC3" s="8"/>
+      <c r="EB3" s="8">
+        <v>128035</v>
+      </c>
+      <c r="EC3" s="8">
+        <v>130598</v>
+      </c>
+      <c r="ED3" s="8">
+        <v>132560</v>
+      </c>
+      <c r="EE3" s="8">
+        <v>134046</v>
+      </c>
+      <c r="EF3" s="8">
+        <v>135846</v>
+      </c>
+      <c r="EG3" s="8"/>
+      <c r="EH3" s="8"/>
     </row>
-    <row r="4" spans="1:133" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:138" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -3131,10 +3211,25 @@
       <c r="EA4" s="8">
         <v>21946</v>
       </c>
-      <c r="EB4" s="8"/>
-      <c r="EC4" s="8"/>
+      <c r="EB4" s="8">
+        <v>21735</v>
+      </c>
+      <c r="EC4" s="8">
+        <v>21915</v>
+      </c>
+      <c r="ED4" s="8">
+        <v>22126</v>
+      </c>
+      <c r="EE4" s="8">
+        <v>21901</v>
+      </c>
+      <c r="EF4" s="8">
+        <v>21640</v>
+      </c>
+      <c r="EG4" s="8"/>
+      <c r="EH4" s="8"/>
     </row>
-    <row r="5" spans="1:133" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:138" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -3437,10 +3532,25 @@
       <c r="EA5" s="8">
         <v>620</v>
       </c>
-      <c r="EB5" s="8"/>
-      <c r="EC5" s="8"/>
+      <c r="EB5" s="8">
+        <v>640</v>
+      </c>
+      <c r="EC5" s="8">
+        <v>654</v>
+      </c>
+      <c r="ED5" s="8">
+        <v>680</v>
+      </c>
+      <c r="EE5" s="8">
+        <v>698</v>
+      </c>
+      <c r="EF5" s="8">
+        <v>651</v>
+      </c>
+      <c r="EG5" s="8"/>
+      <c r="EH5" s="8"/>
     </row>
-    <row r="6" spans="1:133" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:138" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -3830,10 +3940,25 @@
       <c r="EA6" s="8">
         <v>1117</v>
       </c>
-      <c r="EB6" s="8"/>
-      <c r="EC6" s="8"/>
+      <c r="EB6" s="8">
+        <v>1148</v>
+      </c>
+      <c r="EC6" s="8">
+        <v>1146</v>
+      </c>
+      <c r="ED6" s="8">
+        <v>1159</v>
+      </c>
+      <c r="EE6" s="8">
+        <v>1156</v>
+      </c>
+      <c r="EF6" s="8">
+        <v>1155</v>
+      </c>
+      <c r="EG6" s="8"/>
+      <c r="EH6" s="8"/>
     </row>
-    <row r="7" spans="1:133" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:138" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -4225,10 +4350,25 @@
       <c r="EA7" s="8">
         <v>167</v>
       </c>
-      <c r="EB7" s="8"/>
-      <c r="EC7" s="8"/>
+      <c r="EB7" s="8">
+        <v>173</v>
+      </c>
+      <c r="EC7" s="8">
+        <v>175</v>
+      </c>
+      <c r="ED7" s="8">
+        <v>170</v>
+      </c>
+      <c r="EE7" s="8">
+        <v>164</v>
+      </c>
+      <c r="EF7" s="8">
+        <v>158</v>
+      </c>
+      <c r="EG7" s="8"/>
+      <c r="EH7" s="8"/>
     </row>
-    <row r="8" spans="1:133" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:138" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4323,29 +4463,44 @@
       <c r="CO8" s="8"/>
       <c r="DI8" s="15"/>
       <c r="DO8" s="8"/>
+      <c r="DP8" s="8"/>
+      <c r="DQ8" s="8"/>
+      <c r="DR8" s="8"/>
+      <c r="DS8" s="8"/>
+      <c r="DT8" s="8"/>
+      <c r="DU8" s="8"/>
+      <c r="DV8" s="8"/>
+      <c r="DW8" s="8"/>
+      <c r="DX8" s="8"/>
+      <c r="DY8" s="8"/>
+      <c r="DZ8" s="8"/>
+      <c r="EA8" s="8"/>
+      <c r="EB8" s="8"/>
+      <c r="EC8" s="8"/>
+      <c r="ED8" s="8"/>
     </row>
-    <row r="9" spans="1:133" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:138" x14ac:dyDescent="0.2">
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:133" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:138" x14ac:dyDescent="0.2">
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:133" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:138" x14ac:dyDescent="0.2">
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:133" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:138" x14ac:dyDescent="0.2">
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:133" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:138" x14ac:dyDescent="0.2">
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:133" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:138" x14ac:dyDescent="0.2">
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:133" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:138" x14ac:dyDescent="0.2">
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:133" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:138" x14ac:dyDescent="0.2">
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
@@ -4812,7 +4967,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44029</v>
+        <v>44034</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -25129,7 +25284,7 @@
       </c>
       <c r="B136" s="12" t="str">
         <f t="shared" si="57"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C136" s="12">
         <v>130</v>
@@ -25282,7 +25437,7 @@
     <row r="137" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A137" s="12" t="str">
         <f t="shared" si="56"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B137" s="12" t="str">
         <f t="shared" si="57"/>
@@ -25301,145 +25456,145 @@
       </c>
       <c r="F137" cm="1">
         <f t="array" ref="F137">+INDEX(Hoja1!$B$2:$MO$7,1,E137)</f>
-        <v>0</v>
+        <v>183261</v>
       </c>
       <c r="G137">
         <f t="shared" ref="G137:G200" si="70">+F137-F136</f>
-        <v>-180814</v>
+        <v>2447</v>
       </c>
       <c r="H137" cm="1">
         <f t="array" ref="H137">+INDEX(Hoja1!$B$2:$MO$7,2,$E137)</f>
-        <v>0</v>
+        <v>128035</v>
       </c>
       <c r="I137">
         <f t="shared" ref="I137:I200" si="71">+H137-H136</f>
-        <v>-126411</v>
+        <v>1624</v>
       </c>
       <c r="J137">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>55226</v>
       </c>
       <c r="K137">
         <f t="shared" ref="K137:K200" si="72">+J137-J136</f>
-        <v>-54403</v>
+        <v>823</v>
       </c>
       <c r="L137" cm="1">
         <f t="array" ref="L137">+INDEX(Hoja1!$B$2:$MO$7,3,$E137)</f>
-        <v>0</v>
+        <v>21735</v>
       </c>
       <c r="M137" cm="1">
         <f t="array" ref="M137">+INDEX(Hoja1!$B$2:$MO$7,4,$E137)</f>
-        <v>0</v>
+        <v>640</v>
       </c>
       <c r="N137" cm="1">
         <f t="array" ref="N137">+INDEX(Hoja1!$B$2:$MO$7,5,$E137)</f>
-        <v>0</v>
+        <v>1148</v>
       </c>
       <c r="O137" cm="1">
         <f t="array" ref="O137">+INDEX(Hoja1!$B$2:$MO$7,6,$E137)</f>
-        <v>0</v>
+        <v>173</v>
       </c>
       <c r="P137" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.69864837581373018</v>
       </c>
       <c r="Q137" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.30135162418626987</v>
       </c>
       <c r="R137">
         <f t="shared" ref="R137:R200" si="73">+G137-G136</f>
-        <v>-183785</v>
+        <v>-524</v>
       </c>
       <c r="S137">
         <f t="shared" ref="S137:S200" si="74">+J137-J136</f>
-        <v>-54403</v>
+        <v>823</v>
       </c>
       <c r="T137">
         <f t="shared" ref="T137:T200" si="75">+L137-L136</f>
-        <v>-21946</v>
+        <v>-211</v>
       </c>
       <c r="U137">
         <f t="shared" ref="U137:U200" si="76">+M137-M136</f>
-        <v>-620</v>
+        <v>20</v>
       </c>
       <c r="V137">
         <f t="shared" ref="V137:V200" si="77">+N137-N136</f>
-        <v>-1117</v>
+        <v>31</v>
       </c>
       <c r="W137">
         <f t="shared" ref="W137:W200" si="78">+O137-O136</f>
-        <v>-167</v>
+        <v>6</v>
       </c>
       <c r="X137">
         <f t="shared" ref="X137:X200" si="79">+IFERROR(R137/G136,0)</f>
-        <v>-61.859643217771797</v>
+        <v>-0.17637159205654662</v>
       </c>
       <c r="Y137">
         <f t="shared" ref="Y137:Y200" si="80">+IFERROR(S137/J136,0)</f>
-        <v>-1</v>
+        <v>1.5127842214583754E-2</v>
       </c>
       <c r="Z137">
         <f t="shared" ref="Z137:Z200" si="81">+IFERROR(L137/L136,0)</f>
-        <v>0</v>
+        <v>0.99038549166135059</v>
       </c>
       <c r="AA137">
         <f t="shared" ref="AA137:AA200" si="82">+IFERROR(M137/M136,0)</f>
-        <v>0</v>
+        <v>1.032258064516129</v>
       </c>
       <c r="AB137">
         <f t="shared" ref="AB137:AB200" si="83">+IFERROR(N137/N136,0)</f>
-        <v>0</v>
+        <v>1.0277529095792302</v>
       </c>
       <c r="AC137">
         <f t="shared" ref="AC137:AC200" si="84">+IFERROR(O137/O136,0)</f>
-        <v>0</v>
+        <v>1.0359281437125749</v>
       </c>
       <c r="AD137">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>44063.717239721089</v>
       </c>
       <c r="AE137">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>13278.67275787449</v>
       </c>
       <c r="AF137">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>5226.0158691993274</v>
       </c>
       <c r="AG137">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>153.88314498677568</v>
       </c>
       <c r="AH137">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>276.02789132002886</v>
       </c>
       <c r="AI137">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>41.596537629237801</v>
       </c>
       <c r="AJ137">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>23696</v>
       </c>
       <c r="AK137">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>5697.5234431353692</v>
       </c>
       <c r="AL137">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ136</f>
-        <v>-23850</v>
+        <v>-154</v>
       </c>
       <c r="AM137">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ136,0)</f>
-        <v>-1</v>
+        <v>-6.4570230607966456E-3</v>
       </c>
     </row>
     <row r="138" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A138" s="12" t="str">
         <f t="shared" ref="A138:A201" si="85">+IF(D138&gt;$D$4,"OUT TIME","ON")</f>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B138" s="12" t="str">
         <f t="shared" ref="B138:B201" si="86">IF(D138=$D$4,"ultima","no")</f>
@@ -25458,145 +25613,145 @@
       </c>
       <c r="F138" cm="1">
         <f t="array" ref="F138">+INDEX(Hoja1!$B$2:$MO$7,1,E138)</f>
-        <v>0</v>
+        <v>187041</v>
       </c>
       <c r="G138">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>3780</v>
       </c>
       <c r="H138" cm="1">
         <f t="array" ref="H138">+INDEX(Hoja1!$B$2:$MO$7,2,$E138)</f>
-        <v>0</v>
+        <v>130598</v>
       </c>
       <c r="I138">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>2563</v>
       </c>
       <c r="J138">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>56443</v>
       </c>
       <c r="K138">
         <f t="shared" si="72"/>
-        <v>0</v>
+        <v>1217</v>
       </c>
       <c r="L138" cm="1">
         <f t="array" ref="L138">+INDEX(Hoja1!$B$2:$MO$7,3,$E138)</f>
-        <v>0</v>
+        <v>21915</v>
       </c>
       <c r="M138" cm="1">
         <f t="array" ref="M138">+INDEX(Hoja1!$B$2:$MO$7,4,$E138)</f>
-        <v>0</v>
+        <v>654</v>
       </c>
       <c r="N138" cm="1">
         <f t="array" ref="N138">+INDEX(Hoja1!$B$2:$MO$7,5,$E138)</f>
-        <v>0</v>
+        <v>1146</v>
       </c>
       <c r="O138" cm="1">
         <f t="array" ref="O138">+INDEX(Hoja1!$B$2:$MO$7,6,$E138)</f>
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="P138" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.69823193845199716</v>
       </c>
       <c r="Q138" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.30176806154800284</v>
       </c>
       <c r="R138">
         <f t="shared" si="73"/>
-        <v>180814</v>
+        <v>1333</v>
       </c>
       <c r="S138">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>1217</v>
       </c>
       <c r="T138">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="U138">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="V138">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="W138">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X138">
         <f t="shared" si="79"/>
-        <v>-1</v>
+        <v>0.54474867184307318</v>
       </c>
       <c r="Y138">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>2.2036721833918808E-2</v>
       </c>
       <c r="Z138">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>1.0082815734989647</v>
       </c>
       <c r="AA138">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>1.0218750000000001</v>
       </c>
       <c r="AB138">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>0.99825783972125437</v>
       </c>
       <c r="AC138">
         <f t="shared" si="84"/>
-        <v>0</v>
+        <v>1.0115606936416186</v>
       </c>
       <c r="AD138">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>44972.589564799229</v>
       </c>
       <c r="AE138">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>13571.291175763405</v>
       </c>
       <c r="AF138">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>5269.2955037268575</v>
       </c>
       <c r="AG138">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>157.2493387833614</v>
       </c>
       <c r="AH138">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>275.54700649194518</v>
       </c>
       <c r="AI138">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>42.077422457321475</v>
       </c>
       <c r="AJ138">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>23890</v>
       </c>
       <c r="AK138">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>5744.1692714594856</v>
       </c>
       <c r="AL138">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ137</f>
-        <v>0</v>
+        <v>194</v>
       </c>
       <c r="AM138">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ137,0)</f>
-        <v>0</v>
+        <v>8.1870357866306552E-3</v>
       </c>
     </row>
     <row r="139" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A139" s="12" t="str">
         <f t="shared" si="85"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B139" s="12" t="str">
         <f t="shared" si="86"/>
@@ -25615,145 +25770,145 @@
       </c>
       <c r="F139" cm="1">
         <f t="array" ref="F139">+INDEX(Hoja1!$B$2:$MO$7,1,E139)</f>
-        <v>0</v>
+        <v>189941</v>
       </c>
       <c r="G139">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>2900</v>
       </c>
       <c r="H139" cm="1">
         <f t="array" ref="H139">+INDEX(Hoja1!$B$2:$MO$7,2,$E139)</f>
-        <v>0</v>
+        <v>132560</v>
       </c>
       <c r="I139">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>1962</v>
       </c>
       <c r="J139">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>57381</v>
       </c>
       <c r="K139">
         <f t="shared" si="72"/>
-        <v>0</v>
+        <v>938</v>
       </c>
       <c r="L139" cm="1">
         <f t="array" ref="L139">+INDEX(Hoja1!$B$2:$MO$7,3,$E139)</f>
-        <v>0</v>
+        <v>22126</v>
       </c>
       <c r="M139" cm="1">
         <f t="array" ref="M139">+INDEX(Hoja1!$B$2:$MO$7,4,$E139)</f>
-        <v>0</v>
+        <v>680</v>
       </c>
       <c r="N139" cm="1">
         <f t="array" ref="N139">+INDEX(Hoja1!$B$2:$MO$7,5,$E139)</f>
-        <v>0</v>
+        <v>1159</v>
       </c>
       <c r="O139" cm="1">
         <f t="array" ref="O139">+INDEX(Hoja1!$B$2:$MO$7,6,$E139)</f>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="P139" s="13">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>0.69790092713000351</v>
       </c>
       <c r="Q139" s="13">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>0.30209907286999649</v>
       </c>
       <c r="R139">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>-880</v>
       </c>
       <c r="S139">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>938</v>
       </c>
       <c r="T139">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>211</v>
       </c>
       <c r="U139">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="V139">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="W139">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="X139">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>-0.23280423280423279</v>
       </c>
       <c r="Y139">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>1.661853551370409E-2</v>
       </c>
       <c r="Z139">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>1.0096281086014145</v>
       </c>
       <c r="AA139">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>1.0397553516819571</v>
       </c>
       <c r="AB139">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>1.0113438045375218</v>
       </c>
       <c r="AC139">
         <f t="shared" si="84"/>
-        <v>0</v>
+        <v>0.97142857142857142</v>
       </c>
       <c r="AD139">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>45669.872565520564</v>
       </c>
       <c r="AE139">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>13796.826160134648</v>
       </c>
       <c r="AF139">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>5320.0288530896851</v>
       </c>
       <c r="AG139">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>163.50084154844916</v>
       </c>
       <c r="AH139">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>278.67275787448909</v>
       </c>
       <c r="AI139">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>40.87521038711229</v>
       </c>
       <c r="AJ139">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>24135</v>
       </c>
       <c r="AK139">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>5803.0776628997355</v>
       </c>
       <c r="AL139">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ138</f>
-        <v>0</v>
+        <v>245</v>
       </c>
       <c r="AM139">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ138,0)</f>
-        <v>0</v>
+        <v>1.0255336961071579E-2</v>
       </c>
     </row>
     <row r="140" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A140" s="12" t="str">
         <f t="shared" si="85"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B140" s="12" t="str">
         <f t="shared" si="86"/>
@@ -25772,149 +25927,149 @@
       </c>
       <c r="F140" cm="1">
         <f t="array" ref="F140">+INDEX(Hoja1!$B$2:$MO$7,1,E140)</f>
-        <v>0</v>
+        <v>192085</v>
       </c>
       <c r="G140">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>2144</v>
       </c>
       <c r="H140" cm="1">
         <f t="array" ref="H140">+INDEX(Hoja1!$B$2:$MO$7,2,$E140)</f>
-        <v>0</v>
+        <v>134046</v>
       </c>
       <c r="I140">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>1486</v>
       </c>
       <c r="J140">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>58039</v>
       </c>
       <c r="K140">
         <f t="shared" si="72"/>
-        <v>0</v>
+        <v>658</v>
       </c>
       <c r="L140" cm="1">
         <f t="array" ref="L140">+INDEX(Hoja1!$B$2:$MO$7,3,$E140)</f>
-        <v>0</v>
+        <v>21901</v>
       </c>
       <c r="M140" cm="1">
         <f t="array" ref="M140">+INDEX(Hoja1!$B$2:$MO$7,4,$E140)</f>
-        <v>0</v>
+        <v>698</v>
       </c>
       <c r="N140" cm="1">
         <f t="array" ref="N140">+INDEX(Hoja1!$B$2:$MO$7,5,$E140)</f>
-        <v>0</v>
+        <v>1156</v>
       </c>
       <c r="O140" cm="1">
         <f t="array" ref="O140">+INDEX(Hoja1!$B$2:$MO$7,6,$E140)</f>
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="P140" s="13">
         <f t="shared" ref="P140:P203" si="89">+IFERROR(H140/F140,0)</f>
-        <v>0</v>
+        <v>0.69784730718171639</v>
       </c>
       <c r="Q140" s="13">
         <f t="shared" ref="Q140:Q203" si="90">+IFERROR(J140/F140,0)</f>
-        <v>0</v>
+        <v>0.30215269281828355</v>
       </c>
       <c r="R140">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>-756</v>
       </c>
       <c r="S140">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>658</v>
       </c>
       <c r="T140">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>-225</v>
       </c>
       <c r="U140">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="V140">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="W140">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="X140">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>-0.26068965517241377</v>
       </c>
       <c r="Y140">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>1.146721040065527E-2</v>
       </c>
       <c r="Z140">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>0.98983096809183768</v>
       </c>
       <c r="AA140">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>1.026470588235294</v>
       </c>
       <c r="AB140">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>0.997411561691113</v>
       </c>
       <c r="AC140">
         <f t="shared" si="84"/>
-        <v>0</v>
+        <v>0.96470588235294119</v>
       </c>
       <c r="AD140">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>46185.381101226259</v>
       </c>
       <c r="AE140">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>13955.037268574177</v>
       </c>
       <c r="AF140">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>5265.9293099302722</v>
       </c>
       <c r="AG140">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>167.82880500120223</v>
       </c>
       <c r="AH140">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>277.95143063236355</v>
       </c>
       <c r="AI140">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>39.432555902861267</v>
       </c>
       <c r="AJ140">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>23919</v>
       </c>
       <c r="AK140">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>5751.1421014666994</v>
       </c>
       <c r="AL140">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ139</f>
-        <v>0</v>
+        <v>-216</v>
       </c>
       <c r="AM140">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ139,0)</f>
-        <v>0</v>
+        <v>-8.9496581727781226E-3</v>
       </c>
     </row>
     <row r="141" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A141" s="12" t="str">
         <f t="shared" si="85"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B141" s="12" t="str">
         <f t="shared" si="86"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C141" s="12">
         <v>135</v>
@@ -25929,139 +26084,139 @@
       </c>
       <c r="F141" cm="1">
         <f t="array" ref="F141">+INDEX(Hoja1!$B$2:$MO$7,1,E141)</f>
-        <v>0</v>
+        <v>194599</v>
       </c>
       <c r="G141">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>2514</v>
       </c>
       <c r="H141" cm="1">
         <f t="array" ref="H141">+INDEX(Hoja1!$B$2:$MO$7,2,$E141)</f>
-        <v>0</v>
+        <v>135846</v>
       </c>
       <c r="I141">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>1800</v>
       </c>
       <c r="J141">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>58753</v>
       </c>
       <c r="K141">
         <f t="shared" si="72"/>
-        <v>0</v>
+        <v>714</v>
       </c>
       <c r="L141" cm="1">
         <f t="array" ref="L141">+INDEX(Hoja1!$B$2:$MO$7,3,$E141)</f>
-        <v>0</v>
+        <v>21640</v>
       </c>
       <c r="M141" cm="1">
         <f t="array" ref="M141">+INDEX(Hoja1!$B$2:$MO$7,4,$E141)</f>
-        <v>0</v>
+        <v>651</v>
       </c>
       <c r="N141" cm="1">
         <f t="array" ref="N141">+INDEX(Hoja1!$B$2:$MO$7,5,$E141)</f>
-        <v>0</v>
+        <v>1155</v>
       </c>
       <c r="O141" cm="1">
         <f t="array" ref="O141">+INDEX(Hoja1!$B$2:$MO$7,6,$E141)</f>
-        <v>0</v>
+        <v>158</v>
       </c>
       <c r="P141" s="13">
         <f t="shared" si="89"/>
-        <v>0</v>
+        <v>0.69808169620604421</v>
       </c>
       <c r="Q141" s="13">
         <f t="shared" si="90"/>
-        <v>0</v>
+        <v>0.30191830379395579</v>
       </c>
       <c r="R141">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>370</v>
       </c>
       <c r="S141">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>714</v>
       </c>
       <c r="T141">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>-261</v>
       </c>
       <c r="U141">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>-47</v>
       </c>
       <c r="V141">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="W141">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="X141">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>0.17257462686567165</v>
       </c>
       <c r="Y141">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>1.2302072744189253E-2</v>
       </c>
       <c r="Z141">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>0.98808273594813023</v>
       </c>
       <c r="AA141">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>0.93266475644699143</v>
       </c>
       <c r="AB141">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>0.99913494809688586</v>
       </c>
       <c r="AC141">
         <f t="shared" si="84"/>
-        <v>0</v>
+        <v>0.96341463414634143</v>
       </c>
       <c r="AD141">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>46789.853330127436</v>
       </c>
       <c r="AE141">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>14126.713152200049</v>
       </c>
       <c r="AF141">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>5203.1738398653524</v>
       </c>
       <c r="AG141">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>156.52801154123588</v>
       </c>
       <c r="AH141">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>277.71098821832175</v>
       </c>
       <c r="AI141">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>37.989901418610245</v>
       </c>
       <c r="AJ141">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>23604</v>
       </c>
       <c r="AK141">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>5675.4027410435201</v>
       </c>
       <c r="AL141">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ140</f>
-        <v>0</v>
+        <v>-315</v>
       </c>
       <c r="AM141">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ140,0)</f>
-        <v>0</v>
+        <v>-1.3169446883230905E-2</v>
       </c>
     </row>
     <row r="142" spans="1:39" x14ac:dyDescent="0.2">
@@ -26090,7 +26245,7 @@
       </c>
       <c r="G142">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>-194599</v>
       </c>
       <c r="H142" cm="1">
         <f t="array" ref="H142">+INDEX(Hoja1!$B$2:$MO$7,2,$E142)</f>
@@ -26098,7 +26253,7 @@
       </c>
       <c r="I142">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>-135846</v>
       </c>
       <c r="J142">
         <f t="shared" si="62"/>
@@ -26106,7 +26261,7 @@
       </c>
       <c r="K142">
         <f t="shared" si="72"/>
-        <v>0</v>
+        <v>-58753</v>
       </c>
       <c r="L142" cm="1">
         <f t="array" ref="L142">+INDEX(Hoja1!$B$2:$MO$7,3,$E142)</f>
@@ -26134,35 +26289,35 @@
       </c>
       <c r="R142">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>-197113</v>
       </c>
       <c r="S142">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>-58753</v>
       </c>
       <c r="T142">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>-21640</v>
       </c>
       <c r="U142">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>-651</v>
       </c>
       <c r="V142">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>-1155</v>
       </c>
       <c r="W142">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>-158</v>
       </c>
       <c r="X142">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>-78.406125696101824</v>
       </c>
       <c r="Y142">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z142">
         <f t="shared" si="81"/>
@@ -26214,11 +26369,11 @@
       </c>
       <c r="AL142">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ141</f>
-        <v>0</v>
+        <v>-23604</v>
       </c>
       <c r="AM142">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ141,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="143" spans="1:39" x14ac:dyDescent="0.2">
@@ -26291,7 +26446,7 @@
       </c>
       <c r="R143">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>194599</v>
       </c>
       <c r="S143">
         <f t="shared" si="74"/>
@@ -26315,7 +26470,7 @@
       </c>
       <c r="X143">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y143">
         <f t="shared" si="80"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-27-2020 16-39-32
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1698" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0E71B09F-D36B-D04F-AF93-2195303FF2ED}"/>
+  <xr:revisionPtr revIDLastSave="1729" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6A119A04-897A-3C46-83C1-D8D34277D5BB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="180">
   <si>
     <t>Columna1</t>
   </si>
@@ -574,12 +574,6 @@
     <t>19-07-20</t>
   </si>
   <si>
-    <t>19-07-24</t>
-  </si>
-  <si>
-    <t>19-07-25</t>
-  </si>
-  <si>
     <t>20-07-20</t>
   </si>
   <si>
@@ -587,6 +581,21 @@
   </si>
   <si>
     <t>22-07-20</t>
+  </si>
+  <si>
+    <t>23-07-20</t>
+  </si>
+  <si>
+    <t>24-07-20</t>
+  </si>
+  <si>
+    <t>25-07-20</t>
+  </si>
+  <si>
+    <t>26-07-20</t>
+  </si>
+  <si>
+    <t>27-07-20</t>
   </si>
 </sst>
 </file>
@@ -710,7 +719,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="56">
     <dxf>
       <font>
         <b val="0"/>
@@ -908,6 +917,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -992,9 +1010,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:EH7" totalsRowShown="0">
-  <autoFilter ref="A1:EH7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
-  <tableColumns count="138">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:EK7" totalsRowShown="0">
+  <autoFilter ref="A1:EK7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
+  <tableColumns count="141">
     <tableColumn id="76" xr3:uid="{CA01250B-8685-4250-AAEF-D6E482663B6F}" name="Columna1"/>
     <tableColumn id="77" xr3:uid="{BC38B0B2-3229-42F8-9C9A-52EE74902839}" name="10-03-2020"/>
     <tableColumn id="78" xr3:uid="{4BB74E2E-62F3-4EED-8537-96C80CD1ED37}" name="11-03-2020"/>
@@ -1088,51 +1106,54 @@
     <tableColumn id="4" xr3:uid="{2FE879E2-2128-42AE-A0E3-647EE2D0C94F}" name="07-06-2020"/>
     <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="08-06-2020"/>
     <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-2020"/>
-    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="52"/>
-    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="51"/>
-    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="50"/>
-    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="49"/>
-    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="48"/>
-    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="47"/>
-    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="46"/>
-    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="45"/>
-    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="44"/>
-    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="43"/>
-    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="42"/>
-    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="41"/>
-    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="40"/>
-    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="39"/>
-    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="38"/>
-    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="37"/>
-    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="36"/>
-    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="35"/>
-    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="34"/>
-    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="33"/>
-    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="32"/>
-    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="31"/>
-    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="30"/>
-    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="29"/>
-    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="28"/>
-    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="27"/>
-    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="26"/>
-    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="25"/>
-    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="24"/>
-    <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="23"/>
-    <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="10-07-20" dataDxfId="22"/>
-    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="11-07-20" dataDxfId="21"/>
-    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="12-07-20" dataDxfId="20"/>
-    <tableColumn id="127" xr3:uid="{2B284A50-3213-EF46-904E-73679622D22C}" name="13-07-20" dataDxfId="19"/>
-    <tableColumn id="128" xr3:uid="{30C66AA6-47A6-FB40-A335-1BA9A696E85B}" name="14-07-20" dataDxfId="18"/>
-    <tableColumn id="129" xr3:uid="{041D18C8-807A-0949-898D-C4880EDA94DD}" name="15-07-20" dataDxfId="17"/>
-    <tableColumn id="130" xr3:uid="{61B56DA5-913C-EF4F-B703-9A52B436E7DD}" name="16-07-20" dataDxfId="16"/>
-    <tableColumn id="131" xr3:uid="{877B5AA5-D97A-8D40-B352-6FFA59645351}" name="17-07-20" dataDxfId="15"/>
-    <tableColumn id="132" xr3:uid="{3FADF8C3-57FC-5D47-913A-C0C36C8E59FE}" name="18-07-20" dataDxfId="14"/>
-    <tableColumn id="133" xr3:uid="{1226D8E9-4582-2342-A7CC-4D09D093B768}" name="19-07-20" dataDxfId="13"/>
-    <tableColumn id="134" xr3:uid="{7101E8B8-49A5-1A49-8532-994B0A3FB01B}" name="20-07-20" dataDxfId="12"/>
-    <tableColumn id="135" xr3:uid="{94611A1B-D923-9546-A8DC-9CCC7B65A729}" name="21-07-20" dataDxfId="11"/>
-    <tableColumn id="136" xr3:uid="{58AE38DE-BFD7-4249-AB7A-15BF37E8B591}" name="22-07-20" dataDxfId="10"/>
-    <tableColumn id="137" xr3:uid="{55C5FB87-1CA4-3F45-887B-DBB3DAAA5369}" name="19-07-24" dataDxfId="9"/>
-    <tableColumn id="138" xr3:uid="{437CA53C-B11E-BF47-AF09-040913B3FCD0}" name="19-07-25" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="55"/>
+    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="54"/>
+    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="53"/>
+    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="52"/>
+    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="51"/>
+    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="50"/>
+    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="49"/>
+    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="48"/>
+    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="47"/>
+    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="46"/>
+    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="45"/>
+    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="44"/>
+    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="43"/>
+    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="42"/>
+    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="41"/>
+    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="40"/>
+    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="39"/>
+    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="38"/>
+    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="37"/>
+    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="36"/>
+    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="35"/>
+    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="34"/>
+    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="33"/>
+    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="32"/>
+    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="31"/>
+    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="30"/>
+    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="29"/>
+    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="28"/>
+    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="27"/>
+    <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="26"/>
+    <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="10-07-20" dataDxfId="25"/>
+    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="11-07-20" dataDxfId="24"/>
+    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="12-07-20" dataDxfId="23"/>
+    <tableColumn id="127" xr3:uid="{2B284A50-3213-EF46-904E-73679622D22C}" name="13-07-20" dataDxfId="22"/>
+    <tableColumn id="128" xr3:uid="{30C66AA6-47A6-FB40-A335-1BA9A696E85B}" name="14-07-20" dataDxfId="21"/>
+    <tableColumn id="129" xr3:uid="{041D18C8-807A-0949-898D-C4880EDA94DD}" name="15-07-20" dataDxfId="20"/>
+    <tableColumn id="130" xr3:uid="{61B56DA5-913C-EF4F-B703-9A52B436E7DD}" name="16-07-20" dataDxfId="19"/>
+    <tableColumn id="131" xr3:uid="{877B5AA5-D97A-8D40-B352-6FFA59645351}" name="17-07-20" dataDxfId="18"/>
+    <tableColumn id="132" xr3:uid="{3FADF8C3-57FC-5D47-913A-C0C36C8E59FE}" name="18-07-20" dataDxfId="17"/>
+    <tableColumn id="133" xr3:uid="{1226D8E9-4582-2342-A7CC-4D09D093B768}" name="19-07-20" dataDxfId="16"/>
+    <tableColumn id="134" xr3:uid="{7101E8B8-49A5-1A49-8532-994B0A3FB01B}" name="20-07-20" dataDxfId="15"/>
+    <tableColumn id="135" xr3:uid="{94611A1B-D923-9546-A8DC-9CCC7B65A729}" name="21-07-20" dataDxfId="14"/>
+    <tableColumn id="136" xr3:uid="{58AE38DE-BFD7-4249-AB7A-15BF37E8B591}" name="22-07-20" dataDxfId="13"/>
+    <tableColumn id="137" xr3:uid="{55C5FB87-1CA4-3F45-887B-DBB3DAAA5369}" name="23-07-20" dataDxfId="12"/>
+    <tableColumn id="138" xr3:uid="{437CA53C-B11E-BF47-AF09-040913B3FCD0}" name="24-07-20" dataDxfId="11"/>
+    <tableColumn id="139" xr3:uid="{202231FA-82F9-BF4E-8D60-B218C26A354A}" name="25-07-20" dataDxfId="10"/>
+    <tableColumn id="140" xr3:uid="{24F2106B-9F5D-1E4C-A42B-E2AA613BEE08}" name="26-07-20" dataDxfId="9"/>
+    <tableColumn id="141" xr3:uid="{8BDBD0BC-D9B1-B445-9A72-EF935A438E09}" name="27-07-20" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1555,12 +1576,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B32E72-8F4B-408A-9B01-FAD2807C0C88}">
-  <dimension ref="A1:EH52"/>
+  <dimension ref="A1:EK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="ED1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="EI1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="EF8" sqref="EF8"/>
+      <selection pane="topRight" activeCell="EK2" sqref="EK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1577,7 +1598,7 @@
     <col min="116" max="118" width="11.43359375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:141" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1978,22 +1999,31 @@
         <v>171</v>
       </c>
       <c r="ED1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="EE1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="EF1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="EE1" s="1" t="s">
+      <c r="EG1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="EF1" s="1" t="s">
+      <c r="EH1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="EG1" t="s">
-        <v>172</v>
-      </c>
-      <c r="EH1" t="s">
-        <v>173</v>
+      <c r="EI1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="EJ1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="EK1" s="1" t="s">
+        <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:141" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2402,10 +2432,21 @@
       <c r="EF2" s="8">
         <v>194599</v>
       </c>
-      <c r="EG2" s="8"/>
-      <c r="EH2" s="8"/>
+      <c r="EG2" s="8">
+        <v>197605</v>
+      </c>
+      <c r="EH2" s="8">
+        <v>200986</v>
+      </c>
+      <c r="EI2" s="8">
+        <v>203600</v>
+      </c>
+      <c r="EJ2" s="8">
+        <v>207908</v>
+      </c>
+      <c r="EK2" s="8"/>
     </row>
-    <row r="3" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:141" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -2814,10 +2855,21 @@
       <c r="EF3" s="8">
         <v>135846</v>
       </c>
-      <c r="EG3" s="8"/>
-      <c r="EH3" s="8"/>
+      <c r="EG3" s="8">
+        <v>137956</v>
+      </c>
+      <c r="EH3" s="8">
+        <v>140252</v>
+      </c>
+      <c r="EI3" s="8">
+        <v>142071</v>
+      </c>
+      <c r="EJ3" s="8">
+        <v>144913</v>
+      </c>
+      <c r="EK3" s="8"/>
     </row>
-    <row r="4" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:141" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -3226,10 +3278,21 @@
       <c r="EF4" s="8">
         <v>21640</v>
       </c>
-      <c r="EG4" s="8"/>
-      <c r="EH4" s="8"/>
+      <c r="EG4" s="8">
+        <v>21783</v>
+      </c>
+      <c r="EH4" s="8">
+        <v>21967</v>
+      </c>
+      <c r="EI4" s="8">
+        <v>22110</v>
+      </c>
+      <c r="EJ4" s="8">
+        <v>22803</v>
+      </c>
+      <c r="EK4" s="8"/>
     </row>
-    <row r="5" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:141" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -3547,10 +3610,21 @@
       <c r="EF5" s="8">
         <v>651</v>
       </c>
-      <c r="EG5" s="8"/>
-      <c r="EH5" s="8"/>
+      <c r="EG5" s="8">
+        <v>670</v>
+      </c>
+      <c r="EH5" s="8">
+        <v>674</v>
+      </c>
+      <c r="EI5" s="8">
+        <v>652</v>
+      </c>
+      <c r="EJ5" s="8">
+        <v>680</v>
+      </c>
+      <c r="EK5" s="8"/>
     </row>
-    <row r="6" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:141" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -3955,10 +4029,21 @@
       <c r="EF6" s="8">
         <v>1155</v>
       </c>
-      <c r="EG6" s="8"/>
-      <c r="EH6" s="8"/>
+      <c r="EG6" s="8">
+        <v>1169</v>
+      </c>
+      <c r="EH6" s="8">
+        <v>1243</v>
+      </c>
+      <c r="EI6" s="8">
+        <v>1247</v>
+      </c>
+      <c r="EJ6" s="8">
+        <v>1237</v>
+      </c>
+      <c r="EK6" s="8"/>
     </row>
-    <row r="7" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:141" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -4365,10 +4450,21 @@
       <c r="EF7" s="8">
         <v>158</v>
       </c>
-      <c r="EG7" s="8"/>
-      <c r="EH7" s="8"/>
+      <c r="EG7" s="8">
+        <v>158</v>
+      </c>
+      <c r="EH7" s="8">
+        <v>155</v>
+      </c>
+      <c r="EI7" s="8">
+        <v>152</v>
+      </c>
+      <c r="EJ7" s="8">
+        <v>151</v>
+      </c>
+      <c r="EK7" s="8"/>
     </row>
-    <row r="8" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:141" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4479,28 +4575,28 @@
       <c r="EC8" s="8"/>
       <c r="ED8" s="8"/>
     </row>
-    <row r="9" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:141" x14ac:dyDescent="0.2">
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:141" x14ac:dyDescent="0.2">
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:141" x14ac:dyDescent="0.2">
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:141" x14ac:dyDescent="0.2">
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:141" x14ac:dyDescent="0.2">
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:141" x14ac:dyDescent="0.2">
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:141" x14ac:dyDescent="0.2">
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:138" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:141" x14ac:dyDescent="0.2">
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
@@ -4967,7 +5063,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44034</v>
+        <v>44038</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -26069,7 +26165,7 @@
       </c>
       <c r="B141" s="12" t="str">
         <f t="shared" si="86"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C141" s="12">
         <v>135</v>
@@ -26222,7 +26318,7 @@
     <row r="142" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A142" s="12" t="str">
         <f t="shared" si="85"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B142" s="12" t="str">
         <f t="shared" si="86"/>
@@ -26241,145 +26337,145 @@
       </c>
       <c r="F142" cm="1">
         <f t="array" ref="F142">+INDEX(Hoja1!$B$2:$MO$7,1,E142)</f>
-        <v>0</v>
+        <v>197605</v>
       </c>
       <c r="G142">
         <f t="shared" si="70"/>
-        <v>-194599</v>
+        <v>3006</v>
       </c>
       <c r="H142" cm="1">
         <f t="array" ref="H142">+INDEX(Hoja1!$B$2:$MO$7,2,$E142)</f>
-        <v>0</v>
+        <v>137956</v>
       </c>
       <c r="I142">
         <f t="shared" si="71"/>
-        <v>-135846</v>
+        <v>2110</v>
       </c>
       <c r="J142">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>59649</v>
       </c>
       <c r="K142">
         <f t="shared" si="72"/>
-        <v>-58753</v>
+        <v>896</v>
       </c>
       <c r="L142" cm="1">
         <f t="array" ref="L142">+INDEX(Hoja1!$B$2:$MO$7,3,$E142)</f>
-        <v>0</v>
+        <v>21783</v>
       </c>
       <c r="M142" cm="1">
         <f t="array" ref="M142">+INDEX(Hoja1!$B$2:$MO$7,4,$E142)</f>
-        <v>0</v>
+        <v>670</v>
       </c>
       <c r="N142" cm="1">
         <f t="array" ref="N142">+INDEX(Hoja1!$B$2:$MO$7,5,$E142)</f>
-        <v>0</v>
+        <v>1169</v>
       </c>
       <c r="O142" cm="1">
         <f t="array" ref="O142">+INDEX(Hoja1!$B$2:$MO$7,6,$E142)</f>
-        <v>0</v>
+        <v>158</v>
       </c>
       <c r="P142" s="13">
         <f t="shared" si="89"/>
-        <v>0</v>
+        <v>0.69814022924521135</v>
       </c>
       <c r="Q142" s="13">
         <f t="shared" si="90"/>
-        <v>0</v>
+        <v>0.30185977075478859</v>
       </c>
       <c r="R142">
         <f t="shared" si="73"/>
-        <v>-197113</v>
+        <v>492</v>
       </c>
       <c r="S142">
         <f t="shared" si="74"/>
-        <v>-58753</v>
+        <v>896</v>
       </c>
       <c r="T142">
         <f t="shared" si="75"/>
-        <v>-21640</v>
+        <v>143</v>
       </c>
       <c r="U142">
         <f t="shared" si="76"/>
-        <v>-651</v>
+        <v>19</v>
       </c>
       <c r="V142">
         <f t="shared" si="77"/>
-        <v>-1155</v>
+        <v>14</v>
       </c>
       <c r="W142">
         <f t="shared" si="78"/>
-        <v>-158</v>
+        <v>0</v>
       </c>
       <c r="X142">
         <f t="shared" si="79"/>
-        <v>-78.406125696101824</v>
+        <v>0.19570405727923629</v>
       </c>
       <c r="Y142">
         <f t="shared" si="80"/>
-        <v>-1</v>
+        <v>1.5250285091825098E-2</v>
       </c>
       <c r="Z142">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>1.0066081330868761</v>
       </c>
       <c r="AA142">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>1.0291858678955452</v>
       </c>
       <c r="AB142">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>1.0121212121212122</v>
       </c>
       <c r="AC142">
         <f t="shared" si="84"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD142">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>47512.623226737196</v>
       </c>
       <c r="AE142">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>14342.149555181535</v>
       </c>
       <c r="AF142">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>5237.5571050733352</v>
       </c>
       <c r="AG142">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>161.09641740803079</v>
       </c>
       <c r="AH142">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>281.07718201490746</v>
       </c>
       <c r="AI142">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>37.989901418610245</v>
       </c>
       <c r="AJ142">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>23780</v>
       </c>
       <c r="AK142">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>5717.7206059148839</v>
       </c>
       <c r="AL142">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ141</f>
-        <v>-23604</v>
+        <v>176</v>
       </c>
       <c r="AM142">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ141,0)</f>
-        <v>-1</v>
+        <v>7.456363328249449E-3</v>
       </c>
     </row>
     <row r="143" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A143" s="12" t="str">
         <f t="shared" si="85"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B143" s="12" t="str">
         <f t="shared" si="86"/>
@@ -26398,145 +26494,145 @@
       </c>
       <c r="F143" cm="1">
         <f t="array" ref="F143">+INDEX(Hoja1!$B$2:$MO$7,1,E143)</f>
-        <v>0</v>
+        <v>200986</v>
       </c>
       <c r="G143">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>3381</v>
       </c>
       <c r="H143" cm="1">
         <f t="array" ref="H143">+INDEX(Hoja1!$B$2:$MO$7,2,$E143)</f>
-        <v>0</v>
+        <v>140252</v>
       </c>
       <c r="I143">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>2296</v>
       </c>
       <c r="J143">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>60734</v>
       </c>
       <c r="K143">
         <f t="shared" si="72"/>
-        <v>0</v>
+        <v>1085</v>
       </c>
       <c r="L143" cm="1">
         <f t="array" ref="L143">+INDEX(Hoja1!$B$2:$MO$7,3,$E143)</f>
-        <v>0</v>
+        <v>21967</v>
       </c>
       <c r="M143" cm="1">
         <f t="array" ref="M143">+INDEX(Hoja1!$B$2:$MO$7,4,$E143)</f>
-        <v>0</v>
+        <v>674</v>
       </c>
       <c r="N143" cm="1">
         <f t="array" ref="N143">+INDEX(Hoja1!$B$2:$MO$7,5,$E143)</f>
-        <v>0</v>
+        <v>1243</v>
       </c>
       <c r="O143" cm="1">
         <f t="array" ref="O143">+INDEX(Hoja1!$B$2:$MO$7,6,$E143)</f>
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="P143" s="13">
         <f t="shared" si="89"/>
-        <v>0</v>
+        <v>0.6978197486392087</v>
       </c>
       <c r="Q143" s="13">
         <f t="shared" si="90"/>
-        <v>0</v>
+        <v>0.3021802513607913</v>
       </c>
       <c r="R143">
         <f t="shared" si="73"/>
-        <v>194599</v>
+        <v>375</v>
       </c>
       <c r="S143">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>1085</v>
       </c>
       <c r="T143">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>184</v>
       </c>
       <c r="U143">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V143">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="W143">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="X143">
         <f t="shared" si="79"/>
-        <v>-1</v>
+        <v>0.124750499001996</v>
       </c>
       <c r="Y143">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>1.8189743331824507E-2</v>
       </c>
       <c r="Z143">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>1.0084469540467338</v>
       </c>
       <c r="AA143">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>1.0059701492537314</v>
       </c>
       <c r="AB143">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>1.0633019674935842</v>
       </c>
       <c r="AC143">
         <f t="shared" si="84"/>
-        <v>0</v>
+        <v>0.98101265822784811</v>
       </c>
       <c r="AD143">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>48325.559028612646</v>
       </c>
       <c r="AE143">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>14603.029574416927</v>
       </c>
       <c r="AF143">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>5281.7985092570334</v>
       </c>
       <c r="AG143">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>162.05818706419814</v>
       </c>
       <c r="AH143">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>298.86992065400341</v>
       </c>
       <c r="AI143">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>37.268574176484734</v>
       </c>
       <c r="AJ143">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>24039</v>
       </c>
       <c r="AK143">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>5779.9951911517192</v>
       </c>
       <c r="AL143">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ142</f>
-        <v>0</v>
+        <v>259</v>
       </c>
       <c r="AM143">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ142,0)</f>
-        <v>0</v>
+        <v>1.0891505466778806E-2</v>
       </c>
     </row>
     <row r="144" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A144" s="12" t="str">
         <f t="shared" si="85"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B144" s="12" t="str">
         <f t="shared" si="86"/>
@@ -26555,149 +26651,149 @@
       </c>
       <c r="F144" cm="1">
         <f t="array" ref="F144">+INDEX(Hoja1!$B$2:$MO$7,1,E144)</f>
-        <v>0</v>
+        <v>203600</v>
       </c>
       <c r="G144">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>2614</v>
       </c>
       <c r="H144" cm="1">
         <f t="array" ref="H144">+INDEX(Hoja1!$B$2:$MO$7,2,$E144)</f>
-        <v>0</v>
+        <v>142071</v>
       </c>
       <c r="I144">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>1819</v>
       </c>
       <c r="J144">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>61529</v>
       </c>
       <c r="K144">
         <f t="shared" si="72"/>
-        <v>0</v>
+        <v>795</v>
       </c>
       <c r="L144" cm="1">
         <f t="array" ref="L144">+INDEX(Hoja1!$B$2:$MO$7,3,$E144)</f>
-        <v>0</v>
+        <v>22110</v>
       </c>
       <c r="M144" cm="1">
         <f t="array" ref="M144">+INDEX(Hoja1!$B$2:$MO$7,4,$E144)</f>
-        <v>0</v>
+        <v>652</v>
       </c>
       <c r="N144" cm="1">
         <f t="array" ref="N144">+INDEX(Hoja1!$B$2:$MO$7,5,$E144)</f>
-        <v>0</v>
+        <v>1247</v>
       </c>
       <c r="O144" cm="1">
         <f t="array" ref="O144">+INDEX(Hoja1!$B$2:$MO$7,6,$E144)</f>
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="P144" s="13">
         <f t="shared" si="89"/>
-        <v>0</v>
+        <v>0.69779469548133599</v>
       </c>
       <c r="Q144" s="13">
         <f t="shared" si="90"/>
-        <v>0</v>
+        <v>0.30220530451866406</v>
       </c>
       <c r="R144">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>-767</v>
       </c>
       <c r="S144">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>795</v>
       </c>
       <c r="T144">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="U144">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>-22</v>
       </c>
       <c r="V144">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W144">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="X144">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>-0.22685595977521444</v>
       </c>
       <c r="Y144">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>1.3089867290150492E-2</v>
       </c>
       <c r="Z144">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>1.0065097646469705</v>
       </c>
       <c r="AA144">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>0.96735905044510384</v>
       </c>
       <c r="AB144">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>1.003218020917136</v>
       </c>
       <c r="AC144">
         <f t="shared" si="84"/>
-        <v>0</v>
+        <v>0.98064516129032253</v>
       </c>
       <c r="AD144">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>48954.075498918013</v>
       </c>
       <c r="AE144">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>14794.181293580188</v>
       </c>
       <c r="AF144">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>5316.1817744650161</v>
       </c>
       <c r="AG144">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>156.76845395527772</v>
       </c>
       <c r="AH144">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>299.8316903101707</v>
       </c>
       <c r="AI144">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>36.547246934359222</v>
       </c>
       <c r="AJ144">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>24161</v>
       </c>
       <c r="AK144">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>5809.3291656648234</v>
       </c>
       <c r="AL144">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ143</f>
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="AM144">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ143,0)</f>
-        <v>0</v>
+        <v>5.0750863180664754E-3</v>
       </c>
     </row>
     <row r="145" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A145" s="12" t="str">
         <f t="shared" si="85"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B145" s="12" t="str">
         <f t="shared" si="86"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C145" s="12">
         <v>139</v>
@@ -26712,139 +26808,139 @@
       </c>
       <c r="F145" cm="1">
         <f t="array" ref="F145">+INDEX(Hoja1!$B$2:$MO$7,1,E145)</f>
-        <v>0</v>
+        <v>207908</v>
       </c>
       <c r="G145">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>4308</v>
       </c>
       <c r="H145" cm="1">
         <f t="array" ref="H145">+INDEX(Hoja1!$B$2:$MO$7,2,$E145)</f>
-        <v>0</v>
+        <v>144913</v>
       </c>
       <c r="I145">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>2842</v>
       </c>
       <c r="J145">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>62995</v>
       </c>
       <c r="K145">
         <f t="shared" si="72"/>
-        <v>0</v>
+        <v>1466</v>
       </c>
       <c r="L145" cm="1">
         <f t="array" ref="L145">+INDEX(Hoja1!$B$2:$MO$7,3,$E145)</f>
-        <v>0</v>
+        <v>22803</v>
       </c>
       <c r="M145" cm="1">
         <f t="array" ref="M145">+INDEX(Hoja1!$B$2:$MO$7,4,$E145)</f>
-        <v>0</v>
+        <v>680</v>
       </c>
       <c r="N145" cm="1">
         <f t="array" ref="N145">+INDEX(Hoja1!$B$2:$MO$7,5,$E145)</f>
-        <v>0</v>
+        <v>1237</v>
       </c>
       <c r="O145" cm="1">
         <f t="array" ref="O145">+INDEX(Hoja1!$B$2:$MO$7,6,$E145)</f>
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="P145" s="13">
         <f t="shared" si="89"/>
-        <v>0</v>
+        <v>0.69700540623737417</v>
       </c>
       <c r="Q145" s="13">
         <f t="shared" si="90"/>
-        <v>0</v>
+        <v>0.30299459376262577</v>
       </c>
       <c r="R145">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>1694</v>
       </c>
       <c r="S145">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>1466</v>
       </c>
       <c r="T145">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>693</v>
       </c>
       <c r="U145">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="V145">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="W145">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X145">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>0.64804896710022952</v>
       </c>
       <c r="Y145">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>2.3826163272603163E-2</v>
       </c>
       <c r="Z145">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>1.0313432835820895</v>
       </c>
       <c r="AA145">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>1.0429447852760736</v>
       </c>
       <c r="AB145">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>0.99198075380914197</v>
       </c>
       <c r="AC145">
         <f t="shared" si="84"/>
-        <v>0</v>
+        <v>0.99342105263157898</v>
       </c>
       <c r="AD145">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>49989.901418610243</v>
       </c>
       <c r="AE145">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>15146.669872565521</v>
       </c>
       <c r="AF145">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>5482.8083673960091</v>
       </c>
       <c r="AG145">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>163.50084154844916</v>
       </c>
       <c r="AH145">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>297.42726616975239</v>
       </c>
       <c r="AI145">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>36.306804520317385</v>
       </c>
       <c r="AJ145">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>24871</v>
       </c>
       <c r="AK145">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>5980.0432796345276</v>
       </c>
       <c r="AL145">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ144</f>
-        <v>0</v>
+        <v>710</v>
       </c>
       <c r="AM145">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ144,0)</f>
-        <v>0</v>
+        <v>2.9386200902280536E-2</v>
       </c>
     </row>
     <row r="146" spans="1:39" x14ac:dyDescent="0.2">
@@ -26873,7 +26969,7 @@
       </c>
       <c r="G146">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>-207908</v>
       </c>
       <c r="H146" cm="1">
         <f t="array" ref="H146">+INDEX(Hoja1!$B$2:$MO$7,2,$E146)</f>
@@ -26881,7 +26977,7 @@
       </c>
       <c r="I146">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>-144913</v>
       </c>
       <c r="J146">
         <f t="shared" si="62"/>
@@ -26889,7 +26985,7 @@
       </c>
       <c r="K146">
         <f t="shared" si="72"/>
-        <v>0</v>
+        <v>-62995</v>
       </c>
       <c r="L146" cm="1">
         <f t="array" ref="L146">+INDEX(Hoja1!$B$2:$MO$7,3,$E146)</f>
@@ -26917,35 +27013,35 @@
       </c>
       <c r="R146">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>-212216</v>
       </c>
       <c r="S146">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>-62995</v>
       </c>
       <c r="T146">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>-22803</v>
       </c>
       <c r="U146">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>-680</v>
       </c>
       <c r="V146">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>-1237</v>
       </c>
       <c r="W146">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>-151</v>
       </c>
       <c r="X146">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>-49.260909935004641</v>
       </c>
       <c r="Y146">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z146">
         <f t="shared" si="81"/>
@@ -26997,11 +27093,11 @@
       </c>
       <c r="AL146">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ145</f>
-        <v>0</v>
+        <v>-24871</v>
       </c>
       <c r="AM146">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ145,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="147" spans="1:39" x14ac:dyDescent="0.2">
@@ -27074,7 +27170,7 @@
       </c>
       <c r="R147">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>207908</v>
       </c>
       <c r="S147">
         <f t="shared" si="74"/>
@@ -27098,7 +27194,7 @@
       </c>
       <c r="X147">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y147">
         <f t="shared" si="80"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-28-2020 00-40-13
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1729" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6A119A04-897A-3C46-83C1-D8D34277D5BB}"/>
+  <xr:revisionPtr revIDLastSave="1735" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D090C562-A94B-7349-A33F-8EB513357C04}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -1578,10 +1578,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B32E72-8F4B-408A-9B01-FAD2807C0C88}">
   <dimension ref="A1:EK52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="EI1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="EL3" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="EK2" sqref="EK2"/>
+      <selection pane="topRight" activeCell="EK8" sqref="EK8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2444,7 +2444,9 @@
       <c r="EJ2" s="8">
         <v>207908</v>
       </c>
-      <c r="EK2" s="8"/>
+      <c r="EK2" s="8">
+        <v>211373</v>
+      </c>
     </row>
     <row r="3" spans="1:141" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2867,7 +2869,9 @@
       <c r="EJ3" s="8">
         <v>144913</v>
       </c>
-      <c r="EK3" s="8"/>
+      <c r="EK3" s="8">
+        <v>147217</v>
+      </c>
     </row>
     <row r="4" spans="1:141" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -3290,7 +3294,9 @@
       <c r="EJ4" s="8">
         <v>22803</v>
       </c>
-      <c r="EK4" s="8"/>
+      <c r="EK4" s="8">
+        <v>22898</v>
+      </c>
     </row>
     <row r="5" spans="1:141" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -3622,7 +3628,9 @@
       <c r="EJ5" s="8">
         <v>680</v>
       </c>
-      <c r="EK5" s="8"/>
+      <c r="EK5" s="8">
+        <v>726</v>
+      </c>
     </row>
     <row r="6" spans="1:141" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -4041,7 +4049,9 @@
       <c r="EJ6" s="8">
         <v>1237</v>
       </c>
-      <c r="EK6" s="8"/>
+      <c r="EK6" s="8">
+        <v>1255</v>
+      </c>
     </row>
     <row r="7" spans="1:141" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -4462,7 +4472,9 @@
       <c r="EJ7" s="8">
         <v>151</v>
       </c>
-      <c r="EK7" s="8"/>
+      <c r="EK7" s="8">
+        <v>155</v>
+      </c>
     </row>
     <row r="8" spans="1:141" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
@@ -5063,7 +5075,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -26793,7 +26805,7 @@
       </c>
       <c r="B145" s="12" t="str">
         <f t="shared" si="86"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C145" s="12">
         <v>139</v>
@@ -26946,11 +26958,11 @@
     <row r="146" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A146" s="12" t="str">
         <f t="shared" si="85"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B146" s="12" t="str">
         <f t="shared" si="86"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C146" s="12">
         <v>140</v>
@@ -26965,139 +26977,139 @@
       </c>
       <c r="F146" cm="1">
         <f t="array" ref="F146">+INDEX(Hoja1!$B$2:$MO$7,1,E146)</f>
-        <v>0</v>
+        <v>211373</v>
       </c>
       <c r="G146">
         <f t="shared" si="70"/>
-        <v>-207908</v>
+        <v>3465</v>
       </c>
       <c r="H146" cm="1">
         <f t="array" ref="H146">+INDEX(Hoja1!$B$2:$MO$7,2,$E146)</f>
-        <v>0</v>
+        <v>147217</v>
       </c>
       <c r="I146">
         <f t="shared" si="71"/>
-        <v>-144913</v>
+        <v>2304</v>
       </c>
       <c r="J146">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>64156</v>
       </c>
       <c r="K146">
         <f t="shared" si="72"/>
-        <v>-62995</v>
+        <v>1161</v>
       </c>
       <c r="L146" cm="1">
         <f t="array" ref="L146">+INDEX(Hoja1!$B$2:$MO$7,3,$E146)</f>
-        <v>0</v>
+        <v>22898</v>
       </c>
       <c r="M146" cm="1">
         <f t="array" ref="M146">+INDEX(Hoja1!$B$2:$MO$7,4,$E146)</f>
-        <v>0</v>
+        <v>726</v>
       </c>
       <c r="N146" cm="1">
         <f t="array" ref="N146">+INDEX(Hoja1!$B$2:$MO$7,5,$E146)</f>
-        <v>0</v>
+        <v>1255</v>
       </c>
       <c r="O146" cm="1">
         <f t="array" ref="O146">+INDEX(Hoja1!$B$2:$MO$7,6,$E146)</f>
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="P146" s="13">
         <f t="shared" si="89"/>
-        <v>0</v>
+        <v>0.69647968283555606</v>
       </c>
       <c r="Q146" s="13">
         <f t="shared" si="90"/>
-        <v>0</v>
+        <v>0.30352031716444389</v>
       </c>
       <c r="R146">
         <f t="shared" si="73"/>
-        <v>-212216</v>
+        <v>-843</v>
       </c>
       <c r="S146">
         <f t="shared" si="74"/>
-        <v>-62995</v>
+        <v>1161</v>
       </c>
       <c r="T146">
         <f t="shared" si="75"/>
-        <v>-22803</v>
+        <v>95</v>
       </c>
       <c r="U146">
         <f t="shared" si="76"/>
-        <v>-680</v>
+        <v>46</v>
       </c>
       <c r="V146">
         <f t="shared" si="77"/>
-        <v>-1237</v>
+        <v>18</v>
       </c>
       <c r="W146">
         <f t="shared" si="78"/>
-        <v>-151</v>
+        <v>4</v>
       </c>
       <c r="X146">
         <f t="shared" si="79"/>
-        <v>-49.260909935004641</v>
+        <v>-0.19568245125348188</v>
       </c>
       <c r="Y146">
         <f t="shared" si="80"/>
-        <v>-1</v>
+        <v>1.8430034129692834E-2</v>
       </c>
       <c r="Z146">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>1.0041661184931807</v>
       </c>
       <c r="AA146">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>1.0676470588235294</v>
       </c>
       <c r="AB146">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>1.0145513338722716</v>
       </c>
       <c r="AC146">
         <f t="shared" si="84"/>
-        <v>0</v>
+        <v>1.0264900662251655</v>
       </c>
       <c r="AD146">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>50823.034383265207</v>
       </c>
       <c r="AE146">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>15425.823515268094</v>
       </c>
       <c r="AF146">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>5505.6503967299832</v>
       </c>
       <c r="AG146">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>174.56119259437367</v>
       </c>
       <c r="AH146">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>301.7552296225054</v>
       </c>
       <c r="AI146">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>37.268574176484734</v>
       </c>
       <c r="AJ146">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>25034</v>
       </c>
       <c r="AK146">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>6019.2353931233474</v>
       </c>
       <c r="AL146">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ145</f>
-        <v>-24871</v>
+        <v>163</v>
       </c>
       <c r="AM146">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ145,0)</f>
-        <v>-1</v>
+        <v>6.5538176993285352E-3</v>
       </c>
     </row>
     <row r="147" spans="1:39" x14ac:dyDescent="0.2">
@@ -27126,7 +27138,7 @@
       </c>
       <c r="G147">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>-211373</v>
       </c>
       <c r="H147" cm="1">
         <f t="array" ref="H147">+INDEX(Hoja1!$B$2:$MO$7,2,$E147)</f>
@@ -27134,7 +27146,7 @@
       </c>
       <c r="I147">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>-147217</v>
       </c>
       <c r="J147">
         <f t="shared" si="62"/>
@@ -27142,7 +27154,7 @@
       </c>
       <c r="K147">
         <f t="shared" si="72"/>
-        <v>0</v>
+        <v>-64156</v>
       </c>
       <c r="L147" cm="1">
         <f t="array" ref="L147">+INDEX(Hoja1!$B$2:$MO$7,3,$E147)</f>
@@ -27170,35 +27182,35 @@
       </c>
       <c r="R147">
         <f t="shared" si="73"/>
-        <v>207908</v>
+        <v>-214838</v>
       </c>
       <c r="S147">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>-64156</v>
       </c>
       <c r="T147">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>-22898</v>
       </c>
       <c r="U147">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>-726</v>
       </c>
       <c r="V147">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>-1255</v>
       </c>
       <c r="W147">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>-155</v>
       </c>
       <c r="X147">
         <f t="shared" si="79"/>
-        <v>-1</v>
+        <v>-62.002308802308804</v>
       </c>
       <c r="Y147">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z147">
         <f t="shared" si="81"/>
@@ -27250,11 +27262,11 @@
       </c>
       <c r="AL147">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ146</f>
-        <v>0</v>
+        <v>-25034</v>
       </c>
       <c r="AM147">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ146,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="148" spans="1:39" x14ac:dyDescent="0.2">
@@ -27327,7 +27339,7 @@
       </c>
       <c r="R148">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>211373</v>
       </c>
       <c r="S148">
         <f t="shared" si="74"/>
@@ -27351,7 +27363,7 @@
       </c>
       <c r="X148">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y148">
         <f t="shared" si="80"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-29-2020 04-43-14
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1735" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D090C562-A94B-7349-A33F-8EB513357C04}"/>
+  <xr:revisionPtr revIDLastSave="1739" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{977F587F-01D8-B94C-BC62-3959A1DA826D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="183">
   <si>
     <t>Columna1</t>
   </si>
@@ -597,6 +597,12 @@
   <si>
     <t>27-07-20</t>
   </si>
+  <si>
+    <t>27-07-22</t>
+  </si>
+  <si>
+    <t>28-07-20</t>
+  </si>
 </sst>
 </file>
 
@@ -719,7 +725,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="58">
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1010,9 +1022,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:EK7" totalsRowShown="0">
-  <autoFilter ref="A1:EK7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
-  <tableColumns count="141">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:EM7" totalsRowShown="0">
+  <autoFilter ref="A1:EM7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
+  <tableColumns count="143">
     <tableColumn id="76" xr3:uid="{CA01250B-8685-4250-AAEF-D6E482663B6F}" name="Columna1"/>
     <tableColumn id="77" xr3:uid="{BC38B0B2-3229-42F8-9C9A-52EE74902839}" name="10-03-2020"/>
     <tableColumn id="78" xr3:uid="{4BB74E2E-62F3-4EED-8537-96C80CD1ED37}" name="11-03-2020"/>
@@ -1106,74 +1118,76 @@
     <tableColumn id="4" xr3:uid="{2FE879E2-2128-42AE-A0E3-647EE2D0C94F}" name="07-06-2020"/>
     <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="08-06-2020"/>
     <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-2020"/>
-    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="55"/>
-    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="54"/>
-    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="53"/>
-    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="52"/>
-    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="51"/>
-    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="50"/>
-    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="49"/>
-    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="48"/>
-    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="47"/>
-    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="46"/>
-    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="45"/>
-    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="44"/>
-    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="43"/>
-    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="42"/>
-    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="41"/>
-    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="40"/>
-    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="39"/>
-    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="38"/>
-    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="37"/>
-    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="36"/>
-    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="35"/>
-    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="34"/>
-    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="33"/>
-    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="32"/>
-    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="31"/>
-    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="30"/>
-    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="29"/>
-    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="28"/>
-    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="27"/>
-    <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="26"/>
-    <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="10-07-20" dataDxfId="25"/>
-    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="11-07-20" dataDxfId="24"/>
-    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="12-07-20" dataDxfId="23"/>
-    <tableColumn id="127" xr3:uid="{2B284A50-3213-EF46-904E-73679622D22C}" name="13-07-20" dataDxfId="22"/>
-    <tableColumn id="128" xr3:uid="{30C66AA6-47A6-FB40-A335-1BA9A696E85B}" name="14-07-20" dataDxfId="21"/>
-    <tableColumn id="129" xr3:uid="{041D18C8-807A-0949-898D-C4880EDA94DD}" name="15-07-20" dataDxfId="20"/>
-    <tableColumn id="130" xr3:uid="{61B56DA5-913C-EF4F-B703-9A52B436E7DD}" name="16-07-20" dataDxfId="19"/>
-    <tableColumn id="131" xr3:uid="{877B5AA5-D97A-8D40-B352-6FFA59645351}" name="17-07-20" dataDxfId="18"/>
-    <tableColumn id="132" xr3:uid="{3FADF8C3-57FC-5D47-913A-C0C36C8E59FE}" name="18-07-20" dataDxfId="17"/>
-    <tableColumn id="133" xr3:uid="{1226D8E9-4582-2342-A7CC-4D09D093B768}" name="19-07-20" dataDxfId="16"/>
-    <tableColumn id="134" xr3:uid="{7101E8B8-49A5-1A49-8532-994B0A3FB01B}" name="20-07-20" dataDxfId="15"/>
-    <tableColumn id="135" xr3:uid="{94611A1B-D923-9546-A8DC-9CCC7B65A729}" name="21-07-20" dataDxfId="14"/>
-    <tableColumn id="136" xr3:uid="{58AE38DE-BFD7-4249-AB7A-15BF37E8B591}" name="22-07-20" dataDxfId="13"/>
-    <tableColumn id="137" xr3:uid="{55C5FB87-1CA4-3F45-887B-DBB3DAAA5369}" name="23-07-20" dataDxfId="12"/>
-    <tableColumn id="138" xr3:uid="{437CA53C-B11E-BF47-AF09-040913B3FCD0}" name="24-07-20" dataDxfId="11"/>
-    <tableColumn id="139" xr3:uid="{202231FA-82F9-BF4E-8D60-B218C26A354A}" name="25-07-20" dataDxfId="10"/>
-    <tableColumn id="140" xr3:uid="{24F2106B-9F5D-1E4C-A42B-E2AA613BEE08}" name="26-07-20" dataDxfId="9"/>
-    <tableColumn id="141" xr3:uid="{8BDBD0BC-D9B1-B445-9A72-EF935A438E09}" name="27-07-20" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="56"/>
+    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="55"/>
+    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="54"/>
+    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="53"/>
+    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="52"/>
+    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="51"/>
+    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="50"/>
+    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="49"/>
+    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="48"/>
+    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="47"/>
+    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="46"/>
+    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="45"/>
+    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="44"/>
+    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="43"/>
+    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="42"/>
+    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="41"/>
+    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="40"/>
+    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="39"/>
+    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="38"/>
+    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="37"/>
+    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="36"/>
+    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="35"/>
+    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="34"/>
+    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="33"/>
+    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="32"/>
+    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="31"/>
+    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="30"/>
+    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="29"/>
+    <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="28"/>
+    <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="10-07-20" dataDxfId="27"/>
+    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="11-07-20" dataDxfId="26"/>
+    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="12-07-20" dataDxfId="25"/>
+    <tableColumn id="127" xr3:uid="{2B284A50-3213-EF46-904E-73679622D22C}" name="13-07-20" dataDxfId="24"/>
+    <tableColumn id="128" xr3:uid="{30C66AA6-47A6-FB40-A335-1BA9A696E85B}" name="14-07-20" dataDxfId="23"/>
+    <tableColumn id="129" xr3:uid="{041D18C8-807A-0949-898D-C4880EDA94DD}" name="15-07-20" dataDxfId="22"/>
+    <tableColumn id="130" xr3:uid="{61B56DA5-913C-EF4F-B703-9A52B436E7DD}" name="16-07-20" dataDxfId="21"/>
+    <tableColumn id="131" xr3:uid="{877B5AA5-D97A-8D40-B352-6FFA59645351}" name="17-07-20" dataDxfId="20"/>
+    <tableColumn id="132" xr3:uid="{3FADF8C3-57FC-5D47-913A-C0C36C8E59FE}" name="18-07-20" dataDxfId="19"/>
+    <tableColumn id="133" xr3:uid="{1226D8E9-4582-2342-A7CC-4D09D093B768}" name="19-07-20" dataDxfId="18"/>
+    <tableColumn id="134" xr3:uid="{7101E8B8-49A5-1A49-8532-994B0A3FB01B}" name="20-07-20" dataDxfId="17"/>
+    <tableColumn id="135" xr3:uid="{94611A1B-D923-9546-A8DC-9CCC7B65A729}" name="21-07-20" dataDxfId="16"/>
+    <tableColumn id="136" xr3:uid="{58AE38DE-BFD7-4249-AB7A-15BF37E8B591}" name="22-07-20" dataDxfId="15"/>
+    <tableColumn id="137" xr3:uid="{55C5FB87-1CA4-3F45-887B-DBB3DAAA5369}" name="23-07-20" dataDxfId="14"/>
+    <tableColumn id="138" xr3:uid="{437CA53C-B11E-BF47-AF09-040913B3FCD0}" name="24-07-20" dataDxfId="13"/>
+    <tableColumn id="139" xr3:uid="{202231FA-82F9-BF4E-8D60-B218C26A354A}" name="25-07-20" dataDxfId="12"/>
+    <tableColumn id="140" xr3:uid="{24F2106B-9F5D-1E4C-A42B-E2AA613BEE08}" name="26-07-20" dataDxfId="11"/>
+    <tableColumn id="141" xr3:uid="{8BDBD0BC-D9B1-B445-9A72-EF935A438E09}" name="27-07-20" dataDxfId="10"/>
+    <tableColumn id="142" xr3:uid="{6A7EFE4A-AA3A-C34C-891A-3E9FCC0E701D}" name="28-07-20" dataDxfId="1"/>
+    <tableColumn id="143" xr3:uid="{68B87CBE-2A2E-ED49-BF07-4D169F13B444}" name="27-07-22" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="8">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="7">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="5">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="4">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -1206,10 +1220,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="1">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="3">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="2">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1576,12 +1590,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B32E72-8F4B-408A-9B01-FAD2807C0C88}">
-  <dimension ref="A1:EK52"/>
+  <dimension ref="A1:EM52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="EL3" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="EJ1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="EK8" sqref="EK8"/>
+      <selection pane="topRight" activeCell="EL2" sqref="EL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1598,7 +1612,7 @@
     <col min="116" max="118" width="11.43359375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:141" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2022,8 +2036,14 @@
       <c r="EK1" s="1" t="s">
         <v>179</v>
       </c>
+      <c r="EL1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="EM1" t="s">
+        <v>180</v>
+      </c>
     </row>
-    <row r="2" spans="1:141" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2447,8 +2467,10 @@
       <c r="EK2" s="8">
         <v>211373</v>
       </c>
+      <c r="EL2" s="8"/>
+      <c r="EM2" s="8"/>
     </row>
-    <row r="3" spans="1:141" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -2872,8 +2894,10 @@
       <c r="EK3" s="8">
         <v>147217</v>
       </c>
+      <c r="EL3" s="8"/>
+      <c r="EM3" s="8"/>
     </row>
-    <row r="4" spans="1:141" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -3297,8 +3321,10 @@
       <c r="EK4" s="8">
         <v>22898</v>
       </c>
+      <c r="EL4" s="8"/>
+      <c r="EM4" s="8"/>
     </row>
-    <row r="5" spans="1:141" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -3631,8 +3657,10 @@
       <c r="EK5" s="8">
         <v>726</v>
       </c>
+      <c r="EL5" s="8"/>
+      <c r="EM5" s="8"/>
     </row>
-    <row r="6" spans="1:141" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -4052,8 +4080,10 @@
       <c r="EK6" s="8">
         <v>1255</v>
       </c>
+      <c r="EL6" s="8"/>
+      <c r="EM6" s="8"/>
     </row>
-    <row r="7" spans="1:141" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -4475,8 +4505,10 @@
       <c r="EK7" s="8">
         <v>155</v>
       </c>
+      <c r="EL7" s="8"/>
+      <c r="EM7" s="8"/>
     </row>
-    <row r="8" spans="1:141" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4587,28 +4619,28 @@
       <c r="EC8" s="8"/>
       <c r="ED8" s="8"/>
     </row>
-    <row r="9" spans="1:141" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:143" x14ac:dyDescent="0.2">
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:141" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:143" x14ac:dyDescent="0.2">
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:141" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:143" x14ac:dyDescent="0.2">
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:141" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:143" x14ac:dyDescent="0.2">
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:141" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:143" x14ac:dyDescent="0.2">
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:141" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:143" x14ac:dyDescent="0.2">
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:141" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:143" x14ac:dyDescent="0.2">
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:141" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:143" x14ac:dyDescent="0.2">
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-30-2020 00-45-30
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1739" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{977F587F-01D8-B94C-BC62-3959A1DA826D}"/>
+  <xr:revisionPtr revIDLastSave="1752" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7D2C3325-E848-CB4F-A66B-80A9780F8C59}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -598,10 +598,10 @@
     <t>27-07-20</t>
   </si>
   <si>
-    <t>27-07-22</t>
+    <t>28-07-20</t>
   </si>
   <si>
-    <t>28-07-20</t>
+    <t>29-07-20</t>
   </si>
 </sst>
 </file>
@@ -727,12 +727,6 @@
   </cellStyles>
   <dxfs count="58">
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -851,6 +845,12 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
@@ -1166,28 +1166,28 @@
     <tableColumn id="139" xr3:uid="{202231FA-82F9-BF4E-8D60-B218C26A354A}" name="25-07-20" dataDxfId="12"/>
     <tableColumn id="140" xr3:uid="{24F2106B-9F5D-1E4C-A42B-E2AA613BEE08}" name="26-07-20" dataDxfId="11"/>
     <tableColumn id="141" xr3:uid="{8BDBD0BC-D9B1-B445-9A72-EF935A438E09}" name="27-07-20" dataDxfId="10"/>
-    <tableColumn id="142" xr3:uid="{6A7EFE4A-AA3A-C34C-891A-3E9FCC0E701D}" name="28-07-20" dataDxfId="1"/>
-    <tableColumn id="143" xr3:uid="{68B87CBE-2A2E-ED49-BF07-4D169F13B444}" name="27-07-22" dataDxfId="0"/>
+    <tableColumn id="142" xr3:uid="{6A7EFE4A-AA3A-C34C-891A-3E9FCC0E701D}" name="28-07-20" dataDxfId="9"/>
+    <tableColumn id="143" xr3:uid="{68B87CBE-2A2E-ED49-BF07-4D169F13B444}" name="29-07-20" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="6">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="5">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="5">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="3">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="4">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="2">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -1220,10 +1220,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="3">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="1">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="2">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="0">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1593,9 +1593,9 @@
   <dimension ref="A1:EM52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="EJ1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="EK1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="EL2" sqref="EL2"/>
+      <selection pane="topRight" activeCell="EM1" sqref="EM1:EM7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2037,10 +2037,10 @@
         <v>179</v>
       </c>
       <c r="EL1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="EM1" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="EM1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:143" x14ac:dyDescent="0.2">
@@ -2467,8 +2467,12 @@
       <c r="EK2" s="8">
         <v>211373</v>
       </c>
-      <c r="EL2" s="8"/>
-      <c r="EM2" s="8"/>
+      <c r="EL2" s="8">
+        <v>213597</v>
+      </c>
+      <c r="EM2" s="8">
+        <v>216730</v>
+      </c>
     </row>
     <row r="3" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2894,8 +2898,12 @@
       <c r="EK3" s="8">
         <v>147217</v>
       </c>
-      <c r="EL3" s="8"/>
-      <c r="EM3" s="8"/>
+      <c r="EL3" s="8">
+        <v>148715</v>
+      </c>
+      <c r="EM3" s="8">
+        <v>150836</v>
+      </c>
     </row>
     <row r="4" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -3321,8 +3329,12 @@
       <c r="EK4" s="8">
         <v>22898</v>
       </c>
-      <c r="EL4" s="8"/>
-      <c r="EM4" s="8"/>
+      <c r="EL4" s="8">
+        <v>22577</v>
+      </c>
+      <c r="EM4" s="8">
+        <v>22430</v>
+      </c>
     </row>
     <row r="5" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -3657,8 +3669,12 @@
       <c r="EK5" s="8">
         <v>726</v>
       </c>
-      <c r="EL5" s="8"/>
-      <c r="EM5" s="8"/>
+      <c r="EL5" s="8">
+        <v>694</v>
+      </c>
+      <c r="EM5" s="8">
+        <v>689</v>
+      </c>
     </row>
     <row r="6" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -4080,8 +4096,12 @@
       <c r="EK6" s="8">
         <v>1255</v>
       </c>
-      <c r="EL6" s="8"/>
-      <c r="EM6" s="8"/>
+      <c r="EL6" s="8">
+        <v>1274</v>
+      </c>
+      <c r="EM6" s="8">
+        <v>1302</v>
+      </c>
     </row>
     <row r="7" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -4505,8 +4525,12 @@
       <c r="EK7" s="8">
         <v>155</v>
       </c>
-      <c r="EL7" s="8"/>
-      <c r="EM7" s="8"/>
+      <c r="EL7" s="8">
+        <v>148</v>
+      </c>
+      <c r="EM7" s="8">
+        <v>158</v>
+      </c>
     </row>
     <row r="8" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
@@ -5107,7 +5131,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44039</v>
+        <v>44041</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -26994,7 +27018,7 @@
       </c>
       <c r="B146" s="12" t="str">
         <f t="shared" si="86"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C146" s="12">
         <v>140</v>
@@ -27147,7 +27171,7 @@
     <row r="147" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A147" s="12" t="str">
         <f t="shared" si="85"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B147" s="12" t="str">
         <f t="shared" si="86"/>
@@ -27166,149 +27190,149 @@
       </c>
       <c r="F147" cm="1">
         <f t="array" ref="F147">+INDEX(Hoja1!$B$2:$MO$7,1,E147)</f>
-        <v>0</v>
+        <v>213597</v>
       </c>
       <c r="G147">
         <f t="shared" si="70"/>
-        <v>-211373</v>
+        <v>2224</v>
       </c>
       <c r="H147" cm="1">
         <f t="array" ref="H147">+INDEX(Hoja1!$B$2:$MO$7,2,$E147)</f>
-        <v>0</v>
+        <v>148715</v>
       </c>
       <c r="I147">
         <f t="shared" si="71"/>
-        <v>-147217</v>
+        <v>1498</v>
       </c>
       <c r="J147">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>64882</v>
       </c>
       <c r="K147">
         <f t="shared" si="72"/>
-        <v>-64156</v>
+        <v>726</v>
       </c>
       <c r="L147" cm="1">
         <f t="array" ref="L147">+INDEX(Hoja1!$B$2:$MO$7,3,$E147)</f>
-        <v>0</v>
+        <v>22577</v>
       </c>
       <c r="M147" cm="1">
         <f t="array" ref="M147">+INDEX(Hoja1!$B$2:$MO$7,4,$E147)</f>
-        <v>0</v>
+        <v>694</v>
       </c>
       <c r="N147" cm="1">
         <f t="array" ref="N147">+INDEX(Hoja1!$B$2:$MO$7,5,$E147)</f>
-        <v>0</v>
+        <v>1274</v>
       </c>
       <c r="O147" cm="1">
         <f t="array" ref="O147">+INDEX(Hoja1!$B$2:$MO$7,6,$E147)</f>
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="P147" s="13">
         <f t="shared" si="89"/>
-        <v>0</v>
+        <v>0.69624105207470144</v>
       </c>
       <c r="Q147" s="13">
         <f t="shared" si="90"/>
-        <v>0</v>
+        <v>0.30375894792529856</v>
       </c>
       <c r="R147">
         <f t="shared" si="73"/>
-        <v>-214838</v>
+        <v>-1241</v>
       </c>
       <c r="S147">
         <f t="shared" si="74"/>
-        <v>-64156</v>
+        <v>726</v>
       </c>
       <c r="T147">
         <f t="shared" si="75"/>
-        <v>-22898</v>
+        <v>-321</v>
       </c>
       <c r="U147">
         <f t="shared" si="76"/>
-        <v>-726</v>
+        <v>-32</v>
       </c>
       <c r="V147">
         <f t="shared" si="77"/>
-        <v>-1255</v>
+        <v>19</v>
       </c>
       <c r="W147">
         <f t="shared" si="78"/>
-        <v>-155</v>
+        <v>-7</v>
       </c>
       <c r="X147">
         <f t="shared" si="79"/>
-        <v>-62.002308802308804</v>
+        <v>-0.35815295815295817</v>
       </c>
       <c r="Y147">
         <f t="shared" si="80"/>
-        <v>-1</v>
+        <v>1.1316166843319408E-2</v>
       </c>
       <c r="Z147">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>0.98598130841121501</v>
       </c>
       <c r="AA147">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>0.9559228650137741</v>
       </c>
       <c r="AB147">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>1.0151394422310758</v>
       </c>
       <c r="AC147">
         <f t="shared" si="84"/>
-        <v>0</v>
+        <v>0.95483870967741935</v>
       </c>
       <c r="AD147">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>51357.778312094255</v>
       </c>
       <c r="AE147">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>15600.384707862468</v>
       </c>
       <c r="AF147">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>5428.468381822554</v>
       </c>
       <c r="AG147">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>166.86703534503488</v>
       </c>
       <c r="AH147">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>306.32363548930033</v>
       </c>
       <c r="AI147">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>35.585477278191874</v>
       </c>
       <c r="AJ147">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>24693</v>
       </c>
       <c r="AK147">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>5937.2445299350811</v>
       </c>
       <c r="AL147">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ146</f>
-        <v>-25034</v>
+        <v>-341</v>
       </c>
       <c r="AM147">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ146,0)</f>
-        <v>-1</v>
+        <v>-1.3621474794279779E-2</v>
       </c>
     </row>
     <row r="148" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A148" s="12" t="str">
         <f t="shared" si="85"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B148" s="12" t="str">
         <f t="shared" si="86"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C148" s="12">
         <v>142</v>
@@ -27323,139 +27347,139 @@
       </c>
       <c r="F148" cm="1">
         <f t="array" ref="F148">+INDEX(Hoja1!$B$2:$MO$7,1,E148)</f>
-        <v>0</v>
+        <v>216730</v>
       </c>
       <c r="G148">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>3133</v>
       </c>
       <c r="H148" cm="1">
         <f t="array" ref="H148">+INDEX(Hoja1!$B$2:$MO$7,2,$E148)</f>
-        <v>0</v>
+        <v>150836</v>
       </c>
       <c r="I148">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>2121</v>
       </c>
       <c r="J148">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>65894</v>
       </c>
       <c r="K148">
         <f t="shared" si="72"/>
-        <v>0</v>
+        <v>1012</v>
       </c>
       <c r="L148" cm="1">
         <f t="array" ref="L148">+INDEX(Hoja1!$B$2:$MO$7,3,$E148)</f>
-        <v>0</v>
+        <v>22430</v>
       </c>
       <c r="M148" cm="1">
         <f t="array" ref="M148">+INDEX(Hoja1!$B$2:$MO$7,4,$E148)</f>
-        <v>0</v>
+        <v>689</v>
       </c>
       <c r="N148" cm="1">
         <f t="array" ref="N148">+INDEX(Hoja1!$B$2:$MO$7,5,$E148)</f>
-        <v>0</v>
+        <v>1302</v>
       </c>
       <c r="O148" cm="1">
         <f t="array" ref="O148">+INDEX(Hoja1!$B$2:$MO$7,6,$E148)</f>
-        <v>0</v>
+        <v>158</v>
       </c>
       <c r="P148" s="13">
         <f t="shared" si="89"/>
-        <v>0</v>
+        <v>0.69596271858995062</v>
       </c>
       <c r="Q148" s="13">
         <f t="shared" si="90"/>
-        <v>0</v>
+        <v>0.30403728141004938</v>
       </c>
       <c r="R148">
         <f t="shared" si="73"/>
-        <v>211373</v>
+        <v>909</v>
       </c>
       <c r="S148">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>1012</v>
       </c>
       <c r="T148">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>-147</v>
       </c>
       <c r="U148">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="V148">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="W148">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X148">
         <f t="shared" si="79"/>
-        <v>-1</v>
+        <v>0.40872302158273383</v>
       </c>
       <c r="Y148">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>1.5597546314848495E-2</v>
       </c>
       <c r="Z148">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>0.99348894893032735</v>
       </c>
       <c r="AA148">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>0.99279538904899134</v>
       </c>
       <c r="AB148">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>1.0219780219780219</v>
       </c>
       <c r="AC148">
         <f t="shared" si="84"/>
-        <v>0</v>
+        <v>1.0675675675675675</v>
       </c>
       <c r="AD148">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>52111.084395287333</v>
       </c>
       <c r="AE148">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>15843.712430872807</v>
       </c>
       <c r="AF148">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>5393.123346958404</v>
       </c>
       <c r="AG148">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>165.66482327482569</v>
       </c>
       <c r="AH148">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>313.05602308247177</v>
       </c>
       <c r="AI148">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>37.989901418610245</v>
       </c>
       <c r="AJ148">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>24579</v>
       </c>
       <c r="AK148">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>5909.8340947343113</v>
       </c>
       <c r="AL148">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ147</f>
-        <v>0</v>
+        <v>-114</v>
       </c>
       <c r="AM148">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ147,0)</f>
-        <v>0</v>
+        <v>-4.6166929899161702E-3</v>
       </c>
     </row>
     <row r="149" spans="1:39" x14ac:dyDescent="0.2">
@@ -27484,7 +27508,7 @@
       </c>
       <c r="G149">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>-216730</v>
       </c>
       <c r="H149" cm="1">
         <f t="array" ref="H149">+INDEX(Hoja1!$B$2:$MO$7,2,$E149)</f>
@@ -27492,7 +27516,7 @@
       </c>
       <c r="I149">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>-150836</v>
       </c>
       <c r="J149">
         <f t="shared" si="62"/>
@@ -27500,7 +27524,7 @@
       </c>
       <c r="K149">
         <f t="shared" si="72"/>
-        <v>0</v>
+        <v>-65894</v>
       </c>
       <c r="L149" cm="1">
         <f t="array" ref="L149">+INDEX(Hoja1!$B$2:$MO$7,3,$E149)</f>
@@ -27528,35 +27552,35 @@
       </c>
       <c r="R149">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>-219863</v>
       </c>
       <c r="S149">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>-65894</v>
       </c>
       <c r="T149">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>-22430</v>
       </c>
       <c r="U149">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>-689</v>
       </c>
       <c r="V149">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>-1302</v>
       </c>
       <c r="W149">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>-158</v>
       </c>
       <c r="X149">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>-70.176508139163744</v>
       </c>
       <c r="Y149">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z149">
         <f t="shared" si="81"/>
@@ -27608,11 +27632,11 @@
       </c>
       <c r="AL149">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ148</f>
-        <v>0</v>
+        <v>-24579</v>
       </c>
       <c r="AM149">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ148,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="150" spans="1:39" x14ac:dyDescent="0.2">
@@ -27685,7 +27709,7 @@
       </c>
       <c r="R150">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>216730</v>
       </c>
       <c r="S150">
         <f t="shared" si="74"/>
@@ -27709,7 +27733,7 @@
       </c>
       <c r="X150">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y150">
         <f t="shared" si="80"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-01-2020 04-52-10
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1752" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7D2C3325-E848-CB4F-A66B-80A9780F8C59}"/>
+  <xr:revisionPtr revIDLastSave="1754" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DBCBC4C5-C09B-BD42-ADF7-B2B89210EC04}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="185">
   <si>
     <t>Columna1</t>
   </si>
@@ -603,6 +603,12 @@
   <si>
     <t>29-07-20</t>
   </si>
+  <si>
+    <t>29-07-22</t>
+  </si>
+  <si>
+    <t>30-07-20</t>
+  </si>
 </sst>
 </file>
 
@@ -725,7 +731,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="60">
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1022,9 +1034,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:EM7" totalsRowShown="0">
-  <autoFilter ref="A1:EM7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
-  <tableColumns count="143">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:EO7" totalsRowShown="0">
+  <autoFilter ref="A1:EO7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
+  <tableColumns count="145">
     <tableColumn id="76" xr3:uid="{CA01250B-8685-4250-AAEF-D6E482663B6F}" name="Columna1"/>
     <tableColumn id="77" xr3:uid="{BC38B0B2-3229-42F8-9C9A-52EE74902839}" name="10-03-2020"/>
     <tableColumn id="78" xr3:uid="{4BB74E2E-62F3-4EED-8537-96C80CD1ED37}" name="11-03-2020"/>
@@ -1118,76 +1130,78 @@
     <tableColumn id="4" xr3:uid="{2FE879E2-2128-42AE-A0E3-647EE2D0C94F}" name="07-06-2020"/>
     <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="08-06-2020"/>
     <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-2020"/>
-    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="57"/>
-    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="56"/>
-    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="55"/>
-    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="54"/>
-    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="53"/>
-    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="52"/>
-    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="51"/>
-    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="50"/>
-    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="49"/>
-    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="48"/>
-    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="47"/>
-    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="46"/>
-    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="45"/>
-    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="44"/>
-    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="43"/>
-    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="42"/>
-    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="41"/>
-    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="40"/>
-    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="39"/>
-    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="38"/>
-    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="37"/>
-    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="36"/>
-    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="35"/>
-    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="34"/>
-    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="33"/>
-    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="32"/>
-    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="31"/>
-    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="30"/>
-    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="29"/>
-    <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="28"/>
-    <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="10-07-20" dataDxfId="27"/>
-    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="11-07-20" dataDxfId="26"/>
-    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="12-07-20" dataDxfId="25"/>
-    <tableColumn id="127" xr3:uid="{2B284A50-3213-EF46-904E-73679622D22C}" name="13-07-20" dataDxfId="24"/>
-    <tableColumn id="128" xr3:uid="{30C66AA6-47A6-FB40-A335-1BA9A696E85B}" name="14-07-20" dataDxfId="23"/>
-    <tableColumn id="129" xr3:uid="{041D18C8-807A-0949-898D-C4880EDA94DD}" name="15-07-20" dataDxfId="22"/>
-    <tableColumn id="130" xr3:uid="{61B56DA5-913C-EF4F-B703-9A52B436E7DD}" name="16-07-20" dataDxfId="21"/>
-    <tableColumn id="131" xr3:uid="{877B5AA5-D97A-8D40-B352-6FFA59645351}" name="17-07-20" dataDxfId="20"/>
-    <tableColumn id="132" xr3:uid="{3FADF8C3-57FC-5D47-913A-C0C36C8E59FE}" name="18-07-20" dataDxfId="19"/>
-    <tableColumn id="133" xr3:uid="{1226D8E9-4582-2342-A7CC-4D09D093B768}" name="19-07-20" dataDxfId="18"/>
-    <tableColumn id="134" xr3:uid="{7101E8B8-49A5-1A49-8532-994B0A3FB01B}" name="20-07-20" dataDxfId="17"/>
-    <tableColumn id="135" xr3:uid="{94611A1B-D923-9546-A8DC-9CCC7B65A729}" name="21-07-20" dataDxfId="16"/>
-    <tableColumn id="136" xr3:uid="{58AE38DE-BFD7-4249-AB7A-15BF37E8B591}" name="22-07-20" dataDxfId="15"/>
-    <tableColumn id="137" xr3:uid="{55C5FB87-1CA4-3F45-887B-DBB3DAAA5369}" name="23-07-20" dataDxfId="14"/>
-    <tableColumn id="138" xr3:uid="{437CA53C-B11E-BF47-AF09-040913B3FCD0}" name="24-07-20" dataDxfId="13"/>
-    <tableColumn id="139" xr3:uid="{202231FA-82F9-BF4E-8D60-B218C26A354A}" name="25-07-20" dataDxfId="12"/>
-    <tableColumn id="140" xr3:uid="{24F2106B-9F5D-1E4C-A42B-E2AA613BEE08}" name="26-07-20" dataDxfId="11"/>
-    <tableColumn id="141" xr3:uid="{8BDBD0BC-D9B1-B445-9A72-EF935A438E09}" name="27-07-20" dataDxfId="10"/>
-    <tableColumn id="142" xr3:uid="{6A7EFE4A-AA3A-C34C-891A-3E9FCC0E701D}" name="28-07-20" dataDxfId="9"/>
-    <tableColumn id="143" xr3:uid="{68B87CBE-2A2E-ED49-BF07-4D169F13B444}" name="29-07-20" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="59"/>
+    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="58"/>
+    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="57"/>
+    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="56"/>
+    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="55"/>
+    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="54"/>
+    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="53"/>
+    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="52"/>
+    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="51"/>
+    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="50"/>
+    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="49"/>
+    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="48"/>
+    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="47"/>
+    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="46"/>
+    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="45"/>
+    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="44"/>
+    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="43"/>
+    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="42"/>
+    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="41"/>
+    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="40"/>
+    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="39"/>
+    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="38"/>
+    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="37"/>
+    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="36"/>
+    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="35"/>
+    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="34"/>
+    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="33"/>
+    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="32"/>
+    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="31"/>
+    <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="30"/>
+    <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="10-07-20" dataDxfId="29"/>
+    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="11-07-20" dataDxfId="28"/>
+    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="12-07-20" dataDxfId="27"/>
+    <tableColumn id="127" xr3:uid="{2B284A50-3213-EF46-904E-73679622D22C}" name="13-07-20" dataDxfId="26"/>
+    <tableColumn id="128" xr3:uid="{30C66AA6-47A6-FB40-A335-1BA9A696E85B}" name="14-07-20" dataDxfId="25"/>
+    <tableColumn id="129" xr3:uid="{041D18C8-807A-0949-898D-C4880EDA94DD}" name="15-07-20" dataDxfId="24"/>
+    <tableColumn id="130" xr3:uid="{61B56DA5-913C-EF4F-B703-9A52B436E7DD}" name="16-07-20" dataDxfId="23"/>
+    <tableColumn id="131" xr3:uid="{877B5AA5-D97A-8D40-B352-6FFA59645351}" name="17-07-20" dataDxfId="22"/>
+    <tableColumn id="132" xr3:uid="{3FADF8C3-57FC-5D47-913A-C0C36C8E59FE}" name="18-07-20" dataDxfId="21"/>
+    <tableColumn id="133" xr3:uid="{1226D8E9-4582-2342-A7CC-4D09D093B768}" name="19-07-20" dataDxfId="20"/>
+    <tableColumn id="134" xr3:uid="{7101E8B8-49A5-1A49-8532-994B0A3FB01B}" name="20-07-20" dataDxfId="19"/>
+    <tableColumn id="135" xr3:uid="{94611A1B-D923-9546-A8DC-9CCC7B65A729}" name="21-07-20" dataDxfId="18"/>
+    <tableColumn id="136" xr3:uid="{58AE38DE-BFD7-4249-AB7A-15BF37E8B591}" name="22-07-20" dataDxfId="17"/>
+    <tableColumn id="137" xr3:uid="{55C5FB87-1CA4-3F45-887B-DBB3DAAA5369}" name="23-07-20" dataDxfId="16"/>
+    <tableColumn id="138" xr3:uid="{437CA53C-B11E-BF47-AF09-040913B3FCD0}" name="24-07-20" dataDxfId="15"/>
+    <tableColumn id="139" xr3:uid="{202231FA-82F9-BF4E-8D60-B218C26A354A}" name="25-07-20" dataDxfId="14"/>
+    <tableColumn id="140" xr3:uid="{24F2106B-9F5D-1E4C-A42B-E2AA613BEE08}" name="26-07-20" dataDxfId="13"/>
+    <tableColumn id="141" xr3:uid="{8BDBD0BC-D9B1-B445-9A72-EF935A438E09}" name="27-07-20" dataDxfId="12"/>
+    <tableColumn id="142" xr3:uid="{6A7EFE4A-AA3A-C34C-891A-3E9FCC0E701D}" name="28-07-20" dataDxfId="11"/>
+    <tableColumn id="143" xr3:uid="{68B87CBE-2A2E-ED49-BF07-4D169F13B444}" name="29-07-20" dataDxfId="10"/>
+    <tableColumn id="144" xr3:uid="{64D5EFBB-AC65-FF4A-AA5B-44CA608EC21F}" name="30-07-20" dataDxfId="1"/>
+    <tableColumn id="145" xr3:uid="{EC753F0D-EF8A-BB47-914F-F8123749FA51}" name="29-07-22" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="8">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="7">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="5">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="4">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -1220,10 +1234,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="1">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="3">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="2">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1590,12 +1604,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B32E72-8F4B-408A-9B01-FAD2807C0C88}">
-  <dimension ref="A1:EM52"/>
+  <dimension ref="A1:EO52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="EK1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="EL1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="EM1" sqref="EM1:EM7"/>
+      <selection pane="topRight" activeCell="EN2" sqref="EN1:EN7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1612,7 +1626,7 @@
     <col min="116" max="118" width="11.43359375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:143" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:145" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2042,8 +2056,14 @@
       <c r="EM1" s="1" t="s">
         <v>181</v>
       </c>
+      <c r="EN1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="EO1" t="s">
+        <v>182</v>
+      </c>
     </row>
-    <row r="2" spans="1:143" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:145" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2473,8 +2493,10 @@
       <c r="EM2" s="8">
         <v>216730</v>
       </c>
+      <c r="EN2" s="8"/>
+      <c r="EO2" s="8"/>
     </row>
-    <row r="3" spans="1:143" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:145" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -2904,8 +2926,10 @@
       <c r="EM3" s="8">
         <v>150836</v>
       </c>
+      <c r="EN3" s="8"/>
+      <c r="EO3" s="8"/>
     </row>
-    <row r="4" spans="1:143" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:145" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -3335,8 +3359,10 @@
       <c r="EM4" s="8">
         <v>22430</v>
       </c>
+      <c r="EN4" s="8"/>
+      <c r="EO4" s="8"/>
     </row>
-    <row r="5" spans="1:143" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:145" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -3675,8 +3701,10 @@
       <c r="EM5" s="8">
         <v>689</v>
       </c>
+      <c r="EN5" s="8"/>
+      <c r="EO5" s="8"/>
     </row>
-    <row r="6" spans="1:143" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:145" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -4102,8 +4130,10 @@
       <c r="EM6" s="8">
         <v>1302</v>
       </c>
+      <c r="EN6" s="8"/>
+      <c r="EO6" s="8"/>
     </row>
-    <row r="7" spans="1:143" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:145" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -4531,8 +4561,10 @@
       <c r="EM7" s="8">
         <v>158</v>
       </c>
+      <c r="EN7" s="8"/>
+      <c r="EO7" s="8"/>
     </row>
-    <row r="8" spans="1:143" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:145" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4643,28 +4675,28 @@
       <c r="EC8" s="8"/>
       <c r="ED8" s="8"/>
     </row>
-    <row r="9" spans="1:143" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:145" x14ac:dyDescent="0.2">
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:143" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:145" x14ac:dyDescent="0.2">
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:143" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:145" x14ac:dyDescent="0.2">
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:143" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:145" x14ac:dyDescent="0.2">
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:143" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:145" x14ac:dyDescent="0.2">
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:143" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:145" x14ac:dyDescent="0.2">
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:143" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:145" x14ac:dyDescent="0.2">
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:143" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:145" x14ac:dyDescent="0.2">
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-03-2020 00-56-35
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1754" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DBCBC4C5-C09B-BD42-ADF7-B2B89210EC04}"/>
+  <xr:revisionPtr revIDLastSave="1775" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5697EA0C-5043-D844-8EAB-08A772771530}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="191">
   <si>
     <t>Columna1</t>
   </si>
@@ -604,10 +604,22 @@
     <t>29-07-20</t>
   </si>
   <si>
-    <t>29-07-22</t>
+    <t>30-07-20</t>
   </si>
   <si>
-    <t>30-07-20</t>
+    <t>31-07-20</t>
+  </si>
+  <si>
+    <t>31-07-23</t>
+  </si>
+  <si>
+    <t>31-07-24</t>
+  </si>
+  <si>
+    <t>01-08-20</t>
+  </si>
+  <si>
+    <t>02-08-20</t>
   </si>
 </sst>
 </file>
@@ -731,7 +743,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="60">
+  <dxfs count="64">
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
@@ -950,6 +968,12 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1034,9 +1058,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:EO7" totalsRowShown="0">
-  <autoFilter ref="A1:EO7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
-  <tableColumns count="145">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E193F5BD-2E98-4B10-8297-254046EF9753}" name="Condicion_Pacientes" displayName="Condicion_Pacientes" ref="A1:ES7" totalsRowShown="0">
+  <autoFilter ref="A1:ES7" xr:uid="{65EBD142-070D-4A8A-9712-8E08F9BC999A}"/>
+  <tableColumns count="149">
     <tableColumn id="76" xr3:uid="{CA01250B-8685-4250-AAEF-D6E482663B6F}" name="Columna1"/>
     <tableColumn id="77" xr3:uid="{BC38B0B2-3229-42F8-9C9A-52EE74902839}" name="10-03-2020"/>
     <tableColumn id="78" xr3:uid="{4BB74E2E-62F3-4EED-8537-96C80CD1ED37}" name="11-03-2020"/>
@@ -1130,78 +1154,82 @@
     <tableColumn id="4" xr3:uid="{2FE879E2-2128-42AE-A0E3-647EE2D0C94F}" name="07-06-2020"/>
     <tableColumn id="5" xr3:uid="{909AC0E5-B9B2-4C03-B9B1-43F5A05B9F43}" name="08-06-2020"/>
     <tableColumn id="6" xr3:uid="{4C33D573-DF75-4285-9A83-30276C29EFD4}" name="09-06-2020"/>
-    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="59"/>
-    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="58"/>
-    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="57"/>
-    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="56"/>
-    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="55"/>
-    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="54"/>
-    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="53"/>
-    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="52"/>
-    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="51"/>
-    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="50"/>
-    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="49"/>
-    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="48"/>
-    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="47"/>
-    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="46"/>
-    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="45"/>
-    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="44"/>
-    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="43"/>
-    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="42"/>
-    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="41"/>
-    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="40"/>
-    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="39"/>
-    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="38"/>
-    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="37"/>
-    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="36"/>
-    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="35"/>
-    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="34"/>
-    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="33"/>
-    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="32"/>
-    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="31"/>
-    <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="30"/>
-    <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="10-07-20" dataDxfId="29"/>
-    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="11-07-20" dataDxfId="28"/>
-    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="12-07-20" dataDxfId="27"/>
-    <tableColumn id="127" xr3:uid="{2B284A50-3213-EF46-904E-73679622D22C}" name="13-07-20" dataDxfId="26"/>
-    <tableColumn id="128" xr3:uid="{30C66AA6-47A6-FB40-A335-1BA9A696E85B}" name="14-07-20" dataDxfId="25"/>
-    <tableColumn id="129" xr3:uid="{041D18C8-807A-0949-898D-C4880EDA94DD}" name="15-07-20" dataDxfId="24"/>
-    <tableColumn id="130" xr3:uid="{61B56DA5-913C-EF4F-B703-9A52B436E7DD}" name="16-07-20" dataDxfId="23"/>
-    <tableColumn id="131" xr3:uid="{877B5AA5-D97A-8D40-B352-6FFA59645351}" name="17-07-20" dataDxfId="22"/>
-    <tableColumn id="132" xr3:uid="{3FADF8C3-57FC-5D47-913A-C0C36C8E59FE}" name="18-07-20" dataDxfId="21"/>
-    <tableColumn id="133" xr3:uid="{1226D8E9-4582-2342-A7CC-4D09D093B768}" name="19-07-20" dataDxfId="20"/>
-    <tableColumn id="134" xr3:uid="{7101E8B8-49A5-1A49-8532-994B0A3FB01B}" name="20-07-20" dataDxfId="19"/>
-    <tableColumn id="135" xr3:uid="{94611A1B-D923-9546-A8DC-9CCC7B65A729}" name="21-07-20" dataDxfId="18"/>
-    <tableColumn id="136" xr3:uid="{58AE38DE-BFD7-4249-AB7A-15BF37E8B591}" name="22-07-20" dataDxfId="17"/>
-    <tableColumn id="137" xr3:uid="{55C5FB87-1CA4-3F45-887B-DBB3DAAA5369}" name="23-07-20" dataDxfId="16"/>
-    <tableColumn id="138" xr3:uid="{437CA53C-B11E-BF47-AF09-040913B3FCD0}" name="24-07-20" dataDxfId="15"/>
-    <tableColumn id="139" xr3:uid="{202231FA-82F9-BF4E-8D60-B218C26A354A}" name="25-07-20" dataDxfId="14"/>
-    <tableColumn id="140" xr3:uid="{24F2106B-9F5D-1E4C-A42B-E2AA613BEE08}" name="26-07-20" dataDxfId="13"/>
-    <tableColumn id="141" xr3:uid="{8BDBD0BC-D9B1-B445-9A72-EF935A438E09}" name="27-07-20" dataDxfId="12"/>
-    <tableColumn id="142" xr3:uid="{6A7EFE4A-AA3A-C34C-891A-3E9FCC0E701D}" name="28-07-20" dataDxfId="11"/>
-    <tableColumn id="143" xr3:uid="{68B87CBE-2A2E-ED49-BF07-4D169F13B444}" name="29-07-20" dataDxfId="10"/>
-    <tableColumn id="144" xr3:uid="{64D5EFBB-AC65-FF4A-AA5B-44CA608EC21F}" name="30-07-20" dataDxfId="1"/>
-    <tableColumn id="145" xr3:uid="{EC753F0D-EF8A-BB47-914F-F8123749FA51}" name="29-07-22" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{95F17C21-0267-4474-93CA-09A2CCA37449}" name="10-06-2020" dataDxfId="63"/>
+    <tableColumn id="8" xr3:uid="{F74063BD-5DCD-4BB4-9589-556329FB26A8}" name="11-06-2020" dataDxfId="62"/>
+    <tableColumn id="9" xr3:uid="{649F498F-D961-48D9-B03E-7696FE365482}" name="12-06-2020" dataDxfId="61"/>
+    <tableColumn id="97" xr3:uid="{A5C46252-53A6-4C20-9528-EBBB46C70C09}" name="13-06-20" dataDxfId="60"/>
+    <tableColumn id="98" xr3:uid="{906D3465-B7AE-4BEA-B15E-BF4AFA9B17FB}" name="14-06-20" dataDxfId="59"/>
+    <tableColumn id="99" xr3:uid="{D4054379-978C-4004-A172-E45CCD7387C8}" name="15-06-20" dataDxfId="58"/>
+    <tableColumn id="100" xr3:uid="{B8F2504B-914D-40CA-89AF-1A51923EE234}" name="16-06-20" dataDxfId="57"/>
+    <tableColumn id="101" xr3:uid="{A08E839E-61A6-476B-86AD-BC3F1C31B6F7}" name="17-06-20" dataDxfId="56"/>
+    <tableColumn id="102" xr3:uid="{1925CCF1-0C7C-484C-818E-28B0B29E2B65}" name="18-06-20" dataDxfId="55"/>
+    <tableColumn id="103" xr3:uid="{7705B3CE-4EED-4361-85B1-ED555A9C3A4E}" name="19-06-20" dataDxfId="54"/>
+    <tableColumn id="104" xr3:uid="{4CF234B2-A1BA-4E57-B85B-0B16844337FB}" name="20-06-20" dataDxfId="53"/>
+    <tableColumn id="105" xr3:uid="{E05FE28E-6EEE-4AB3-B14B-C49FB57E415A}" name="21-06-20" dataDxfId="52"/>
+    <tableColumn id="106" xr3:uid="{7FA93533-0664-4F66-8C27-79E1AAD1F1D5}" name="22-06-20" dataDxfId="51"/>
+    <tableColumn id="107" xr3:uid="{F04ACC92-96E1-4BCA-9CE5-3E3038C08C05}" name="23-06-20" dataDxfId="50"/>
+    <tableColumn id="108" xr3:uid="{8AA85728-B7A4-4846-AD35-9DA2869791FA}" name="24-06-20" dataDxfId="49"/>
+    <tableColumn id="109" xr3:uid="{D4C3E08C-EB48-435F-9E11-B34A55EB3A2E}" name="25-06-20" dataDxfId="48"/>
+    <tableColumn id="110" xr3:uid="{D686EF51-E376-4076-8007-316C16FBDBCC}" name="26-06-20" dataDxfId="47"/>
+    <tableColumn id="111" xr3:uid="{3D163CAF-BABE-4D11-8523-51B7BDF7A2E0}" name="27-06-20" dataDxfId="46"/>
+    <tableColumn id="112" xr3:uid="{F5011FA0-0F27-4C66-9945-9108C8263A1F}" name="28-06-20" dataDxfId="45"/>
+    <tableColumn id="113" xr3:uid="{45A50112-213E-479B-8A5A-6240F859FD1E}" name="29-06-20" dataDxfId="44"/>
+    <tableColumn id="114" xr3:uid="{72B232D5-9A82-4772-9114-9458E03DF764}" name="30-06-20" dataDxfId="43"/>
+    <tableColumn id="115" xr3:uid="{45D977E4-5C5D-4F34-A1FA-4D0065194B2E}" name="01-07-20" dataDxfId="42"/>
+    <tableColumn id="116" xr3:uid="{8E9A6A7A-D809-7747-90C8-0871BFB774C9}" name="02-07-20" dataDxfId="41"/>
+    <tableColumn id="117" xr3:uid="{69AA80D0-14FC-C54A-8E37-04EF18CDE697}" name="03-07-20" dataDxfId="40"/>
+    <tableColumn id="118" xr3:uid="{FD812150-1658-B344-9E5C-CF900C811CAC}" name="04-07-20" dataDxfId="39"/>
+    <tableColumn id="119" xr3:uid="{CF5C86C6-44F6-604E-BFA3-D8D4C003425A}" name="05-07-20" dataDxfId="38"/>
+    <tableColumn id="120" xr3:uid="{B32FA352-85FB-1F4D-8EA7-97AFBE6A3712}" name="06-07-20" dataDxfId="37"/>
+    <tableColumn id="121" xr3:uid="{3850ADEE-D7EB-9E49-BBB5-6B9F1F54CD95}" name="07-06-20" dataDxfId="36"/>
+    <tableColumn id="122" xr3:uid="{320DDD59-5C45-2040-9D89-C4544F091C5A}" name="08-07-20" dataDxfId="35"/>
+    <tableColumn id="123" xr3:uid="{0ACFB9AB-6D30-3A45-9547-D95BC47690DD}" name="09-07-20" dataDxfId="34"/>
+    <tableColumn id="124" xr3:uid="{81FD73C7-D816-3F4E-A9DF-1C421C2EFC23}" name="10-07-20" dataDxfId="33"/>
+    <tableColumn id="125" xr3:uid="{56DFBF65-88C7-5646-8896-48E8D3FF2198}" name="11-07-20" dataDxfId="32"/>
+    <tableColumn id="126" xr3:uid="{18F6DF39-9721-384A-A899-DB40D6B4785E}" name="12-07-20" dataDxfId="31"/>
+    <tableColumn id="127" xr3:uid="{2B284A50-3213-EF46-904E-73679622D22C}" name="13-07-20" dataDxfId="30"/>
+    <tableColumn id="128" xr3:uid="{30C66AA6-47A6-FB40-A335-1BA9A696E85B}" name="14-07-20" dataDxfId="29"/>
+    <tableColumn id="129" xr3:uid="{041D18C8-807A-0949-898D-C4880EDA94DD}" name="15-07-20" dataDxfId="28"/>
+    <tableColumn id="130" xr3:uid="{61B56DA5-913C-EF4F-B703-9A52B436E7DD}" name="16-07-20" dataDxfId="27"/>
+    <tableColumn id="131" xr3:uid="{877B5AA5-D97A-8D40-B352-6FFA59645351}" name="17-07-20" dataDxfId="26"/>
+    <tableColumn id="132" xr3:uid="{3FADF8C3-57FC-5D47-913A-C0C36C8E59FE}" name="18-07-20" dataDxfId="25"/>
+    <tableColumn id="133" xr3:uid="{1226D8E9-4582-2342-A7CC-4D09D093B768}" name="19-07-20" dataDxfId="24"/>
+    <tableColumn id="134" xr3:uid="{7101E8B8-49A5-1A49-8532-994B0A3FB01B}" name="20-07-20" dataDxfId="23"/>
+    <tableColumn id="135" xr3:uid="{94611A1B-D923-9546-A8DC-9CCC7B65A729}" name="21-07-20" dataDxfId="22"/>
+    <tableColumn id="136" xr3:uid="{58AE38DE-BFD7-4249-AB7A-15BF37E8B591}" name="22-07-20" dataDxfId="21"/>
+    <tableColumn id="137" xr3:uid="{55C5FB87-1CA4-3F45-887B-DBB3DAAA5369}" name="23-07-20" dataDxfId="20"/>
+    <tableColumn id="138" xr3:uid="{437CA53C-B11E-BF47-AF09-040913B3FCD0}" name="24-07-20" dataDxfId="19"/>
+    <tableColumn id="139" xr3:uid="{202231FA-82F9-BF4E-8D60-B218C26A354A}" name="25-07-20" dataDxfId="18"/>
+    <tableColumn id="140" xr3:uid="{24F2106B-9F5D-1E4C-A42B-E2AA613BEE08}" name="26-07-20" dataDxfId="17"/>
+    <tableColumn id="141" xr3:uid="{8BDBD0BC-D9B1-B445-9A72-EF935A438E09}" name="27-07-20" dataDxfId="16"/>
+    <tableColumn id="142" xr3:uid="{6A7EFE4A-AA3A-C34C-891A-3E9FCC0E701D}" name="28-07-20" dataDxfId="15"/>
+    <tableColumn id="143" xr3:uid="{68B87CBE-2A2E-ED49-BF07-4D169F13B444}" name="29-07-20" dataDxfId="14"/>
+    <tableColumn id="144" xr3:uid="{64D5EFBB-AC65-FF4A-AA5B-44CA608EC21F}" name="30-07-20" dataDxfId="13"/>
+    <tableColumn id="145" xr3:uid="{EC753F0D-EF8A-BB47-914F-F8123749FA51}" name="31-07-20" dataDxfId="12"/>
+    <tableColumn id="146" xr3:uid="{5EAED391-39D4-DB4D-9C41-D6293831A1D6}" name="01-08-20" dataDxfId="3"/>
+    <tableColumn id="147" xr3:uid="{29CD9BB6-921C-EC4A-84EB-6022FDCA9F77}" name="02-08-20" dataDxfId="2"/>
+    <tableColumn id="148" xr3:uid="{7A6B2633-DA48-844B-B2A7-4FC596D36087}" name="31-07-23" dataDxfId="1"/>
+    <tableColumn id="149" xr3:uid="{B5E62901-93E8-AB4A-A55E-33F107A754BE}" name="31-07-24" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="10">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="9">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="5">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="7">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="4">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="6">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -1234,10 +1262,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="3">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="5">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="2">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="4">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1604,12 +1632,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B32E72-8F4B-408A-9B01-FAD2807C0C88}">
-  <dimension ref="A1:EO52"/>
+  <dimension ref="A1:ES52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="EL1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="EN1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="EN2" sqref="EN1:EN7"/>
+      <selection pane="topRight" activeCell="EP4" sqref="EP4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1626,7 +1654,7 @@
     <col min="116" max="118" width="11.43359375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:145" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2057,13 +2085,25 @@
         <v>181</v>
       </c>
       <c r="EN1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="EO1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="EO1" t="s">
-        <v>182</v>
+      <c r="EP1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="EQ1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="ER1" t="s">
+        <v>184</v>
+      </c>
+      <c r="ES1" t="s">
+        <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:145" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2493,10 +2533,20 @@
       <c r="EM2" s="8">
         <v>216730</v>
       </c>
-      <c r="EN2" s="8"/>
-      <c r="EO2" s="8"/>
+      <c r="EN2" s="8">
+        <v>219942</v>
+      </c>
+      <c r="EO2" s="8">
+        <v>222990</v>
+      </c>
+      <c r="EP2" s="8">
+        <v>226596</v>
+      </c>
+      <c r="EQ2" s="8"/>
+      <c r="ER2" s="8"/>
+      <c r="ES2" s="8"/>
     </row>
-    <row r="3" spans="1:145" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -2926,10 +2976,20 @@
       <c r="EM3" s="8">
         <v>150836</v>
       </c>
-      <c r="EN3" s="8"/>
-      <c r="EO3" s="8"/>
+      <c r="EN3" s="8">
+        <v>153132</v>
+      </c>
+      <c r="EO3" s="8">
+        <v>155165</v>
+      </c>
+      <c r="EP3" s="8">
+        <v>157706</v>
+      </c>
+      <c r="EQ3" s="8"/>
+      <c r="ER3" s="8"/>
+      <c r="ES3" s="8"/>
     </row>
-    <row r="4" spans="1:145" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -3359,10 +3419,18 @@
       <c r="EM4" s="8">
         <v>22430</v>
       </c>
-      <c r="EN4" s="8"/>
-      <c r="EO4" s="8"/>
+      <c r="EN4" s="8">
+        <v>22457</v>
+      </c>
+      <c r="EO4" s="8">
+        <v>22528</v>
+      </c>
+      <c r="EP4" s="8"/>
+      <c r="EQ4" s="8"/>
+      <c r="ER4" s="8"/>
+      <c r="ES4" s="8"/>
     </row>
-    <row r="5" spans="1:145" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -3701,10 +3769,18 @@
       <c r="EM5" s="8">
         <v>689</v>
       </c>
-      <c r="EN5" s="8"/>
-      <c r="EO5" s="8"/>
+      <c r="EN5" s="8">
+        <v>666</v>
+      </c>
+      <c r="EO5" s="8">
+        <v>673</v>
+      </c>
+      <c r="EP5" s="8"/>
+      <c r="EQ5" s="8"/>
+      <c r="ER5" s="8"/>
+      <c r="ES5" s="8"/>
     </row>
-    <row r="6" spans="1:145" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -4130,10 +4206,18 @@
       <c r="EM6" s="8">
         <v>1302</v>
       </c>
-      <c r="EN6" s="8"/>
-      <c r="EO6" s="8"/>
+      <c r="EN6" s="8">
+        <v>1292</v>
+      </c>
+      <c r="EO6" s="8">
+        <v>1302</v>
+      </c>
+      <c r="EP6" s="8"/>
+      <c r="EQ6" s="8"/>
+      <c r="ER6" s="8"/>
+      <c r="ES6" s="8"/>
     </row>
-    <row r="7" spans="1:145" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -4561,10 +4645,18 @@
       <c r="EM7" s="8">
         <v>158</v>
       </c>
-      <c r="EN7" s="8"/>
-      <c r="EO7" s="8"/>
+      <c r="EN7" s="8">
+        <v>161</v>
+      </c>
+      <c r="EO7" s="8">
+        <v>166</v>
+      </c>
+      <c r="EP7" s="8"/>
+      <c r="EQ7" s="8"/>
+      <c r="ER7" s="8"/>
+      <c r="ES7" s="8"/>
     </row>
-    <row r="8" spans="1:145" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4674,29 +4766,42 @@
       <c r="EB8" s="8"/>
       <c r="EC8" s="8"/>
       <c r="ED8" s="8"/>
+      <c r="EE8" s="8"/>
+      <c r="EF8" s="8"/>
+      <c r="EG8" s="8"/>
+      <c r="EH8" s="8"/>
+      <c r="EI8" s="8"/>
+      <c r="EJ8" s="8"/>
+      <c r="EK8" s="8"/>
+      <c r="EL8" s="8"/>
+      <c r="EM8" s="8"/>
+      <c r="EN8" s="8"/>
+      <c r="EO8" s="8"/>
+      <c r="EP8" s="8"/>
+      <c r="EQ8" s="8"/>
     </row>
-    <row r="9" spans="1:145" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:149" x14ac:dyDescent="0.2">
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:145" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:149" x14ac:dyDescent="0.2">
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:145" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:149" x14ac:dyDescent="0.2">
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:145" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:149" x14ac:dyDescent="0.2">
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:145" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:149" x14ac:dyDescent="0.2">
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:145" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:149" x14ac:dyDescent="0.2">
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:145" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:149" x14ac:dyDescent="0.2">
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:145" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:149" x14ac:dyDescent="0.2">
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
@@ -5163,7 +5268,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44041</v>
+        <v>44044</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -27364,7 +27469,7 @@
       </c>
       <c r="B148" s="12" t="str">
         <f t="shared" si="86"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C148" s="12">
         <v>142</v>
@@ -27517,7 +27622,7 @@
     <row r="149" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A149" s="12" t="str">
         <f t="shared" si="85"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B149" s="12" t="str">
         <f t="shared" si="86"/>
@@ -27536,145 +27641,145 @@
       </c>
       <c r="F149" cm="1">
         <f t="array" ref="F149">+INDEX(Hoja1!$B$2:$MO$7,1,E149)</f>
-        <v>0</v>
+        <v>219942</v>
       </c>
       <c r="G149">
         <f t="shared" si="70"/>
-        <v>-216730</v>
+        <v>3212</v>
       </c>
       <c r="H149" cm="1">
         <f t="array" ref="H149">+INDEX(Hoja1!$B$2:$MO$7,2,$E149)</f>
-        <v>0</v>
+        <v>153132</v>
       </c>
       <c r="I149">
         <f t="shared" si="71"/>
-        <v>-150836</v>
+        <v>2296</v>
       </c>
       <c r="J149">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>66810</v>
       </c>
       <c r="K149">
         <f t="shared" si="72"/>
-        <v>-65894</v>
+        <v>916</v>
       </c>
       <c r="L149" cm="1">
         <f t="array" ref="L149">+INDEX(Hoja1!$B$2:$MO$7,3,$E149)</f>
-        <v>0</v>
+        <v>22457</v>
       </c>
       <c r="M149" cm="1">
         <f t="array" ref="M149">+INDEX(Hoja1!$B$2:$MO$7,4,$E149)</f>
-        <v>0</v>
+        <v>666</v>
       </c>
       <c r="N149" cm="1">
         <f t="array" ref="N149">+INDEX(Hoja1!$B$2:$MO$7,5,$E149)</f>
-        <v>0</v>
+        <v>1292</v>
       </c>
       <c r="O149" cm="1">
         <f t="array" ref="O149">+INDEX(Hoja1!$B$2:$MO$7,6,$E149)</f>
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="P149" s="13">
         <f t="shared" si="89"/>
-        <v>0</v>
+        <v>0.69623809913522661</v>
       </c>
       <c r="Q149" s="13">
         <f t="shared" si="90"/>
-        <v>0</v>
+        <v>0.30376190086477345</v>
       </c>
       <c r="R149">
         <f t="shared" si="73"/>
-        <v>-219863</v>
+        <v>79</v>
       </c>
       <c r="S149">
         <f t="shared" si="74"/>
-        <v>-65894</v>
+        <v>916</v>
       </c>
       <c r="T149">
         <f t="shared" si="75"/>
-        <v>-22430</v>
+        <v>27</v>
       </c>
       <c r="U149">
         <f t="shared" si="76"/>
-        <v>-689</v>
+        <v>-23</v>
       </c>
       <c r="V149">
         <f t="shared" si="77"/>
-        <v>-1302</v>
+        <v>-10</v>
       </c>
       <c r="W149">
         <f t="shared" si="78"/>
-        <v>-158</v>
+        <v>3</v>
       </c>
       <c r="X149">
         <f t="shared" si="79"/>
-        <v>-70.176508139163744</v>
+        <v>2.5215448451962975E-2</v>
       </c>
       <c r="Y149">
         <f t="shared" si="80"/>
-        <v>-1</v>
+        <v>1.3901113910219443E-2</v>
       </c>
       <c r="Z149">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>1.0012037449843958</v>
       </c>
       <c r="AA149">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>0.96661828737300437</v>
       </c>
       <c r="AB149">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>0.99231950844854067</v>
       </c>
       <c r="AC149">
         <f t="shared" si="84"/>
-        <v>0</v>
+        <v>1.018987341772152</v>
       </c>
       <c r="AD149">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>52883.385429189715</v>
       </c>
       <c r="AE149">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>16063.957682135129</v>
       </c>
       <c r="AF149">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>5399.6152921375333</v>
       </c>
       <c r="AG149">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>160.13464775186344</v>
       </c>
       <c r="AH149">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>310.6515989420534</v>
       </c>
       <c r="AI149">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>38.711228660735756</v>
       </c>
       <c r="AJ149">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>24576</v>
       </c>
       <c r="AK149">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>5909.1127674921863</v>
       </c>
       <c r="AL149">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ148</f>
-        <v>-24579</v>
+        <v>-3</v>
       </c>
       <c r="AM149">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ148,0)</f>
-        <v>-1</v>
+        <v>-1.2205541315757354E-4</v>
       </c>
     </row>
     <row r="150" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A150" s="12" t="str">
         <f t="shared" si="85"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B150" s="12" t="str">
         <f t="shared" si="86"/>
@@ -27693,149 +27798,149 @@
       </c>
       <c r="F150" cm="1">
         <f t="array" ref="F150">+INDEX(Hoja1!$B$2:$MO$7,1,E150)</f>
-        <v>0</v>
+        <v>222990</v>
       </c>
       <c r="G150">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>3048</v>
       </c>
       <c r="H150" cm="1">
         <f t="array" ref="H150">+INDEX(Hoja1!$B$2:$MO$7,2,$E150)</f>
-        <v>0</v>
+        <v>155165</v>
       </c>
       <c r="I150">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>2033</v>
       </c>
       <c r="J150">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>67825</v>
       </c>
       <c r="K150">
         <f t="shared" si="72"/>
-        <v>0</v>
+        <v>1015</v>
       </c>
       <c r="L150" cm="1">
         <f t="array" ref="L150">+INDEX(Hoja1!$B$2:$MO$7,3,$E150)</f>
-        <v>0</v>
+        <v>22528</v>
       </c>
       <c r="M150" cm="1">
         <f t="array" ref="M150">+INDEX(Hoja1!$B$2:$MO$7,4,$E150)</f>
-        <v>0</v>
+        <v>673</v>
       </c>
       <c r="N150" cm="1">
         <f t="array" ref="N150">+INDEX(Hoja1!$B$2:$MO$7,5,$E150)</f>
-        <v>0</v>
+        <v>1302</v>
       </c>
       <c r="O150" cm="1">
         <f t="array" ref="O150">+INDEX(Hoja1!$B$2:$MO$7,6,$E150)</f>
-        <v>0</v>
+        <v>166</v>
       </c>
       <c r="P150" s="13">
         <f t="shared" si="89"/>
-        <v>0</v>
+        <v>0.69583837840261897</v>
       </c>
       <c r="Q150" s="13">
         <f t="shared" si="90"/>
-        <v>0</v>
+        <v>0.30416162159738103</v>
       </c>
       <c r="R150">
         <f t="shared" si="73"/>
-        <v>216730</v>
+        <v>-164</v>
       </c>
       <c r="S150">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>1015</v>
       </c>
       <c r="T150">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="U150">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="V150">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W150">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X150">
         <f t="shared" si="79"/>
-        <v>-1</v>
+        <v>-5.1058530510585308E-2</v>
       </c>
       <c r="Y150">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>1.5192336476575363E-2</v>
       </c>
       <c r="Z150">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>1.0031615977200872</v>
       </c>
       <c r="AA150">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>1.0105105105105106</v>
       </c>
       <c r="AB150">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>1.0077399380804954</v>
       </c>
       <c r="AC150">
         <f t="shared" si="84"/>
-        <v>0</v>
+        <v>1.031055900621118</v>
       </c>
       <c r="AD150">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>53616.253907189232</v>
       </c>
       <c r="AE150">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>16308.006732387594</v>
       </c>
       <c r="AF150">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>5416.686703534504</v>
       </c>
       <c r="AG150">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>161.8177446501563</v>
       </c>
       <c r="AH150">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>313.05602308247177</v>
       </c>
       <c r="AI150">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>39.913440730944941</v>
       </c>
       <c r="AJ150">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>24669</v>
       </c>
       <c r="AK150">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>5931.4739119980768</v>
       </c>
       <c r="AL150">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ149</f>
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="AM150">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ149,0)</f>
-        <v>0</v>
+        <v>3.7841796875E-3</v>
       </c>
     </row>
     <row r="151" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A151" s="12" t="str">
         <f t="shared" si="85"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B151" s="12" t="str">
         <f t="shared" si="86"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C151" s="12">
         <v>145</v>
@@ -27850,27 +27955,27 @@
       </c>
       <c r="F151" cm="1">
         <f t="array" ref="F151">+INDEX(Hoja1!$B$2:$MO$7,1,E151)</f>
-        <v>0</v>
+        <v>226596</v>
       </c>
       <c r="G151">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>3606</v>
       </c>
       <c r="H151" cm="1">
         <f t="array" ref="H151">+INDEX(Hoja1!$B$2:$MO$7,2,$E151)</f>
-        <v>0</v>
+        <v>157706</v>
       </c>
       <c r="I151">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>2541</v>
       </c>
       <c r="J151">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>68890</v>
       </c>
       <c r="K151">
         <f t="shared" si="72"/>
-        <v>0</v>
+        <v>1065</v>
       </c>
       <c r="L151" cm="1">
         <f t="array" ref="L151">+INDEX(Hoja1!$B$2:$MO$7,3,$E151)</f>
@@ -27890,43 +27995,43 @@
       </c>
       <c r="P151" s="13">
         <f t="shared" si="89"/>
-        <v>0</v>
+        <v>0.69597874631502765</v>
       </c>
       <c r="Q151" s="13">
         <f t="shared" si="90"/>
-        <v>0</v>
+        <v>0.30402125368497235</v>
       </c>
       <c r="R151">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>558</v>
       </c>
       <c r="S151">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>1065</v>
       </c>
       <c r="T151">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>-22528</v>
       </c>
       <c r="U151">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>-673</v>
       </c>
       <c r="V151">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>-1302</v>
       </c>
       <c r="W151">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>-166</v>
       </c>
       <c r="X151">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>0.18307086614173229</v>
       </c>
       <c r="Y151">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>1.5702174714338372E-2</v>
       </c>
       <c r="Z151">
         <f t="shared" si="81"/>
@@ -27946,11 +28051,11 @@
       </c>
       <c r="AD151">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>54483.289252224095</v>
       </c>
       <c r="AE151">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>16564.07790334215</v>
       </c>
       <c r="AF151">
         <f t="shared" si="65"/>
@@ -27978,11 +28083,11 @@
       </c>
       <c r="AL151">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ150</f>
-        <v>0</v>
+        <v>-24669</v>
       </c>
       <c r="AM151">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ150,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="152" spans="1:39" x14ac:dyDescent="0.2">
@@ -28011,7 +28116,7 @@
       </c>
       <c r="G152">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>-226596</v>
       </c>
       <c r="H152" cm="1">
         <f t="array" ref="H152">+INDEX(Hoja1!$B$2:$MO$7,2,$E152)</f>
@@ -28019,7 +28124,7 @@
       </c>
       <c r="I152">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>-157706</v>
       </c>
       <c r="J152">
         <f t="shared" si="62"/>
@@ -28027,7 +28132,7 @@
       </c>
       <c r="K152">
         <f t="shared" si="72"/>
-        <v>0</v>
+        <v>-68890</v>
       </c>
       <c r="L152" cm="1">
         <f t="array" ref="L152">+INDEX(Hoja1!$B$2:$MO$7,3,$E152)</f>
@@ -28055,11 +28160,11 @@
       </c>
       <c r="R152">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>-230202</v>
       </c>
       <c r="S152">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>-68890</v>
       </c>
       <c r="T152">
         <f t="shared" si="75"/>
@@ -28079,11 +28184,11 @@
       </c>
       <c r="X152">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>-63.838602329450914</v>
       </c>
       <c r="Y152">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z152">
         <f t="shared" si="81"/>
@@ -28212,7 +28317,7 @@
       </c>
       <c r="R153">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>226596</v>
       </c>
       <c r="S153">
         <f t="shared" si="74"/>
@@ -28236,7 +28341,7 @@
       </c>
       <c r="X153">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y153">
         <f t="shared" si="80"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-03-2020 04-56-59
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1775" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5697EA0C-5043-D844-8EAB-08A772771530}"/>
+  <xr:revisionPtr revIDLastSave="1785" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{95D17A22-1A8D-294F-840F-A1C85242A581}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="188">
   <si>
     <t>Columna1</t>
   </si>
@@ -745,18 +745,6 @@
   </cellStyles>
   <dxfs count="64">
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -875,6 +863,18 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
@@ -1206,30 +1206,30 @@
     <tableColumn id="143" xr3:uid="{68B87CBE-2A2E-ED49-BF07-4D169F13B444}" name="29-07-20" dataDxfId="14"/>
     <tableColumn id="144" xr3:uid="{64D5EFBB-AC65-FF4A-AA5B-44CA608EC21F}" name="30-07-20" dataDxfId="13"/>
     <tableColumn id="145" xr3:uid="{EC753F0D-EF8A-BB47-914F-F8123749FA51}" name="31-07-20" dataDxfId="12"/>
-    <tableColumn id="146" xr3:uid="{5EAED391-39D4-DB4D-9C41-D6293831A1D6}" name="01-08-20" dataDxfId="3"/>
-    <tableColumn id="147" xr3:uid="{29CD9BB6-921C-EC4A-84EB-6022FDCA9F77}" name="02-08-20" dataDxfId="2"/>
-    <tableColumn id="148" xr3:uid="{7A6B2633-DA48-844B-B2A7-4FC596D36087}" name="31-07-23" dataDxfId="1"/>
-    <tableColumn id="149" xr3:uid="{B5E62901-93E8-AB4A-A55E-33F107A754BE}" name="31-07-24" dataDxfId="0"/>
+    <tableColumn id="146" xr3:uid="{5EAED391-39D4-DB4D-9C41-D6293831A1D6}" name="01-08-20" dataDxfId="11"/>
+    <tableColumn id="147" xr3:uid="{29CD9BB6-921C-EC4A-84EB-6022FDCA9F77}" name="02-08-20" dataDxfId="10"/>
+    <tableColumn id="148" xr3:uid="{7A6B2633-DA48-844B-B2A7-4FC596D36087}" name="31-07-23" dataDxfId="9"/>
+    <tableColumn id="149" xr3:uid="{B5E62901-93E8-AB4A-A55E-33F107A754BE}" name="31-07-24" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BEBC99C-0E00-45D9-B659-C8FF033A96AB}" name="TODO_PACIENTES" displayName="TODO_PACIENTES" ref="A6:AM303" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A6:AM303" xr:uid="{DE0B32F3-6185-43E1-8784-A837F07BC110}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{8C9A4ABF-9AC7-46D8-BB8F-7A7936F45A5C}" name="ON" dataDxfId="6">
       <calculatedColumnFormula>+IF(D7&gt;$D$4,"OUT TIME","ON")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="9">
+    <tableColumn id="2" xr3:uid="{2D69C1D4-551E-473B-8D60-DB76DBCD5269}" name="Ultimo" dataDxfId="5">
       <calculatedColumnFormula>IF(D7=$D$4,"ultima","no")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{F289EBF6-6CE0-41C5-9B24-07FEE0D98514}" name="Indice" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{CAD719F0-6451-4240-A36D-21196A38055A}" name="Fecha" dataDxfId="3">
       <calculatedColumnFormula>+D6+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="6">
+    <tableColumn id="5" xr3:uid="{E0CB7D30-F77C-4BEC-A223-78C24B518326}" name="DIA" dataDxfId="2">
       <calculatedColumnFormula>+E6+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{55FC4DBE-D639-4B4C-87A2-D20476A5BE01}" name="Pruebas Realizadas">
@@ -1262,10 +1262,10 @@
     <tableColumn id="15" xr3:uid="{5E5DF55F-A32B-4739-BE3E-02DB52D2A1CC}" name="Hospitalizados en UCI">
       <calculatedColumnFormula array="1">+INDEX(Hoja1!$B$2:$MO$7,6,$E7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="5">
+    <tableColumn id="16" xr3:uid="{9417BBCA-C31B-4386-8AA4-9905D9B24D21}" name="%Pruebas Negativas" dataDxfId="1">
       <calculatedColumnFormula>+IFERROR(H7/F7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="4">
+    <tableColumn id="17" xr3:uid="{376DF500-B5B1-4162-ACDF-AA62A93C172F}" name="%Pruebas Positivas" dataDxfId="0">
       <calculatedColumnFormula>+IFERROR(J7/F7,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{E2CB7125-1D2A-4977-8FF3-CA9D5FB95EF1}" name="Variación Pruebas Realizadas">
@@ -1637,7 +1637,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="EN1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="EP4" sqref="EP4"/>
+      <selection pane="topRight" activeCell="EQ7" sqref="EQ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2542,7 +2542,9 @@
       <c r="EP2" s="8">
         <v>226596</v>
       </c>
-      <c r="EQ2" s="8"/>
+      <c r="EQ2" s="8">
+        <v>229831</v>
+      </c>
       <c r="ER2" s="8"/>
       <c r="ES2" s="8"/>
     </row>
@@ -2985,7 +2987,9 @@
       <c r="EP3" s="8">
         <v>157706</v>
       </c>
-      <c r="EQ3" s="8"/>
+      <c r="EQ3" s="8">
+        <v>159856</v>
+      </c>
       <c r="ER3" s="8"/>
       <c r="ES3" s="8"/>
     </row>
@@ -3425,8 +3429,12 @@
       <c r="EO4" s="8">
         <v>22528</v>
       </c>
-      <c r="EP4" s="8"/>
-      <c r="EQ4" s="8"/>
+      <c r="EP4" s="8">
+        <v>22743</v>
+      </c>
+      <c r="EQ4" s="8">
+        <v>22806</v>
+      </c>
       <c r="ER4" s="8"/>
       <c r="ES4" s="8"/>
     </row>
@@ -3775,8 +3783,12 @@
       <c r="EO5" s="8">
         <v>673</v>
       </c>
-      <c r="EP5" s="8"/>
-      <c r="EQ5" s="8"/>
+      <c r="EP5" s="8">
+        <v>641</v>
+      </c>
+      <c r="EQ5" s="8">
+        <v>674</v>
+      </c>
       <c r="ER5" s="8"/>
       <c r="ES5" s="8"/>
     </row>
@@ -4212,8 +4224,12 @@
       <c r="EO6" s="8">
         <v>1302</v>
       </c>
-      <c r="EP6" s="8"/>
-      <c r="EQ6" s="8"/>
+      <c r="EP6" s="8">
+        <v>1303</v>
+      </c>
+      <c r="EQ6" s="8">
+        <v>1300</v>
+      </c>
       <c r="ER6" s="8"/>
       <c r="ES6" s="8"/>
     </row>
@@ -4651,8 +4667,12 @@
       <c r="EO7" s="8">
         <v>166</v>
       </c>
-      <c r="EP7" s="8"/>
-      <c r="EQ7" s="8"/>
+      <c r="EP7" s="8">
+        <v>166</v>
+      </c>
+      <c r="EQ7" s="8">
+        <v>164</v>
+      </c>
       <c r="ER7" s="8"/>
       <c r="ES7" s="8"/>
     </row>
@@ -5268,7 +5288,7 @@
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
-        <v>44044</v>
+        <v>44045</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -27940,7 +27960,7 @@
       </c>
       <c r="B151" s="12" t="str">
         <f t="shared" si="86"/>
-        <v>ultima</v>
+        <v>no</v>
       </c>
       <c r="C151" s="12">
         <v>145</v>
@@ -27979,19 +27999,19 @@
       </c>
       <c r="L151" cm="1">
         <f t="array" ref="L151">+INDEX(Hoja1!$B$2:$MO$7,3,$E151)</f>
-        <v>0</v>
+        <v>22743</v>
       </c>
       <c r="M151" cm="1">
         <f t="array" ref="M151">+INDEX(Hoja1!$B$2:$MO$7,4,$E151)</f>
-        <v>0</v>
+        <v>641</v>
       </c>
       <c r="N151" cm="1">
         <f t="array" ref="N151">+INDEX(Hoja1!$B$2:$MO$7,5,$E151)</f>
-        <v>0</v>
+        <v>1303</v>
       </c>
       <c r="O151" cm="1">
         <f t="array" ref="O151">+INDEX(Hoja1!$B$2:$MO$7,6,$E151)</f>
-        <v>0</v>
+        <v>166</v>
       </c>
       <c r="P151" s="13">
         <f t="shared" si="89"/>
@@ -28011,19 +28031,19 @@
       </c>
       <c r="T151">
         <f t="shared" si="75"/>
-        <v>-22528</v>
+        <v>215</v>
       </c>
       <c r="U151">
         <f t="shared" si="76"/>
-        <v>-673</v>
+        <v>-32</v>
       </c>
       <c r="V151">
         <f t="shared" si="77"/>
-        <v>-1302</v>
+        <v>1</v>
       </c>
       <c r="W151">
         <f t="shared" si="78"/>
-        <v>-166</v>
+        <v>0</v>
       </c>
       <c r="X151">
         <f t="shared" si="79"/>
@@ -28035,19 +28055,19 @@
       </c>
       <c r="Z151">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>1.0095436789772727</v>
       </c>
       <c r="AA151">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>0.95245170876671614</v>
       </c>
       <c r="AB151">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>1.0007680491551458</v>
       </c>
       <c r="AC151">
         <f t="shared" si="84"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD151">
         <f t="shared" si="63"/>
@@ -28059,45 +28079,45 @@
       </c>
       <c r="AF151">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>5468.3818225534988</v>
       </c>
       <c r="AG151">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>154.12358740081751</v>
       </c>
       <c r="AH151">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>313.29646549651358</v>
       </c>
       <c r="AI151">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>39.913440730944941</v>
       </c>
       <c r="AJ151">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>24853</v>
       </c>
       <c r="AK151">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>5975.7153161817751</v>
       </c>
       <c r="AL151">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ150</f>
-        <v>-24669</v>
+        <v>184</v>
       </c>
       <c r="AM151">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ150,0)</f>
-        <v>-1</v>
+        <v>7.4587539016579517E-3</v>
       </c>
     </row>
     <row r="152" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A152" s="12" t="str">
         <f t="shared" si="85"/>
-        <v>OUT TIME</v>
+        <v>ON</v>
       </c>
       <c r="B152" s="12" t="str">
         <f t="shared" si="86"/>
-        <v>no</v>
+        <v>ultima</v>
       </c>
       <c r="C152" s="12">
         <v>146</v>
@@ -28112,139 +28132,139 @@
       </c>
       <c r="F152" cm="1">
         <f t="array" ref="F152">+INDEX(Hoja1!$B$2:$MO$7,1,E152)</f>
-        <v>0</v>
+        <v>229831</v>
       </c>
       <c r="G152">
         <f t="shared" si="70"/>
-        <v>-226596</v>
+        <v>3235</v>
       </c>
       <c r="H152" cm="1">
         <f t="array" ref="H152">+INDEX(Hoja1!$B$2:$MO$7,2,$E152)</f>
-        <v>0</v>
+        <v>159856</v>
       </c>
       <c r="I152">
         <f t="shared" si="71"/>
-        <v>-157706</v>
+        <v>2150</v>
       </c>
       <c r="J152">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>69975</v>
       </c>
       <c r="K152">
         <f t="shared" si="72"/>
-        <v>-68890</v>
+        <v>1085</v>
       </c>
       <c r="L152" cm="1">
         <f t="array" ref="L152">+INDEX(Hoja1!$B$2:$MO$7,3,$E152)</f>
-        <v>0</v>
+        <v>22806</v>
       </c>
       <c r="M152" cm="1">
         <f t="array" ref="M152">+INDEX(Hoja1!$B$2:$MO$7,4,$E152)</f>
-        <v>0</v>
+        <v>674</v>
       </c>
       <c r="N152" cm="1">
         <f t="array" ref="N152">+INDEX(Hoja1!$B$2:$MO$7,5,$E152)</f>
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="O152" cm="1">
         <f t="array" ref="O152">+INDEX(Hoja1!$B$2:$MO$7,6,$E152)</f>
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="P152" s="13">
         <f t="shared" si="89"/>
-        <v>0</v>
+        <v>0.69553715556213047</v>
       </c>
       <c r="Q152" s="13">
         <f t="shared" si="90"/>
-        <v>0</v>
+        <v>0.30446284443786958</v>
       </c>
       <c r="R152">
         <f t="shared" si="73"/>
-        <v>-230202</v>
+        <v>-371</v>
       </c>
       <c r="S152">
         <f t="shared" si="74"/>
-        <v>-68890</v>
+        <v>1085</v>
       </c>
       <c r="T152">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="U152">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="V152">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="W152">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X152">
         <f t="shared" si="79"/>
-        <v>-63.838602329450914</v>
+        <v>-0.10288408208541321</v>
       </c>
       <c r="Y152">
         <f t="shared" si="80"/>
-        <v>-1</v>
+        <v>1.5749745971839164E-2</v>
       </c>
       <c r="Z152">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>1.002770083102493</v>
       </c>
       <c r="AA152">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>1.0514820592823713</v>
       </c>
       <c r="AB152">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>0.9976976208749041</v>
       </c>
       <c r="AC152">
         <f t="shared" si="84"/>
-        <v>0</v>
+        <v>0.98795180722891562</v>
       </c>
       <c r="AD152">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>55261.120461649436</v>
       </c>
       <c r="AE152">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>16824.957922577545</v>
       </c>
       <c r="AF152">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>5483.5296946381341</v>
       </c>
       <c r="AG152">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>162.05818706419814</v>
       </c>
       <c r="AH152">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>312.57513825438809</v>
       </c>
       <c r="AI152">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>39.432555902861267</v>
       </c>
       <c r="AJ152">
         <f>+TODO_PACIENTES[[#This Row],[Aislamiento Domiciliario]]+TODO_PACIENTES[[#This Row],[Aislamiento en Hoteles]]+TODO_PACIENTES[[#This Row],[Hospitalizados en Sala]]+TODO_PACIENTES[[#This Row],[Hospitalizados en UCI]]</f>
-        <v>0</v>
+        <v>24944</v>
       </c>
       <c r="AK152">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>5997.5955758595819</v>
       </c>
       <c r="AL152">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ151</f>
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="AM152">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ151,0)</f>
-        <v>0</v>
+        <v>3.661529795195751E-3</v>
       </c>
     </row>
     <row r="153" spans="1:39" x14ac:dyDescent="0.2">
@@ -28273,7 +28293,7 @@
       </c>
       <c r="G153">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>-229831</v>
       </c>
       <c r="H153" cm="1">
         <f t="array" ref="H153">+INDEX(Hoja1!$B$2:$MO$7,2,$E153)</f>
@@ -28281,7 +28301,7 @@
       </c>
       <c r="I153">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>-159856</v>
       </c>
       <c r="J153">
         <f t="shared" si="62"/>
@@ -28289,7 +28309,7 @@
       </c>
       <c r="K153">
         <f t="shared" si="72"/>
-        <v>0</v>
+        <v>-69975</v>
       </c>
       <c r="L153" cm="1">
         <f t="array" ref="L153">+INDEX(Hoja1!$B$2:$MO$7,3,$E153)</f>
@@ -28317,35 +28337,35 @@
       </c>
       <c r="R153">
         <f t="shared" si="73"/>
-        <v>226596</v>
+        <v>-233066</v>
       </c>
       <c r="S153">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>-69975</v>
       </c>
       <c r="T153">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>-22806</v>
       </c>
       <c r="U153">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>-674</v>
       </c>
       <c r="V153">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>-1300</v>
       </c>
       <c r="W153">
         <f t="shared" si="78"/>
-        <v>0</v>
+        <v>-164</v>
       </c>
       <c r="X153">
         <f t="shared" si="79"/>
-        <v>-1</v>
+        <v>-72.045131375579601</v>
       </c>
       <c r="Y153">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z153">
         <f t="shared" si="81"/>
@@ -28397,11 +28417,11 @@
       </c>
       <c r="AL153">
         <f>+TODO_PACIENTES[[#This Row],[Personas con Medidas Sanitarias]]-AJ152</f>
-        <v>0</v>
+        <v>-24944</v>
       </c>
       <c r="AM153">
         <f>+IFERROR(TODO_PACIENTES[[#This Row],[Variación Personas Medidas Sanitarias]]/AJ152,0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="154" spans="1:39" x14ac:dyDescent="0.2">
@@ -28474,7 +28494,7 @@
       </c>
       <c r="R154">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>229831</v>
       </c>
       <c r="S154">
         <f t="shared" si="74"/>
@@ -28498,7 +28518,7 @@
       </c>
       <c r="X154">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y154">
         <f t="shared" si="80"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-04-2020 15-02-32
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,13 +10,13 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1794" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5DFD2064-3112-497A-B00C-01B680B33F0A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="TODO PACIENTES" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,14 +34,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -625,9 +627,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -715,9 +717,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -726,11 +728,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -739,7 +741,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="64">
     <dxf>
@@ -759,7 +761,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="0.0%"/>
+      <numFmt numFmtId="165" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <font>
@@ -778,13 +780,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="0.0%"/>
+      <numFmt numFmtId="165" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -863,184 +865,184 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1334,7 +1336,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1632,27 +1634,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B32E72-8F4B-408A-9B01-FAD2807C0C88}">
   <dimension ref="A1:ES52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="EE1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="EM20" sqref="EM20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="87" width="11.28515625" customWidth="1"/>
-    <col min="94" max="101" width="11.42578125" style="8"/>
-    <col min="102" max="103" width="11.42578125" style="15"/>
-    <col min="104" max="104" width="12.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="105" max="112" width="11.42578125" style="15"/>
-    <col min="113" max="113" width="11.42578125" style="8"/>
-    <col min="114" max="114" width="10" style="8" customWidth="1"/>
-    <col min="115" max="115" width="10.85546875" style="8" customWidth="1"/>
-    <col min="116" max="118" width="11.42578125" style="8"/>
+    <col min="1" max="1" width="26.09765625" customWidth="1"/>
+    <col min="2" max="87" width="11.296875" customWidth="1"/>
+    <col min="94" max="101" width="11.43359375" style="8"/>
+    <col min="102" max="103" width="11.43359375" style="15"/>
+    <col min="104" max="104" width="12.9140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="105" max="112" width="11.43359375" style="15"/>
+    <col min="113" max="113" width="11.43359375" style="8"/>
+    <col min="114" max="114" width="9.953125" style="8" customWidth="1"/>
+    <col min="115" max="115" width="10.89453125" style="8" customWidth="1"/>
+    <col min="116" max="118" width="11.43359375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2101,7 +2103,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2548,7 +2550,7 @@
       </c>
       <c r="ES2" s="8"/>
     </row>
-    <row r="3" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -2995,7 +2997,7 @@
       </c>
       <c r="ES3" s="8"/>
     </row>
-    <row r="4" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -3442,7 +3444,7 @@
       </c>
       <c r="ES4" s="8"/>
     </row>
-    <row r="5" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -3798,7 +3800,7 @@
       </c>
       <c r="ES5" s="8"/>
     </row>
-    <row r="6" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -4241,7 +4243,7 @@
       </c>
       <c r="ES6" s="8"/>
     </row>
-    <row r="7" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -4686,7 +4688,7 @@
       </c>
       <c r="ES7" s="8"/>
     </row>
-    <row r="8" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4810,46 +4812,46 @@
       <c r="EP8" s="8"/>
       <c r="EQ8" s="8"/>
     </row>
-    <row r="9" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:149" x14ac:dyDescent="0.2">
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:149" x14ac:dyDescent="0.2">
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:149" x14ac:dyDescent="0.2">
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:149" x14ac:dyDescent="0.2">
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:149" x14ac:dyDescent="0.2">
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:149" x14ac:dyDescent="0.2">
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:149" x14ac:dyDescent="0.2">
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:149" x14ac:dyDescent="0.2">
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W17" s="3"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W18" s="3"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W19" s="3"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W20" s="3"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W21" s="3"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -4872,52 +4874,52 @@
       <c r="T22" s="2"/>
       <c r="W22" s="3"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W23" s="3"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W24" s="3"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W25" s="4"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W26" s="4"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W27" s="4"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W28" s="4"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W29" s="4"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W30" s="4"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W31" s="4"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W32" s="4"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W33" s="4"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W34" s="4"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W35" s="1"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W36" s="1"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W37" s="1"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -4940,7 +4942,7 @@
       <c r="T38" s="2"/>
       <c r="W38" s="1"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -4963,7 +4965,7 @@
       <c r="T39" s="2"/>
       <c r="W39" s="1"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -4986,7 +4988,7 @@
       <c r="T40" s="2"/>
       <c r="W40" s="1"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -5009,7 +5011,7 @@
       <c r="T41" s="2"/>
       <c r="W41" s="1"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -5032,7 +5034,7 @@
       <c r="T42" s="2"/>
       <c r="W42" s="1"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -5055,7 +5057,7 @@
       <c r="T43" s="2"/>
       <c r="W43" s="1"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -5078,7 +5080,7 @@
       <c r="T44" s="2"/>
       <c r="W44" s="1"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -5101,7 +5103,7 @@
       <c r="T45" s="2"/>
       <c r="W45" s="1"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -5124,7 +5126,7 @@
       <c r="T46" s="2"/>
       <c r="W46" s="1"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -5147,7 +5149,7 @@
       <c r="T47" s="2"/>
       <c r="W47" s="3"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -5170,7 +5172,7 @@
       <c r="T48" s="2"/>
       <c r="W48" s="3"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -5193,7 +5195,7 @@
       <c r="T49" s="2"/>
       <c r="W49" s="3"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -5216,7 +5218,7 @@
       <c r="T50" s="2"/>
       <c r="W50" s="3"/>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -5239,7 +5241,7 @@
       <c r="T51" s="2"/>
       <c r="W51" s="3"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="W52" s="3"/>
     </row>
   </sheetData>
@@ -5258,54 +5260,54 @@
   </sheetPr>
   <dimension ref="A4:AM304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AL4" sqref="AL4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" customWidth="1"/>
-    <col min="16" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="12.7109375" customWidth="1"/>
-    <col min="23" max="23" width="10.85546875" customWidth="1"/>
-    <col min="24" max="24" width="10.42578125" customWidth="1"/>
-    <col min="25" max="25" width="10.85546875" customWidth="1"/>
-    <col min="26" max="30" width="14" customWidth="1"/>
-    <col min="31" max="32" width="11" customWidth="1"/>
-    <col min="33" max="33" width="11.7109375" customWidth="1"/>
-    <col min="34" max="34" width="12.28515625" customWidth="1"/>
-    <col min="35" max="35" width="12" customWidth="1"/>
-    <col min="37" max="37" width="13.5703125" customWidth="1"/>
-    <col min="38" max="38" width="13.28515625" customWidth="1"/>
-    <col min="39" max="39" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7.12890625" customWidth="1"/>
+    <col min="4" max="4" width="10.35546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.37890625" customWidth="1"/>
+    <col min="6" max="6" width="12.64453125" customWidth="1"/>
+    <col min="7" max="7" width="8.875" customWidth="1"/>
+    <col min="8" max="8" width="11.97265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.14453125" customWidth="1"/>
+    <col min="11" max="11" width="8.7421875" customWidth="1"/>
+    <col min="12" max="12" width="10.35546875" customWidth="1"/>
+    <col min="13" max="13" width="10.89453125" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" customWidth="1"/>
+    <col min="15" max="15" width="10.76171875" customWidth="1"/>
+    <col min="16" max="17" width="11.97265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.64453125" customWidth="1"/>
+    <col min="19" max="19" width="11.703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="12.64453125" customWidth="1"/>
+    <col min="23" max="23" width="10.89453125" customWidth="1"/>
+    <col min="24" max="24" width="10.35546875" customWidth="1"/>
+    <col min="25" max="25" width="10.89453125" customWidth="1"/>
+    <col min="26" max="30" width="13.98828125" customWidth="1"/>
+    <col min="31" max="32" width="11.02734375" customWidth="1"/>
+    <col min="33" max="33" width="11.703125" customWidth="1"/>
+    <col min="34" max="34" width="12.23828125" customWidth="1"/>
+    <col min="35" max="35" width="11.97265625" customWidth="1"/>
+    <col min="37" max="37" width="13.5859375" customWidth="1"/>
+    <col min="38" max="38" width="13.31640625" customWidth="1"/>
+    <col min="39" max="39" width="14.2578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
         <v>44046</v>
       </c>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:39" ht="48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>102</v>
       </c>
@@ -5424,7 +5426,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="str">
         <f>+IF(D7&gt;$D$4,"OUT TIME","ON")</f>
         <v>ON</v>
@@ -5512,7 +5514,7 @@
         <v>1.6830968982928589</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="str">
         <f t="shared" ref="A8:A9" si="0">+IF(D8&gt;$D$4,"OUT TIME","ON")</f>
         <v>ON</v>
@@ -5669,7 +5671,7 @@
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>ON</v>
@@ -5826,7 +5828,7 @@
         <v>1.3636363636363635</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="str">
         <f t="shared" ref="A10:A73" si="27">+IF(D10&gt;$D$4,"OUT TIME","ON")</f>
         <v>ON</v>
@@ -5983,7 +5985,7 @@
         <v>0.15384615384615385</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -6140,7 +6142,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -6297,7 +6299,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -6454,7 +6456,7 @@
         <v>0.25925925925925924</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -6611,7 +6613,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -6768,7 +6770,7 @@
         <v>0.27058823529411763</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -6925,7 +6927,7 @@
         <v>0.25925925925925924</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -7082,7 +7084,7 @@
         <v>0.46323529411764708</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -7239,7 +7241,7 @@
         <v>0.21608040201005024</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -7396,7 +7398,7 @@
         <v>0.29338842975206614</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -7553,7 +7555,7 @@
         <v>8.3067092651757185E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -7710,7 +7712,7 @@
         <v>0.28908554572271389</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -7867,7 +7869,7 @@
         <v>0.2585812356979405</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -8024,7 +8026,7 @@
         <v>0.20545454545454545</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -8181,7 +8183,7 @@
         <v>0.20361990950226244</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -8338,7 +8340,7 @@
         <v>0.10776942355889724</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -8495,7 +8497,7 @@
         <v>8.7104072398190041E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -8652,7 +8654,7 @@
         <v>4.7866805411030174E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -8809,7 +8811,7 @@
         <v>0.13406156901688182</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -8966,7 +8968,7 @@
         <v>0.11733800350262696</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -9123,7 +9125,7 @@
         <v>0.11912225705329153</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -9280,7 +9282,7 @@
         <v>0.13375350140056022</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -9437,7 +9439,7 @@
         <v>0.26003705991352688</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -9594,7 +9596,7 @@
         <v>6.4705882352941183E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -9751,7 +9753,7 @@
         <v>0.10082872928176796</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -9908,7 +9910,7 @@
         <v>6.775407779171895E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -10065,7 +10067,7 @@
         <v>-4.0736388562475516E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -10222,7 +10224,7 @@
         <v>9.0240914659044505E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -10379,7 +10381,7 @@
         <v>0.27827715355805244</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -10536,7 +10538,7 @@
         <v>8.5555230002929972E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -10693,7 +10695,7 @@
         <v>6.2078272604588397E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -10850,7 +10852,7 @@
         <v>-0.15705209656925032</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -11007,7 +11009,7 @@
         <v>0.24781429002110342</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -11164,7 +11166,7 @@
         <v>-0.13674800676491905</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -11321,7 +11323,7 @@
         <v>0.28547439126784213</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -11478,7 +11480,7 @@
         <v>-0.13520574787720444</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -11635,7 +11637,7 @@
         <v>1.0322255790533736E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -11792,7 +11794,7 @@
         <v>-0.41016695738848741</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -11949,7 +11951,7 @@
         <v>5.4921841994085341E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A49" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -12106,7 +12108,7 @@
         <v>0.78173808570284342</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -12263,7 +12265,7 @@
         <v>3.2366824005394472E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A51" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -12420,7 +12422,7 @@
         <v>3.3964728935336384E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -12577,7 +12579,7 @@
         <v>2.4426194988418616E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -12734,7 +12736,7 @@
         <v>3.6176772867420347E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -12891,7 +12893,7 @@
         <v>4.0468161079150959E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -13048,7 +13050,7 @@
         <v>2.9361296472831269E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A56" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -13205,7 +13207,7 @@
         <v>2.6115947397666234E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A57" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -13362,7 +13364,7 @@
         <v>2.4007220216606499E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A58" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -13519,7 +13521,7 @@
         <v>-0.42111757447558612</v>
       </c>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A59" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -13676,7 +13678,7 @@
         <v>4.2021924482338609E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -13833,7 +13835,7 @@
         <v>0.40736411455289306</v>
       </c>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A61" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -13990,7 +13992,7 @@
         <v>2.7408637873754152E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -14147,7 +14149,7 @@
         <v>1.5561843168957154E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A63" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -14304,7 +14306,7 @@
         <v>-0.21830845771144278</v>
       </c>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -14461,7 +14463,7 @@
         <v>2.6476578411405296E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A65" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -14618,7 +14620,7 @@
         <v>1.0912698412698412E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A66" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -14775,7 +14777,7 @@
         <v>5.9617271835132483E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A67" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -14932,7 +14934,7 @@
         <v>5.116925214169947E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A68" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -15089,7 +15091,7 @@
         <v>-5.9471365638766524E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A69" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -15246,7 +15248,7 @@
         <v>1.1079104808331486E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A70" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -15403,7 +15405,7 @@
         <v>-0.44444444444444442</v>
       </c>
     </row>
-    <row r="71" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A71" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -15560,7 +15562,7 @@
         <v>0.35219123505976097</v>
       </c>
     </row>
-    <row r="72" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A72" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -15717,7 +15719,7 @@
         <v>3.5651149086623452E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A73" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -15874,7 +15876,7 @@
         <v>4.2958748221906116E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A74" s="12" t="str">
         <f t="shared" ref="A74:A137" si="56">+IF(D74&gt;$D$4,"OUT TIME","ON")</f>
         <v>ON</v>
@@ -16031,7 +16033,7 @@
         <v>4.4189852700491E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A75" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -16188,7 +16190,7 @@
         <v>4.5454545454545456E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A76" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -16345,7 +16347,7 @@
         <v>2.6736631684157922E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A77" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -16502,7 +16504,7 @@
         <v>-8.5178875638841564E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A78" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -16659,7 +16661,7 @@
         <v>2.5036818851251842E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A79" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -16816,7 +16818,7 @@
         <v>1.2691570881226053E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A80" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -16973,7 +16975,7 @@
         <v>2.1045164341451879E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A81" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -17130,7 +17132,7 @@
         <v>0.61625752663270028</v>
       </c>
     </row>
-    <row r="82" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A82" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -17287,7 +17289,7 @@
         <v>-0.29345178392319815</v>
       </c>
     </row>
-    <row r="83" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A83" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -17444,7 +17446,7 @@
         <v>-6.8343135266680191E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A84" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -17601,7 +17603,7 @@
         <v>3.5045711797997391E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A85" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -17758,7 +17760,7 @@
         <v>-0.1516298633017876</v>
       </c>
     </row>
-    <row r="86" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A86" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -17915,7 +17917,7 @@
         <v>9.8661378284581061E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A87" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -18072,7 +18074,7 @@
         <v>5.257220216606498E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A88" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -18229,7 +18231,7 @@
         <v>-0.29817792068595927</v>
       </c>
     </row>
-    <row r="89" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A89" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -18386,7 +18388,7 @@
         <v>0.10354306658521686</v>
       </c>
     </row>
-    <row r="90" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A90" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -18543,7 +18545,7 @@
         <v>0.1013008580127318</v>
       </c>
     </row>
-    <row r="91" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A91" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -18700,7 +18702,7 @@
         <v>6.2829856747926613E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A92" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -18857,7 +18859,7 @@
         <v>0.11917711042799717</v>
       </c>
     </row>
-    <row r="93" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A93" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -19014,7 +19016,7 @@
         <v>6.9511937460384532E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A94" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -19171,7 +19173,7 @@
         <v>6.1635717107862503E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A95" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -19328,7 +19330,7 @@
         <v>2.3446222553033122E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A96" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -19485,7 +19487,7 @@
         <v>5.7090909090909088E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A97" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -19642,7 +19644,7 @@
         <v>4.1451668386652908E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A98" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -19799,7 +19801,7 @@
         <v>3.5342691990090831E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A99" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -19956,7 +19958,7 @@
         <v>3.6688467060137182E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A100" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -20113,7 +20115,7 @@
         <v>9.1090937067241112E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A101" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -20270,7 +20272,7 @@
         <v>-0.2905090960372303</v>
       </c>
     </row>
-    <row r="102" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A102" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -20427,7 +20429,7 @@
         <v>0.16696481812760883</v>
       </c>
     </row>
-    <row r="103" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A103" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -20584,7 +20586,7 @@
         <v>0.10424118548799183</v>
       </c>
     </row>
-    <row r="104" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A104" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -20741,7 +20743,7 @@
         <v>0.11183094246490823</v>
       </c>
     </row>
-    <row r="105" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A105" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -20898,7 +20900,7 @@
         <v>7.2558268590455055E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A106" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -21055,7 +21057,7 @@
         <v>8.0455309791747504E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A107" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -21212,7 +21214,7 @@
         <v>8.8710642882796606E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A108" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -21369,7 +21371,7 @@
         <v>3.6947437871123819E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A109" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -21526,7 +21528,7 @@
         <v>9.9681866383881226E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A110" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -21683,7 +21685,7 @@
         <v>7.7145612343297976E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A111" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -21840,7 +21842,7 @@
         <v>3.5541629364368846E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A112" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -21997,7 +21999,7 @@
         <v>4.469611826748509E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A113" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -22154,7 +22156,7 @@
         <v>4.932141674942072E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A114" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -22311,7 +22313,7 @@
         <v>7.8312302839116721E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A115" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -22468,7 +22470,7 @@
         <v>2.8303956702991295E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A116" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -22625,7 +22627,7 @@
         <v>4.5234708392603129E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A117" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -22782,7 +22784,7 @@
         <v>6.2329885683179098E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A118" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -22939,7 +22941,7 @@
         <v>6.1363054060978736E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A119" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -23096,7 +23098,7 @@
         <v>3.645141822570911E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A120" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -23253,7 +23255,7 @@
         <v>4.0701059741469661E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A121" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -23410,7 +23412,7 @@
         <v>1.4099479662060091E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A122" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -23567,7 +23569,7 @@
         <v>1.2524137931034483E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A123" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -23724,7 +23726,7 @@
         <v>8.1734960767218829E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A124" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -23881,7 +23883,7 @@
         <v>4.9400064857853206E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A125" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -24038,7 +24040,7 @@
         <v>5.727235269880511E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A126" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -24195,7 +24197,7 @@
         <v>1.1593920498830864E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A127" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -24352,7 +24354,7 @@
         <v>9.4866608879899828E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A128" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -24509,7 +24511,7 @@
         <v>-1.0971712064112961E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A129" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -24666,7 +24668,7 @@
         <v>1.3371537726838587E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A130" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -24823,7 +24825,7 @@
         <v>1.4355207935902328E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A131" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -24980,7 +24982,7 @@
         <v>1.9558982556772769E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A132" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -25137,7 +25139,7 @@
         <v>2.9375144108830988E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A133" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -25294,7 +25296,7 @@
         <v>6.5854314129558285E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A134" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -25451,7 +25453,7 @@
         <v>1.6689661311139792E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A135" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -25608,7 +25610,7 @@
         <v>3.0073542286814917E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A136" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -25765,7 +25767,7 @@
         <v>1.3556584930517189E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A137" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -25922,7 +25924,7 @@
         <v>-6.4570230607966456E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A138" s="12" t="str">
         <f t="shared" ref="A138:A201" si="85">+IF(D138&gt;$D$4,"OUT TIME","ON")</f>
         <v>ON</v>
@@ -26079,7 +26081,7 @@
         <v>8.1870357866306552E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A139" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -26236,7 +26238,7 @@
         <v>1.0255336961071579E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A140" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -26393,7 +26395,7 @@
         <v>-8.9496581727781226E-3</v>
       </c>
     </row>
-    <row r="141" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A141" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -26550,7 +26552,7 @@
         <v>-1.3169446883230905E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A142" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -26707,7 +26709,7 @@
         <v>7.456363328249449E-3</v>
       </c>
     </row>
-    <row r="143" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A143" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -26864,7 +26866,7 @@
         <v>1.0891505466778806E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A144" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -27021,7 +27023,7 @@
         <v>5.0750863180664754E-3</v>
       </c>
     </row>
-    <row r="145" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A145" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -27178,7 +27180,7 @@
         <v>2.9386200902280536E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A146" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -27335,7 +27337,7 @@
         <v>6.5538176993285352E-3</v>
       </c>
     </row>
-    <row r="147" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A147" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -27492,7 +27494,7 @@
         <v>-1.3621474794279779E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A148" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -27649,7 +27651,7 @@
         <v>-4.6166929899161702E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A149" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -27806,7 +27808,7 @@
         <v>-1.2205541315757354E-4</v>
       </c>
     </row>
-    <row r="150" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A150" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -27963,7 +27965,7 @@
         <v>3.7841796875E-3</v>
       </c>
     </row>
-    <row r="151" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A151" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -28120,7 +28122,7 @@
         <v>7.4587539016579517E-3</v>
       </c>
     </row>
-    <row r="152" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A152" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -28277,7 +28279,7 @@
         <v>3.661529795195751E-3</v>
       </c>
     </row>
-    <row r="153" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A153" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -28434,7 +28436,7 @@
         <v>-3.1270044900577293E-3</v>
       </c>
     </row>
-    <row r="154" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A154" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -28591,7 +28593,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="155" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A155" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -28748,7 +28750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A156" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -28905,7 +28907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A157" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -29062,7 +29064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A158" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -29219,7 +29221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A159" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -29376,7 +29378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A160" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -29533,7 +29535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A161" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -29690,7 +29692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A162" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -29847,7 +29849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A163" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -30004,7 +30006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A164" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -30161,7 +30163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A165" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -30318,7 +30320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A166" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -30475,7 +30477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A167" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -30632,7 +30634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A168" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -30789,7 +30791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A169" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -30946,7 +30948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A170" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -31103,7 +31105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A171" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -31260,7 +31262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A172" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -31417,7 +31419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A173" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -31574,7 +31576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A174" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -31731,7 +31733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A175" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -31888,7 +31890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A176" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -32045,7 +32047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A177" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -32202,7 +32204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A178" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -32359,7 +32361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A179" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -32516,7 +32518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A180" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -32673,7 +32675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A181" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -32830,7 +32832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A182" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -32987,7 +32989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A183" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -33144,7 +33146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A184" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -33301,7 +33303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A185" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -33458,7 +33460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A186" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -33615,7 +33617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A187" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -33772,7 +33774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A188" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -33929,7 +33931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A189" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -34086,7 +34088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A190" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -34243,7 +34245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A191" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -34400,7 +34402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A192" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -34557,7 +34559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A193" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -34714,7 +34716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A194" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -34871,7 +34873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A195" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -35028,7 +35030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A196" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -35185,7 +35187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A197" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -35342,7 +35344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A198" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -35499,7 +35501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A199" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -35656,7 +35658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A200" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -35813,7 +35815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A201" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -35970,7 +35972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A202" s="12" t="str">
         <f t="shared" ref="A202:A265" si="114">+IF(D202&gt;$D$4,"OUT TIME","ON")</f>
         <v>OUT TIME</v>
@@ -36127,7 +36129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A203" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -36284,7 +36286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A204" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -36441,7 +36443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A205" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -36598,7 +36600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A206" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -36755,7 +36757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A207" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -36912,7 +36914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A208" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -37069,7 +37071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A209" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -37226,7 +37228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A210" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -37383,7 +37385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A211" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -37540,7 +37542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A212" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -37697,7 +37699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A213" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -37854,7 +37856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A214" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -38011,7 +38013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A215" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -38168,7 +38170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A216" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -38325,7 +38327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A217" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -38482,7 +38484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A218" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -38639,7 +38641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A219" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -38796,7 +38798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A220" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -38953,7 +38955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A221" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -39110,7 +39112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A222" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -39267,7 +39269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A223" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -39424,7 +39426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A224" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -39581,7 +39583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A225" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -39738,7 +39740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A226" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -39895,7 +39897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A227" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -40052,7 +40054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A228" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -40209,7 +40211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A229" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -40366,7 +40368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A230" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -40523,7 +40525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A231" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -40680,7 +40682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A232" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -40837,7 +40839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A233" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -40994,7 +40996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A234" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -41151,7 +41153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A235" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -41308,7 +41310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A236" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -41465,7 +41467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A237" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -41622,7 +41624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A238" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -41779,7 +41781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A239" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -41936,7 +41938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A240" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -42093,7 +42095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A241" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -42250,7 +42252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A242" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -42407,7 +42409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A243" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -42564,7 +42566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A244" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -42721,7 +42723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A245" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -42878,7 +42880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A246" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -43035,7 +43037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A247" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -43192,7 +43194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A248" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -43349,7 +43351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A249" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -43506,7 +43508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A250" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -43663,7 +43665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A251" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -43820,7 +43822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A252" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -43977,7 +43979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A253" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -44134,7 +44136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A254" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -44291,7 +44293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A255" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -44448,7 +44450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A256" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -44605,7 +44607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A257" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -44762,7 +44764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A258" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -44919,7 +44921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A259" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -45076,7 +45078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A260" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -45233,7 +45235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A261" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -45390,7 +45392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A262" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -45547,7 +45549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A263" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -45704,7 +45706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A264" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -45861,7 +45863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A265" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -46018,7 +46020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A266" s="12" t="str">
         <f t="shared" ref="A266:A303" si="143">+IF(D266&gt;$D$4,"OUT TIME","ON")</f>
         <v>OUT TIME</v>
@@ -46175,7 +46177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A267" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -46332,7 +46334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A268" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -46489,7 +46491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A269" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -46646,7 +46648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A270" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -46803,7 +46805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A271" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -46960,7 +46962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A272" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -47117,7 +47119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A273" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -47274,7 +47276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A274" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -47431,7 +47433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A275" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -47588,7 +47590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A276" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -47745,7 +47747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A277" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -47902,7 +47904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A278" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -48059,7 +48061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A279" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -48216,7 +48218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A280" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -48373,7 +48375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A281" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -48530,7 +48532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A282" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -48687,7 +48689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A283" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -48844,7 +48846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A284" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -49001,7 +49003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A285" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -49158,7 +49160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A286" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -49315,7 +49317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A287" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -49472,7 +49474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A288" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -49629,7 +49631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A289" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -49786,7 +49788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A290" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -49943,7 +49945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A291" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -50100,7 +50102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A292" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -50257,7 +50259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A293" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -50414,7 +50416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A294" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -50571,7 +50573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A295" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -50728,7 +50730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A296" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -50885,7 +50887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A297" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -51042,7 +51044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A298" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -51199,7 +51201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A299" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -51356,7 +51358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A300" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -51513,7 +51515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A301" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -51670,7 +51672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A302" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -51827,7 +51829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A303" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -51984,7 +51986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A304" s="12"/>
       <c r="B304" s="12"/>
       <c r="C304" s="12"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-04-2020 23-03-59
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1794" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5DFD2064-3112-497A-B00C-01B680B33F0A}"/>
+  <xr:revisionPtr revIDLastSave="1796" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{25C071D4-CF1E-4A80-BD72-24927DE78522}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="TODO PACIENTES" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -346,123 +346,6 @@
     <t>12-06-2020</t>
   </si>
   <si>
-    <t>Pruebas Realizadas</t>
-  </si>
-  <si>
-    <t>Pruebas Negativas</t>
-  </si>
-  <si>
-    <t>Aislamiento Domiciliario</t>
-  </si>
-  <si>
-    <t>Aislamiento en Hoteles</t>
-  </si>
-  <si>
-    <t>Hospitalizados en Sala</t>
-  </si>
-  <si>
-    <t>Hospitalizados en UCI</t>
-  </si>
-  <si>
-    <t>ON</t>
-  </si>
-  <si>
-    <t>Ultimo</t>
-  </si>
-  <si>
-    <t>Indice</t>
-  </si>
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t>DIA</t>
-  </si>
-  <si>
-    <t>Pruebas Diarias</t>
-  </si>
-  <si>
-    <t>Pruebas Negativas Diarias</t>
-  </si>
-  <si>
-    <t>Pruebas Positivas</t>
-  </si>
-  <si>
-    <t>Pruebas Positivas Diarias</t>
-  </si>
-  <si>
-    <t>%Pruebas Negativas</t>
-  </si>
-  <si>
-    <t>%Pruebas Positivas</t>
-  </si>
-  <si>
-    <t>Variación Pruebas Positivas</t>
-  </si>
-  <si>
-    <t>Variación Pruebas Realizadas</t>
-  </si>
-  <si>
-    <t>Variación Aislamiento Domiciliario</t>
-  </si>
-  <si>
-    <t>Variación Aislamiento Hoteles</t>
-  </si>
-  <si>
-    <t>Variación Hospitalizados en Sala</t>
-  </si>
-  <si>
-    <t>Variación Hospitalizados en UCI</t>
-  </si>
-  <si>
-    <t>Pruebas Realizadas/1MM hab</t>
-  </si>
-  <si>
-    <t>Pruebas Positivas/1MM hab</t>
-  </si>
-  <si>
-    <t>%Variación Pruebas Realizadas</t>
-  </si>
-  <si>
-    <t>%Variación Pruebas Positivas</t>
-  </si>
-  <si>
-    <t>%Variación Aislamiento Domiciliario</t>
-  </si>
-  <si>
-    <t>%Variación Aislamiento Hoteles</t>
-  </si>
-  <si>
-    <t>%Variación Hospitalizados en Sala</t>
-  </si>
-  <si>
-    <t>%Variación Hospitalizados en UCI</t>
-  </si>
-  <si>
-    <t>Aislamiento Domiciliario/1MM hab</t>
-  </si>
-  <si>
-    <t>Aislamiento Hoteles/1MM hab</t>
-  </si>
-  <si>
-    <t>Hospitalizados en Sala/1MM hab</t>
-  </si>
-  <si>
-    <t>Hospitalizados en UCI/1MM hab</t>
-  </si>
-  <si>
-    <t>Personas con Medidas Sanitarias</t>
-  </si>
-  <si>
-    <t>Variación Personas Medidas Sanitarias</t>
-  </si>
-  <si>
-    <t>Personas Medidas Sanitarias/1MM hab</t>
-  </si>
-  <si>
-    <t>%Variación Personas Medidas Sanitarias</t>
-  </si>
-  <si>
     <t>13-06-20</t>
   </si>
   <si>
@@ -621,17 +504,134 @@
   <si>
     <t>04-08-2020</t>
   </si>
+  <si>
+    <t>Pruebas Realizadas</t>
+  </si>
+  <si>
+    <t>Pruebas Negativas</t>
+  </si>
+  <si>
+    <t>Aislamiento Domiciliario</t>
+  </si>
+  <si>
+    <t>Aislamiento en Hoteles</t>
+  </si>
+  <si>
+    <t>Hospitalizados en Sala</t>
+  </si>
+  <si>
+    <t>Hospitalizados en UCI</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>Ultimo</t>
+  </si>
+  <si>
+    <t>Indice</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>DIA</t>
+  </si>
+  <si>
+    <t>Pruebas Diarias</t>
+  </si>
+  <si>
+    <t>Pruebas Negativas Diarias</t>
+  </si>
+  <si>
+    <t>Pruebas Positivas</t>
+  </si>
+  <si>
+    <t>Pruebas Positivas Diarias</t>
+  </si>
+  <si>
+    <t>%Pruebas Negativas</t>
+  </si>
+  <si>
+    <t>%Pruebas Positivas</t>
+  </si>
+  <si>
+    <t>Variación Pruebas Realizadas</t>
+  </si>
+  <si>
+    <t>Variación Pruebas Positivas</t>
+  </si>
+  <si>
+    <t>Variación Aislamiento Domiciliario</t>
+  </si>
+  <si>
+    <t>Variación Aislamiento Hoteles</t>
+  </si>
+  <si>
+    <t>Variación Hospitalizados en Sala</t>
+  </si>
+  <si>
+    <t>Variación Hospitalizados en UCI</t>
+  </si>
+  <si>
+    <t>%Variación Pruebas Realizadas</t>
+  </si>
+  <si>
+    <t>%Variación Pruebas Positivas</t>
+  </si>
+  <si>
+    <t>%Variación Aislamiento Domiciliario</t>
+  </si>
+  <si>
+    <t>%Variación Aislamiento Hoteles</t>
+  </si>
+  <si>
+    <t>%Variación Hospitalizados en Sala</t>
+  </si>
+  <si>
+    <t>%Variación Hospitalizados en UCI</t>
+  </si>
+  <si>
+    <t>Pruebas Realizadas/1MM hab</t>
+  </si>
+  <si>
+    <t>Pruebas Positivas/1MM hab</t>
+  </si>
+  <si>
+    <t>Aislamiento Domiciliario/1MM hab</t>
+  </si>
+  <si>
+    <t>Aislamiento Hoteles/1MM hab</t>
+  </si>
+  <si>
+    <t>Hospitalizados en Sala/1MM hab</t>
+  </si>
+  <si>
+    <t>Hospitalizados en UCI/1MM hab</t>
+  </si>
+  <si>
+    <t>Personas con Medidas Sanitarias</t>
+  </si>
+  <si>
+    <t>Personas Medidas Sanitarias/1MM hab</t>
+  </si>
+  <si>
+    <t>Variación Personas Medidas Sanitarias</t>
+  </si>
+  <si>
+    <t>%Variación Personas Medidas Sanitarias</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -717,9 +717,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -728,11 +728,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -741,7 +741,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="64">
     <dxf>
@@ -761,7 +761,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
+      <numFmt numFmtId="166" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <font>
@@ -780,13 +780,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="0.0%"/>
+      <numFmt numFmtId="166" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="167" formatCode="d/m/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -865,184 +865,184 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1634,27 +1634,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B32E72-8F4B-408A-9B01-FAD2807C0C88}">
   <dimension ref="A1:ES52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="EE1" activePane="topRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="FH2" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="EM20" sqref="EM20"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="EM20" sqref="EM20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.09765625" customWidth="1"/>
-    <col min="2" max="87" width="11.296875" customWidth="1"/>
-    <col min="94" max="101" width="11.43359375" style="8"/>
-    <col min="102" max="103" width="11.43359375" style="15"/>
-    <col min="104" max="104" width="12.9140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="105" max="112" width="11.43359375" style="15"/>
-    <col min="113" max="113" width="11.43359375" style="8"/>
-    <col min="114" max="114" width="9.953125" style="8" customWidth="1"/>
-    <col min="115" max="115" width="10.89453125" style="8" customWidth="1"/>
-    <col min="116" max="118" width="11.43359375" style="8"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="87" width="11.28515625" customWidth="1"/>
+    <col min="94" max="101" width="11.42578125" style="8"/>
+    <col min="102" max="103" width="11.42578125" style="15"/>
+    <col min="104" max="104" width="12.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="105" max="112" width="11.42578125" style="15"/>
+    <col min="113" max="113" width="11.42578125" style="8"/>
+    <col min="114" max="114" width="10" style="8" customWidth="1"/>
+    <col min="115" max="115" width="10.85546875" style="8" customWidth="1"/>
+    <col min="116" max="118" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:149">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1944,168 +1944,168 @@
         <v>95</v>
       </c>
       <c r="CS1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="CT1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="CU1" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="CV1" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="CW1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="CX1" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="CY1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="CZ1" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="DA1" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="DB1" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="DC1" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="DD1" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="DE1" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="DF1" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="DG1" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="DH1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="DI1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="DJ1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="DK1" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="DL1" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="DM1" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="DN1" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="DO1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="DP1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="DR1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="DS1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="DT1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DU1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DV1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="DW1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="DX1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="DY1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="DZ1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="EA1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="EB1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="EC1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="ED1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="EE1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="EF1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="CT1" s="8" t="s">
+      <c r="EG1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="CU1" s="8" t="s">
+      <c r="EH1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="CV1" s="8" t="s">
+      <c r="EI1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="CW1" s="8" t="s">
+      <c r="EJ1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="CX1" s="15" t="s">
+      <c r="EK1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="CY1" s="16" t="s">
+      <c r="EL1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="CZ1" s="16" t="s">
+      <c r="EM1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="DA1" s="16" t="s">
+      <c r="EN1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="DB1" s="16" t="s">
+      <c r="EO1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="DC1" s="16" t="s">
+      <c r="EP1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="DD1" s="16" t="s">
+      <c r="EQ1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="DE1" s="16" t="s">
+      <c r="ER1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="DF1" s="16" t="s">
+      <c r="ES1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="DG1" s="16" t="s">
+    </row>
+    <row r="2" spans="1:149">
+      <c r="A2" t="s">
         <v>149</v>
-      </c>
-      <c r="DH1" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="DI1" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="DJ1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="DK1" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="DL1" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="DM1" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="DN1" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="DO1" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="DP1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="DQ1" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="DR1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="DS1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="DT1" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="DU1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="DV1" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="DW1" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="DX1" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="DY1" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="DZ1" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="EA1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="EB1" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="EC1" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="ED1" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="EE1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="EF1" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="EG1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="EH1" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="EI1" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="EJ1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="EK1" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="EL1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="EM1" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="EN1" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="EO1" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="EP1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="EQ1" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="ER1" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="ES1" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:149" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>96</v>
       </c>
       <c r="B2" s="7">
         <v>146</v>
@@ -2550,9 +2550,9 @@
       </c>
       <c r="ES2" s="8"/>
     </row>
-    <row r="3" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:149">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>150</v>
       </c>
       <c r="B3" s="7">
         <v>138</v>
@@ -2997,9 +2997,9 @@
       </c>
       <c r="ES3" s="8"/>
     </row>
-    <row r="4" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:149">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>151</v>
       </c>
       <c r="B4" s="7">
         <v>6</v>
@@ -3444,9 +3444,9 @@
       </c>
       <c r="ES4" s="8"/>
     </row>
-    <row r="5" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:149">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>152</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -3800,9 +3800,9 @@
       </c>
       <c r="ES5" s="8"/>
     </row>
-    <row r="6" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:149">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>153</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -4243,9 +4243,9 @@
       </c>
       <c r="ES6" s="8"/>
     </row>
-    <row r="7" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:149">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -4688,7 +4688,7 @@
       </c>
       <c r="ES7" s="8"/>
     </row>
-    <row r="8" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:149">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4812,46 +4812,46 @@
       <c r="EP8" s="8"/>
       <c r="EQ8" s="8"/>
     </row>
-    <row r="9" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:149">
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:149">
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:149">
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:149">
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:149">
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:149">
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:149">
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:149">
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23">
       <c r="W17" s="3"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23">
       <c r="W18" s="3"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23">
       <c r="W19" s="3"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23">
       <c r="W20" s="3"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23">
       <c r="W21" s="3"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -4874,52 +4874,52 @@
       <c r="T22" s="2"/>
       <c r="W22" s="3"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23">
       <c r="W23" s="3"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23">
       <c r="W24" s="3"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23">
       <c r="W25" s="4"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23">
       <c r="W26" s="4"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23">
       <c r="W27" s="4"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23">
       <c r="W28" s="4"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23">
       <c r="W29" s="4"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23">
       <c r="W30" s="4"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23">
       <c r="W31" s="4"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23">
       <c r="W32" s="4"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23">
       <c r="W33" s="4"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23">
       <c r="W34" s="4"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23">
       <c r="W35" s="1"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23">
       <c r="W36" s="1"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23">
       <c r="W37" s="1"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -4942,7 +4942,7 @@
       <c r="T38" s="2"/>
       <c r="W38" s="1"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -4965,7 +4965,7 @@
       <c r="T39" s="2"/>
       <c r="W39" s="1"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -4988,7 +4988,7 @@
       <c r="T40" s="2"/>
       <c r="W40" s="1"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -5011,7 +5011,7 @@
       <c r="T41" s="2"/>
       <c r="W41" s="1"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -5034,7 +5034,7 @@
       <c r="T42" s="2"/>
       <c r="W42" s="1"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -5057,7 +5057,7 @@
       <c r="T43" s="2"/>
       <c r="W43" s="1"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -5080,7 +5080,7 @@
       <c r="T44" s="2"/>
       <c r="W44" s="1"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -5103,7 +5103,7 @@
       <c r="T45" s="2"/>
       <c r="W45" s="1"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -5126,7 +5126,7 @@
       <c r="T46" s="2"/>
       <c r="W46" s="1"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -5149,7 +5149,7 @@
       <c r="T47" s="2"/>
       <c r="W47" s="3"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -5172,7 +5172,7 @@
       <c r="T48" s="2"/>
       <c r="W48" s="3"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -5195,7 +5195,7 @@
       <c r="T49" s="2"/>
       <c r="W49" s="3"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -5218,7 +5218,7 @@
       <c r="T50" s="2"/>
       <c r="W50" s="3"/>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -5241,7 +5241,7 @@
       <c r="T51" s="2"/>
       <c r="W51" s="3"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23">
       <c r="W52" s="3"/>
     </row>
   </sheetData>
@@ -5260,173 +5260,173 @@
   </sheetPr>
   <dimension ref="A4:AM304"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AL4" sqref="AL4"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AJ7" sqref="AJ7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="7.12890625" customWidth="1"/>
-    <col min="4" max="4" width="10.35546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.37890625" customWidth="1"/>
-    <col min="6" max="6" width="12.64453125" customWidth="1"/>
-    <col min="7" max="7" width="8.875" customWidth="1"/>
-    <col min="8" max="8" width="11.97265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.14453125" customWidth="1"/>
-    <col min="11" max="11" width="8.7421875" customWidth="1"/>
-    <col min="12" max="12" width="10.35546875" customWidth="1"/>
-    <col min="13" max="13" width="10.89453125" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" customWidth="1"/>
-    <col min="15" max="15" width="10.76171875" customWidth="1"/>
-    <col min="16" max="17" width="11.97265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.64453125" customWidth="1"/>
-    <col min="19" max="19" width="11.703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="12.64453125" customWidth="1"/>
-    <col min="23" max="23" width="10.89453125" customWidth="1"/>
-    <col min="24" max="24" width="10.35546875" customWidth="1"/>
-    <col min="25" max="25" width="10.89453125" customWidth="1"/>
-    <col min="26" max="30" width="13.98828125" customWidth="1"/>
-    <col min="31" max="32" width="11.02734375" customWidth="1"/>
-    <col min="33" max="33" width="11.703125" customWidth="1"/>
-    <col min="34" max="34" width="12.23828125" customWidth="1"/>
-    <col min="35" max="35" width="11.97265625" customWidth="1"/>
-    <col min="37" max="37" width="13.5859375" customWidth="1"/>
-    <col min="38" max="38" width="13.31640625" customWidth="1"/>
-    <col min="39" max="39" width="14.2578125" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="12.7109375" customWidth="1"/>
+    <col min="23" max="23" width="10.85546875" customWidth="1"/>
+    <col min="24" max="24" width="10.28515625" customWidth="1"/>
+    <col min="25" max="25" width="10.85546875" customWidth="1"/>
+    <col min="26" max="30" width="14" customWidth="1"/>
+    <col min="31" max="32" width="11" customWidth="1"/>
+    <col min="33" max="33" width="11.7109375" customWidth="1"/>
+    <col min="34" max="34" width="12.28515625" customWidth="1"/>
+    <col min="35" max="35" width="12" customWidth="1"/>
+    <col min="37" max="37" width="13.5703125" customWidth="1"/>
+    <col min="38" max="38" width="13.28515625" customWidth="1"/>
+    <col min="39" max="39" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39">
       <c r="D4" s="9">
         <f>+D7+COUNTA(Hoja1!$C$2:$MO$2)</f>
         <v>44046</v>
       </c>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39">
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:39" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" ht="56.25">
       <c r="A6" s="14" t="s">
-        <v>102</v>
+        <v>155</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>103</v>
+        <v>156</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>104</v>
+        <v>157</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>105</v>
+        <v>158</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>106</v>
+        <v>159</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>96</v>
+        <v>149</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>107</v>
+        <v>160</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>97</v>
+        <v>150</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>109</v>
+        <v>162</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>110</v>
+        <v>163</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>98</v>
+        <v>151</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>99</v>
+        <v>152</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>100</v>
+        <v>153</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>111</v>
+        <v>164</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>112</v>
+        <v>165</v>
       </c>
       <c r="R6" s="14" t="s">
-        <v>114</v>
+        <v>166</v>
       </c>
       <c r="S6" s="14" t="s">
-        <v>113</v>
+        <v>167</v>
       </c>
       <c r="T6" s="14" t="s">
-        <v>115</v>
+        <v>168</v>
       </c>
       <c r="U6" s="14" t="s">
-        <v>116</v>
+        <v>169</v>
       </c>
       <c r="V6" s="14" t="s">
-        <v>117</v>
+        <v>170</v>
       </c>
       <c r="W6" s="14" t="s">
-        <v>118</v>
+        <v>171</v>
       </c>
       <c r="X6" s="14" t="s">
-        <v>121</v>
+        <v>172</v>
       </c>
       <c r="Y6" s="14" t="s">
-        <v>122</v>
+        <v>173</v>
       </c>
       <c r="Z6" s="14" t="s">
-        <v>123</v>
+        <v>174</v>
       </c>
       <c r="AA6" s="14" t="s">
-        <v>124</v>
+        <v>175</v>
       </c>
       <c r="AB6" s="14" t="s">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="AC6" s="14" t="s">
-        <v>126</v>
+        <v>177</v>
       </c>
       <c r="AD6" s="14" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
       <c r="AE6" s="14" t="s">
-        <v>120</v>
+        <v>179</v>
       </c>
       <c r="AF6" s="14" t="s">
-        <v>127</v>
+        <v>180</v>
       </c>
       <c r="AG6" s="14" t="s">
-        <v>128</v>
+        <v>181</v>
       </c>
       <c r="AH6" s="14" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="AI6" s="14" t="s">
-        <v>130</v>
+        <v>183</v>
       </c>
       <c r="AJ6" s="14" t="s">
-        <v>131</v>
+        <v>184</v>
       </c>
       <c r="AK6" s="14" t="s">
-        <v>133</v>
+        <v>185</v>
       </c>
       <c r="AL6" s="14" t="s">
-        <v>132</v>
+        <v>186</v>
       </c>
       <c r="AM6" s="14" t="s">
-        <v>134</v>
+        <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39">
       <c r="A7" s="12" t="str">
         <f>+IF(D7&gt;$D$4,"OUT TIME","ON")</f>
         <v>ON</v>
@@ -5514,7 +5514,7 @@
         <v>1.6830968982928589</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39">
       <c r="A8" s="12" t="str">
         <f t="shared" ref="A8:A9" si="0">+IF(D8&gt;$D$4,"OUT TIME","ON")</f>
         <v>ON</v>
@@ -5671,7 +5671,7 @@
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39">
       <c r="A9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>ON</v>
@@ -5828,7 +5828,7 @@
         <v>1.3636363636363635</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39">
       <c r="A10" s="12" t="str">
         <f t="shared" ref="A10:A73" si="27">+IF(D10&gt;$D$4,"OUT TIME","ON")</f>
         <v>ON</v>
@@ -5985,7 +5985,7 @@
         <v>0.15384615384615385</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39">
       <c r="A11" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -6142,7 +6142,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39">
       <c r="A12" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -6299,7 +6299,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39">
       <c r="A13" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -6456,7 +6456,7 @@
         <v>0.25925925925925924</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:39">
       <c r="A14" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -6613,7 +6613,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:39">
       <c r="A15" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -6770,7 +6770,7 @@
         <v>0.27058823529411763</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39">
       <c r="A16" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -6927,7 +6927,7 @@
         <v>0.25925925925925924</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:39">
       <c r="A17" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -7084,7 +7084,7 @@
         <v>0.46323529411764708</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:39">
       <c r="A18" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -7241,7 +7241,7 @@
         <v>0.21608040201005024</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:39">
       <c r="A19" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -7398,7 +7398,7 @@
         <v>0.29338842975206614</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:39">
       <c r="A20" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -7555,7 +7555,7 @@
         <v>8.3067092651757185E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:39">
       <c r="A21" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -7712,7 +7712,7 @@
         <v>0.28908554572271389</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:39">
       <c r="A22" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -7869,7 +7869,7 @@
         <v>0.2585812356979405</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:39">
       <c r="A23" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -8026,7 +8026,7 @@
         <v>0.20545454545454545</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:39">
       <c r="A24" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -8183,7 +8183,7 @@
         <v>0.20361990950226244</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:39">
       <c r="A25" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -8340,7 +8340,7 @@
         <v>0.10776942355889724</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:39">
       <c r="A26" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -8497,7 +8497,7 @@
         <v>8.7104072398190041E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:39">
       <c r="A27" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -8654,7 +8654,7 @@
         <v>4.7866805411030174E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:39">
       <c r="A28" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -8811,7 +8811,7 @@
         <v>0.13406156901688182</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:39">
       <c r="A29" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -8968,7 +8968,7 @@
         <v>0.11733800350262696</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:39">
       <c r="A30" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -9125,7 +9125,7 @@
         <v>0.11912225705329153</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:39">
       <c r="A31" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -9282,7 +9282,7 @@
         <v>0.13375350140056022</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:39">
       <c r="A32" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -9439,7 +9439,7 @@
         <v>0.26003705991352688</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:39">
       <c r="A33" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -9596,7 +9596,7 @@
         <v>6.4705882352941183E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:39">
       <c r="A34" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -9753,7 +9753,7 @@
         <v>0.10082872928176796</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:39">
       <c r="A35" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -9910,7 +9910,7 @@
         <v>6.775407779171895E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:39">
       <c r="A36" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -10067,7 +10067,7 @@
         <v>-4.0736388562475516E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:39">
       <c r="A37" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -10224,7 +10224,7 @@
         <v>9.0240914659044505E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:39">
       <c r="A38" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -10381,7 +10381,7 @@
         <v>0.27827715355805244</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:39">
       <c r="A39" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -10538,7 +10538,7 @@
         <v>8.5555230002929972E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:39">
       <c r="A40" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -10695,7 +10695,7 @@
         <v>6.2078272604588397E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:39">
       <c r="A41" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -10852,7 +10852,7 @@
         <v>-0.15705209656925032</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:39">
       <c r="A42" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -11009,7 +11009,7 @@
         <v>0.24781429002110342</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:39">
       <c r="A43" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -11166,7 +11166,7 @@
         <v>-0.13674800676491905</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:39">
       <c r="A44" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -11323,7 +11323,7 @@
         <v>0.28547439126784213</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:39">
       <c r="A45" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -11480,7 +11480,7 @@
         <v>-0.13520574787720444</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:39">
       <c r="A46" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -11637,7 +11637,7 @@
         <v>1.0322255790533736E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:39">
       <c r="A47" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -11794,7 +11794,7 @@
         <v>-0.41016695738848741</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:39">
       <c r="A48" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -11951,7 +11951,7 @@
         <v>5.4921841994085341E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:39">
       <c r="A49" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -12108,7 +12108,7 @@
         <v>0.78173808570284342</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:39">
       <c r="A50" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -12265,7 +12265,7 @@
         <v>3.2366824005394472E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:39">
       <c r="A51" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -12422,7 +12422,7 @@
         <v>3.3964728935336384E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:39">
       <c r="A52" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -12579,7 +12579,7 @@
         <v>2.4426194988418616E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:39">
       <c r="A53" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -12736,7 +12736,7 @@
         <v>3.6176772867420347E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:39">
       <c r="A54" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -12893,7 +12893,7 @@
         <v>4.0468161079150959E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:39">
       <c r="A55" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -13050,7 +13050,7 @@
         <v>2.9361296472831269E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:39">
       <c r="A56" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -13207,7 +13207,7 @@
         <v>2.6115947397666234E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:39">
       <c r="A57" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -13364,7 +13364,7 @@
         <v>2.4007220216606499E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:39">
       <c r="A58" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -13521,7 +13521,7 @@
         <v>-0.42111757447558612</v>
       </c>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:39">
       <c r="A59" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -13678,7 +13678,7 @@
         <v>4.2021924482338609E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:39">
       <c r="A60" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -13835,7 +13835,7 @@
         <v>0.40736411455289306</v>
       </c>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:39">
       <c r="A61" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -13992,7 +13992,7 @@
         <v>2.7408637873754152E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:39">
       <c r="A62" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -14149,7 +14149,7 @@
         <v>1.5561843168957154E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:39">
       <c r="A63" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -14306,7 +14306,7 @@
         <v>-0.21830845771144278</v>
       </c>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:39">
       <c r="A64" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -14463,7 +14463,7 @@
         <v>2.6476578411405296E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:39">
       <c r="A65" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -14620,7 +14620,7 @@
         <v>1.0912698412698412E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:39">
       <c r="A66" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -14777,7 +14777,7 @@
         <v>5.9617271835132483E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:39">
       <c r="A67" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -14934,7 +14934,7 @@
         <v>5.116925214169947E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:39">
       <c r="A68" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -15091,7 +15091,7 @@
         <v>-5.9471365638766524E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:39">
       <c r="A69" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -15248,7 +15248,7 @@
         <v>1.1079104808331486E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:39">
       <c r="A70" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -15405,7 +15405,7 @@
         <v>-0.44444444444444442</v>
       </c>
     </row>
-    <row r="71" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:39">
       <c r="A71" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -15562,7 +15562,7 @@
         <v>0.35219123505976097</v>
       </c>
     </row>
-    <row r="72" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:39">
       <c r="A72" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -15719,7 +15719,7 @@
         <v>3.5651149086623452E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:39">
       <c r="A73" s="12" t="str">
         <f t="shared" si="27"/>
         <v>ON</v>
@@ -15876,7 +15876,7 @@
         <v>4.2958748221906116E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:39">
       <c r="A74" s="12" t="str">
         <f t="shared" ref="A74:A137" si="56">+IF(D74&gt;$D$4,"OUT TIME","ON")</f>
         <v>ON</v>
@@ -16033,7 +16033,7 @@
         <v>4.4189852700491E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:39">
       <c r="A75" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -16190,7 +16190,7 @@
         <v>4.5454545454545456E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:39">
       <c r="A76" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -16347,7 +16347,7 @@
         <v>2.6736631684157922E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:39">
       <c r="A77" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -16504,7 +16504,7 @@
         <v>-8.5178875638841564E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:39">
       <c r="A78" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -16661,7 +16661,7 @@
         <v>2.5036818851251842E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:39">
       <c r="A79" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -16818,7 +16818,7 @@
         <v>1.2691570881226053E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:39">
       <c r="A80" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -16975,7 +16975,7 @@
         <v>2.1045164341451879E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:39">
       <c r="A81" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -17132,7 +17132,7 @@
         <v>0.61625752663270028</v>
       </c>
     </row>
-    <row r="82" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:39">
       <c r="A82" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -17289,7 +17289,7 @@
         <v>-0.29345178392319815</v>
       </c>
     </row>
-    <row r="83" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:39">
       <c r="A83" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -17446,7 +17446,7 @@
         <v>-6.8343135266680191E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:39">
       <c r="A84" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -17603,7 +17603,7 @@
         <v>3.5045711797997391E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:39">
       <c r="A85" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -17760,7 +17760,7 @@
         <v>-0.1516298633017876</v>
       </c>
     </row>
-    <row r="86" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:39">
       <c r="A86" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -17917,7 +17917,7 @@
         <v>9.8661378284581061E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:39">
       <c r="A87" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -18074,7 +18074,7 @@
         <v>5.257220216606498E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:39">
       <c r="A88" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -18231,7 +18231,7 @@
         <v>-0.29817792068595927</v>
       </c>
     </row>
-    <row r="89" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:39">
       <c r="A89" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -18388,7 +18388,7 @@
         <v>0.10354306658521686</v>
       </c>
     </row>
-    <row r="90" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:39">
       <c r="A90" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -18545,7 +18545,7 @@
         <v>0.1013008580127318</v>
       </c>
     </row>
-    <row r="91" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:39">
       <c r="A91" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -18702,7 +18702,7 @@
         <v>6.2829856747926613E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:39">
       <c r="A92" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -18859,7 +18859,7 @@
         <v>0.11917711042799717</v>
       </c>
     </row>
-    <row r="93" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:39">
       <c r="A93" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -19016,7 +19016,7 @@
         <v>6.9511937460384532E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:39">
       <c r="A94" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -19173,7 +19173,7 @@
         <v>6.1635717107862503E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:39">
       <c r="A95" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -19330,7 +19330,7 @@
         <v>2.3446222553033122E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:39">
       <c r="A96" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -19487,7 +19487,7 @@
         <v>5.7090909090909088E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:39">
       <c r="A97" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -19644,7 +19644,7 @@
         <v>4.1451668386652908E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:39">
       <c r="A98" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -19801,7 +19801,7 @@
         <v>3.5342691990090831E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:39">
       <c r="A99" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -19958,7 +19958,7 @@
         <v>3.6688467060137182E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:39">
       <c r="A100" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -20115,7 +20115,7 @@
         <v>9.1090937067241112E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:39">
       <c r="A101" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -20272,7 +20272,7 @@
         <v>-0.2905090960372303</v>
       </c>
     </row>
-    <row r="102" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:39">
       <c r="A102" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -20429,7 +20429,7 @@
         <v>0.16696481812760883</v>
       </c>
     </row>
-    <row r="103" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:39">
       <c r="A103" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -20586,7 +20586,7 @@
         <v>0.10424118548799183</v>
       </c>
     </row>
-    <row r="104" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:39">
       <c r="A104" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -20743,7 +20743,7 @@
         <v>0.11183094246490823</v>
       </c>
     </row>
-    <row r="105" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:39">
       <c r="A105" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -20900,7 +20900,7 @@
         <v>7.2558268590455055E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:39">
       <c r="A106" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -21057,7 +21057,7 @@
         <v>8.0455309791747504E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:39">
       <c r="A107" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -21214,7 +21214,7 @@
         <v>8.8710642882796606E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:39">
       <c r="A108" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -21371,7 +21371,7 @@
         <v>3.6947437871123819E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:39">
       <c r="A109" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -21528,7 +21528,7 @@
         <v>9.9681866383881226E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:39">
       <c r="A110" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -21685,7 +21685,7 @@
         <v>7.7145612343297976E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:39">
       <c r="A111" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -21842,7 +21842,7 @@
         <v>3.5541629364368846E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:39">
       <c r="A112" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -21999,7 +21999,7 @@
         <v>4.469611826748509E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:39">
       <c r="A113" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -22156,7 +22156,7 @@
         <v>4.932141674942072E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:39">
       <c r="A114" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -22313,7 +22313,7 @@
         <v>7.8312302839116721E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:39">
       <c r="A115" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -22470,7 +22470,7 @@
         <v>2.8303956702991295E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:39">
       <c r="A116" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -22627,7 +22627,7 @@
         <v>4.5234708392603129E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:39">
       <c r="A117" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -22784,7 +22784,7 @@
         <v>6.2329885683179098E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:39">
       <c r="A118" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -22941,7 +22941,7 @@
         <v>6.1363054060978736E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:39">
       <c r="A119" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -23098,7 +23098,7 @@
         <v>3.645141822570911E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:39">
       <c r="A120" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -23255,7 +23255,7 @@
         <v>4.0701059741469661E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:39">
       <c r="A121" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -23412,7 +23412,7 @@
         <v>1.4099479662060091E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:39">
       <c r="A122" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -23569,7 +23569,7 @@
         <v>1.2524137931034483E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:39">
       <c r="A123" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -23726,7 +23726,7 @@
         <v>8.1734960767218829E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:39">
       <c r="A124" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -23883,7 +23883,7 @@
         <v>4.9400064857853206E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:39">
       <c r="A125" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -24040,7 +24040,7 @@
         <v>5.727235269880511E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:39">
       <c r="A126" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -24197,7 +24197,7 @@
         <v>1.1593920498830864E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:39">
       <c r="A127" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -24354,7 +24354,7 @@
         <v>9.4866608879899828E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:39">
       <c r="A128" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -24511,7 +24511,7 @@
         <v>-1.0971712064112961E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:39">
       <c r="A129" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -24668,7 +24668,7 @@
         <v>1.3371537726838587E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:39">
       <c r="A130" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -24825,7 +24825,7 @@
         <v>1.4355207935902328E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:39">
       <c r="A131" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -24982,7 +24982,7 @@
         <v>1.9558982556772769E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:39">
       <c r="A132" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -25139,7 +25139,7 @@
         <v>2.9375144108830988E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:39">
       <c r="A133" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -25296,7 +25296,7 @@
         <v>6.5854314129558285E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:39">
       <c r="A134" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -25453,7 +25453,7 @@
         <v>1.6689661311139792E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:39">
       <c r="A135" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -25610,7 +25610,7 @@
         <v>3.0073542286814917E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:39">
       <c r="A136" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -25767,7 +25767,7 @@
         <v>1.3556584930517189E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:39">
       <c r="A137" s="12" t="str">
         <f t="shared" si="56"/>
         <v>ON</v>
@@ -25924,7 +25924,7 @@
         <v>-6.4570230607966456E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:39">
       <c r="A138" s="12" t="str">
         <f t="shared" ref="A138:A201" si="85">+IF(D138&gt;$D$4,"OUT TIME","ON")</f>
         <v>ON</v>
@@ -26081,7 +26081,7 @@
         <v>8.1870357866306552E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:39">
       <c r="A139" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -26238,7 +26238,7 @@
         <v>1.0255336961071579E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:39">
       <c r="A140" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -26395,7 +26395,7 @@
         <v>-8.9496581727781226E-3</v>
       </c>
     </row>
-    <row r="141" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:39">
       <c r="A141" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -26552,7 +26552,7 @@
         <v>-1.3169446883230905E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:39">
       <c r="A142" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -26709,7 +26709,7 @@
         <v>7.456363328249449E-3</v>
       </c>
     </row>
-    <row r="143" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:39">
       <c r="A143" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -26866,7 +26866,7 @@
         <v>1.0891505466778806E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:39">
       <c r="A144" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -27023,7 +27023,7 @@
         <v>5.0750863180664754E-3</v>
       </c>
     </row>
-    <row r="145" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:39">
       <c r="A145" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -27180,7 +27180,7 @@
         <v>2.9386200902280536E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:39">
       <c r="A146" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -27337,7 +27337,7 @@
         <v>6.5538176993285352E-3</v>
       </c>
     </row>
-    <row r="147" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:39">
       <c r="A147" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -27494,7 +27494,7 @@
         <v>-1.3621474794279779E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:39">
       <c r="A148" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -27651,7 +27651,7 @@
         <v>-4.6166929899161702E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:39">
       <c r="A149" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -27808,7 +27808,7 @@
         <v>-1.2205541315757354E-4</v>
       </c>
     </row>
-    <row r="150" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:39">
       <c r="A150" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -27965,7 +27965,7 @@
         <v>3.7841796875E-3</v>
       </c>
     </row>
-    <row r="151" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:39">
       <c r="A151" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -28122,7 +28122,7 @@
         <v>7.4587539016579517E-3</v>
       </c>
     </row>
-    <row r="152" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:39">
       <c r="A152" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -28279,7 +28279,7 @@
         <v>3.661529795195751E-3</v>
       </c>
     </row>
-    <row r="153" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:39">
       <c r="A153" s="12" t="str">
         <f t="shared" si="85"/>
         <v>ON</v>
@@ -28436,7 +28436,7 @@
         <v>-3.1270044900577293E-3</v>
       </c>
     </row>
-    <row r="154" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:39">
       <c r="A154" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -28593,7 +28593,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="155" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:39">
       <c r="A155" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -28750,7 +28750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:39">
       <c r="A156" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -28907,7 +28907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:39">
       <c r="A157" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -29064,7 +29064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:39">
       <c r="A158" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -29221,7 +29221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:39">
       <c r="A159" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -29378,7 +29378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:39">
       <c r="A160" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -29535,7 +29535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:39">
       <c r="A161" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -29692,7 +29692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:39">
       <c r="A162" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -29849,7 +29849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:39">
       <c r="A163" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -30006,7 +30006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:39">
       <c r="A164" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -30163,7 +30163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:39">
       <c r="A165" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -30320,7 +30320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:39">
       <c r="A166" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -30477,7 +30477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:39">
       <c r="A167" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -30634,7 +30634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:39">
       <c r="A168" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -30791,7 +30791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:39">
       <c r="A169" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -30948,7 +30948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:39">
       <c r="A170" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -31105,7 +31105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:39">
       <c r="A171" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -31262,7 +31262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:39">
       <c r="A172" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -31419,7 +31419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:39">
       <c r="A173" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -31576,7 +31576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:39">
       <c r="A174" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -31733,7 +31733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:39">
       <c r="A175" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -31890,7 +31890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:39">
       <c r="A176" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -32047,7 +32047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:39">
       <c r="A177" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -32204,7 +32204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:39">
       <c r="A178" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -32361,7 +32361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:39">
       <c r="A179" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -32518,7 +32518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:39">
       <c r="A180" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -32675,7 +32675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:39">
       <c r="A181" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -32832,7 +32832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:39">
       <c r="A182" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -32989,7 +32989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:39">
       <c r="A183" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -33146,7 +33146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:39">
       <c r="A184" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -33303,7 +33303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:39">
       <c r="A185" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -33460,7 +33460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:39">
       <c r="A186" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -33617,7 +33617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:39">
       <c r="A187" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -33774,7 +33774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:39">
       <c r="A188" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -33931,7 +33931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:39">
       <c r="A189" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -34088,7 +34088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:39">
       <c r="A190" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -34245,7 +34245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:39">
       <c r="A191" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -34402,7 +34402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:39">
       <c r="A192" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -34559,7 +34559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:39">
       <c r="A193" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -34716,7 +34716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:39">
       <c r="A194" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -34873,7 +34873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:39">
       <c r="A195" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -35030,7 +35030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:39">
       <c r="A196" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -35187,7 +35187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:39">
       <c r="A197" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -35344,7 +35344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:39">
       <c r="A198" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -35501,7 +35501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:39">
       <c r="A199" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -35658,7 +35658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:39">
       <c r="A200" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -35815,7 +35815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:39">
       <c r="A201" s="12" t="str">
         <f t="shared" si="85"/>
         <v>OUT TIME</v>
@@ -35972,7 +35972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:39">
       <c r="A202" s="12" t="str">
         <f t="shared" ref="A202:A265" si="114">+IF(D202&gt;$D$4,"OUT TIME","ON")</f>
         <v>OUT TIME</v>
@@ -36129,7 +36129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:39">
       <c r="A203" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -36286,7 +36286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:39">
       <c r="A204" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -36443,7 +36443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:39">
       <c r="A205" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -36600,7 +36600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:39">
       <c r="A206" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -36757,7 +36757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:39">
       <c r="A207" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -36914,7 +36914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:39">
       <c r="A208" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -37071,7 +37071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:39">
       <c r="A209" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -37228,7 +37228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:39">
       <c r="A210" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -37385,7 +37385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:39">
       <c r="A211" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -37542,7 +37542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:39">
       <c r="A212" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -37699,7 +37699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:39">
       <c r="A213" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -37856,7 +37856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:39">
       <c r="A214" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -38013,7 +38013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:39">
       <c r="A215" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -38170,7 +38170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:39">
       <c r="A216" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -38327,7 +38327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:39">
       <c r="A217" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -38484,7 +38484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:39">
       <c r="A218" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -38641,7 +38641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:39">
       <c r="A219" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -38798,7 +38798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:39">
       <c r="A220" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -38955,7 +38955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:39">
       <c r="A221" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -39112,7 +39112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:39">
       <c r="A222" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -39269,7 +39269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:39">
       <c r="A223" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -39426,7 +39426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:39">
       <c r="A224" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -39583,7 +39583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:39">
       <c r="A225" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -39740,7 +39740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:39">
       <c r="A226" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -39897,7 +39897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:39">
       <c r="A227" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -40054,7 +40054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:39">
       <c r="A228" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -40211,7 +40211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:39">
       <c r="A229" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -40368,7 +40368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:39">
       <c r="A230" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -40525,7 +40525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:39">
       <c r="A231" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -40682,7 +40682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:39">
       <c r="A232" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -40839,7 +40839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:39">
       <c r="A233" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -40996,7 +40996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:39">
       <c r="A234" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -41153,7 +41153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:39">
       <c r="A235" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -41310,7 +41310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:39">
       <c r="A236" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -41467,7 +41467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:39">
       <c r="A237" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -41624,7 +41624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:39">
       <c r="A238" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -41781,7 +41781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:39">
       <c r="A239" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -41938,7 +41938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:39">
       <c r="A240" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -42095,7 +42095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:39">
       <c r="A241" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -42252,7 +42252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:39">
       <c r="A242" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -42409,7 +42409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:39">
       <c r="A243" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -42566,7 +42566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:39">
       <c r="A244" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -42723,7 +42723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:39">
       <c r="A245" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -42880,7 +42880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:39">
       <c r="A246" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -43037,7 +43037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:39">
       <c r="A247" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -43194,7 +43194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:39">
       <c r="A248" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -43351,7 +43351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:39">
       <c r="A249" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -43508,7 +43508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:39">
       <c r="A250" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -43665,7 +43665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:39">
       <c r="A251" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -43822,7 +43822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:39">
       <c r="A252" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -43979,7 +43979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:39">
       <c r="A253" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -44136,7 +44136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:39">
       <c r="A254" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -44293,7 +44293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:39">
       <c r="A255" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -44450,7 +44450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:39">
       <c r="A256" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -44607,7 +44607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:39">
       <c r="A257" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -44764,7 +44764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:39">
       <c r="A258" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -44921,7 +44921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:39">
       <c r="A259" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -45078,7 +45078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:39">
       <c r="A260" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -45235,7 +45235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:39">
       <c r="A261" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -45392,7 +45392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:39">
       <c r="A262" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -45549,7 +45549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:39">
       <c r="A263" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -45706,7 +45706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:39">
       <c r="A264" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -45863,7 +45863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:39">
       <c r="A265" s="12" t="str">
         <f t="shared" si="114"/>
         <v>OUT TIME</v>
@@ -46020,7 +46020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:39">
       <c r="A266" s="12" t="str">
         <f t="shared" ref="A266:A303" si="143">+IF(D266&gt;$D$4,"OUT TIME","ON")</f>
         <v>OUT TIME</v>
@@ -46177,7 +46177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:39">
       <c r="A267" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -46334,7 +46334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:39">
       <c r="A268" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -46491,7 +46491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:39">
       <c r="A269" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -46648,7 +46648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:39">
       <c r="A270" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -46805,7 +46805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:39">
       <c r="A271" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -46962,7 +46962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:39">
       <c r="A272" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -47119,7 +47119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:39">
       <c r="A273" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -47276,7 +47276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:39">
       <c r="A274" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -47433,7 +47433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:39">
       <c r="A275" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -47590,7 +47590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:39">
       <c r="A276" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -47747,7 +47747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:39">
       <c r="A277" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -47904,7 +47904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:39">
       <c r="A278" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -48061,7 +48061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:39">
       <c r="A279" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -48218,7 +48218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:39">
       <c r="A280" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -48375,7 +48375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:39">
       <c r="A281" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -48532,7 +48532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:39">
       <c r="A282" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -48689,7 +48689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:39">
       <c r="A283" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -48846,7 +48846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:39">
       <c r="A284" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -49003,7 +49003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:39">
       <c r="A285" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -49160,7 +49160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:39">
       <c r="A286" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -49317,7 +49317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:39">
       <c r="A287" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -49474,7 +49474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:39">
       <c r="A288" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -49631,7 +49631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:39">
       <c r="A289" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -49788,7 +49788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:39">
       <c r="A290" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -49945,7 +49945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:39">
       <c r="A291" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -50102,7 +50102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:39">
       <c r="A292" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -50259,7 +50259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:39">
       <c r="A293" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -50416,7 +50416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:39">
       <c r="A294" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -50573,7 +50573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:39">
       <c r="A295" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -50730,7 +50730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:39">
       <c r="A296" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -50887,7 +50887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:39">
       <c r="A297" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -51044,7 +51044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:39">
       <c r="A298" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -51201,7 +51201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:39">
       <c r="A299" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -51358,7 +51358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:39">
       <c r="A300" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -51515,7 +51515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:39">
       <c r="A301" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -51672,7 +51672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:39">
       <c r="A302" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -51829,7 +51829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:39">
       <c r="A303" s="12" t="str">
         <f t="shared" si="143"/>
         <v>OUT TIME</v>
@@ -51986,7 +51986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:39">
       <c r="A304" s="12"/>
       <c r="B304" s="12"/>
       <c r="C304" s="12"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-05-2020 03-04-49
</commit_message>
<xml_diff>
--- a/datacovidpa/Condición_Pacientes PN.xlsx
+++ b/datacovidpa/Condición_Pacientes PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1796" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{25C071D4-CF1E-4A80-BD72-24927DE78522}"/>
+  <xr:revisionPtr revIDLastSave="1798" documentId="8_{EB53E55E-EEC3-4F21-8E7D-52E27AC5BA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E5F6CBEE-C44A-4710-AB54-9D5AD93B30D4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{2AF9DF2C-A2C8-45B1-80FF-162E42031A82}"/>
   </bookViews>
@@ -5260,8 +5260,8 @@
   </sheetPr>
   <dimension ref="A4:AM304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AJ7" sqref="AJ7"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AN8" sqref="AN8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -5307,7 +5307,7 @@
     <row r="5" spans="1:39">
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:39" ht="56.25">
+    <row r="6" spans="1:39" ht="60">
       <c r="A6" s="14" t="s">
         <v>155</v>
       </c>

</xml_diff>